<commit_message>
add sync var example
</commit_message>
<xml_diff>
--- a/Task_Result.xlsx
+++ b/Task_Result.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\beetech\java\stage1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A36AD92-93E1-4FE9-9F97-B1D422CD0035}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAE1C9DB-3032-4186-AAB9-108DA247DCD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,17 +16,28 @@
     <sheet name="day2 " sheetId="1" r:id="rId1"/>
     <sheet name="day3" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="55">
   <si>
     <t>STT</t>
   </si>
@@ -182,6 +193,34 @@
   </si>
   <si>
     <t>Với chương trình trên thì ta thấy được khi 1 "Bank Account" được nhiều ngườidùng cùng "withdraw" or "deposit" cùng 1 thời điểm nhờ có  "method synchronized" đã không còn sự bất đồng bộ (tránh tình trạng nhiều người cùng rút tại 1 thời điểm dẫn tới sai lệch số tiền)</t>
+  </si>
+  <si>
+    <t>thread</t>
+  </si>
+  <si>
+    <t>mutilthread</t>
+  </si>
+  <si>
+    <t>là một đối tượng trong Java được sử dụng để thực hiện nhiều tác vụ cùng một lúc. 
+Mỗi thread đại diện cho một luồng thực thi độc lập trong chương trình. Khi một chương trình Java được thực thi, nó sẽ tạo ra ít nhất một thread - thread chính, còn được gọi là main thread. Các thread khác có thể được tạo ra từ main thread hoặc từ một thread khác để thực hiện các tác vụ cụ thể, giúp chương trình có thể thực hiện nhiều tác vụ đồng thời và nhanh chóng hơn.</t>
+  </si>
+  <si>
+    <t>là kỹ thuật lập trình cho phép chương trình có thể thực hiện đồng thời nhiều tác vụ khác nhau trong một thời điểm. 
+Nó cho phép một chương trình được phân chia thành các phần nhỏ và chạy đồng thời trên nhiều luồng (threads) khác nhau để cải thiện hiệu năng và tăng khả năng đáp ứng của chương trình. Khi sử dụng multithreading, một chương trình có thể thực hiện nhiều tác vụ cùng lúc, giúp tăng tốc độ xử lý và giảm thời gian phản hồi của chương trình.</t>
+  </si>
+  <si>
+    <t>là một biến đồng bộ hóa trong Java, được sử dụng để đảm bảo rằng chỉ có một luồng có thể truy cập vào biến đó cùng một lúc. 
+Nếu một luồng đang sử dụng biến synchronized, các luồng khác phải chờ đợi cho đến khi luồng đang sử dụng kết thúc và giải phóng biến synchronized trước khi truy cập vào nó. Việc sử dụng biến synchronized giúp đảm bảo tính đúng đắn và tránh được các tình huống đua nhau (race condition) trong quá trình thực thi đa luồng.</t>
+  </si>
+  <si>
+    <t>https://www.baeldung.com/java-synchronized#4-reentrancy</t>
+  </si>
+  <si>
+    <t>Sự kiểm chứng cho biến synchronized</t>
+  </si>
+  <si>
+    <t>Như có thể thấy thì khi thay đối tượng đại diện cho 2 phương thức thì có kết quả khác nhau. 
+Vậy khi 2 phương thức có đối tượng đại diện khác nhau sẽ dẫn tới hiện tượng bất đồng bộ</t>
   </si>
 </sst>
 </file>
@@ -253,7 +292,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -285,21 +324,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -325,6 +355,28 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -337,38 +389,40 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -524,8 +578,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="20266" y="3658005"/>
-          <a:ext cx="7557986" cy="5369263"/>
+          <a:off x="20266" y="3462476"/>
+          <a:ext cx="7568494" cy="5411296"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -648,6 +702,128 @@
         <a:xfrm>
           <a:off x="81642" y="10736035"/>
           <a:ext cx="7866289" cy="3924300"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>6164036</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>81643</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>12246</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>2792186</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Picture 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BBC6DC59-7923-68A4-D695-EBC49F584EC2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="8477250" y="1020536"/>
+          <a:ext cx="7713889" cy="5105400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>367393</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>54429</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>5729968</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>2694215</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Picture 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{98D4A44F-C5E2-485F-A563-BE344F2CE2B6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="367393" y="993322"/>
+          <a:ext cx="7675789" cy="5034643"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -950,27 +1126,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="16:22" x14ac:dyDescent="0.25">
-      <c r="P1" s="12" t="s">
+      <c r="P1" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="Q1" s="13"/>
-      <c r="R1" s="13"/>
-      <c r="S1" s="13"/>
-      <c r="T1" s="13"/>
+      <c r="Q1" s="21"/>
+      <c r="R1" s="21"/>
+      <c r="S1" s="21"/>
+      <c r="T1" s="21"/>
     </row>
     <row r="2" spans="16:22" x14ac:dyDescent="0.25">
-      <c r="P2" s="13"/>
-      <c r="Q2" s="13"/>
-      <c r="R2" s="13"/>
-      <c r="S2" s="13"/>
-      <c r="T2" s="13"/>
+      <c r="P2" s="21"/>
+      <c r="Q2" s="21"/>
+      <c r="R2" s="21"/>
+      <c r="S2" s="21"/>
+      <c r="T2" s="21"/>
     </row>
     <row r="3" spans="16:22" x14ac:dyDescent="0.25">
-      <c r="P3" s="14"/>
-      <c r="Q3" s="14"/>
-      <c r="R3" s="14"/>
-      <c r="S3" s="14"/>
-      <c r="T3" s="14"/>
+      <c r="P3" s="22"/>
+      <c r="Q3" s="22"/>
+      <c r="R3" s="22"/>
+      <c r="S3" s="22"/>
+      <c r="T3" s="22"/>
     </row>
     <row r="4" spans="16:22" x14ac:dyDescent="0.25">
       <c r="P4" s="7" t="s">
@@ -979,11 +1155,11 @@
       <c r="Q4" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="R4" s="11" t="s">
+      <c r="R4" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="S4" s="11"/>
-      <c r="T4" s="11"/>
+      <c r="S4" s="19"/>
+      <c r="T4" s="19"/>
       <c r="U4" s="7" t="s">
         <v>18</v>
       </c>
@@ -1157,10 +1333,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25977106-C04A-4BDF-83D6-AA6BE76B6728}">
-  <dimension ref="A1:K70"/>
+  <dimension ref="A1:N70"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="54" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M46" sqref="M46"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1169,285 +1345,300 @@
     <col min="3" max="3" width="127.140625" customWidth="1"/>
     <col min="4" max="4" width="71.7109375" customWidth="1"/>
     <col min="10" max="10" width="24.85546875" customWidth="1"/>
+    <col min="11" max="11" width="39.140625" customWidth="1"/>
+    <col min="12" max="12" width="72.140625" customWidth="1"/>
+    <col min="13" max="13" width="74.7109375" customWidth="1"/>
+    <col min="14" max="14" width="82.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:14" ht="74.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="34" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="L1" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="M1" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="N1" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
-    </row>
-    <row r="2" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="A2" s="3">
+    </row>
+    <row r="2" spans="1:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="32"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="K2" s="3">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="L2" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="M2" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="N2" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
-      <c r="I2" s="17"/>
-      <c r="J2" s="17"/>
-    </row>
-    <row r="3" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
+    </row>
+    <row r="3" spans="1:14" ht="90" x14ac:dyDescent="0.25">
+      <c r="A3" s="14"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="17"/>
+      <c r="K3" s="3">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="L3" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="M3" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="D3" s="16" t="s">
+      <c r="N3" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="17"/>
-      <c r="I3" s="17"/>
-      <c r="J3" s="17"/>
-    </row>
-    <row r="4" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
+    </row>
+    <row r="4" spans="1:14" ht="75" x14ac:dyDescent="0.25">
+      <c r="A4" s="14"/>
+      <c r="B4" s="15"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="18"/>
+      <c r="K4" s="3">
         <v>3</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="L4" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="M4" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="D4" s="15" t="s">
+      <c r="N4" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="17"/>
-      <c r="H4" s="17"/>
-      <c r="I4" s="17"/>
-      <c r="J4" s="17"/>
-    </row>
-    <row r="5" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
+    </row>
+    <row r="5" spans="1:14" ht="238.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="14"/>
+      <c r="B5" s="15"/>
+      <c r="C5" s="16"/>
+      <c r="D5" s="18"/>
+      <c r="K5" s="3">
         <v>4</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="L5" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="M5" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="D5" s="15" t="s">
+      <c r="N5" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="E5" s="17"/>
-      <c r="F5" s="17"/>
-      <c r="G5" s="17"/>
-      <c r="H5" s="17"/>
-      <c r="I5" s="17"/>
-      <c r="J5" s="17"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
+    </row>
+    <row r="6" spans="1:14" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="35" t="s">
+        <v>54</v>
+      </c>
+      <c r="B6" s="29"/>
+      <c r="C6" s="29"/>
+      <c r="D6" s="29"/>
+      <c r="E6" s="29"/>
+      <c r="K6" s="3">
         <v>5</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="L6" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="17"/>
-      <c r="G6" s="17"/>
-      <c r="H6" s="17"/>
-      <c r="I6" s="17"/>
-      <c r="J6" s="17"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M6" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="N6" s="9" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="6.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="25" t="s">
         <v>42</v>
       </c>
       <c r="B7" s="25"/>
       <c r="C7" s="25"/>
-      <c r="D7" s="26" t="s">
+      <c r="D7" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="E7" s="27"/>
-      <c r="F7" s="27"/>
-      <c r="G7" s="27"/>
-      <c r="H7" s="27"/>
-      <c r="I7" s="27"/>
-      <c r="J7" s="27"/>
-      <c r="K7" s="20"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="26"/>
-      <c r="B8" s="26"/>
-      <c r="C8" s="26"/>
-      <c r="D8" s="27"/>
-      <c r="E8" s="27"/>
-      <c r="F8" s="27"/>
-      <c r="G8" s="27"/>
-      <c r="H8" s="27"/>
-      <c r="I8" s="27"/>
-      <c r="J8" s="27"/>
-      <c r="K8" s="20"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="17"/>
-      <c r="B9" s="17"/>
-      <c r="C9" s="17"/>
-      <c r="D9" s="20"/>
-      <c r="E9" s="20"/>
-      <c r="F9" s="20"/>
-      <c r="G9" s="20"/>
-      <c r="H9" s="20"/>
-      <c r="I9" s="20"/>
-      <c r="J9" s="20"/>
-      <c r="K9" s="20"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="17"/>
-      <c r="B10" s="17"/>
-      <c r="C10" s="17"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="17"/>
-      <c r="G10" s="17"/>
-      <c r="H10" s="17"/>
-      <c r="I10" s="17"/>
-      <c r="J10" s="17"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="17"/>
-      <c r="B11" s="17"/>
-      <c r="C11" s="17"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="17"/>
-      <c r="G11" s="17"/>
-      <c r="H11" s="17"/>
-      <c r="I11" s="17"/>
-      <c r="J11" s="17"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="17"/>
-      <c r="B12" s="17"/>
-      <c r="C12" s="17"/>
-      <c r="D12" s="17"/>
-      <c r="E12" s="17"/>
-      <c r="F12" s="17"/>
-      <c r="G12" s="17"/>
-      <c r="H12" s="17"/>
-      <c r="I12" s="17"/>
-      <c r="J12" s="17"/>
+      <c r="E7" s="26"/>
+      <c r="F7" s="26"/>
+      <c r="G7" s="26"/>
+      <c r="H7" s="26"/>
+      <c r="I7" s="26"/>
+      <c r="J7" s="26"/>
+      <c r="K7" s="3">
+        <v>6</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="M7" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="N7" s="1"/>
+    </row>
+    <row r="8" spans="1:14" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="25"/>
+      <c r="B8" s="25"/>
+      <c r="C8" s="25"/>
+      <c r="D8" s="26"/>
+      <c r="E8" s="26"/>
+      <c r="F8" s="26"/>
+      <c r="G8" s="26"/>
+      <c r="H8" s="26"/>
+      <c r="I8" s="26"/>
+      <c r="J8" s="26"/>
+      <c r="K8" s="3">
+        <v>7</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="M8" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="N8" s="1"/>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D35" s="21" t="s">
+      <c r="D35" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="E35" s="13"/>
-      <c r="F35" s="13"/>
-      <c r="G35" s="13"/>
-      <c r="H35" s="13"/>
-      <c r="I35" s="13"/>
-      <c r="J35" s="13"/>
+      <c r="E35" s="21"/>
+      <c r="F35" s="21"/>
+      <c r="G35" s="21"/>
+      <c r="H35" s="21"/>
+      <c r="I35" s="21"/>
+      <c r="J35" s="21"/>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D36" s="13"/>
-      <c r="E36" s="13"/>
-      <c r="F36" s="13"/>
-      <c r="G36" s="13"/>
-      <c r="H36" s="13"/>
-      <c r="I36" s="13"/>
-      <c r="J36" s="13"/>
+      <c r="D36" s="21"/>
+      <c r="E36" s="21"/>
+      <c r="F36" s="21"/>
+      <c r="G36" s="21"/>
+      <c r="H36" s="21"/>
+      <c r="I36" s="21"/>
+      <c r="J36" s="21"/>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D37" s="13"/>
-      <c r="E37" s="13"/>
-      <c r="F37" s="13"/>
-      <c r="G37" s="13"/>
-      <c r="H37" s="13"/>
-      <c r="I37" s="13"/>
-      <c r="J37" s="13"/>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A39" s="19" t="s">
+      <c r="D37" s="21"/>
+      <c r="E37" s="21"/>
+      <c r="F37" s="21"/>
+      <c r="G37" s="21"/>
+      <c r="H37" s="21"/>
+      <c r="I37" s="21"/>
+      <c r="J37" s="21"/>
+    </row>
+    <row r="39" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A39" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="B39" s="19"/>
-      <c r="C39" s="19"/>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A40" s="19"/>
-      <c r="B40" s="19"/>
-      <c r="C40" s="19"/>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A41" s="19"/>
-      <c r="B41" s="19"/>
-      <c r="C41" s="19"/>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A42" s="19"/>
-      <c r="B42" s="19"/>
-      <c r="C42" s="19"/>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A43" s="24" t="s">
+      <c r="B39" s="24"/>
+      <c r="C39" s="24"/>
+      <c r="D39" s="30"/>
+      <c r="E39" s="31"/>
+      <c r="F39" s="31"/>
+      <c r="G39" s="31"/>
+      <c r="H39" s="31"/>
+      <c r="I39" s="31"/>
+      <c r="J39" s="31"/>
+    </row>
+    <row r="40" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="24"/>
+      <c r="B40" s="24"/>
+      <c r="C40" s="24"/>
+      <c r="D40" s="31"/>
+      <c r="E40" s="31"/>
+      <c r="F40" s="31"/>
+      <c r="G40" s="31"/>
+      <c r="H40" s="31"/>
+      <c r="I40" s="31"/>
+      <c r="J40" s="31"/>
+    </row>
+    <row r="41" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="24"/>
+      <c r="B41" s="24"/>
+      <c r="C41" s="24"/>
+      <c r="D41" s="31"/>
+      <c r="E41" s="31"/>
+      <c r="F41" s="31"/>
+      <c r="G41" s="31"/>
+      <c r="H41" s="31"/>
+      <c r="I41" s="31"/>
+      <c r="J41" s="31"/>
+    </row>
+    <row r="42" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="24"/>
+      <c r="B42" s="24"/>
+      <c r="C42" s="24"/>
+      <c r="D42" s="31"/>
+      <c r="E42" s="31"/>
+      <c r="F42" s="31"/>
+      <c r="G42" s="31"/>
+      <c r="H42" s="31"/>
+      <c r="I42" s="31"/>
+      <c r="J42" s="31"/>
+    </row>
+    <row r="43" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="B43" s="13"/>
-      <c r="C43" s="13"/>
+      <c r="B43" s="25"/>
+      <c r="C43" s="25"/>
+      <c r="D43" s="31"/>
+      <c r="E43" s="31"/>
+      <c r="F43" s="31"/>
+      <c r="G43" s="31"/>
+      <c r="H43" s="31"/>
+      <c r="I43" s="31"/>
+      <c r="J43" s="31"/>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A44" s="13"/>
-      <c r="B44" s="13"/>
-      <c r="C44" s="13"/>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="25"/>
+      <c r="B44" s="25"/>
+      <c r="C44" s="25"/>
+    </row>
+    <row r="68" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="23" t="s">
         <v>46</v>
       </c>
-      <c r="B68" s="22"/>
-      <c r="C68" s="22"/>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A69" s="22"/>
-      <c r="B69" s="22"/>
-      <c r="C69" s="22"/>
+      <c r="B68" s="23"/>
+      <c r="C68" s="23"/>
+    </row>
+    <row r="69" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="23"/>
+      <c r="B69" s="23"/>
+      <c r="C69" s="23"/>
     </row>
     <row r="70" spans="1:3" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="22"/>
-      <c r="B70" s="22"/>
-      <c r="C70" s="22"/>
+      <c r="A70" s="23"/>
+      <c r="B70" s="23"/>
+      <c r="C70" s="23"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="8">
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A6:E6"/>
     <mergeCell ref="A68:C70"/>
     <mergeCell ref="A39:C42"/>
     <mergeCell ref="A7:C8"/>
@@ -1456,13 +1647,14 @@
     <mergeCell ref="A43:C44"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" display="https://stackoverflow.com/questions/15070513/how-to-test-a-non-thread-safe-class" xr:uid="{099E06CC-9B91-4197-87D0-C20037FCDD31}"/>
-    <hyperlink ref="D3" r:id="rId2" display="https://www.baeldung.com/java-thread-safety" xr:uid="{38025520-86A2-467A-A1B7-7A2F5813FD38}"/>
-    <hyperlink ref="D4" r:id="rId3" xr:uid="{67109424-1466-4B6B-9C24-42F7B661600F}"/>
-    <hyperlink ref="D5" r:id="rId4" xr:uid="{5D163F4B-4A2A-427E-8ABC-EBDDEB47C63C}"/>
+    <hyperlink ref="N2" r:id="rId1" display="https://stackoverflow.com/questions/15070513/how-to-test-a-non-thread-safe-class" xr:uid="{AF80577A-A125-48C9-AA50-5BBE662AA378}"/>
+    <hyperlink ref="N3" r:id="rId2" display="https://www.baeldung.com/java-thread-safety" xr:uid="{C1945518-65A5-43C4-A7C3-0AB5B0EA6DE6}"/>
+    <hyperlink ref="N4" r:id="rId3" xr:uid="{F6BBD934-A547-4D3A-A18E-DBB296712BB7}"/>
+    <hyperlink ref="N5" r:id="rId4" xr:uid="{AB87879D-41CA-4D0A-BC91-EEAA9A792E8B}"/>
+    <hyperlink ref="N6" r:id="rId5" location="4-reentrancy" xr:uid="{F4526B1D-3B6D-4BBD-A91D-7781541ECE62}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId5"/>
-  <drawing r:id="rId6"/>
+  <pageSetup orientation="portrait" r:id="rId6"/>
+  <drawing r:id="rId7"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update day6 task remaining
</commit_message>
<xml_diff>
--- a/Task_Result.xlsx
+++ b/Task_Result.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\beetech\java\stage1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{959C88B3-B9DB-4E67-B6F4-F326752B5A66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1556FF22-67F1-4963-B038-6C5F299C253F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="172">
   <si>
     <t>STT</t>
   </si>
@@ -570,10 +570,66 @@
     <t>Sealed classes</t>
   </si>
   <si>
-    <t xml:space="preserve"> là một tính năng mới trong Java 15, nó giới hạn các lớp con của một lớp cụ thể chỉ có thể được định nghĩa bởi lớp cha hoặc trong cùng một module. Điều này cung cấp một cách để xác định và giới hạn các lớp được kế thừa từ một lớp cơ sở nhất định.
+    <t>Từ Java 9 trở đi thì cho phép "diamon operator" có thể sử dụng "anonymous inner class"</t>
+  </si>
+  <si>
+    <t>https://docs.oracle.com/javase/tutorial/java/IandI/defaultmethods.html</t>
+  </si>
+  <si>
+    <t>https://reflectoring.io/java-release-notes/#java-module-system</t>
+  </si>
+  <si>
+    <t>https://docs.oracle.com/javase/tutorial/essential/exceptions/tryResourceClose.html</t>
+  </si>
+  <si>
+    <t>https://viblo.asia/p/java-anonymous-class-n157G5J3vAje</t>
+  </si>
+  <si>
+    <t>https://www.geeksforgeeks.org/diamond-operator-for-anonymous-inner-class-with-examples-in-java/</t>
+  </si>
+  <si>
+    <t>https://reflectoring.io/java-release-notes/#private-interface-methods</t>
+  </si>
+  <si>
+    <t>https://reflectoring.io/java-release-notes/#local-variable-type-inference</t>
+  </si>
+  <si>
+    <t>https://reflectoring.io/java-release-notes/#switch-expressions</t>
+  </si>
+  <si>
+    <t>https://docs.oracle.com/en/java/javase/14/language/switch-expressions.html</t>
+  </si>
+  <si>
+    <t>https://docs.oracle.com/en/java/javase/15/text-blocks/index.html#using-text-blocks</t>
+  </si>
+  <si>
+    <t>https://docs.oracle.com/en/java/javase/16/language/pattern-matching-instanceof-operator.html</t>
+  </si>
+  <si>
+    <t>https://docs.oracle.com/en/java/javase/16/language/records.html</t>
+  </si>
+  <si>
+    <t>https://docs.oracle.com/en/java/javase/16/language/sealed-classes-and-interfaces.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> là một tính năng mới trong Java 16, nó giới hạn các lớp con của một lớp cụ thể chỉ có thể được định nghĩa bởi lớp cha hoặc trong cùng một module. Điều này cung cấp một cách để xác định và giới hạn các lớp được kế thừa từ một lớp cơ sở nhất định.
 Một lớp được đánh dấu là sealed bằng cách sử dụng từ khóa sealed trước khai báo lớp và sau đó liệt kê các lớp con được phép kế thừa nó. Các lớp được liệt kê phải được định nghĩa trong cùng một file hoặc package.
 Một lớp con không được liệt kê trong danh sách permits sẽ không thể kế thừa lớp cha sealed. Khi ta cố gắng định nghĩa một lớp con không được phép, chương trình sẽ bị lỗi biên dịch.
+Permitted subclasses phải có các từ khóa sau:
+final
+sealed
+non-sealed
 </t>
+  </si>
+  <si>
+    <t>Repeating Annotation</t>
+  </si>
+  <si>
+    <t>là một tính năng mới được giới thiệu trong Java 8, cho phép chúng ta sử dụng nhiều annotation cùng một loại trên một phần tử. 
+Trước khi tính năng này được giới thiệu, ta chỉ có thể sử dụng một annotation cùng một loại cho một phần tử. Để sử dụng repeating annotations, ta cần đánh dấu annotation bằng @Repeatable và định nghĩa một annotation container.</t>
+  </si>
+  <si>
+    <t>https://reflectoring.io/java-release-notes/#repeating-annotations</t>
   </si>
 </sst>
 </file>
@@ -734,7 +790,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -801,6 +857,13 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -849,15 +912,11 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -897,7 +956,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9F5F04C2-D3A7-F489-C193-480B74E20109}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -941,7 +1000,7 @@
         <xdr:cNvPr id="6" name="Picture 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{83BCA204-DD3E-45CF-95EC-B0CF7DF3594B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -990,7 +1049,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C2E90FB0-7484-0B1E-E402-D4AB3E4924F9}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1051,7 +1110,7 @@
         <xdr:cNvPr id="4" name="Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AAB8C5B5-D205-4333-A452-468DF7719274}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1112,7 +1171,7 @@
         <xdr:cNvPr id="6" name="Picture 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2188C6C2-B02B-BEF2-8FD3-203FC631A871}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1173,7 +1232,7 @@
         <xdr:cNvPr id="10" name="Picture 9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BBC6DC59-7923-68A4-D695-EBC49F584EC2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000A000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1234,7 +1293,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{07DF58DD-D311-AE9E-8A5D-CEF88AB3ED77}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1300,7 +1359,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2920738E-093E-43D0-36CF-9E30AE0AF704}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1361,7 +1420,7 @@
         <xdr:cNvPr id="6" name="Picture 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{889DFBD5-9EE0-35BC-4666-DA48E8CCAF22}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1422,7 +1481,7 @@
         <xdr:cNvPr id="7" name="Picture 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E93C5651-8182-51F6-7FC4-8BC0C1303C15}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1803,27 +1862,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="16:22" x14ac:dyDescent="0.25">
-      <c r="P1" s="31" t="s">
+      <c r="P1" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="Q1" s="32"/>
-      <c r="R1" s="32"/>
-      <c r="S1" s="32"/>
-      <c r="T1" s="32"/>
+      <c r="Q1" s="35"/>
+      <c r="R1" s="35"/>
+      <c r="S1" s="35"/>
+      <c r="T1" s="35"/>
     </row>
     <row r="2" spans="16:22" x14ac:dyDescent="0.25">
-      <c r="P2" s="32"/>
-      <c r="Q2" s="32"/>
-      <c r="R2" s="32"/>
-      <c r="S2" s="32"/>
-      <c r="T2" s="32"/>
+      <c r="P2" s="35"/>
+      <c r="Q2" s="35"/>
+      <c r="R2" s="35"/>
+      <c r="S2" s="35"/>
+      <c r="T2" s="35"/>
     </row>
     <row r="3" spans="16:22" x14ac:dyDescent="0.25">
-      <c r="P3" s="33"/>
-      <c r="Q3" s="33"/>
-      <c r="R3" s="33"/>
-      <c r="S3" s="33"/>
-      <c r="T3" s="33"/>
+      <c r="P3" s="36"/>
+      <c r="Q3" s="36"/>
+      <c r="R3" s="36"/>
+      <c r="S3" s="36"/>
+      <c r="T3" s="36"/>
     </row>
     <row r="4" spans="16:22" x14ac:dyDescent="0.25">
       <c r="P4" s="7" t="s">
@@ -1832,11 +1891,11 @@
       <c r="Q4" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="R4" s="30" t="s">
+      <c r="R4" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="S4" s="30"/>
-      <c r="T4" s="30"/>
+      <c r="S4" s="33"/>
+      <c r="T4" s="33"/>
       <c r="U4" s="7" t="s">
         <v>18</v>
       </c>
@@ -1990,24 +2049,24 @@
       </c>
     </row>
     <row r="14" spans="16:22" x14ac:dyDescent="0.25">
-      <c r="P14" s="34" t="s">
+      <c r="P14" s="37" t="s">
         <v>73</v>
       </c>
-      <c r="Q14" s="32"/>
-      <c r="R14" s="32"/>
-      <c r="S14" s="32"/>
+      <c r="Q14" s="35"/>
+      <c r="R14" s="35"/>
+      <c r="S14" s="35"/>
     </row>
     <row r="15" spans="16:22" x14ac:dyDescent="0.25">
-      <c r="P15" s="32"/>
-      <c r="Q15" s="32"/>
-      <c r="R15" s="32"/>
-      <c r="S15" s="32"/>
+      <c r="P15" s="35"/>
+      <c r="Q15" s="35"/>
+      <c r="R15" s="35"/>
+      <c r="S15" s="35"/>
     </row>
     <row r="16" spans="16:22" x14ac:dyDescent="0.25">
-      <c r="P16" s="32"/>
-      <c r="Q16" s="32"/>
-      <c r="R16" s="32"/>
-      <c r="S16" s="32"/>
+      <c r="P16" s="35"/>
+      <c r="Q16" s="35"/>
+      <c r="R16" s="35"/>
+      <c r="S16" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -2050,17 +2109,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="49.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="38" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
-      <c r="I1" s="36"/>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="39"/>
+      <c r="I1" s="39"/>
       <c r="J1" s="13"/>
       <c r="K1" s="7" t="s">
         <v>0</v>
@@ -2150,13 +2209,13 @@
       </c>
     </row>
     <row r="6" spans="1:14" ht="129.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="37" t="s">
+      <c r="A6" s="40" t="s">
         <v>54</v>
       </c>
-      <c r="B6" s="38"/>
-      <c r="C6" s="38"/>
-      <c r="D6" s="38"/>
-      <c r="E6" s="38"/>
+      <c r="B6" s="41"/>
+      <c r="C6" s="41"/>
+      <c r="D6" s="41"/>
+      <c r="E6" s="41"/>
       <c r="K6" s="3">
         <v>5</v>
       </c>
@@ -2171,20 +2230,20 @@
       </c>
     </row>
     <row r="7" spans="1:14" ht="108" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="34" t="s">
+      <c r="A7" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="B7" s="34"/>
-      <c r="C7" s="34"/>
-      <c r="D7" s="34" t="s">
+      <c r="B7" s="37"/>
+      <c r="C7" s="37"/>
+      <c r="D7" s="37" t="s">
         <v>43</v>
       </c>
-      <c r="E7" s="41"/>
-      <c r="F7" s="41"/>
-      <c r="G7" s="41"/>
-      <c r="H7" s="41"/>
-      <c r="I7" s="41"/>
-      <c r="J7" s="41"/>
+      <c r="E7" s="44"/>
+      <c r="F7" s="44"/>
+      <c r="G7" s="44"/>
+      <c r="H7" s="44"/>
+      <c r="I7" s="44"/>
+      <c r="J7" s="44"/>
       <c r="K7" s="3">
         <v>6</v>
       </c>
@@ -2197,16 +2256,16 @@
       <c r="N7" s="1"/>
     </row>
     <row r="8" spans="1:14" ht="139.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="34"/>
-      <c r="B8" s="34"/>
-      <c r="C8" s="34"/>
-      <c r="D8" s="41"/>
-      <c r="E8" s="41"/>
-      <c r="F8" s="41"/>
-      <c r="G8" s="41"/>
-      <c r="H8" s="41"/>
-      <c r="I8" s="41"/>
-      <c r="J8" s="41"/>
+      <c r="A8" s="37"/>
+      <c r="B8" s="37"/>
+      <c r="C8" s="37"/>
+      <c r="D8" s="44"/>
+      <c r="E8" s="44"/>
+      <c r="F8" s="44"/>
+      <c r="G8" s="44"/>
+      <c r="H8" s="44"/>
+      <c r="I8" s="44"/>
+      <c r="J8" s="44"/>
       <c r="K8" s="3">
         <v>7</v>
       </c>
@@ -2219,85 +2278,85 @@
       <c r="N8" s="1"/>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D35" s="42" t="s">
+      <c r="D35" s="45" t="s">
         <v>44</v>
       </c>
-      <c r="E35" s="32"/>
-      <c r="F35" s="32"/>
-      <c r="G35" s="32"/>
-      <c r="H35" s="32"/>
-      <c r="I35" s="32"/>
-      <c r="J35" s="32"/>
+      <c r="E35" s="35"/>
+      <c r="F35" s="35"/>
+      <c r="G35" s="35"/>
+      <c r="H35" s="35"/>
+      <c r="I35" s="35"/>
+      <c r="J35" s="35"/>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D36" s="32"/>
-      <c r="E36" s="32"/>
-      <c r="F36" s="32"/>
-      <c r="G36" s="32"/>
-      <c r="H36" s="32"/>
-      <c r="I36" s="32"/>
-      <c r="J36" s="32"/>
+      <c r="D36" s="35"/>
+      <c r="E36" s="35"/>
+      <c r="F36" s="35"/>
+      <c r="G36" s="35"/>
+      <c r="H36" s="35"/>
+      <c r="I36" s="35"/>
+      <c r="J36" s="35"/>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D37" s="32"/>
-      <c r="E37" s="32"/>
-      <c r="F37" s="32"/>
-      <c r="G37" s="32"/>
-      <c r="H37" s="32"/>
-      <c r="I37" s="32"/>
-      <c r="J37" s="32"/>
+      <c r="D37" s="35"/>
+      <c r="E37" s="35"/>
+      <c r="F37" s="35"/>
+      <c r="G37" s="35"/>
+      <c r="H37" s="35"/>
+      <c r="I37" s="35"/>
+      <c r="J37" s="35"/>
     </row>
     <row r="39" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A39" s="40" t="s">
+      <c r="A39" s="43" t="s">
         <v>41</v>
       </c>
-      <c r="B39" s="40"/>
-      <c r="C39" s="40"/>
+      <c r="B39" s="43"/>
+      <c r="C39" s="43"/>
       <c r="D39" s="20"/>
     </row>
     <row r="40" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="40"/>
-      <c r="B40" s="40"/>
-      <c r="C40" s="40"/>
+      <c r="A40" s="43"/>
+      <c r="B40" s="43"/>
+      <c r="C40" s="43"/>
     </row>
     <row r="41" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="40"/>
-      <c r="B41" s="40"/>
-      <c r="C41" s="40"/>
+      <c r="A41" s="43"/>
+      <c r="B41" s="43"/>
+      <c r="C41" s="43"/>
     </row>
     <row r="42" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="40"/>
-      <c r="B42" s="40"/>
-      <c r="C42" s="40"/>
+      <c r="A42" s="43"/>
+      <c r="B42" s="43"/>
+      <c r="C42" s="43"/>
     </row>
     <row r="43" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="34" t="s">
+      <c r="A43" s="37" t="s">
         <v>45</v>
       </c>
-      <c r="B43" s="34"/>
-      <c r="C43" s="34"/>
+      <c r="B43" s="37"/>
+      <c r="C43" s="37"/>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A44" s="34"/>
-      <c r="B44" s="34"/>
-      <c r="C44" s="34"/>
+      <c r="A44" s="37"/>
+      <c r="B44" s="37"/>
+      <c r="C44" s="37"/>
     </row>
     <row r="68" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="39" t="s">
+      <c r="A68" s="42" t="s">
         <v>46</v>
       </c>
-      <c r="B68" s="39"/>
-      <c r="C68" s="39"/>
+      <c r="B68" s="42"/>
+      <c r="C68" s="42"/>
     </row>
     <row r="69" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="39"/>
-      <c r="B69" s="39"/>
-      <c r="C69" s="39"/>
+      <c r="A69" s="42"/>
+      <c r="B69" s="42"/>
+      <c r="C69" s="42"/>
     </row>
     <row r="70" spans="1:3" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="39"/>
-      <c r="B70" s="39"/>
-      <c r="C70" s="39"/>
+      <c r="A70" s="42"/>
+      <c r="B70" s="42"/>
+      <c r="C70" s="42"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -2373,20 +2432,20 @@
       <c r="D2" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="F2" s="34" t="s">
+      <c r="F2" s="37" t="s">
         <v>68</v>
       </c>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32"/>
-      <c r="K2" s="32"/>
-      <c r="L2" s="32"/>
-      <c r="M2" s="32"/>
-      <c r="N2" s="32"/>
-      <c r="O2" s="32"/>
-      <c r="P2" s="32"/>
-      <c r="Q2" s="32"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="35"/>
+      <c r="I2" s="35"/>
+      <c r="J2" s="35"/>
+      <c r="K2" s="35"/>
+      <c r="L2" s="35"/>
+      <c r="M2" s="35"/>
+      <c r="N2" s="35"/>
+      <c r="O2" s="35"/>
+      <c r="P2" s="35"/>
+      <c r="Q2" s="35"/>
     </row>
     <row r="3" spans="1:17" ht="110.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
@@ -2428,21 +2487,21 @@
         <v>65</v>
       </c>
       <c r="D5" s="3"/>
-      <c r="E5" s="43" t="s">
+      <c r="E5" s="46" t="s">
         <v>69</v>
       </c>
-      <c r="F5" s="32"/>
-      <c r="G5" s="32"/>
-      <c r="H5" s="32"/>
-      <c r="I5" s="32"/>
-      <c r="J5" s="32"/>
-      <c r="K5" s="32"/>
-      <c r="L5" s="32"/>
-      <c r="M5" s="32"/>
-      <c r="N5" s="32"/>
-      <c r="O5" s="32"/>
-      <c r="P5" s="32"/>
-      <c r="Q5" s="32"/>
+      <c r="F5" s="35"/>
+      <c r="G5" s="35"/>
+      <c r="H5" s="35"/>
+      <c r="I5" s="35"/>
+      <c r="J5" s="35"/>
+      <c r="K5" s="35"/>
+      <c r="L5" s="35"/>
+      <c r="M5" s="35"/>
+      <c r="N5" s="35"/>
+      <c r="O5" s="35"/>
+      <c r="P5" s="35"/>
+      <c r="Q5" s="35"/>
     </row>
     <row r="6" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
@@ -2455,19 +2514,19 @@
         <v>67</v>
       </c>
       <c r="D6" s="3"/>
-      <c r="E6" s="44"/>
-      <c r="F6" s="32"/>
-      <c r="G6" s="32"/>
-      <c r="H6" s="32"/>
-      <c r="I6" s="32"/>
-      <c r="J6" s="32"/>
-      <c r="K6" s="32"/>
-      <c r="L6" s="32"/>
-      <c r="M6" s="32"/>
-      <c r="N6" s="32"/>
-      <c r="O6" s="32"/>
-      <c r="P6" s="32"/>
-      <c r="Q6" s="32"/>
+      <c r="E6" s="47"/>
+      <c r="F6" s="35"/>
+      <c r="G6" s="35"/>
+      <c r="H6" s="35"/>
+      <c r="I6" s="35"/>
+      <c r="J6" s="35"/>
+      <c r="K6" s="35"/>
+      <c r="L6" s="35"/>
+      <c r="M6" s="35"/>
+      <c r="N6" s="35"/>
+      <c r="O6" s="35"/>
+      <c r="P6" s="35"/>
+      <c r="Q6" s="35"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="14"/>
@@ -2531,78 +2590,78 @@
       <c r="D16" s="14"/>
     </row>
     <row r="22" spans="5:16" x14ac:dyDescent="0.25">
-      <c r="E22" s="34" t="s">
+      <c r="E22" s="37" t="s">
         <v>70</v>
       </c>
-      <c r="F22" s="32"/>
-      <c r="G22" s="32"/>
-      <c r="H22" s="32"/>
-      <c r="I22" s="32"/>
-      <c r="J22" s="32"/>
-      <c r="K22" s="32"/>
-      <c r="L22" s="32"/>
-      <c r="M22" s="32"/>
-      <c r="N22" s="32"/>
-      <c r="O22" s="32"/>
-      <c r="P22" s="32"/>
+      <c r="F22" s="35"/>
+      <c r="G22" s="35"/>
+      <c r="H22" s="35"/>
+      <c r="I22" s="35"/>
+      <c r="J22" s="35"/>
+      <c r="K22" s="35"/>
+      <c r="L22" s="35"/>
+      <c r="M22" s="35"/>
+      <c r="N22" s="35"/>
+      <c r="O22" s="35"/>
+      <c r="P22" s="35"/>
     </row>
     <row r="23" spans="5:16" x14ac:dyDescent="0.25">
-      <c r="E23" s="32"/>
-      <c r="F23" s="32"/>
-      <c r="G23" s="32"/>
-      <c r="H23" s="32"/>
-      <c r="I23" s="32"/>
-      <c r="J23" s="32"/>
-      <c r="K23" s="32"/>
-      <c r="L23" s="32"/>
-      <c r="M23" s="32"/>
-      <c r="N23" s="32"/>
-      <c r="O23" s="32"/>
-      <c r="P23" s="32"/>
+      <c r="E23" s="35"/>
+      <c r="F23" s="35"/>
+      <c r="G23" s="35"/>
+      <c r="H23" s="35"/>
+      <c r="I23" s="35"/>
+      <c r="J23" s="35"/>
+      <c r="K23" s="35"/>
+      <c r="L23" s="35"/>
+      <c r="M23" s="35"/>
+      <c r="N23" s="35"/>
+      <c r="O23" s="35"/>
+      <c r="P23" s="35"/>
     </row>
     <row r="24" spans="5:16" x14ac:dyDescent="0.25">
-      <c r="E24" s="32"/>
-      <c r="F24" s="32"/>
-      <c r="G24" s="32"/>
-      <c r="H24" s="32"/>
-      <c r="I24" s="32"/>
-      <c r="J24" s="32"/>
-      <c r="K24" s="32"/>
-      <c r="L24" s="32"/>
-      <c r="M24" s="32"/>
-      <c r="N24" s="32"/>
-      <c r="O24" s="32"/>
-      <c r="P24" s="32"/>
+      <c r="E24" s="35"/>
+      <c r="F24" s="35"/>
+      <c r="G24" s="35"/>
+      <c r="H24" s="35"/>
+      <c r="I24" s="35"/>
+      <c r="J24" s="35"/>
+      <c r="K24" s="35"/>
+      <c r="L24" s="35"/>
+      <c r="M24" s="35"/>
+      <c r="N24" s="35"/>
+      <c r="O24" s="35"/>
+      <c r="P24" s="35"/>
     </row>
     <row r="40" spans="5:16" x14ac:dyDescent="0.25">
-      <c r="E40" s="42" t="s">
+      <c r="E40" s="45" t="s">
         <v>71</v>
       </c>
-      <c r="F40" s="32"/>
-      <c r="G40" s="32"/>
-      <c r="H40" s="32"/>
-      <c r="I40" s="32"/>
-      <c r="J40" s="32"/>
-      <c r="K40" s="32"/>
-      <c r="L40" s="32"/>
-      <c r="M40" s="32"/>
-      <c r="N40" s="32"/>
-      <c r="O40" s="32"/>
-      <c r="P40" s="32"/>
+      <c r="F40" s="35"/>
+      <c r="G40" s="35"/>
+      <c r="H40" s="35"/>
+      <c r="I40" s="35"/>
+      <c r="J40" s="35"/>
+      <c r="K40" s="35"/>
+      <c r="L40" s="35"/>
+      <c r="M40" s="35"/>
+      <c r="N40" s="35"/>
+      <c r="O40" s="35"/>
+      <c r="P40" s="35"/>
     </row>
     <row r="41" spans="5:16" x14ac:dyDescent="0.25">
-      <c r="E41" s="32"/>
-      <c r="F41" s="32"/>
-      <c r="G41" s="32"/>
-      <c r="H41" s="32"/>
-      <c r="I41" s="32"/>
-      <c r="J41" s="32"/>
-      <c r="K41" s="32"/>
-      <c r="L41" s="32"/>
-      <c r="M41" s="32"/>
-      <c r="N41" s="32"/>
-      <c r="O41" s="32"/>
-      <c r="P41" s="32"/>
+      <c r="E41" s="35"/>
+      <c r="F41" s="35"/>
+      <c r="G41" s="35"/>
+      <c r="H41" s="35"/>
+      <c r="I41" s="35"/>
+      <c r="J41" s="35"/>
+      <c r="K41" s="35"/>
+      <c r="L41" s="35"/>
+      <c r="M41" s="35"/>
+      <c r="N41" s="35"/>
+      <c r="O41" s="35"/>
+      <c r="P41" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -2680,14 +2739,14 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="45" t="s">
+      <c r="A7" s="48" t="s">
         <v>79</v>
       </c>
-      <c r="B7" s="32"/>
+      <c r="B7" s="35"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="32"/>
-      <c r="B8" s="32"/>
+      <c r="A8" s="35"/>
+      <c r="B8" s="35"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
@@ -2856,7 +2915,7 @@
   <oleObjects>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <oleObject progId="Word.Document.12" dvAspect="DVASPECT_ICON" link="[1]!''''" oleUpdate="OLEUPDATE_ONCALL" shapeId="4099">
+        <oleObject dvAspect="DVASPECT_ICON" link="[1]!''''" oleUpdate="OLEUPDATE_ONCALL" shapeId="4099">
           <objectPr defaultSize="0" dde="1" r:id="rId4">
             <anchor moveWithCells="1">
               <from>
@@ -2876,7 +2935,7 @@
         </oleObject>
       </mc:Choice>
       <mc:Fallback>
-        <oleObject progId="Word.Document.12" dvAspect="DVASPECT_ICON" link="[1]!''''" oleUpdate="OLEUPDATE_ONCALL" shapeId="4099"/>
+        <oleObject dvAspect="DVASPECT_ICON" link="[1]!''''" oleUpdate="OLEUPDATE_ONCALL" shapeId="4099"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </oleObjects>
@@ -2887,8 +2946,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D5CC180-ABEC-4096-BF7B-D59D7E76A5ED}">
   <dimension ref="A1:M19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2900,29 +2959,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="46" t="s">
+      <c r="B1" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="46" t="s">
+      <c r="C1" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="46" t="s">
+      <c r="D1" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="46" t="s">
+      <c r="E1" s="49" t="s">
         <v>121</v>
       </c>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
-      <c r="I1" s="46"/>
-      <c r="J1" s="46"/>
-      <c r="K1" s="46"/>
-      <c r="L1" s="46"/>
-      <c r="M1" s="46"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
+      <c r="J1" s="30"/>
+      <c r="K1" s="30"/>
+      <c r="L1" s="30"/>
+      <c r="M1" s="30"/>
     </row>
     <row r="2" spans="1:13" ht="112.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
@@ -2937,7 +2996,7 @@
       <c r="D2" s="11" t="s">
         <v>120</v>
       </c>
-      <c r="E2" s="47">
+      <c r="E2" s="3">
         <v>8</v>
       </c>
       <c r="F2" s="1"/>
@@ -2962,7 +3021,7 @@
       <c r="D3" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="E3" s="47">
+      <c r="E3" s="3">
         <v>8</v>
       </c>
       <c r="F3" s="1"/>
@@ -2975,7 +3034,7 @@
       <c r="M3" s="1"/>
     </row>
     <row r="4" spans="1:13" ht="210" x14ac:dyDescent="0.25">
-      <c r="A4" s="48">
+      <c r="A4" s="31">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -2987,7 +3046,7 @@
       <c r="D4" s="9" t="s">
         <v>126</v>
       </c>
-      <c r="E4" s="47">
+      <c r="E4" s="3">
         <v>8</v>
       </c>
       <c r="F4" s="1"/>
@@ -3000,7 +3059,7 @@
       <c r="M4" s="1"/>
     </row>
     <row r="5" spans="1:13" ht="150" x14ac:dyDescent="0.25">
-      <c r="A5" s="48">
+      <c r="A5" s="31">
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -3009,8 +3068,10 @@
       <c r="C5" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1">
+      <c r="D5" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="E5" s="31">
         <v>8</v>
       </c>
       <c r="F5" s="1"/>
@@ -3023,7 +3084,7 @@
       <c r="M5" s="1"/>
     </row>
     <row r="6" spans="1:13" ht="270" x14ac:dyDescent="0.25">
-      <c r="A6" s="48">
+      <c r="A6" s="31">
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
@@ -3032,8 +3093,12 @@
       <c r="C6" s="6" t="s">
         <v>131</v>
       </c>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
+      <c r="D6" s="9" t="s">
+        <v>156</v>
+      </c>
+      <c r="E6" s="31">
+        <v>9</v>
+      </c>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
@@ -3044,7 +3109,7 @@
       <c r="M6" s="1"/>
     </row>
     <row r="7" spans="1:13" ht="75" x14ac:dyDescent="0.25">
-      <c r="A7" s="48">
+      <c r="A7" s="31">
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
@@ -3053,8 +3118,12 @@
       <c r="C7" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
+      <c r="D7" s="9" t="s">
+        <v>157</v>
+      </c>
+      <c r="E7" s="31">
+        <v>8</v>
+      </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
@@ -3075,7 +3144,9 @@
         <v>135</v>
       </c>
       <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
+      <c r="E8" s="31">
+        <v>7</v>
+      </c>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
@@ -3095,8 +3166,12 @@
       <c r="C9" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
+      <c r="D9" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="E9" s="31">
+        <v>1.1000000000000001</v>
+      </c>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
@@ -3107,15 +3182,21 @@
       <c r="M9" s="1"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="48">
+      <c r="A10" s="31">
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
+      <c r="C10" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="E10" s="31">
+        <v>9</v>
+      </c>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
@@ -3126,7 +3207,7 @@
       <c r="M10" s="1"/>
     </row>
     <row r="11" spans="1:13" ht="90" x14ac:dyDescent="0.25">
-      <c r="A11" s="48">
+      <c r="A11" s="31">
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
@@ -3135,8 +3216,12 @@
       <c r="C11" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
+      <c r="D11" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="E11" s="50">
+        <v>9</v>
+      </c>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
@@ -3147,7 +3232,7 @@
       <c r="M11" s="1"/>
     </row>
     <row r="12" spans="1:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" s="48">
+      <c r="A12" s="31">
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -3156,8 +3241,12 @@
       <c r="C12" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
+      <c r="D12" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="E12" s="31">
+        <v>10</v>
+      </c>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
@@ -3168,7 +3257,7 @@
       <c r="M12" s="1"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="48">
+      <c r="A13" s="31">
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
@@ -3177,8 +3266,12 @@
       <c r="C13" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
+      <c r="D13" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="E13" s="31">
+        <v>12</v>
+      </c>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
@@ -3189,7 +3282,7 @@
       <c r="M13" s="1"/>
     </row>
     <row r="14" spans="1:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="A14" s="48">
+      <c r="A14" s="31">
         <v>13</v>
       </c>
       <c r="B14" s="3" t="s">
@@ -3198,8 +3291,12 @@
       <c r="C14" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
+      <c r="D14" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="E14" s="31">
+        <v>14</v>
+      </c>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
@@ -3210,7 +3307,7 @@
       <c r="M14" s="1"/>
     </row>
     <row r="15" spans="1:13" ht="135" x14ac:dyDescent="0.25">
-      <c r="A15" s="48">
+      <c r="A15" s="31">
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
@@ -3219,8 +3316,12 @@
       <c r="C15" s="6" t="s">
         <v>148</v>
       </c>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
+      <c r="D15" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="E15" s="31">
+        <v>15</v>
+      </c>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
@@ -3231,7 +3332,7 @@
       <c r="M15" s="1"/>
     </row>
     <row r="16" spans="1:13" ht="75" x14ac:dyDescent="0.25">
-      <c r="A16" s="48">
+      <c r="A16" s="31">
         <v>15</v>
       </c>
       <c r="B16" s="3" t="s">
@@ -3240,8 +3341,12 @@
       <c r="C16" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
+      <c r="D16" s="9" t="s">
+        <v>165</v>
+      </c>
+      <c r="E16" s="31">
+        <v>16</v>
+      </c>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
@@ -3252,7 +3357,7 @@
       <c r="M16" s="1"/>
     </row>
     <row r="17" spans="1:13" ht="150" x14ac:dyDescent="0.25">
-      <c r="A17" s="49">
+      <c r="A17" s="32">
         <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
@@ -3261,8 +3366,12 @@
       <c r="C17" s="6" t="s">
         <v>152</v>
       </c>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
+      <c r="D17" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="E17" s="31">
+        <v>16</v>
+      </c>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
@@ -3272,7 +3381,7 @@
       <c r="L17" s="1"/>
       <c r="M17" s="1"/>
     </row>
-    <row r="18" spans="1:13" ht="135" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" ht="195" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>17</v>
       </c>
@@ -3280,10 +3389,14 @@
         <v>153</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
+        <v>168</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="E18" s="31">
+        <v>16</v>
+      </c>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
@@ -3293,12 +3406,22 @@
       <c r="L18" s="1"/>
       <c r="M18" s="1"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
+    <row r="19" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+      <c r="A19" s="31">
+        <v>18</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="E19" s="31">
+        <v>8</v>
+      </c>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
@@ -3312,8 +3435,22 @@
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" xr:uid="{BD266EE8-9EE9-410E-A73B-7BCBE7209954}"/>
     <hyperlink ref="D4" r:id="rId2" xr:uid="{61BCAF91-187D-4E55-9A08-AC7DFBC537EF}"/>
+    <hyperlink ref="D5" r:id="rId3" xr:uid="{265D7779-3692-4D46-8D2F-36DDAC43DD3A}"/>
+    <hyperlink ref="D6" r:id="rId4" location="java-module-system" xr:uid="{7CF071A5-697F-456A-857B-6B68A89A54E2}"/>
+    <hyperlink ref="D7" r:id="rId5" xr:uid="{5E418898-2A4E-495A-A104-C7A030278692}"/>
+    <hyperlink ref="D9" r:id="rId6" xr:uid="{CB359587-5F3C-4D3B-B2F0-2FB99D3A9967}"/>
+    <hyperlink ref="D10" r:id="rId7" xr:uid="{BDB8C26B-4ABE-45A2-B5D1-4544AD7FA68B}"/>
+    <hyperlink ref="D11" r:id="rId8" location="private-interface-methods" xr:uid="{03D7CE78-B00A-40EC-B5F3-2AA3BD25A3F8}"/>
+    <hyperlink ref="D12" r:id="rId9" location="local-variable-type-inference" xr:uid="{ABC6A97A-A492-4F1E-B376-6B08FCF1FF79}"/>
+    <hyperlink ref="D13" r:id="rId10" xr:uid="{C5C0004D-306F-4C4E-8BB7-B950CCF159EA}"/>
+    <hyperlink ref="D14" r:id="rId11" location="switch-expressions" xr:uid="{9C27DA53-F783-4DE8-BF63-0D5BC42DFF78}"/>
+    <hyperlink ref="D15" r:id="rId12" location="using-text-blocks" xr:uid="{AF940015-A731-45B2-AF55-D061E7728FA6}"/>
+    <hyperlink ref="D16" r:id="rId13" xr:uid="{B62A518E-DC89-418B-A066-017A0CDEEBDB}"/>
+    <hyperlink ref="D17" r:id="rId14" xr:uid="{1673A8AC-A268-453A-A526-36C81C723CFF}"/>
+    <hyperlink ref="D18" r:id="rId15" xr:uid="{24EB30BC-5EF8-4524-9F31-9D4139905188}"/>
+    <hyperlink ref="D19" r:id="rId16" location="repeating-annotations" xr:uid="{056F707C-428B-48F4-87B1-E2564C8A4EC9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId17"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
tóm tắt lại day 3 và day 4
</commit_message>
<xml_diff>
--- a/Task_Result.xlsx
+++ b/Task_Result.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\beetech\java\stage1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{822770F4-1078-48BE-8ADE-30AAE786DF94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E458E459-9F28-4323-9B24-69E9706C2653}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="day2 " sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="268">
   <si>
     <t>STT</t>
   </si>
@@ -2260,12 +2260,171 @@
       <t xml:space="preserve"> được dùng để chỉ định một mảng các Exception class mà transaction sẽ không rollback khi chúng xảy ra.</t>
     </r>
   </si>
+  <si>
+    <t xml:space="preserve">Ưu điểm: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nhược điểm: </t>
+  </si>
+  <si>
+    <t>vì được sử dụng bởi nhiều luồng nên có thể bị xung đột dẫn tới kết quả không chính xác</t>
+  </si>
+  <si>
+    <t>Ưu điểm:</t>
+  </si>
+  <si>
+    <t>không cần quan tâm tới việc đồng bộ giữa các thread khác</t>
+  </si>
+  <si>
+    <t>có hiệu suất cao hơn vì đỡ chi phí đồng bộ giữa các thread</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Biến thread safe: </t>
+  </si>
+  <si>
+    <t>là biến được thiết kế đảm bảo an toàn khi thao tác trên nhiều thread mà không cần đồng bộ hóa</t>
+  </si>
+  <si>
+    <t>Dễ tồn memory vì phải tạo ra bản sao như là CopyOnWriteArrayList</t>
+  </si>
+  <si>
+    <t>Chỉ thực hiện được các phép toán đơn giản như AtomicInteger</t>
+  </si>
+  <si>
+    <t>đảm bảo tính đúng đắn mà không cần phải đồng bộ giữa các luồng</t>
+  </si>
+  <si>
+    <t>Method synchronize:</t>
+  </si>
+  <si>
+    <t>Là phương thức được đánh dấu bởi keyword synchronize để đảm bảo rằng chỉ có một thread được vào cùng một thời điểm</t>
+  </si>
+  <si>
+    <t>Tránh các tình trạng xung đột giữa các thread</t>
+  </si>
+  <si>
+    <t>DĐảm bảo nhất quán dữ liệu khi một thread đang sửa thread còn lại đang đọc</t>
+  </si>
+  <si>
+    <t>Giảm hiệu suất vì phải đồng bộ các thread với nhau</t>
+  </si>
+  <si>
+    <t>Block synchronize:</t>
+  </si>
+  <si>
+    <t>Cô lập được phần cần phải đồng bộ</t>
+  </si>
+  <si>
+    <t>Là một khối đồng bộ mà ở đó sự dụng một đối tượng để đại diên cho block đó</t>
+  </si>
+  <si>
+    <t>biến synchronized:</t>
+  </si>
+  <si>
+    <t>Là một biến được dùng để đại diện cho một khối hoặc trên chính thực thể đó khi đồng bộ giữa các thread</t>
+  </si>
+  <si>
+    <t>Thread:</t>
+  </si>
+  <si>
+    <t>Là một đối tượng trong Java đại diện cho một luồng thực thi độc lập</t>
+  </si>
+  <si>
+    <t>có thể tạo ra nhiều luồng con từ một luồng chính gia tăng hiệu suất</t>
+  </si>
+  <si>
+    <t>Dễ gây bất đồng bộ khi sử dụng nhiều luồng</t>
+  </si>
+  <si>
+    <t>mutilthread:</t>
+  </si>
+  <si>
+    <t>Là một kỹ thuật lập trình thực hiện nhiều tác vụ trong một thời điểm</t>
+  </si>
+  <si>
+    <t>Tăng hiệu suất khi thực nhiều nhiều tác vụ cùng một lúc</t>
+  </si>
+  <si>
+    <t>Dễ bị bất đồng bộ giữa các thread với nhau</t>
+  </si>
+  <si>
+    <t>Biến non-thread safe:</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> là một biến được sử dụng bởi nhiều luồng cùng một lúc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thread pool: </t>
+  </si>
+  <si>
+    <t>là một pool chứa các thread thực hiện các tác vụ trong ứng dụng đa luồng</t>
+  </si>
+  <si>
+    <t>Thay vì phải tạo 1 thread cho 1 tác vụ thì có thể tái sử dụng lại thread đang rảnh giảm bớt được memory và tăng hiệu suất</t>
+  </si>
+  <si>
+    <t>Nhược điểm:</t>
+  </si>
+  <si>
+    <t>phải tốn một lượng memory nhất định để duy trì các thread trong pool</t>
+  </si>
+  <si>
+    <t>Dễ bị trì trệ vì các thead phải chờ đợi nhau</t>
+  </si>
+  <si>
+    <t>Connection pool:</t>
+  </si>
+  <si>
+    <t>Là một kỹ thuật để tối ưu hóa việc kết nối và sử dụng cơ sở dữ liệu</t>
+  </si>
+  <si>
+    <t>Có thể tái sử dụng giúp tôi ưu hiệu suất và tài nguyên</t>
+  </si>
+  <si>
+    <t>Giảm thời gian chờ cho việc tạo các kết nối</t>
+  </si>
+  <si>
+    <t>Khó khăn trong việc cấu hình các tham số</t>
+  </si>
+  <si>
+    <t>String pool:</t>
+  </si>
+  <si>
+    <t>là một kỹ thuật được sử dụng để giảm thiểu tạo các String giống nhau</t>
+  </si>
+  <si>
+    <t>Tránh tình trạng tạo các String trùng lặp</t>
+  </si>
+  <si>
+    <t>viêc sử dụng các String khác nhau sẽ không tối ưu</t>
+  </si>
+  <si>
+    <t>Biến tham trị:</t>
+  </si>
+  <si>
+    <t>được sử dụng để truyền giá trị vào phương thức</t>
+  </si>
+  <si>
+    <t>sử dụng khi chỉ muốn truyền giá trị và không ảnh hưởng đến biến ban đầu</t>
+  </si>
+  <si>
+    <t>Không thể thay đổi trên biến được truyền vào</t>
+  </si>
+  <si>
+    <t>được sử dụng khi muốn truyền một đối tượng vào phương thức</t>
+  </si>
+  <si>
+    <t>Có thể thay đổi trực tiếp đối tượng được truyền vào</t>
+  </si>
+  <si>
+    <t>Dễ bị trỏ đến đối tượng chưa được khởi tạo</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2333,6 +2492,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -2453,7 +2619,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="88">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2542,6 +2708,21 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2575,9 +2756,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2590,42 +2768,89 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2744,14 +2969,14 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>20266</xdr:colOff>
-      <xdr:row>8</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>40532</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>5278066</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>400050</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2805,13 +3030,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>40532</xdr:colOff>
-      <xdr:row>8</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>91197</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>27592</xdr:colOff>
-      <xdr:row>33</xdr:row>
+      <xdr:row>52</xdr:row>
       <xdr:rowOff>155440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2866,13 +3091,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>81642</xdr:colOff>
-      <xdr:row>45</xdr:row>
+      <xdr:row>64</xdr:row>
       <xdr:rowOff>68035</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>5634717</xdr:colOff>
-      <xdr:row>65</xdr:row>
+      <xdr:row>84</xdr:row>
       <xdr:rowOff>182335</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2933,8 +3158,8 @@
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>12246</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>900793</xdr:rowOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>57151</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2994,8 +3219,8 @@
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>5359854</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>865413</xdr:rowOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>21771</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3052,16 +3277,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>4</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>525518</xdr:colOff>
-      <xdr:row>2</xdr:row>
+      <xdr:row>5</xdr:row>
       <xdr:rowOff>120431</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
+      <xdr:col>23</xdr:col>
       <xdr:colOff>89339</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>1125702</xdr:rowOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>151305</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3113,15 +3338,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>4</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>394138</xdr:colOff>
-      <xdr:row>6</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>43793</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
+      <xdr:col>21</xdr:col>
       <xdr:colOff>488841</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>31</xdr:row>
       <xdr:rowOff>92404</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3174,15 +3399,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>5</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>580258</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:row>35</xdr:row>
       <xdr:rowOff>65690</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
+      <xdr:col>19</xdr:col>
       <xdr:colOff>152806</xdr:colOff>
-      <xdr:row>38</xdr:row>
+      <xdr:row>49</xdr:row>
       <xdr:rowOff>136899</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3414,7 +3639,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{13A43684-D9FB-C2FA-528B-CC77DBC1FD76}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3719,7 +3944,7 @@
   <dimension ref="P1:V16"/>
   <sheetViews>
     <sheetView topLeftCell="A6" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="U31" sqref="U31"/>
+      <selection activeCell="U18" sqref="U18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3735,27 +3960,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="16:22" x14ac:dyDescent="0.25">
-      <c r="P1" s="39" t="s">
+      <c r="P1" s="44" t="s">
         <v>17</v>
       </c>
-      <c r="Q1" s="40"/>
-      <c r="R1" s="40"/>
-      <c r="S1" s="40"/>
-      <c r="T1" s="40"/>
+      <c r="Q1" s="45"/>
+      <c r="R1" s="45"/>
+      <c r="S1" s="45"/>
+      <c r="T1" s="45"/>
     </row>
     <row r="2" spans="16:22" x14ac:dyDescent="0.25">
-      <c r="P2" s="40"/>
-      <c r="Q2" s="40"/>
-      <c r="R2" s="40"/>
-      <c r="S2" s="40"/>
-      <c r="T2" s="40"/>
+      <c r="P2" s="45"/>
+      <c r="Q2" s="45"/>
+      <c r="R2" s="45"/>
+      <c r="S2" s="45"/>
+      <c r="T2" s="45"/>
     </row>
     <row r="3" spans="16:22" x14ac:dyDescent="0.25">
-      <c r="P3" s="41"/>
-      <c r="Q3" s="41"/>
-      <c r="R3" s="41"/>
-      <c r="S3" s="41"/>
-      <c r="T3" s="41"/>
+      <c r="P3" s="46"/>
+      <c r="Q3" s="46"/>
+      <c r="R3" s="46"/>
+      <c r="S3" s="46"/>
+      <c r="T3" s="46"/>
     </row>
     <row r="4" spans="16:22" x14ac:dyDescent="0.25">
       <c r="P4" s="7" t="s">
@@ -3764,11 +3989,11 @@
       <c r="Q4" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="R4" s="38" t="s">
+      <c r="R4" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="S4" s="38"/>
-      <c r="T4" s="38"/>
+      <c r="S4" s="43"/>
+      <c r="T4" s="43"/>
       <c r="U4" s="7" t="s">
         <v>18</v>
       </c>
@@ -3922,24 +4147,24 @@
       </c>
     </row>
     <row r="14" spans="16:22" x14ac:dyDescent="0.25">
-      <c r="P14" s="42" t="s">
+      <c r="P14" s="47" t="s">
         <v>73</v>
       </c>
-      <c r="Q14" s="40"/>
-      <c r="R14" s="40"/>
-      <c r="S14" s="40"/>
+      <c r="Q14" s="45"/>
+      <c r="R14" s="45"/>
+      <c r="S14" s="45"/>
     </row>
     <row r="15" spans="16:22" x14ac:dyDescent="0.25">
-      <c r="P15" s="40"/>
-      <c r="Q15" s="40"/>
-      <c r="R15" s="40"/>
-      <c r="S15" s="40"/>
+      <c r="P15" s="45"/>
+      <c r="Q15" s="45"/>
+      <c r="R15" s="45"/>
+      <c r="S15" s="45"/>
     </row>
     <row r="16" spans="16:22" x14ac:dyDescent="0.25">
-      <c r="P16" s="40"/>
-      <c r="Q16" s="40"/>
-      <c r="R16" s="40"/>
-      <c r="S16" s="40"/>
+      <c r="P16" s="45"/>
+      <c r="Q16" s="45"/>
+      <c r="R16" s="45"/>
+      <c r="S16" s="45"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -3963,10 +4188,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25977106-C04A-4BDF-83D6-AA6BE76B6728}">
-  <dimension ref="A1:N70"/>
+  <dimension ref="A1:AD89"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3974,280 +4199,759 @@
     <col min="2" max="2" width="25.42578125" customWidth="1"/>
     <col min="3" max="3" width="127.140625" customWidth="1"/>
     <col min="4" max="4" width="71.7109375" customWidth="1"/>
-    <col min="10" max="10" width="24.85546875" customWidth="1"/>
-    <col min="11" max="11" width="39.140625" customWidth="1"/>
-    <col min="12" max="12" width="72.140625" customWidth="1"/>
-    <col min="13" max="13" width="74.7109375" customWidth="1"/>
-    <col min="14" max="14" width="82.85546875" customWidth="1"/>
+    <col min="14" max="14" width="13" customWidth="1"/>
+    <col min="15" max="15" width="13.42578125" customWidth="1"/>
+    <col min="26" max="26" width="24.85546875" customWidth="1"/>
+    <col min="27" max="27" width="39.140625" customWidth="1"/>
+    <col min="28" max="28" width="72.140625" customWidth="1"/>
+    <col min="29" max="29" width="74.7109375" customWidth="1"/>
+    <col min="30" max="30" width="82.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="49.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="43" t="s">
+    <row r="1" spans="1:30" ht="49.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="48" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="44"/>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
-      <c r="F1" s="44"/>
-      <c r="G1" s="44"/>
-      <c r="H1" s="44"/>
-      <c r="I1" s="44"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="7" t="s">
+      <c r="B1" s="49"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="49"/>
+      <c r="G1" s="49"/>
+      <c r="H1" s="49"/>
+      <c r="I1" s="49"/>
+      <c r="J1" s="49"/>
+      <c r="K1" s="49"/>
+      <c r="L1" s="49"/>
+      <c r="M1" s="49"/>
+      <c r="N1" s="49"/>
+      <c r="O1" s="49"/>
+      <c r="P1" s="49"/>
+      <c r="Q1" s="39"/>
+      <c r="R1" s="39"/>
+      <c r="S1" s="39"/>
+      <c r="T1" s="39"/>
+      <c r="U1" s="39"/>
+      <c r="V1" s="39"/>
+      <c r="W1" s="39"/>
+      <c r="X1" s="39"/>
+      <c r="Y1" s="39"/>
+      <c r="Z1" s="13"/>
+      <c r="AA1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="AB1" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="M1" s="7" t="s">
+      <c r="AC1" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="N1" s="7" t="s">
+      <c r="AD1" s="7" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="126.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:30" ht="126.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="21"/>
       <c r="B2" s="19"/>
       <c r="C2" s="19"/>
       <c r="D2" s="19"/>
       <c r="E2" s="19"/>
       <c r="F2" s="19"/>
-      <c r="K2" s="3">
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
+      <c r="K2" s="19"/>
+      <c r="L2" s="19"/>
+      <c r="M2" s="19"/>
+      <c r="N2" s="70" t="s">
+        <v>244</v>
+      </c>
+      <c r="P2" t="s">
+        <v>245</v>
+      </c>
+      <c r="AA2" s="3">
         <v>1</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="AB2" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="M2" s="6" t="s">
+      <c r="AC2" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="N2" s="10" t="s">
+      <c r="AD2" s="10" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="90" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:30" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="14"/>
       <c r="B3" s="15"/>
       <c r="C3" s="16"/>
       <c r="D3" s="17"/>
-      <c r="K3" s="3">
+      <c r="O3" t="s">
+        <v>216</v>
+      </c>
+      <c r="P3" t="s">
+        <v>217</v>
+      </c>
+      <c r="AA3" s="3">
         <v>2</v>
       </c>
-      <c r="L3" s="2" t="s">
+      <c r="AB3" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="M3" s="6" t="s">
+      <c r="AC3" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="N3" s="12" t="s">
+      <c r="AD3" s="12" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:30" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="14"/>
       <c r="B4" s="15"/>
       <c r="C4" s="16"/>
       <c r="D4" s="18"/>
-      <c r="K4" s="3">
+      <c r="O4" t="s">
+        <v>218</v>
+      </c>
+      <c r="P4" t="s">
+        <v>219</v>
+      </c>
+      <c r="AA4" s="64">
         <v>3</v>
       </c>
-      <c r="L4" s="2" t="s">
+      <c r="AB4" s="64" t="s">
         <v>35</v>
       </c>
-      <c r="M4" s="6" t="s">
+      <c r="AC4" s="73" t="s">
         <v>38</v>
       </c>
-      <c r="N4" s="11" t="s">
+      <c r="AD4" s="76" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="238.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="14"/>
       <c r="B5" s="15"/>
       <c r="C5" s="16"/>
       <c r="D5" s="18"/>
-      <c r="K5" s="3">
+      <c r="P5" t="s">
+        <v>220</v>
+      </c>
+      <c r="AA5" s="65"/>
+      <c r="AB5" s="65"/>
+      <c r="AC5" s="74"/>
+      <c r="AD5" s="77"/>
+    </row>
+    <row r="6" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="14"/>
+      <c r="B6" s="15"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="18"/>
+      <c r="N6" s="70" t="s">
+        <v>221</v>
+      </c>
+      <c r="P6" t="s">
+        <v>222</v>
+      </c>
+      <c r="AA6" s="66"/>
+      <c r="AB6" s="66"/>
+      <c r="AC6" s="75"/>
+      <c r="AD6" s="78"/>
+    </row>
+    <row r="7" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="14"/>
+      <c r="B7" s="15"/>
+      <c r="C7" s="16"/>
+      <c r="D7" s="18"/>
+      <c r="O7" t="s">
+        <v>216</v>
+      </c>
+      <c r="P7" t="s">
+        <v>223</v>
+      </c>
+      <c r="AA7" s="64">
         <v>4</v>
       </c>
-      <c r="L5" s="2" t="s">
+      <c r="AB7" s="64" t="s">
         <v>36</v>
       </c>
-      <c r="M5" s="6" t="s">
+      <c r="AC7" s="73" t="s">
         <v>39</v>
       </c>
-      <c r="N5" s="11" t="s">
+      <c r="AD7" s="76" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="129.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="45" t="s">
+    <row r="8" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="14"/>
+      <c r="B8" s="15"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="18"/>
+      <c r="P8" t="s">
+        <v>224</v>
+      </c>
+      <c r="AA8" s="65"/>
+      <c r="AB8" s="65"/>
+      <c r="AC8" s="74"/>
+      <c r="AD8" s="77"/>
+    </row>
+    <row r="9" spans="1:30" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="14"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="18"/>
+      <c r="O9" t="s">
+        <v>215</v>
+      </c>
+      <c r="P9" t="s">
+        <v>225</v>
+      </c>
+      <c r="AA9" s="66"/>
+      <c r="AB9" s="66"/>
+      <c r="AC9" s="75"/>
+      <c r="AD9" s="78"/>
+    </row>
+    <row r="10" spans="1:30" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="50" t="s">
         <v>54</v>
       </c>
-      <c r="B6" s="46"/>
-      <c r="C6" s="46"/>
-      <c r="D6" s="46"/>
-      <c r="E6" s="46"/>
-      <c r="K6" s="3">
+      <c r="B10" s="51"/>
+      <c r="C10" s="51"/>
+      <c r="D10" s="51"/>
+      <c r="E10" s="51"/>
+      <c r="F10" s="19"/>
+      <c r="G10" s="19"/>
+      <c r="H10" s="19"/>
+      <c r="I10" s="19"/>
+      <c r="N10" s="70" t="s">
+        <v>226</v>
+      </c>
+      <c r="P10" t="s">
+        <v>227</v>
+      </c>
+      <c r="AA10" s="63">
         <v>5</v>
       </c>
-      <c r="L6" s="1" t="s">
+      <c r="AB10" s="79" t="s">
         <v>37</v>
       </c>
-      <c r="M6" s="4" t="s">
+      <c r="AC10" s="71" t="s">
         <v>51</v>
       </c>
-      <c r="N6" s="9" t="s">
+      <c r="AD10" s="72" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="108" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="42" t="s">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="O11" t="s">
+        <v>218</v>
+      </c>
+      <c r="P11" t="s">
+        <v>228</v>
+      </c>
+      <c r="AA11" s="63"/>
+      <c r="AB11" s="79"/>
+      <c r="AC11" s="71"/>
+      <c r="AD11" s="72"/>
+    </row>
+    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="P12" t="s">
+        <v>229</v>
+      </c>
+      <c r="AA12" s="63"/>
+      <c r="AB12" s="79"/>
+      <c r="AC12" s="71"/>
+      <c r="AD12" s="72"/>
+    </row>
+    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="O13" t="s">
+        <v>216</v>
+      </c>
+      <c r="P13" t="s">
+        <v>230</v>
+      </c>
+      <c r="AA13" s="63"/>
+      <c r="AB13" s="79"/>
+      <c r="AC13" s="71"/>
+      <c r="AD13" s="72"/>
+    </row>
+    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="N14" s="70" t="s">
+        <v>231</v>
+      </c>
+      <c r="P14" t="s">
+        <v>233</v>
+      </c>
+      <c r="AA14" s="63"/>
+      <c r="AB14" s="79"/>
+      <c r="AC14" s="71"/>
+      <c r="AD14" s="72"/>
+    </row>
+    <row r="15" spans="1:30" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="40"/>
+      <c r="B15" s="19"/>
+      <c r="C15" s="19"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="19"/>
+      <c r="F15" s="19"/>
+      <c r="G15" s="19"/>
+      <c r="H15" s="19"/>
+      <c r="I15" s="19"/>
+      <c r="O15" t="s">
+        <v>218</v>
+      </c>
+      <c r="P15" t="s">
+        <v>232</v>
+      </c>
+      <c r="AA15" s="63"/>
+      <c r="AB15" s="79"/>
+      <c r="AC15" s="71"/>
+      <c r="AD15" s="72"/>
+    </row>
+    <row r="16" spans="1:30" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="40"/>
+      <c r="B16" s="19"/>
+      <c r="C16" s="19"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="19"/>
+      <c r="F16" s="19"/>
+      <c r="G16" s="19"/>
+      <c r="H16" s="19"/>
+      <c r="I16" s="19"/>
+      <c r="P16" t="s">
+        <v>228</v>
+      </c>
+      <c r="AA16" s="63"/>
+      <c r="AB16" s="79"/>
+      <c r="AC16" s="71"/>
+      <c r="AD16" s="72"/>
+    </row>
+    <row r="17" spans="1:30" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="40"/>
+      <c r="B17" s="19"/>
+      <c r="C17" s="19"/>
+      <c r="D17" s="19"/>
+      <c r="E17" s="19"/>
+      <c r="F17" s="19"/>
+      <c r="G17" s="19"/>
+      <c r="H17" s="19"/>
+      <c r="I17" s="19"/>
+      <c r="P17" t="s">
+        <v>229</v>
+      </c>
+      <c r="AA17" s="63"/>
+      <c r="AB17" s="79"/>
+      <c r="AC17" s="71"/>
+      <c r="AD17" s="72"/>
+    </row>
+    <row r="18" spans="1:30" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="40"/>
+      <c r="B18" s="19"/>
+      <c r="C18" s="19"/>
+      <c r="D18" s="19"/>
+      <c r="E18" s="19"/>
+      <c r="F18" s="19"/>
+      <c r="G18" s="19"/>
+      <c r="H18" s="19"/>
+      <c r="I18" s="19"/>
+      <c r="O18" t="s">
+        <v>216</v>
+      </c>
+      <c r="P18" t="s">
+        <v>230</v>
+      </c>
+      <c r="AA18" s="63"/>
+      <c r="AB18" s="79"/>
+      <c r="AC18" s="71"/>
+      <c r="AD18" s="72"/>
+    </row>
+    <row r="19" spans="1:30" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="40"/>
+      <c r="B19" s="19"/>
+      <c r="C19" s="19"/>
+      <c r="D19" s="19"/>
+      <c r="E19" s="19"/>
+      <c r="F19" s="19"/>
+      <c r="G19" s="19"/>
+      <c r="H19" s="19"/>
+      <c r="I19" s="19"/>
+      <c r="N19" s="70" t="s">
+        <v>234</v>
+      </c>
+      <c r="P19" t="s">
+        <v>235</v>
+      </c>
+      <c r="AA19" s="63"/>
+      <c r="AB19" s="79"/>
+      <c r="AC19" s="71"/>
+      <c r="AD19" s="72"/>
+    </row>
+    <row r="20" spans="1:30" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="40"/>
+      <c r="B20" s="19"/>
+      <c r="C20" s="19"/>
+      <c r="D20" s="19"/>
+      <c r="E20" s="19"/>
+      <c r="F20" s="19"/>
+      <c r="G20" s="19"/>
+      <c r="H20" s="19"/>
+      <c r="I20" s="19"/>
+      <c r="N20" s="70" t="s">
+        <v>236</v>
+      </c>
+      <c r="O20" t="s">
+        <v>237</v>
+      </c>
+      <c r="AA20" s="63"/>
+      <c r="AB20" s="79"/>
+      <c r="AC20" s="71"/>
+      <c r="AD20" s="72"/>
+    </row>
+    <row r="21" spans="1:30" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="40"/>
+      <c r="B21" s="19"/>
+      <c r="C21" s="19"/>
+      <c r="D21" s="19"/>
+      <c r="E21" s="19"/>
+      <c r="F21" s="19"/>
+      <c r="G21" s="19"/>
+      <c r="H21" s="19"/>
+      <c r="I21" s="19"/>
+      <c r="O21" t="s">
+        <v>218</v>
+      </c>
+      <c r="P21" t="s">
+        <v>238</v>
+      </c>
+      <c r="AA21" s="63"/>
+      <c r="AB21" s="79"/>
+      <c r="AC21" s="71"/>
+      <c r="AD21" s="72"/>
+    </row>
+    <row r="22" spans="1:30" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="40"/>
+      <c r="B22" s="19"/>
+      <c r="C22" s="19"/>
+      <c r="D22" s="19"/>
+      <c r="E22" s="19"/>
+      <c r="F22" s="19"/>
+      <c r="G22" s="19"/>
+      <c r="H22" s="19"/>
+      <c r="I22" s="19"/>
+      <c r="O22" t="s">
+        <v>216</v>
+      </c>
+      <c r="P22" t="s">
+        <v>239</v>
+      </c>
+      <c r="AA22" s="63"/>
+      <c r="AB22" s="79"/>
+      <c r="AC22" s="71"/>
+      <c r="AD22" s="72"/>
+    </row>
+    <row r="23" spans="1:30" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="40"/>
+      <c r="B23" s="19"/>
+      <c r="C23" s="19"/>
+      <c r="D23" s="19"/>
+      <c r="E23" s="19"/>
+      <c r="F23" s="19"/>
+      <c r="G23" s="19"/>
+      <c r="H23" s="19"/>
+      <c r="I23" s="19"/>
+      <c r="N23" s="70" t="s">
+        <v>240</v>
+      </c>
+      <c r="O23" t="s">
+        <v>241</v>
+      </c>
+      <c r="AA23" s="63"/>
+      <c r="AB23" s="79"/>
+      <c r="AC23" s="71"/>
+      <c r="AD23" s="72"/>
+    </row>
+    <row r="24" spans="1:30" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="40"/>
+      <c r="B24" s="19"/>
+      <c r="C24" s="19"/>
+      <c r="D24" s="19"/>
+      <c r="E24" s="19"/>
+      <c r="F24" s="19"/>
+      <c r="G24" s="19"/>
+      <c r="H24" s="19"/>
+      <c r="I24" s="19"/>
+      <c r="O24" t="s">
+        <v>218</v>
+      </c>
+      <c r="P24" t="s">
+        <v>242</v>
+      </c>
+      <c r="AA24" s="63"/>
+      <c r="AB24" s="79"/>
+      <c r="AC24" s="71"/>
+      <c r="AD24" s="72"/>
+    </row>
+    <row r="25" spans="1:30" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="40"/>
+      <c r="B25" s="19"/>
+      <c r="C25" s="19"/>
+      <c r="D25" s="19"/>
+      <c r="E25" s="19"/>
+      <c r="F25" s="19"/>
+      <c r="G25" s="19"/>
+      <c r="H25" s="19"/>
+      <c r="I25" s="19"/>
+      <c r="O25" t="s">
+        <v>216</v>
+      </c>
+      <c r="P25" t="s">
+        <v>243</v>
+      </c>
+      <c r="AA25" s="63"/>
+      <c r="AB25" s="79"/>
+      <c r="AC25" s="71"/>
+      <c r="AD25" s="72"/>
+    </row>
+    <row r="26" spans="1:30" ht="108" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="47" t="s">
         <v>42</v>
       </c>
-      <c r="B7" s="42"/>
-      <c r="C7" s="42"/>
-      <c r="D7" s="42" t="s">
+      <c r="B26" s="47"/>
+      <c r="C26" s="47"/>
+      <c r="D26" s="47" t="s">
         <v>43</v>
       </c>
-      <c r="E7" s="49"/>
-      <c r="F7" s="49"/>
-      <c r="G7" s="49"/>
-      <c r="H7" s="49"/>
-      <c r="I7" s="49"/>
-      <c r="J7" s="49"/>
-      <c r="K7" s="3">
+      <c r="E26" s="47"/>
+      <c r="F26" s="47"/>
+      <c r="G26" s="47"/>
+      <c r="H26" s="47"/>
+      <c r="I26" s="47"/>
+      <c r="J26" s="67"/>
+      <c r="K26" s="67"/>
+      <c r="L26" s="67"/>
+      <c r="M26" s="67"/>
+      <c r="N26" s="67"/>
+      <c r="O26" s="67"/>
+      <c r="P26" s="67"/>
+      <c r="Q26" s="67"/>
+      <c r="R26" s="67"/>
+      <c r="S26" s="67"/>
+      <c r="T26" s="67"/>
+      <c r="U26" s="67"/>
+      <c r="V26" s="67"/>
+      <c r="W26" s="67"/>
+      <c r="X26" s="67"/>
+      <c r="Y26" s="67"/>
+      <c r="Z26" s="67"/>
+      <c r="AA26" s="3">
         <v>6</v>
       </c>
-      <c r="L7" s="2" t="s">
+      <c r="AB26" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="M7" s="4" t="s">
+      <c r="AC26" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="N7" s="1"/>
-    </row>
-    <row r="8" spans="1:14" ht="139.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="42"/>
-      <c r="B8" s="42"/>
-      <c r="C8" s="42"/>
-      <c r="D8" s="49"/>
-      <c r="E8" s="49"/>
-      <c r="F8" s="49"/>
-      <c r="G8" s="49"/>
-      <c r="H8" s="49"/>
-      <c r="I8" s="49"/>
-      <c r="J8" s="49"/>
-      <c r="K8" s="3">
+      <c r="AD26" s="1"/>
+    </row>
+    <row r="27" spans="1:30" ht="139.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="47"/>
+      <c r="B27" s="47"/>
+      <c r="C27" s="47"/>
+      <c r="D27" s="47"/>
+      <c r="E27" s="47"/>
+      <c r="F27" s="47"/>
+      <c r="G27" s="47"/>
+      <c r="H27" s="47"/>
+      <c r="I27" s="47"/>
+      <c r="J27" s="67"/>
+      <c r="K27" s="67"/>
+      <c r="L27" s="67"/>
+      <c r="M27" s="67"/>
+      <c r="N27" s="67"/>
+      <c r="O27" s="67"/>
+      <c r="P27" s="67"/>
+      <c r="Q27" s="67"/>
+      <c r="R27" s="67"/>
+      <c r="S27" s="67"/>
+      <c r="T27" s="67"/>
+      <c r="U27" s="67"/>
+      <c r="V27" s="67"/>
+      <c r="W27" s="67"/>
+      <c r="X27" s="67"/>
+      <c r="Y27" s="67"/>
+      <c r="Z27" s="67"/>
+      <c r="AA27" s="3">
         <v>7</v>
       </c>
-      <c r="L8" s="2" t="s">
+      <c r="AB27" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="M8" s="4" t="s">
+      <c r="AC27" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="N8" s="1"/>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D35" s="50" t="s">
+      <c r="AD27" s="1"/>
+    </row>
+    <row r="54" spans="1:26" ht="42" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D54" s="54" t="s">
         <v>44</v>
       </c>
-      <c r="E35" s="40"/>
-      <c r="F35" s="40"/>
-      <c r="G35" s="40"/>
-      <c r="H35" s="40"/>
-      <c r="I35" s="40"/>
-      <c r="J35" s="40"/>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D36" s="40"/>
-      <c r="E36" s="40"/>
-      <c r="F36" s="40"/>
-      <c r="G36" s="40"/>
-      <c r="H36" s="40"/>
-      <c r="I36" s="40"/>
-      <c r="J36" s="40"/>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D37" s="40"/>
-      <c r="E37" s="40"/>
-      <c r="F37" s="40"/>
-      <c r="G37" s="40"/>
-      <c r="H37" s="40"/>
-      <c r="I37" s="40"/>
-      <c r="J37" s="40"/>
-    </row>
-    <row r="39" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A39" s="48" t="s">
+      <c r="E54" s="54"/>
+      <c r="F54" s="54"/>
+      <c r="G54" s="54"/>
+      <c r="H54" s="54"/>
+      <c r="I54" s="54"/>
+      <c r="J54" s="54"/>
+      <c r="K54" s="69"/>
+      <c r="L54" s="69"/>
+      <c r="M54" s="69"/>
+      <c r="N54" s="69"/>
+      <c r="O54" s="69"/>
+      <c r="P54" s="69"/>
+      <c r="Q54" s="69"/>
+      <c r="R54" s="69"/>
+      <c r="S54" s="69"/>
+      <c r="T54" s="69"/>
+      <c r="U54" s="69"/>
+      <c r="V54" s="69"/>
+      <c r="W54" s="69"/>
+      <c r="X54" s="69"/>
+      <c r="Y54" s="69"/>
+      <c r="Z54" s="69"/>
+    </row>
+    <row r="55" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="D55" s="69"/>
+      <c r="E55" s="69"/>
+      <c r="F55" s="69"/>
+      <c r="G55" s="69"/>
+      <c r="H55" s="69"/>
+      <c r="I55" s="69"/>
+      <c r="J55" s="69"/>
+      <c r="K55" s="69"/>
+      <c r="L55" s="69"/>
+      <c r="M55" s="69"/>
+      <c r="N55" s="69"/>
+      <c r="O55" s="69"/>
+      <c r="P55" s="69"/>
+      <c r="Q55" s="69"/>
+      <c r="R55" s="69"/>
+      <c r="S55" s="69"/>
+      <c r="T55" s="69"/>
+      <c r="U55" s="69"/>
+      <c r="V55" s="69"/>
+      <c r="W55" s="69"/>
+      <c r="X55" s="69"/>
+      <c r="Y55" s="69"/>
+      <c r="Z55" s="69"/>
+    </row>
+    <row r="56" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="D56" s="69"/>
+      <c r="E56" s="69"/>
+      <c r="F56" s="69"/>
+      <c r="G56" s="69"/>
+      <c r="H56" s="69"/>
+      <c r="I56" s="69"/>
+      <c r="J56" s="69"/>
+      <c r="K56" s="69"/>
+      <c r="L56" s="69"/>
+      <c r="M56" s="69"/>
+      <c r="N56" s="69"/>
+      <c r="O56" s="69"/>
+      <c r="P56" s="69"/>
+      <c r="Q56" s="69"/>
+      <c r="R56" s="69"/>
+      <c r="S56" s="69"/>
+      <c r="T56" s="69"/>
+      <c r="U56" s="69"/>
+      <c r="V56" s="69"/>
+      <c r="W56" s="69"/>
+      <c r="X56" s="69"/>
+      <c r="Y56" s="69"/>
+      <c r="Z56" s="69"/>
+    </row>
+    <row r="58" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A58" s="53" t="s">
         <v>41</v>
       </c>
-      <c r="B39" s="48"/>
-      <c r="C39" s="48"/>
-      <c r="D39" s="20"/>
-    </row>
-    <row r="40" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="48"/>
-      <c r="B40" s="48"/>
-      <c r="C40" s="48"/>
-    </row>
-    <row r="41" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="48"/>
-      <c r="B41" s="48"/>
-      <c r="C41" s="48"/>
-    </row>
-    <row r="42" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="48"/>
-      <c r="B42" s="48"/>
-      <c r="C42" s="48"/>
-    </row>
-    <row r="43" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="42" t="s">
+      <c r="B58" s="53"/>
+      <c r="C58" s="53"/>
+      <c r="D58" s="20"/>
+    </row>
+    <row r="59" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="53"/>
+      <c r="B59" s="53"/>
+      <c r="C59" s="53"/>
+    </row>
+    <row r="60" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="53"/>
+      <c r="B60" s="53"/>
+      <c r="C60" s="53"/>
+    </row>
+    <row r="61" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="53"/>
+      <c r="B61" s="53"/>
+      <c r="C61" s="53"/>
+    </row>
+    <row r="62" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="47" t="s">
         <v>45</v>
       </c>
-      <c r="B43" s="42"/>
-      <c r="C43" s="42"/>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A44" s="42"/>
-      <c r="B44" s="42"/>
-      <c r="C44" s="42"/>
-    </row>
-    <row r="68" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="47" t="s">
+      <c r="B62" s="47"/>
+      <c r="C62" s="47"/>
+    </row>
+    <row r="63" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A63" s="47"/>
+      <c r="B63" s="47"/>
+      <c r="C63" s="47"/>
+    </row>
+    <row r="87" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A87" s="52" t="s">
         <v>46</v>
       </c>
-      <c r="B68" s="47"/>
-      <c r="C68" s="47"/>
-    </row>
-    <row r="69" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="47"/>
-      <c r="B69" s="47"/>
-      <c r="C69" s="47"/>
-    </row>
-    <row r="70" spans="1:3" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="47"/>
-      <c r="B70" s="47"/>
-      <c r="C70" s="47"/>
+      <c r="B87" s="52"/>
+      <c r="C87" s="52"/>
+    </row>
+    <row r="88" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A88" s="52"/>
+      <c r="B88" s="52"/>
+      <c r="C88" s="52"/>
+    </row>
+    <row r="89" spans="1:3" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A89" s="52"/>
+      <c r="B89" s="52"/>
+      <c r="C89" s="52"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A6:E6"/>
-    <mergeCell ref="A68:C70"/>
-    <mergeCell ref="A39:C42"/>
-    <mergeCell ref="A7:C8"/>
-    <mergeCell ref="D7:J8"/>
-    <mergeCell ref="D35:J37"/>
-    <mergeCell ref="A43:C44"/>
+  <mergeCells count="20">
+    <mergeCell ref="AA10:AA25"/>
+    <mergeCell ref="AB10:AB25"/>
+    <mergeCell ref="AC10:AC25"/>
+    <mergeCell ref="AD10:AD25"/>
+    <mergeCell ref="AA4:AA6"/>
+    <mergeCell ref="AB4:AB6"/>
+    <mergeCell ref="AC4:AC6"/>
+    <mergeCell ref="AD4:AD6"/>
+    <mergeCell ref="AA7:AA9"/>
+    <mergeCell ref="AB7:AB9"/>
+    <mergeCell ref="AC7:AC9"/>
+    <mergeCell ref="AD7:AD9"/>
+    <mergeCell ref="A1:P1"/>
+    <mergeCell ref="A10:E10"/>
+    <mergeCell ref="A87:C89"/>
+    <mergeCell ref="A58:C61"/>
+    <mergeCell ref="A26:C27"/>
+    <mergeCell ref="A62:C63"/>
+    <mergeCell ref="D26:I27"/>
+    <mergeCell ref="D54:J54"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="N2" r:id="rId1" display="https://stackoverflow.com/questions/15070513/how-to-test-a-non-thread-safe-class" xr:uid="{AF80577A-A125-48C9-AA50-5BBE662AA378}"/>
-    <hyperlink ref="N3" r:id="rId2" display="https://www.baeldung.com/java-thread-safety" xr:uid="{C1945518-65A5-43C4-A7C3-0AB5B0EA6DE6}"/>
-    <hyperlink ref="N4" r:id="rId3" xr:uid="{F6BBD934-A547-4D3A-A18E-DBB296712BB7}"/>
-    <hyperlink ref="N5" r:id="rId4" xr:uid="{AB87879D-41CA-4D0A-BC91-EEAA9A792E8B}"/>
-    <hyperlink ref="N6" r:id="rId5" location="4-reentrancy" xr:uid="{F4526B1D-3B6D-4BBD-A91D-7781541ECE62}"/>
+    <hyperlink ref="AD2" r:id="rId1" display="https://stackoverflow.com/questions/15070513/how-to-test-a-non-thread-safe-class" xr:uid="{AF80577A-A125-48C9-AA50-5BBE662AA378}"/>
+    <hyperlink ref="AD3" r:id="rId2" display="https://www.baeldung.com/java-thread-safety" xr:uid="{C1945518-65A5-43C4-A7C3-0AB5B0EA6DE6}"/>
+    <hyperlink ref="AD4" r:id="rId3" xr:uid="{F6BBD934-A547-4D3A-A18E-DBB296712BB7}"/>
+    <hyperlink ref="AD7" r:id="rId4" xr:uid="{AB87879D-41CA-4D0A-BC91-EEAA9A792E8B}"/>
+    <hyperlink ref="AD10" r:id="rId5" location="4-reentrancy" xr:uid="{F4526B1D-3B6D-4BBD-A91D-7781541ECE62}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId6"/>
@@ -4257,296 +4961,555 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9C39CBF-243C-46B8-A97D-C9A6BCF6006E}">
-  <dimension ref="A1:Q41"/>
+  <dimension ref="A1:W52"/>
   <sheetViews>
     <sheetView zoomScale="87" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="22.7109375" customWidth="1"/>
-    <col min="3" max="3" width="115.140625" customWidth="1"/>
-    <col min="4" max="4" width="68.7109375" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" customWidth="1"/>
+    <col min="1" max="1" width="15.5703125" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" customWidth="1"/>
+    <col min="6" max="6" width="88.5703125" customWidth="1"/>
+    <col min="8" max="8" width="22.7109375" customWidth="1"/>
+    <col min="9" max="9" width="115.140625" customWidth="1"/>
+    <col min="10" max="10" width="68.7109375" customWidth="1"/>
+    <col min="11" max="11" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="G1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="H1" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="25" t="s">
+      <c r="I1" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="D1" s="24" t="s">
+      <c r="J1" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="13"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
-      <c r="K1" s="28"/>
-    </row>
-    <row r="2" spans="1:17" ht="110.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="3">
+      <c r="K1" s="13"/>
+      <c r="L1" s="28"/>
+      <c r="M1" s="28"/>
+      <c r="N1" s="28"/>
+      <c r="O1" s="28"/>
+      <c r="P1" s="28"/>
+      <c r="Q1" s="28"/>
+    </row>
+    <row r="2" spans="1:23" ht="110.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="70" t="s">
+        <v>246</v>
+      </c>
+      <c r="B2" t="s">
+        <v>247</v>
+      </c>
+      <c r="G2" s="58">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="H2" s="58" t="s">
         <v>56</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="I2" s="73" t="s">
         <v>57</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="J2" s="80" t="s">
         <v>58</v>
       </c>
-      <c r="F2" s="42" t="s">
+      <c r="L2" s="47" t="s">
         <v>68</v>
       </c>
-      <c r="G2" s="40"/>
-      <c r="H2" s="40"/>
-      <c r="I2" s="40"/>
-      <c r="J2" s="40"/>
-      <c r="K2" s="40"/>
-      <c r="L2" s="40"/>
-      <c r="M2" s="40"/>
-      <c r="N2" s="40"/>
-      <c r="O2" s="40"/>
-      <c r="P2" s="40"/>
-      <c r="Q2" s="40"/>
-    </row>
-    <row r="3" spans="1:17" ht="110.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
+      <c r="M2" s="45"/>
+      <c r="N2" s="45"/>
+      <c r="O2" s="45"/>
+      <c r="P2" s="45"/>
+      <c r="Q2" s="45"/>
+      <c r="R2" s="45"/>
+      <c r="S2" s="45"/>
+      <c r="T2" s="45"/>
+      <c r="U2" s="45"/>
+      <c r="V2" s="45"/>
+      <c r="W2" s="45"/>
+    </row>
+    <row r="3" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B3" t="s">
+        <v>218</v>
+      </c>
+      <c r="C3" t="s">
+        <v>248</v>
+      </c>
+      <c r="G3" s="60"/>
+      <c r="H3" s="60"/>
+      <c r="I3" s="74"/>
+      <c r="J3" s="81"/>
+      <c r="L3" s="38"/>
+      <c r="M3" s="23"/>
+      <c r="N3" s="23"/>
+      <c r="O3" s="23"/>
+      <c r="P3" s="23"/>
+      <c r="Q3" s="23"/>
+      <c r="R3" s="23"/>
+      <c r="S3" s="23"/>
+      <c r="T3" s="23"/>
+      <c r="U3" s="23"/>
+      <c r="V3" s="23"/>
+      <c r="W3" s="23"/>
+    </row>
+    <row r="4" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B4" t="s">
+        <v>249</v>
+      </c>
+      <c r="C4" t="s">
+        <v>250</v>
+      </c>
+      <c r="G4" s="60"/>
+      <c r="H4" s="60"/>
+      <c r="I4" s="74"/>
+      <c r="J4" s="81"/>
+      <c r="L4" s="38"/>
+      <c r="M4" s="23"/>
+      <c r="N4" s="23"/>
+      <c r="O4" s="23"/>
+      <c r="P4" s="23"/>
+      <c r="Q4" s="23"/>
+      <c r="R4" s="23"/>
+      <c r="S4" s="23"/>
+      <c r="T4" s="23"/>
+      <c r="U4" s="23"/>
+      <c r="V4" s="23"/>
+      <c r="W4" s="23"/>
+    </row>
+    <row r="5" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="C5" t="s">
+        <v>251</v>
+      </c>
+      <c r="G5" s="59"/>
+      <c r="H5" s="59"/>
+      <c r="I5" s="75"/>
+      <c r="J5" s="82"/>
+      <c r="L5" s="38"/>
+      <c r="M5" s="23"/>
+      <c r="N5" s="23"/>
+      <c r="O5" s="23"/>
+      <c r="P5" s="23"/>
+      <c r="Q5" s="23"/>
+      <c r="R5" s="23"/>
+      <c r="S5" s="23"/>
+      <c r="T5" s="23"/>
+      <c r="U5" s="23"/>
+      <c r="V5" s="23"/>
+      <c r="W5" s="23"/>
+    </row>
+    <row r="6" spans="1:23" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="70" t="s">
+        <v>252</v>
+      </c>
+      <c r="B6" t="s">
+        <v>253</v>
+      </c>
+      <c r="G6" s="58">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="H6" s="58" t="s">
         <v>59</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="I6" s="73" t="s">
         <v>60</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="J6" s="83" t="s">
         <v>72</v>
       </c>
-      <c r="G3" s="26"/>
-    </row>
-    <row r="4" spans="1:17" ht="90" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
+      <c r="M6" s="26"/>
+    </row>
+    <row r="7" spans="1:23" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>218</v>
+      </c>
+      <c r="C7" t="s">
+        <v>254</v>
+      </c>
+      <c r="G7" s="60"/>
+      <c r="H7" s="60"/>
+      <c r="I7" s="74"/>
+      <c r="J7" s="84"/>
+      <c r="M7" s="26"/>
+    </row>
+    <row r="8" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>255</v>
+      </c>
+      <c r="G8" s="60"/>
+      <c r="H8" s="60"/>
+      <c r="I8" s="74"/>
+      <c r="J8" s="84"/>
+      <c r="M8" s="26"/>
+    </row>
+    <row r="9" spans="1:23" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>249</v>
+      </c>
+      <c r="C9" t="s">
+        <v>256</v>
+      </c>
+      <c r="G9" s="59"/>
+      <c r="H9" s="59"/>
+      <c r="I9" s="75"/>
+      <c r="J9" s="85"/>
+      <c r="M9" s="26"/>
+    </row>
+    <row r="10" spans="1:23" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="70" t="s">
+        <v>257</v>
+      </c>
+      <c r="B10" t="s">
+        <v>258</v>
+      </c>
+      <c r="G10" s="58">
         <v>3</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="H10" s="58" t="s">
         <v>61</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="I10" s="73" t="s">
         <v>62</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="J10" s="83" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>218</v>
+      </c>
+      <c r="C11" t="s">
+        <v>259</v>
+      </c>
+      <c r="G11" s="60"/>
+      <c r="H11" s="60"/>
+      <c r="I11" s="74"/>
+      <c r="J11" s="84"/>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>249</v>
+      </c>
+      <c r="C12" t="s">
+        <v>260</v>
+      </c>
+      <c r="G12" s="60"/>
+      <c r="H12" s="60"/>
+      <c r="I12" s="74"/>
+      <c r="J12" s="84"/>
+    </row>
+    <row r="13" spans="1:23" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="70" t="s">
+        <v>261</v>
+      </c>
+      <c r="B13" t="s">
+        <v>262</v>
+      </c>
+      <c r="G13" s="58">
         <v>4</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="H13" s="58" t="s">
         <v>66</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="I13" s="73" t="s">
         <v>65</v>
       </c>
-      <c r="D5" s="3"/>
-      <c r="E5" s="51" t="s">
+      <c r="J13" s="58"/>
+      <c r="K13" s="55" t="s">
         <v>69</v>
       </c>
-      <c r="F5" s="40"/>
-      <c r="G5" s="40"/>
-      <c r="H5" s="40"/>
-      <c r="I5" s="40"/>
-      <c r="J5" s="40"/>
-      <c r="K5" s="40"/>
-      <c r="L5" s="40"/>
-      <c r="M5" s="40"/>
-      <c r="N5" s="40"/>
-      <c r="O5" s="40"/>
-      <c r="P5" s="40"/>
-      <c r="Q5" s="40"/>
-    </row>
-    <row r="6" spans="1:17" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
+      <c r="L13" s="45"/>
+      <c r="M13" s="45"/>
+      <c r="N13" s="45"/>
+      <c r="O13" s="45"/>
+      <c r="P13" s="45"/>
+      <c r="Q13" s="45"/>
+      <c r="R13" s="45"/>
+      <c r="S13" s="45"/>
+      <c r="T13" s="45"/>
+      <c r="U13" s="45"/>
+      <c r="V13" s="45"/>
+      <c r="W13" s="45"/>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>218</v>
+      </c>
+      <c r="C14" t="s">
+        <v>263</v>
+      </c>
+      <c r="G14" s="60"/>
+      <c r="H14" s="60"/>
+      <c r="I14" s="74"/>
+      <c r="J14" s="60"/>
+      <c r="K14" s="55"/>
+      <c r="L14" s="45"/>
+      <c r="M14" s="45"/>
+      <c r="N14" s="45"/>
+      <c r="O14" s="45"/>
+      <c r="P14" s="45"/>
+      <c r="Q14" s="45"/>
+      <c r="R14" s="45"/>
+      <c r="S14" s="45"/>
+      <c r="T14" s="45"/>
+      <c r="U14" s="45"/>
+      <c r="V14" s="45"/>
+      <c r="W14" s="45"/>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>249</v>
+      </c>
+      <c r="C15" t="s">
+        <v>264</v>
+      </c>
+      <c r="G15" s="59"/>
+      <c r="H15" s="59"/>
+      <c r="I15" s="75"/>
+      <c r="J15" s="59"/>
+      <c r="K15" s="55"/>
+      <c r="L15" s="45"/>
+      <c r="M15" s="45"/>
+      <c r="N15" s="45"/>
+      <c r="O15" s="45"/>
+      <c r="P15" s="45"/>
+      <c r="Q15" s="45"/>
+      <c r="R15" s="45"/>
+      <c r="S15" s="45"/>
+      <c r="T15" s="45"/>
+      <c r="U15" s="45"/>
+      <c r="V15" s="45"/>
+      <c r="W15" s="45"/>
+    </row>
+    <row r="16" spans="1:23" ht="45" x14ac:dyDescent="0.25">
+      <c r="A16" s="70" t="s">
+        <v>64</v>
+      </c>
+      <c r="B16" t="s">
+        <v>265</v>
+      </c>
+      <c r="G16" s="3">
         <v>5</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="H16" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="I16" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="D6" s="3"/>
-      <c r="E6" s="52"/>
-      <c r="F6" s="40"/>
-      <c r="G6" s="40"/>
-      <c r="H6" s="40"/>
-      <c r="I6" s="40"/>
-      <c r="J6" s="40"/>
-      <c r="K6" s="40"/>
-      <c r="L6" s="40"/>
-      <c r="M6" s="40"/>
-      <c r="N6" s="40"/>
-      <c r="O6" s="40"/>
-      <c r="P6" s="40"/>
-      <c r="Q6" s="40"/>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A7" s="14"/>
-      <c r="B7" s="14"/>
-      <c r="C7" s="14"/>
-      <c r="D7" s="14"/>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A8" s="14"/>
-      <c r="B8" s="14"/>
-      <c r="C8" s="14"/>
-      <c r="D8" s="14"/>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A9" s="14"/>
-      <c r="B9" s="14"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="14"/>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A10" s="14"/>
-      <c r="B10" s="14"/>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14"/>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A11" s="14"/>
-      <c r="B11" s="14"/>
-      <c r="C11" s="14"/>
-      <c r="D11" s="14"/>
-      <c r="K11" s="27"/>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A12" s="14"/>
-      <c r="B12" s="14"/>
-      <c r="C12" s="14"/>
-      <c r="D12" s="14"/>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A13" s="14"/>
-      <c r="B13" s="14"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A14" s="14"/>
-      <c r="B14" s="14"/>
-      <c r="C14" s="14"/>
-      <c r="D14" s="14"/>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A15" s="14"/>
-      <c r="B15" s="14"/>
-      <c r="C15" s="14"/>
-      <c r="D15" s="14"/>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A16" s="14"/>
-      <c r="B16" s="14"/>
-      <c r="C16" s="14"/>
-      <c r="D16" s="14"/>
-    </row>
-    <row r="22" spans="5:16" x14ac:dyDescent="0.25">
-      <c r="E22" s="42" t="s">
+      <c r="J16" s="3"/>
+      <c r="K16" s="56"/>
+      <c r="L16" s="45"/>
+      <c r="M16" s="45"/>
+      <c r="N16" s="45"/>
+      <c r="O16" s="45"/>
+      <c r="P16" s="45"/>
+      <c r="Q16" s="45"/>
+      <c r="R16" s="45"/>
+      <c r="S16" s="45"/>
+      <c r="T16" s="45"/>
+      <c r="U16" s="45"/>
+      <c r="V16" s="45"/>
+      <c r="W16" s="45"/>
+    </row>
+    <row r="17" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>218</v>
+      </c>
+      <c r="C17" t="s">
+        <v>266</v>
+      </c>
+      <c r="G17" s="68"/>
+      <c r="H17" s="68"/>
+      <c r="I17" s="86"/>
+      <c r="J17" s="68"/>
+      <c r="K17" s="87"/>
+      <c r="L17" s="23"/>
+      <c r="M17" s="23"/>
+      <c r="N17" s="23"/>
+      <c r="O17" s="23"/>
+      <c r="P17" s="23"/>
+      <c r="Q17" s="23"/>
+      <c r="R17" s="23"/>
+      <c r="S17" s="23"/>
+      <c r="T17" s="23"/>
+      <c r="U17" s="23"/>
+      <c r="V17" s="23"/>
+      <c r="W17" s="23"/>
+    </row>
+    <row r="18" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>249</v>
+      </c>
+      <c r="C18" t="s">
+        <v>267</v>
+      </c>
+      <c r="G18" s="14"/>
+      <c r="H18" s="14"/>
+      <c r="I18" s="14"/>
+      <c r="J18" s="14"/>
+    </row>
+    <row r="19" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="G19" s="14"/>
+      <c r="H19" s="14"/>
+      <c r="I19" s="14"/>
+      <c r="J19" s="14"/>
+    </row>
+    <row r="20" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="G20" s="14"/>
+      <c r="H20" s="14"/>
+      <c r="I20" s="14"/>
+      <c r="J20" s="14"/>
+    </row>
+    <row r="21" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="G21" s="14"/>
+      <c r="H21" s="14"/>
+      <c r="I21" s="14"/>
+      <c r="J21" s="14"/>
+    </row>
+    <row r="22" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="G22" s="14"/>
+      <c r="H22" s="14"/>
+      <c r="I22" s="14"/>
+      <c r="J22" s="14"/>
+      <c r="Q22" s="27"/>
+    </row>
+    <row r="23" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="G23" s="14"/>
+      <c r="H23" s="14"/>
+      <c r="I23" s="14"/>
+      <c r="J23" s="14"/>
+    </row>
+    <row r="24" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="G24" s="14"/>
+      <c r="H24" s="14"/>
+      <c r="I24" s="14"/>
+      <c r="J24" s="14"/>
+    </row>
+    <row r="25" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="G25" s="14"/>
+      <c r="H25" s="14"/>
+      <c r="I25" s="14"/>
+      <c r="J25" s="14"/>
+    </row>
+    <row r="26" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="G26" s="14"/>
+      <c r="H26" s="14"/>
+      <c r="I26" s="14"/>
+      <c r="J26" s="14"/>
+    </row>
+    <row r="27" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="G27" s="14"/>
+      <c r="H27" s="14"/>
+      <c r="I27" s="14"/>
+      <c r="J27" s="14"/>
+    </row>
+    <row r="33" spans="11:22" x14ac:dyDescent="0.25">
+      <c r="K33" s="47" t="s">
         <v>70</v>
       </c>
-      <c r="F22" s="40"/>
-      <c r="G22" s="40"/>
-      <c r="H22" s="40"/>
-      <c r="I22" s="40"/>
-      <c r="J22" s="40"/>
-      <c r="K22" s="40"/>
-      <c r="L22" s="40"/>
-      <c r="M22" s="40"/>
-      <c r="N22" s="40"/>
-      <c r="O22" s="40"/>
-      <c r="P22" s="40"/>
-    </row>
-    <row r="23" spans="5:16" x14ac:dyDescent="0.25">
-      <c r="E23" s="40"/>
-      <c r="F23" s="40"/>
-      <c r="G23" s="40"/>
-      <c r="H23" s="40"/>
-      <c r="I23" s="40"/>
-      <c r="J23" s="40"/>
-      <c r="K23" s="40"/>
-      <c r="L23" s="40"/>
-      <c r="M23" s="40"/>
-      <c r="N23" s="40"/>
-      <c r="O23" s="40"/>
-      <c r="P23" s="40"/>
-    </row>
-    <row r="24" spans="5:16" x14ac:dyDescent="0.25">
-      <c r="E24" s="40"/>
-      <c r="F24" s="40"/>
-      <c r="G24" s="40"/>
-      <c r="H24" s="40"/>
-      <c r="I24" s="40"/>
-      <c r="J24" s="40"/>
-      <c r="K24" s="40"/>
-      <c r="L24" s="40"/>
-      <c r="M24" s="40"/>
-      <c r="N24" s="40"/>
-      <c r="O24" s="40"/>
-      <c r="P24" s="40"/>
-    </row>
-    <row r="40" spans="5:16" x14ac:dyDescent="0.25">
-      <c r="E40" s="50" t="s">
+      <c r="L33" s="45"/>
+      <c r="M33" s="45"/>
+      <c r="N33" s="45"/>
+      <c r="O33" s="45"/>
+      <c r="P33" s="45"/>
+      <c r="Q33" s="45"/>
+      <c r="R33" s="45"/>
+      <c r="S33" s="45"/>
+      <c r="T33" s="45"/>
+      <c r="U33" s="45"/>
+      <c r="V33" s="45"/>
+    </row>
+    <row r="34" spans="11:22" x14ac:dyDescent="0.25">
+      <c r="K34" s="45"/>
+      <c r="L34" s="45"/>
+      <c r="M34" s="45"/>
+      <c r="N34" s="45"/>
+      <c r="O34" s="45"/>
+      <c r="P34" s="45"/>
+      <c r="Q34" s="45"/>
+      <c r="R34" s="45"/>
+      <c r="S34" s="45"/>
+      <c r="T34" s="45"/>
+      <c r="U34" s="45"/>
+      <c r="V34" s="45"/>
+    </row>
+    <row r="35" spans="11:22" x14ac:dyDescent="0.25">
+      <c r="K35" s="45"/>
+      <c r="L35" s="45"/>
+      <c r="M35" s="45"/>
+      <c r="N35" s="45"/>
+      <c r="O35" s="45"/>
+      <c r="P35" s="45"/>
+      <c r="Q35" s="45"/>
+      <c r="R35" s="45"/>
+      <c r="S35" s="45"/>
+      <c r="T35" s="45"/>
+      <c r="U35" s="45"/>
+      <c r="V35" s="45"/>
+    </row>
+    <row r="51" spans="11:22" x14ac:dyDescent="0.25">
+      <c r="K51" s="54" t="s">
         <v>71</v>
       </c>
-      <c r="F40" s="40"/>
-      <c r="G40" s="40"/>
-      <c r="H40" s="40"/>
-      <c r="I40" s="40"/>
-      <c r="J40" s="40"/>
-      <c r="K40" s="40"/>
-      <c r="L40" s="40"/>
-      <c r="M40" s="40"/>
-      <c r="N40" s="40"/>
-      <c r="O40" s="40"/>
-      <c r="P40" s="40"/>
-    </row>
-    <row r="41" spans="5:16" x14ac:dyDescent="0.25">
-      <c r="E41" s="40"/>
-      <c r="F41" s="40"/>
-      <c r="G41" s="40"/>
-      <c r="H41" s="40"/>
-      <c r="I41" s="40"/>
-      <c r="J41" s="40"/>
-      <c r="K41" s="40"/>
-      <c r="L41" s="40"/>
-      <c r="M41" s="40"/>
-      <c r="N41" s="40"/>
-      <c r="O41" s="40"/>
-      <c r="P41" s="40"/>
+      <c r="L51" s="45"/>
+      <c r="M51" s="45"/>
+      <c r="N51" s="45"/>
+      <c r="O51" s="45"/>
+      <c r="P51" s="45"/>
+      <c r="Q51" s="45"/>
+      <c r="R51" s="45"/>
+      <c r="S51" s="45"/>
+      <c r="T51" s="45"/>
+      <c r="U51" s="45"/>
+      <c r="V51" s="45"/>
+    </row>
+    <row r="52" spans="11:22" x14ac:dyDescent="0.25">
+      <c r="K52" s="45"/>
+      <c r="L52" s="45"/>
+      <c r="M52" s="45"/>
+      <c r="N52" s="45"/>
+      <c r="O52" s="45"/>
+      <c r="P52" s="45"/>
+      <c r="Q52" s="45"/>
+      <c r="R52" s="45"/>
+      <c r="S52" s="45"/>
+      <c r="T52" s="45"/>
+      <c r="U52" s="45"/>
+      <c r="V52" s="45"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="F2:Q2"/>
-    <mergeCell ref="E5:Q6"/>
-    <mergeCell ref="E22:P24"/>
-    <mergeCell ref="E40:P41"/>
+  <mergeCells count="20">
+    <mergeCell ref="G13:G15"/>
+    <mergeCell ref="H13:H15"/>
+    <mergeCell ref="I13:I15"/>
+    <mergeCell ref="J13:J15"/>
+    <mergeCell ref="L2:W2"/>
+    <mergeCell ref="K13:W16"/>
+    <mergeCell ref="K33:V35"/>
+    <mergeCell ref="K51:V52"/>
+    <mergeCell ref="G2:G5"/>
+    <mergeCell ref="H2:H5"/>
+    <mergeCell ref="I2:I5"/>
+    <mergeCell ref="J2:J5"/>
+    <mergeCell ref="G6:G9"/>
+    <mergeCell ref="H6:H9"/>
+    <mergeCell ref="I6:I9"/>
+    <mergeCell ref="J6:J9"/>
+    <mergeCell ref="G10:G12"/>
+    <mergeCell ref="H10:H12"/>
+    <mergeCell ref="I10:I12"/>
+    <mergeCell ref="J10:J12"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{3D14D563-A18C-4362-B2CD-8D8339C1C427}"/>
-    <hyperlink ref="D3" r:id="rId2" display="https://www.baeldung.com/java-connection-pooling" xr:uid="{C6D19347-A59D-426C-9D1E-C2B07B6CDCC2}"/>
-    <hyperlink ref="D4" r:id="rId3" display="https://viblo.asia/p/string-pool-la-gi-_x000a_" xr:uid="{6F55EEC8-830E-42C3-9431-2030A8B28A12}"/>
+    <hyperlink ref="J2" r:id="rId1" xr:uid="{3D14D563-A18C-4362-B2CD-8D8339C1C427}"/>
+    <hyperlink ref="J6" r:id="rId2" display="https://www.baeldung.com/java-connection-pooling" xr:uid="{C6D19347-A59D-426C-9D1E-C2B07B6CDCC2}"/>
+    <hyperlink ref="J10" r:id="rId3" display="https://viblo.asia/p/string-pool-la-gi-_x000a_" xr:uid="{6F55EEC8-830E-42C3-9431-2030A8B28A12}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId4"/>
@@ -4612,14 +5575,14 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="53" t="s">
+      <c r="A7" s="57" t="s">
         <v>79</v>
       </c>
-      <c r="B7" s="40"/>
+      <c r="B7" s="45"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="40"/>
-      <c r="B8" s="40"/>
+      <c r="A8" s="45"/>
+      <c r="B8" s="45"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
@@ -4819,7 +5782,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D5CC180-ABEC-4096-BF7B-D59D7E76A5ED}">
   <dimension ref="A1:M19"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
@@ -5332,7 +6295,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A3AF180-2B8D-4C19-A7E4-B0AE9B7543FC}">
   <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="D3" sqref="A1:D3"/>
     </sheetView>
   </sheetViews>
@@ -5469,7 +6432,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F79DFAC0-397F-4C98-B2DF-6497ADE191DD}">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
@@ -5593,7 +6556,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83D713CF-1264-4070-BA73-824C7A1D0A05}">
   <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
@@ -5617,11 +6580,11 @@
       <c r="D1" s="30" t="s">
         <v>189</v>
       </c>
-      <c r="E1" s="63"/>
-      <c r="F1" s="63"/>
-      <c r="G1" s="63"/>
-      <c r="H1" s="63"/>
-      <c r="I1" s="63"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
     </row>
     <row r="2" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
@@ -5636,43 +6599,43 @@
       <c r="D2" s="37" t="s">
         <v>207</v>
       </c>
-      <c r="E2" s="62"/>
-      <c r="F2" s="62"/>
-      <c r="G2" s="62"/>
-      <c r="H2" s="62"/>
-      <c r="I2" s="62"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
     </row>
     <row r="3" spans="1:9" ht="297" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="56">
+      <c r="A3" s="58">
         <v>2</v>
       </c>
-      <c r="B3" s="56" t="s">
+      <c r="B3" s="58" t="s">
         <v>192</v>
       </c>
-      <c r="C3" s="54" t="s">
+      <c r="C3" s="41" t="s">
         <v>193</v>
       </c>
-      <c r="D3" s="61" t="s">
+      <c r="D3" s="42" t="s">
         <v>209</v>
       </c>
-      <c r="E3" s="62"/>
-      <c r="F3" s="62"/>
-      <c r="G3" s="62"/>
-      <c r="H3" s="62"/>
-      <c r="I3" s="62"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
     </row>
     <row r="4" spans="1:9" ht="333.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="60"/>
-      <c r="B4" s="57"/>
+      <c r="B4" s="59"/>
       <c r="C4" s="3"/>
       <c r="D4" s="37" t="s">
         <v>208</v>
       </c>
-      <c r="E4" s="62"/>
-      <c r="F4" s="62"/>
-      <c r="G4" s="62"/>
-      <c r="H4" s="62"/>
-      <c r="I4" s="62"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="14"/>
     </row>
     <row r="5" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="60"/>
@@ -5682,14 +6645,14 @@
       <c r="C5" s="5" t="s">
         <v>197</v>
       </c>
-      <c r="D5" s="64" t="s">
+      <c r="D5" s="61" t="s">
         <v>210</v>
       </c>
-      <c r="E5" s="62"/>
-      <c r="F5" s="62"/>
-      <c r="G5" s="62"/>
-      <c r="H5" s="62"/>
-      <c r="I5" s="62"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="14"/>
     </row>
     <row r="6" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="60"/>
@@ -5699,12 +6662,12 @@
       <c r="C6" s="5" t="s">
         <v>199</v>
       </c>
-      <c r="D6" s="55"/>
-      <c r="E6" s="62"/>
-      <c r="F6" s="62"/>
-      <c r="G6" s="62"/>
-      <c r="H6" s="62"/>
-      <c r="I6" s="62"/>
+      <c r="D6" s="62"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="14"/>
     </row>
     <row r="7" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A7" s="60"/>
@@ -5714,15 +6677,15 @@
       <c r="C7" s="5" t="s">
         <v>198</v>
       </c>
-      <c r="D7" s="55"/>
-      <c r="E7" s="62"/>
-      <c r="F7" s="62"/>
-      <c r="G7" s="62"/>
-      <c r="H7" s="62"/>
-      <c r="I7" s="62"/>
+      <c r="D7" s="62"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="14"/>
     </row>
     <row r="8" spans="1:9" ht="90" x14ac:dyDescent="0.25">
-      <c r="A8" s="57"/>
+      <c r="A8" s="59"/>
       <c r="B8" s="3" t="s">
         <v>200</v>
       </c>
@@ -5732,11 +6695,11 @@
       <c r="D8" s="37" t="s">
         <v>208</v>
       </c>
-      <c r="E8" s="62"/>
-      <c r="F8" s="62"/>
-      <c r="G8" s="62"/>
-      <c r="H8" s="62"/>
-      <c r="I8" s="62"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="14"/>
     </row>
     <row r="9" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
@@ -5748,14 +6711,14 @@
       <c r="C9" s="5" t="s">
         <v>203</v>
       </c>
-      <c r="D9" s="61" t="s">
+      <c r="D9" s="42" t="s">
         <v>204</v>
       </c>
-      <c r="E9" s="62"/>
-      <c r="F9" s="62"/>
-      <c r="G9" s="62"/>
-      <c r="H9" s="62"/>
-      <c r="I9" s="62"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="14"/>
+      <c r="I9" s="14"/>
     </row>
     <row r="10" spans="1:9" ht="150" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
@@ -5770,89 +6733,89 @@
       <c r="D10" s="37" t="s">
         <v>207</v>
       </c>
-      <c r="E10" s="62"/>
-      <c r="F10" s="62"/>
-      <c r="G10" s="62"/>
-      <c r="H10" s="62"/>
-      <c r="I10" s="62"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="14"/>
+      <c r="I10" s="14"/>
     </row>
     <row r="11" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="65">
+      <c r="A11" s="63">
         <v>5</v>
       </c>
-      <c r="B11" s="65" t="s">
+      <c r="B11" s="63" t="s">
         <v>211</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>212</v>
       </c>
-      <c r="D11" s="58" t="s">
+      <c r="D11" s="64" t="s">
         <v>207</v>
       </c>
-      <c r="E11" s="62"/>
-      <c r="F11" s="62"/>
-      <c r="G11" s="62"/>
-      <c r="H11" s="62"/>
-      <c r="I11" s="62"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="14"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="65"/>
-      <c r="B12" s="65"/>
+      <c r="A12" s="63"/>
+      <c r="B12" s="63"/>
       <c r="C12" s="3" t="s">
         <v>213</v>
       </c>
-      <c r="D12" s="66"/>
-      <c r="E12" s="62"/>
-      <c r="F12" s="62"/>
-      <c r="G12" s="62"/>
-      <c r="H12" s="62"/>
-      <c r="I12" s="62"/>
+      <c r="D12" s="65"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="14"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="65"/>
-      <c r="B13" s="65"/>
+      <c r="A13" s="63"/>
+      <c r="B13" s="63"/>
       <c r="C13" s="3" t="s">
         <v>214</v>
       </c>
-      <c r="D13" s="59"/>
-      <c r="E13" s="62"/>
-      <c r="F13" s="62"/>
-      <c r="G13" s="62"/>
-      <c r="H13" s="62"/>
-      <c r="I13" s="62"/>
+      <c r="D13" s="66"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="14"/>
+      <c r="I13" s="14"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="62"/>
-      <c r="B14" s="62"/>
-      <c r="C14" s="62"/>
-      <c r="D14" s="62"/>
-      <c r="E14" s="62"/>
-      <c r="F14" s="62"/>
-      <c r="G14" s="62"/>
-      <c r="H14" s="62"/>
-      <c r="I14" s="62"/>
+      <c r="A14" s="14"/>
+      <c r="B14" s="14"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="14"/>
+      <c r="I14" s="14"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="62"/>
-      <c r="B15" s="62"/>
-      <c r="C15" s="62"/>
-      <c r="D15" s="62"/>
-      <c r="E15" s="62"/>
-      <c r="F15" s="62"/>
-      <c r="G15" s="62"/>
-      <c r="H15" s="62"/>
-      <c r="I15" s="62"/>
+      <c r="A15" s="14"/>
+      <c r="B15" s="14"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="14"/>
+      <c r="I15" s="14"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="62"/>
-      <c r="B16" s="62"/>
-      <c r="C16" s="62"/>
-      <c r="D16" s="62"/>
-      <c r="E16" s="62"/>
-      <c r="F16" s="62"/>
-      <c r="G16" s="62"/>
-      <c r="H16" s="62"/>
-      <c r="I16" s="62"/>
+      <c r="A16" s="14"/>
+      <c r="B16" s="14"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="14"/>
+      <c r="H16" s="14"/>
+      <c r="I16" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>

<commit_message>
tóm tắt lại day 6
</commit_message>
<xml_diff>
--- a/Task_Result.xlsx
+++ b/Task_Result.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\beetech\java\stage1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E458E459-9F28-4323-9B24-69E9706C2653}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28260E91-77BE-40AD-8934-45B6D5B06D7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="day2 " sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="340">
   <si>
     <t>STT</t>
   </si>
@@ -2418,6 +2418,222 @@
   </si>
   <si>
     <t>Dễ bị trỏ đến đối tượng chưa được khởi tạo</t>
+  </si>
+  <si>
+    <t>Lambda Expression:</t>
+  </si>
+  <si>
+    <t>là hàm ẩn danh</t>
+  </si>
+  <si>
+    <t>tiện lợi và gọn gàng phù hợp với những phương thức sử dụng 1 lần</t>
+  </si>
+  <si>
+    <t>phù hợp làm tham số của phương thức</t>
+  </si>
+  <si>
+    <t>Khó hiểu đối với người mới</t>
+  </si>
+  <si>
+    <t>Stream API:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">là một tính năng cho phép thao tác xử lý dữ liệu trên một tập hợp các phần </t>
+  </si>
+  <si>
+    <t>Gọn và dễ đọc</t>
+  </si>
+  <si>
+    <t>Hiệu suất cao với xử lý đa luồng</t>
+  </si>
+  <si>
+    <t>Việc xử lý trên nhiều luồng có thể gây bất đồng bộ nên các phần tử phải độc lập</t>
+  </si>
+  <si>
+    <t>là cú pháp để tham chiếu đến phương thức</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Giảm sự lặp lại </t>
+  </si>
+  <si>
+    <t>Có thể tái sử dụng</t>
+  </si>
+  <si>
+    <t>là một tính năng cho phép định nghĩa phương thức ở interface</t>
+  </si>
+  <si>
+    <t>Tránh định nghĩa lại ở các class implement</t>
+  </si>
+  <si>
+    <t>là một tính năng cho phép ứng dụng triển khai module hóa</t>
+  </si>
+  <si>
+    <t>cho phép ứng dụng chia thành các module riêng biệt</t>
+  </si>
+  <si>
+    <t>có thể tái sử dụng lại module</t>
+  </si>
+  <si>
+    <t>kiểm soát sự tương thích giữa các module</t>
+  </si>
+  <si>
+    <t>giúp quản lý các phiên bản của module</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kiểm soát truy cập vào module </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Làm giảm hiệu suất của ứng dụng khi sử dụng quá nhiều module </t>
+  </si>
+  <si>
+    <t>Khó triển khai</t>
+  </si>
+  <si>
+    <t>là cú pháp được sử dụng để tự động giải phóng các tài nguyên trong khối try-catch-finally</t>
+  </si>
+  <si>
+    <t>tự động giải phóng các tài nguyên</t>
+  </si>
+  <si>
+    <t>giảm thiếu viết thêm code giải phóng tài nguyên</t>
+  </si>
+  <si>
+    <t>các tài nguyên đó phải implement interface java.lang.AutoCloseable hoặc java.io.Closeable</t>
+  </si>
+  <si>
+    <t>là một tính năng cho phép khai báo đối tượng generic mà không cần định kiểu generics</t>
+  </si>
+  <si>
+    <t>loại bỏ việc lặp lại kiểu generics ở cả 2 phía của toán tử gán trong khai báo đối tượng</t>
+  </si>
+  <si>
+    <t>Tự động xác định kiểu</t>
+  </si>
+  <si>
+    <t>Không hỗ trợ trước Java 7</t>
+  </si>
+  <si>
+    <t>là một lớp nặc danh được khai báo bên trong một phương thức hoặc một khối lệnh của một lớp khác</t>
+  </si>
+  <si>
+    <t>giúp rút ngắn đoạn mã khi cần định nghĩa một lớp mới để sử dụng một phương thức hoặc ghi đè một phương thức.</t>
+  </si>
+  <si>
+    <t>tiện lợi cho việc sử dụng các class chỉ dùng 1 lần</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> làm cho mã nguồn trở nên phức tạp hơn và khó bảo trì hơn do không có tên lớp, khó để tìm kiếm khi có lỗi.</t>
+  </si>
+  <si>
+    <t>Không thể tái sử dụng lại</t>
+  </si>
+  <si>
+    <t>Các class khác không thể kế thừa</t>
+  </si>
+  <si>
+    <t>Không hỗ trợ trước Java 9</t>
+  </si>
+  <si>
+    <t>là cú pháp sử dụng cho việc khởi tạo một đối tượng anonymous inner class mà không cần chỉ định kiểu generic của lớp.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">giúp rút ngắn đoạn mã </t>
+  </si>
+  <si>
+    <t>là tính năng cho phép định nghĩa phương thức riêng tư trong các interface.</t>
+  </si>
+  <si>
+    <t>đảm bảo tính đóng gói</t>
+  </si>
+  <si>
+    <t>có thể triển khai trên các Default method</t>
+  </si>
+  <si>
+    <t>Chỉ được sử dụng trong cùng 1 interface</t>
+  </si>
+  <si>
+    <t>là tính năng cho phép khai báo biến mà không cần chỉ định kiểu dữ liệu một cách rõ ràng. Thay vào đó, kiểu dữ liệu của biến sẽ được suy ra từ giá trị khởi tạo.</t>
+  </si>
+  <si>
+    <t>Giúp rút ngắn mã nguồn</t>
+  </si>
+  <si>
+    <t>thay đổi kiểu dữ liệu của biến một cách dễ dàng và linh hoạt hơn, mà không cần phải sửa đổi code nhiều</t>
+  </si>
+  <si>
+    <t>Khi kiểu dữ liệu của biến không được chỉ định rõ ràng, điều này có thể làm cho code trở nên khó hiểu hơn đối với những người mới học hoặc những người không quen với tính năng này</t>
+  </si>
+  <si>
+    <t>là một tính năng cho phép sử dụng switch case như một biểu thức trả về một giá trị</t>
+  </si>
+  <si>
+    <t>giảm thiểu mã code</t>
+  </si>
+  <si>
+    <t>gán giá trị cho một biến hoặc làm giá trị trả về</t>
+  </si>
+  <si>
+    <t>Không hỗ trợ các trường hợp default</t>
+  </si>
+  <si>
+    <t>Không hỗ trợ trước Java 12</t>
+  </si>
+  <si>
+    <t>là một keyword được sử dụng trong Switch Expressions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">là một tính năng giúp dễ dàng trong việc khai báo chuỗi dài </t>
+  </si>
+  <si>
+    <t>có thể viết các chuỗi dài hoặc các chuỗi chứa các ký tự đặc biệt một cách dễ dàng và tự nhiên hơn mà không cần sử dụng escape sequences như \n, \r, \t và kết hợp với các toán tử + để nối chuỗi.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> hỗ trợ các trường hợp thực tế như viết HTML, JSON hoặc SQL </t>
+  </si>
+  <si>
+    <t>Không hỗ trợ trước Java 15</t>
+  </si>
+  <si>
+    <t>là một tính năng cho phép kiểm tra một đối tượng có phù hợp với một kiểu nhất định hay không</t>
+  </si>
+  <si>
+    <t>giúp cho code trở nên dễ đọc và dễ hiểu hơn bằng cách cho phép kiểm tra kiểu của một đối tượng một cách dễ dàng và tự nhiên hơn</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> giúp cho code trở nên gọn hơn bằng cách loại bỏ các phép ép kiểu (type casting) không cần thiết.</t>
+  </si>
+  <si>
+    <t>Không hỗ trợ trước Java 16</t>
+  </si>
+  <si>
+    <t>là một tính năng cho phép định nghĩa các lớp đơn giản để chứa dữ liệu, với cú pháp rút gọn và hỗ trợ một số tính năng tiện ích.</t>
+  </si>
+  <si>
+    <t>Định nghĩa nhanh các class chỉ có các field và getter</t>
+  </si>
+  <si>
+    <t>vì bất biến nên không thể sửa đổi các thuộc tính</t>
+  </si>
+  <si>
+    <t>Không cho phép kế thừa</t>
+  </si>
+  <si>
+    <t>là tính năng mà nó giới hạn các lớp con của một lớp cụ thể chỉ có thể được định nghĩa bởi lớp cha và phải trong cùng một module</t>
+  </si>
+  <si>
+    <t>Giới hạn các lớp con có thể được kế thừa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Là tính năng cho phép sử dụng nhiều anonation cùng loại trên cùng </t>
+  </si>
+  <si>
+    <t>Các lớp con được đánh dấu final không được kế thừa</t>
+  </si>
+  <si>
+    <t>Giảm thiểu viết nhiều code lặp đi lặp lại</t>
+  </si>
+  <si>
+    <t>Không hỗ trợ trước Java 8</t>
   </si>
 </sst>
 </file>
@@ -2619,7 +2835,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="88">
+  <cellXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2723,6 +2939,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2759,32 +2983,17 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -2794,18 +3003,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2825,8 +3022,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2846,11 +3049,29 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3960,27 +4181,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="16:22" x14ac:dyDescent="0.25">
-      <c r="P1" s="44" t="s">
+      <c r="P1" s="48" t="s">
         <v>17</v>
       </c>
-      <c r="Q1" s="45"/>
-      <c r="R1" s="45"/>
-      <c r="S1" s="45"/>
-      <c r="T1" s="45"/>
+      <c r="Q1" s="49"/>
+      <c r="R1" s="49"/>
+      <c r="S1" s="49"/>
+      <c r="T1" s="49"/>
     </row>
     <row r="2" spans="16:22" x14ac:dyDescent="0.25">
-      <c r="P2" s="45"/>
-      <c r="Q2" s="45"/>
-      <c r="R2" s="45"/>
-      <c r="S2" s="45"/>
-      <c r="T2" s="45"/>
+      <c r="P2" s="49"/>
+      <c r="Q2" s="49"/>
+      <c r="R2" s="49"/>
+      <c r="S2" s="49"/>
+      <c r="T2" s="49"/>
     </row>
     <row r="3" spans="16:22" x14ac:dyDescent="0.25">
-      <c r="P3" s="46"/>
-      <c r="Q3" s="46"/>
-      <c r="R3" s="46"/>
-      <c r="S3" s="46"/>
-      <c r="T3" s="46"/>
+      <c r="P3" s="50"/>
+      <c r="Q3" s="50"/>
+      <c r="R3" s="50"/>
+      <c r="S3" s="50"/>
+      <c r="T3" s="50"/>
     </row>
     <row r="4" spans="16:22" x14ac:dyDescent="0.25">
       <c r="P4" s="7" t="s">
@@ -3989,11 +4210,11 @@
       <c r="Q4" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="R4" s="43" t="s">
+      <c r="R4" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="S4" s="43"/>
-      <c r="T4" s="43"/>
+      <c r="S4" s="47"/>
+      <c r="T4" s="47"/>
       <c r="U4" s="7" t="s">
         <v>18</v>
       </c>
@@ -4147,24 +4368,24 @@
       </c>
     </row>
     <row r="14" spans="16:22" x14ac:dyDescent="0.25">
-      <c r="P14" s="47" t="s">
+      <c r="P14" s="51" t="s">
         <v>73</v>
       </c>
-      <c r="Q14" s="45"/>
-      <c r="R14" s="45"/>
-      <c r="S14" s="45"/>
+      <c r="Q14" s="49"/>
+      <c r="R14" s="49"/>
+      <c r="S14" s="49"/>
     </row>
     <row r="15" spans="16:22" x14ac:dyDescent="0.25">
-      <c r="P15" s="45"/>
-      <c r="Q15" s="45"/>
-      <c r="R15" s="45"/>
-      <c r="S15" s="45"/>
+      <c r="P15" s="49"/>
+      <c r="Q15" s="49"/>
+      <c r="R15" s="49"/>
+      <c r="S15" s="49"/>
     </row>
     <row r="16" spans="16:22" x14ac:dyDescent="0.25">
-      <c r="P16" s="45"/>
-      <c r="Q16" s="45"/>
-      <c r="R16" s="45"/>
-      <c r="S16" s="45"/>
+      <c r="P16" s="49"/>
+      <c r="Q16" s="49"/>
+      <c r="R16" s="49"/>
+      <c r="S16" s="49"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -4190,7 +4411,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25977106-C04A-4BDF-83D6-AA6BE76B6728}">
   <dimension ref="A1:AD89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="G1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
@@ -4209,24 +4430,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:30" ht="49.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="48" t="s">
+      <c r="A1" s="52" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="49"/>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
-      <c r="F1" s="49"/>
-      <c r="G1" s="49"/>
-      <c r="H1" s="49"/>
-      <c r="I1" s="49"/>
-      <c r="J1" s="49"/>
-      <c r="K1" s="49"/>
-      <c r="L1" s="49"/>
-      <c r="M1" s="49"/>
-      <c r="N1" s="49"/>
-      <c r="O1" s="49"/>
-      <c r="P1" s="49"/>
+      <c r="B1" s="53"/>
+      <c r="C1" s="53"/>
+      <c r="D1" s="53"/>
+      <c r="E1" s="53"/>
+      <c r="F1" s="53"/>
+      <c r="G1" s="53"/>
+      <c r="H1" s="53"/>
+      <c r="I1" s="53"/>
+      <c r="J1" s="53"/>
+      <c r="K1" s="53"/>
+      <c r="L1" s="53"/>
+      <c r="M1" s="53"/>
+      <c r="N1" s="53"/>
+      <c r="O1" s="53"/>
+      <c r="P1" s="53"/>
       <c r="Q1" s="39"/>
       <c r="R1" s="39"/>
       <c r="S1" s="39"/>
@@ -4264,7 +4485,7 @@
       <c r="K2" s="19"/>
       <c r="L2" s="19"/>
       <c r="M2" s="19"/>
-      <c r="N2" s="70" t="s">
+      <c r="N2" s="44" t="s">
         <v>244</v>
       </c>
       <c r="P2" t="s">
@@ -4318,16 +4539,16 @@
       <c r="P4" t="s">
         <v>219</v>
       </c>
-      <c r="AA4" s="64">
+      <c r="AA4" s="63">
         <v>3</v>
       </c>
-      <c r="AB4" s="64" t="s">
+      <c r="AB4" s="63" t="s">
         <v>35</v>
       </c>
-      <c r="AC4" s="73" t="s">
+      <c r="AC4" s="66" t="s">
         <v>38</v>
       </c>
-      <c r="AD4" s="76" t="s">
+      <c r="AD4" s="69" t="s">
         <v>32</v>
       </c>
     </row>
@@ -4339,26 +4560,26 @@
       <c r="P5" t="s">
         <v>220</v>
       </c>
-      <c r="AA5" s="65"/>
-      <c r="AB5" s="65"/>
-      <c r="AC5" s="74"/>
-      <c r="AD5" s="77"/>
+      <c r="AA5" s="64"/>
+      <c r="AB5" s="64"/>
+      <c r="AC5" s="67"/>
+      <c r="AD5" s="70"/>
     </row>
     <row r="6" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="14"/>
       <c r="B6" s="15"/>
       <c r="C6" s="16"/>
       <c r="D6" s="18"/>
-      <c r="N6" s="70" t="s">
+      <c r="N6" s="44" t="s">
         <v>221</v>
       </c>
       <c r="P6" t="s">
         <v>222</v>
       </c>
-      <c r="AA6" s="66"/>
-      <c r="AB6" s="66"/>
-      <c r="AC6" s="75"/>
-      <c r="AD6" s="78"/>
+      <c r="AA6" s="65"/>
+      <c r="AB6" s="65"/>
+      <c r="AC6" s="68"/>
+      <c r="AD6" s="71"/>
     </row>
     <row r="7" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="14"/>
@@ -4371,16 +4592,16 @@
       <c r="P7" t="s">
         <v>223</v>
       </c>
-      <c r="AA7" s="64">
+      <c r="AA7" s="63">
         <v>4</v>
       </c>
-      <c r="AB7" s="64" t="s">
+      <c r="AB7" s="63" t="s">
         <v>36</v>
       </c>
-      <c r="AC7" s="73" t="s">
+      <c r="AC7" s="66" t="s">
         <v>39</v>
       </c>
-      <c r="AD7" s="76" t="s">
+      <c r="AD7" s="69" t="s">
         <v>40</v>
       </c>
     </row>
@@ -4392,10 +4613,10 @@
       <c r="P8" t="s">
         <v>224</v>
       </c>
-      <c r="AA8" s="65"/>
-      <c r="AB8" s="65"/>
-      <c r="AC8" s="74"/>
-      <c r="AD8" s="77"/>
+      <c r="AA8" s="64"/>
+      <c r="AB8" s="64"/>
+      <c r="AC8" s="67"/>
+      <c r="AD8" s="70"/>
     </row>
     <row r="9" spans="1:30" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="14"/>
@@ -4408,39 +4629,39 @@
       <c r="P9" t="s">
         <v>225</v>
       </c>
-      <c r="AA9" s="66"/>
-      <c r="AB9" s="66"/>
-      <c r="AC9" s="75"/>
-      <c r="AD9" s="78"/>
+      <c r="AA9" s="65"/>
+      <c r="AB9" s="65"/>
+      <c r="AC9" s="68"/>
+      <c r="AD9" s="71"/>
     </row>
     <row r="10" spans="1:30" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="50" t="s">
+      <c r="A10" s="54" t="s">
         <v>54</v>
       </c>
-      <c r="B10" s="51"/>
-      <c r="C10" s="51"/>
-      <c r="D10" s="51"/>
-      <c r="E10" s="51"/>
+      <c r="B10" s="55"/>
+      <c r="C10" s="55"/>
+      <c r="D10" s="55"/>
+      <c r="E10" s="55"/>
       <c r="F10" s="19"/>
       <c r="G10" s="19"/>
       <c r="H10" s="19"/>
       <c r="I10" s="19"/>
-      <c r="N10" s="70" t="s">
+      <c r="N10" s="44" t="s">
         <v>226</v>
       </c>
       <c r="P10" t="s">
         <v>227</v>
       </c>
-      <c r="AA10" s="63">
+      <c r="AA10" s="59">
         <v>5</v>
       </c>
-      <c r="AB10" s="79" t="s">
+      <c r="AB10" s="60" t="s">
         <v>37</v>
       </c>
-      <c r="AC10" s="71" t="s">
+      <c r="AC10" s="61" t="s">
         <v>51</v>
       </c>
-      <c r="AD10" s="72" t="s">
+      <c r="AD10" s="62" t="s">
         <v>52</v>
       </c>
     </row>
@@ -4451,19 +4672,19 @@
       <c r="P11" t="s">
         <v>228</v>
       </c>
-      <c r="AA11" s="63"/>
-      <c r="AB11" s="79"/>
-      <c r="AC11" s="71"/>
-      <c r="AD11" s="72"/>
+      <c r="AA11" s="59"/>
+      <c r="AB11" s="60"/>
+      <c r="AC11" s="61"/>
+      <c r="AD11" s="62"/>
     </row>
     <row r="12" spans="1:30" x14ac:dyDescent="0.25">
       <c r="P12" t="s">
         <v>229</v>
       </c>
-      <c r="AA12" s="63"/>
-      <c r="AB12" s="79"/>
-      <c r="AC12" s="71"/>
-      <c r="AD12" s="72"/>
+      <c r="AA12" s="59"/>
+      <c r="AB12" s="60"/>
+      <c r="AC12" s="61"/>
+      <c r="AD12" s="62"/>
     </row>
     <row r="13" spans="1:30" x14ac:dyDescent="0.25">
       <c r="O13" t="s">
@@ -4472,22 +4693,22 @@
       <c r="P13" t="s">
         <v>230</v>
       </c>
-      <c r="AA13" s="63"/>
-      <c r="AB13" s="79"/>
-      <c r="AC13" s="71"/>
-      <c r="AD13" s="72"/>
+      <c r="AA13" s="59"/>
+      <c r="AB13" s="60"/>
+      <c r="AC13" s="61"/>
+      <c r="AD13" s="62"/>
     </row>
     <row r="14" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="N14" s="70" t="s">
+      <c r="N14" s="44" t="s">
         <v>231</v>
       </c>
       <c r="P14" t="s">
         <v>233</v>
       </c>
-      <c r="AA14" s="63"/>
-      <c r="AB14" s="79"/>
-      <c r="AC14" s="71"/>
-      <c r="AD14" s="72"/>
+      <c r="AA14" s="59"/>
+      <c r="AB14" s="60"/>
+      <c r="AC14" s="61"/>
+      <c r="AD14" s="62"/>
     </row>
     <row r="15" spans="1:30" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="40"/>
@@ -4505,10 +4726,10 @@
       <c r="P15" t="s">
         <v>232</v>
       </c>
-      <c r="AA15" s="63"/>
-      <c r="AB15" s="79"/>
-      <c r="AC15" s="71"/>
-      <c r="AD15" s="72"/>
+      <c r="AA15" s="59"/>
+      <c r="AB15" s="60"/>
+      <c r="AC15" s="61"/>
+      <c r="AD15" s="62"/>
     </row>
     <row r="16" spans="1:30" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="40"/>
@@ -4523,10 +4744,10 @@
       <c r="P16" t="s">
         <v>228</v>
       </c>
-      <c r="AA16" s="63"/>
-      <c r="AB16" s="79"/>
-      <c r="AC16" s="71"/>
-      <c r="AD16" s="72"/>
+      <c r="AA16" s="59"/>
+      <c r="AB16" s="60"/>
+      <c r="AC16" s="61"/>
+      <c r="AD16" s="62"/>
     </row>
     <row r="17" spans="1:30" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="40"/>
@@ -4541,10 +4762,10 @@
       <c r="P17" t="s">
         <v>229</v>
       </c>
-      <c r="AA17" s="63"/>
-      <c r="AB17" s="79"/>
-      <c r="AC17" s="71"/>
-      <c r="AD17" s="72"/>
+      <c r="AA17" s="59"/>
+      <c r="AB17" s="60"/>
+      <c r="AC17" s="61"/>
+      <c r="AD17" s="62"/>
     </row>
     <row r="18" spans="1:30" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="40"/>
@@ -4562,10 +4783,10 @@
       <c r="P18" t="s">
         <v>230</v>
       </c>
-      <c r="AA18" s="63"/>
-      <c r="AB18" s="79"/>
-      <c r="AC18" s="71"/>
-      <c r="AD18" s="72"/>
+      <c r="AA18" s="59"/>
+      <c r="AB18" s="60"/>
+      <c r="AC18" s="61"/>
+      <c r="AD18" s="62"/>
     </row>
     <row r="19" spans="1:30" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="40"/>
@@ -4577,16 +4798,16 @@
       <c r="G19" s="19"/>
       <c r="H19" s="19"/>
       <c r="I19" s="19"/>
-      <c r="N19" s="70" t="s">
+      <c r="N19" s="44" t="s">
         <v>234</v>
       </c>
       <c r="P19" t="s">
         <v>235</v>
       </c>
-      <c r="AA19" s="63"/>
-      <c r="AB19" s="79"/>
-      <c r="AC19" s="71"/>
-      <c r="AD19" s="72"/>
+      <c r="AA19" s="59"/>
+      <c r="AB19" s="60"/>
+      <c r="AC19" s="61"/>
+      <c r="AD19" s="62"/>
     </row>
     <row r="20" spans="1:30" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="40"/>
@@ -4598,16 +4819,16 @@
       <c r="G20" s="19"/>
       <c r="H20" s="19"/>
       <c r="I20" s="19"/>
-      <c r="N20" s="70" t="s">
+      <c r="N20" s="44" t="s">
         <v>236</v>
       </c>
       <c r="O20" t="s">
         <v>237</v>
       </c>
-      <c r="AA20" s="63"/>
-      <c r="AB20" s="79"/>
-      <c r="AC20" s="71"/>
-      <c r="AD20" s="72"/>
+      <c r="AA20" s="59"/>
+      <c r="AB20" s="60"/>
+      <c r="AC20" s="61"/>
+      <c r="AD20" s="62"/>
     </row>
     <row r="21" spans="1:30" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="40"/>
@@ -4625,10 +4846,10 @@
       <c r="P21" t="s">
         <v>238</v>
       </c>
-      <c r="AA21" s="63"/>
-      <c r="AB21" s="79"/>
-      <c r="AC21" s="71"/>
-      <c r="AD21" s="72"/>
+      <c r="AA21" s="59"/>
+      <c r="AB21" s="60"/>
+      <c r="AC21" s="61"/>
+      <c r="AD21" s="62"/>
     </row>
     <row r="22" spans="1:30" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="40"/>
@@ -4646,10 +4867,10 @@
       <c r="P22" t="s">
         <v>239</v>
       </c>
-      <c r="AA22" s="63"/>
-      <c r="AB22" s="79"/>
-      <c r="AC22" s="71"/>
-      <c r="AD22" s="72"/>
+      <c r="AA22" s="59"/>
+      <c r="AB22" s="60"/>
+      <c r="AC22" s="61"/>
+      <c r="AD22" s="62"/>
     </row>
     <row r="23" spans="1:30" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="40"/>
@@ -4661,16 +4882,16 @@
       <c r="G23" s="19"/>
       <c r="H23" s="19"/>
       <c r="I23" s="19"/>
-      <c r="N23" s="70" t="s">
+      <c r="N23" s="44" t="s">
         <v>240</v>
       </c>
       <c r="O23" t="s">
         <v>241</v>
       </c>
-      <c r="AA23" s="63"/>
-      <c r="AB23" s="79"/>
-      <c r="AC23" s="71"/>
-      <c r="AD23" s="72"/>
+      <c r="AA23" s="59"/>
+      <c r="AB23" s="60"/>
+      <c r="AC23" s="61"/>
+      <c r="AD23" s="62"/>
     </row>
     <row r="24" spans="1:30" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="40"/>
@@ -4688,10 +4909,10 @@
       <c r="P24" t="s">
         <v>242</v>
       </c>
-      <c r="AA24" s="63"/>
-      <c r="AB24" s="79"/>
-      <c r="AC24" s="71"/>
-      <c r="AD24" s="72"/>
+      <c r="AA24" s="59"/>
+      <c r="AB24" s="60"/>
+      <c r="AC24" s="61"/>
+      <c r="AD24" s="62"/>
     </row>
     <row r="25" spans="1:30" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="40"/>
@@ -4709,42 +4930,42 @@
       <c r="P25" t="s">
         <v>243</v>
       </c>
-      <c r="AA25" s="63"/>
-      <c r="AB25" s="79"/>
-      <c r="AC25" s="71"/>
-      <c r="AD25" s="72"/>
+      <c r="AA25" s="59"/>
+      <c r="AB25" s="60"/>
+      <c r="AC25" s="61"/>
+      <c r="AD25" s="62"/>
     </row>
     <row r="26" spans="1:30" ht="108" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="47" t="s">
+      <c r="A26" s="51" t="s">
         <v>42</v>
       </c>
-      <c r="B26" s="47"/>
-      <c r="C26" s="47"/>
-      <c r="D26" s="47" t="s">
+      <c r="B26" s="51"/>
+      <c r="C26" s="51"/>
+      <c r="D26" s="51" t="s">
         <v>43</v>
       </c>
-      <c r="E26" s="47"/>
-      <c r="F26" s="47"/>
-      <c r="G26" s="47"/>
-      <c r="H26" s="47"/>
-      <c r="I26" s="47"/>
-      <c r="J26" s="67"/>
-      <c r="K26" s="67"/>
-      <c r="L26" s="67"/>
-      <c r="M26" s="67"/>
-      <c r="N26" s="67"/>
-      <c r="O26" s="67"/>
-      <c r="P26" s="67"/>
-      <c r="Q26" s="67"/>
-      <c r="R26" s="67"/>
-      <c r="S26" s="67"/>
-      <c r="T26" s="67"/>
-      <c r="U26" s="67"/>
-      <c r="V26" s="67"/>
-      <c r="W26" s="67"/>
-      <c r="X26" s="67"/>
-      <c r="Y26" s="67"/>
-      <c r="Z26" s="67"/>
+      <c r="E26" s="51"/>
+      <c r="F26" s="51"/>
+      <c r="G26" s="51"/>
+      <c r="H26" s="51"/>
+      <c r="I26" s="51"/>
+      <c r="J26" s="43"/>
+      <c r="K26" s="43"/>
+      <c r="L26" s="43"/>
+      <c r="M26" s="43"/>
+      <c r="N26" s="43"/>
+      <c r="O26" s="43"/>
+      <c r="P26" s="43"/>
+      <c r="Q26" s="43"/>
+      <c r="R26" s="43"/>
+      <c r="S26" s="43"/>
+      <c r="T26" s="43"/>
+      <c r="U26" s="43"/>
+      <c r="V26" s="43"/>
+      <c r="W26" s="43"/>
+      <c r="X26" s="43"/>
+      <c r="Y26" s="43"/>
+      <c r="Z26" s="43"/>
       <c r="AA26" s="3">
         <v>6</v>
       </c>
@@ -4757,32 +4978,32 @@
       <c r="AD26" s="1"/>
     </row>
     <row r="27" spans="1:30" ht="139.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="47"/>
-      <c r="B27" s="47"/>
-      <c r="C27" s="47"/>
-      <c r="D27" s="47"/>
-      <c r="E27" s="47"/>
-      <c r="F27" s="47"/>
-      <c r="G27" s="47"/>
-      <c r="H27" s="47"/>
-      <c r="I27" s="47"/>
-      <c r="J27" s="67"/>
-      <c r="K27" s="67"/>
-      <c r="L27" s="67"/>
-      <c r="M27" s="67"/>
-      <c r="N27" s="67"/>
-      <c r="O27" s="67"/>
-      <c r="P27" s="67"/>
-      <c r="Q27" s="67"/>
-      <c r="R27" s="67"/>
-      <c r="S27" s="67"/>
-      <c r="T27" s="67"/>
-      <c r="U27" s="67"/>
-      <c r="V27" s="67"/>
-      <c r="W27" s="67"/>
-      <c r="X27" s="67"/>
-      <c r="Y27" s="67"/>
-      <c r="Z27" s="67"/>
+      <c r="A27" s="51"/>
+      <c r="B27" s="51"/>
+      <c r="C27" s="51"/>
+      <c r="D27" s="51"/>
+      <c r="E27" s="51"/>
+      <c r="F27" s="51"/>
+      <c r="G27" s="51"/>
+      <c r="H27" s="51"/>
+      <c r="I27" s="51"/>
+      <c r="J27" s="43"/>
+      <c r="K27" s="43"/>
+      <c r="L27" s="43"/>
+      <c r="M27" s="43"/>
+      <c r="N27" s="43"/>
+      <c r="O27" s="43"/>
+      <c r="P27" s="43"/>
+      <c r="Q27" s="43"/>
+      <c r="R27" s="43"/>
+      <c r="S27" s="43"/>
+      <c r="T27" s="43"/>
+      <c r="U27" s="43"/>
+      <c r="V27" s="43"/>
+      <c r="W27" s="43"/>
+      <c r="X27" s="43"/>
+      <c r="Y27" s="43"/>
+      <c r="Z27" s="43"/>
       <c r="AA27" s="3">
         <v>7</v>
       </c>
@@ -4794,134 +5015,68 @@
       </c>
       <c r="AD27" s="1"/>
     </row>
-    <row r="54" spans="1:26" ht="42" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="D54" s="54" t="s">
+    <row r="54" spans="1:10" ht="42" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D54" s="58" t="s">
         <v>44</v>
       </c>
-      <c r="E54" s="54"/>
-      <c r="F54" s="54"/>
-      <c r="G54" s="54"/>
-      <c r="H54" s="54"/>
-      <c r="I54" s="54"/>
-      <c r="J54" s="54"/>
-      <c r="K54" s="69"/>
-      <c r="L54" s="69"/>
-      <c r="M54" s="69"/>
-      <c r="N54" s="69"/>
-      <c r="O54" s="69"/>
-      <c r="P54" s="69"/>
-      <c r="Q54" s="69"/>
-      <c r="R54" s="69"/>
-      <c r="S54" s="69"/>
-      <c r="T54" s="69"/>
-      <c r="U54" s="69"/>
-      <c r="V54" s="69"/>
-      <c r="W54" s="69"/>
-      <c r="X54" s="69"/>
-      <c r="Y54" s="69"/>
-      <c r="Z54" s="69"/>
-    </row>
-    <row r="55" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="D55" s="69"/>
-      <c r="E55" s="69"/>
-      <c r="F55" s="69"/>
-      <c r="G55" s="69"/>
-      <c r="H55" s="69"/>
-      <c r="I55" s="69"/>
-      <c r="J55" s="69"/>
-      <c r="K55" s="69"/>
-      <c r="L55" s="69"/>
-      <c r="M55" s="69"/>
-      <c r="N55" s="69"/>
-      <c r="O55" s="69"/>
-      <c r="P55" s="69"/>
-      <c r="Q55" s="69"/>
-      <c r="R55" s="69"/>
-      <c r="S55" s="69"/>
-      <c r="T55" s="69"/>
-      <c r="U55" s="69"/>
-      <c r="V55" s="69"/>
-      <c r="W55" s="69"/>
-      <c r="X55" s="69"/>
-      <c r="Y55" s="69"/>
-      <c r="Z55" s="69"/>
-    </row>
-    <row r="56" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="D56" s="69"/>
-      <c r="E56" s="69"/>
-      <c r="F56" s="69"/>
-      <c r="G56" s="69"/>
-      <c r="H56" s="69"/>
-      <c r="I56" s="69"/>
-      <c r="J56" s="69"/>
-      <c r="K56" s="69"/>
-      <c r="L56" s="69"/>
-      <c r="M56" s="69"/>
-      <c r="N56" s="69"/>
-      <c r="O56" s="69"/>
-      <c r="P56" s="69"/>
-      <c r="Q56" s="69"/>
-      <c r="R56" s="69"/>
-      <c r="S56" s="69"/>
-      <c r="T56" s="69"/>
-      <c r="U56" s="69"/>
-      <c r="V56" s="69"/>
-      <c r="W56" s="69"/>
-      <c r="X56" s="69"/>
-      <c r="Y56" s="69"/>
-      <c r="Z56" s="69"/>
-    </row>
-    <row r="58" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A58" s="53" t="s">
+      <c r="E54" s="58"/>
+      <c r="F54" s="58"/>
+      <c r="G54" s="58"/>
+      <c r="H54" s="58"/>
+      <c r="I54" s="58"/>
+      <c r="J54" s="58"/>
+    </row>
+    <row r="58" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A58" s="57" t="s">
         <v>41</v>
       </c>
-      <c r="B58" s="53"/>
-      <c r="C58" s="53"/>
+      <c r="B58" s="57"/>
+      <c r="C58" s="57"/>
       <c r="D58" s="20"/>
     </row>
-    <row r="59" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="53"/>
-      <c r="B59" s="53"/>
-      <c r="C59" s="53"/>
-    </row>
-    <row r="60" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="53"/>
-      <c r="B60" s="53"/>
-      <c r="C60" s="53"/>
-    </row>
-    <row r="61" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="53"/>
-      <c r="B61" s="53"/>
-      <c r="C61" s="53"/>
-    </row>
-    <row r="62" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="47" t="s">
+    <row r="59" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="57"/>
+      <c r="B59" s="57"/>
+      <c r="C59" s="57"/>
+    </row>
+    <row r="60" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="57"/>
+      <c r="B60" s="57"/>
+      <c r="C60" s="57"/>
+    </row>
+    <row r="61" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="57"/>
+      <c r="B61" s="57"/>
+      <c r="C61" s="57"/>
+    </row>
+    <row r="62" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="51" t="s">
         <v>45</v>
       </c>
-      <c r="B62" s="47"/>
-      <c r="C62" s="47"/>
-    </row>
-    <row r="63" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A63" s="47"/>
-      <c r="B63" s="47"/>
-      <c r="C63" s="47"/>
+      <c r="B62" s="51"/>
+      <c r="C62" s="51"/>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A63" s="51"/>
+      <c r="B63" s="51"/>
+      <c r="C63" s="51"/>
     </row>
     <row r="87" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="52" t="s">
+      <c r="A87" s="56" t="s">
         <v>46</v>
       </c>
-      <c r="B87" s="52"/>
-      <c r="C87" s="52"/>
+      <c r="B87" s="56"/>
+      <c r="C87" s="56"/>
     </row>
     <row r="88" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="52"/>
-      <c r="B88" s="52"/>
-      <c r="C88" s="52"/>
+      <c r="A88" s="56"/>
+      <c r="B88" s="56"/>
+      <c r="C88" s="56"/>
     </row>
     <row r="89" spans="1:3" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="52"/>
-      <c r="B89" s="52"/>
-      <c r="C89" s="52"/>
+      <c r="A89" s="56"/>
+      <c r="B89" s="56"/>
+      <c r="C89" s="56"/>
     </row>
   </sheetData>
   <mergeCells count="20">
@@ -5000,38 +5155,38 @@
       <c r="Q1" s="28"/>
     </row>
     <row r="2" spans="1:23" ht="110.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="70" t="s">
+      <c r="A2" s="44" t="s">
         <v>246</v>
       </c>
       <c r="B2" t="s">
         <v>247</v>
       </c>
-      <c r="G2" s="58">
+      <c r="G2" s="72">
         <v>1</v>
       </c>
-      <c r="H2" s="58" t="s">
+      <c r="H2" s="72" t="s">
         <v>56</v>
       </c>
-      <c r="I2" s="73" t="s">
+      <c r="I2" s="66" t="s">
         <v>57</v>
       </c>
-      <c r="J2" s="80" t="s">
+      <c r="J2" s="75" t="s">
         <v>58</v>
       </c>
-      <c r="L2" s="47" t="s">
+      <c r="L2" s="51" t="s">
         <v>68</v>
       </c>
-      <c r="M2" s="45"/>
-      <c r="N2" s="45"/>
-      <c r="O2" s="45"/>
-      <c r="P2" s="45"/>
-      <c r="Q2" s="45"/>
-      <c r="R2" s="45"/>
-      <c r="S2" s="45"/>
-      <c r="T2" s="45"/>
-      <c r="U2" s="45"/>
-      <c r="V2" s="45"/>
-      <c r="W2" s="45"/>
+      <c r="M2" s="49"/>
+      <c r="N2" s="49"/>
+      <c r="O2" s="49"/>
+      <c r="P2" s="49"/>
+      <c r="Q2" s="49"/>
+      <c r="R2" s="49"/>
+      <c r="S2" s="49"/>
+      <c r="T2" s="49"/>
+      <c r="U2" s="49"/>
+      <c r="V2" s="49"/>
+      <c r="W2" s="49"/>
     </row>
     <row r="3" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B3" t="s">
@@ -5040,10 +5195,10 @@
       <c r="C3" t="s">
         <v>248</v>
       </c>
-      <c r="G3" s="60"/>
-      <c r="H3" s="60"/>
-      <c r="I3" s="74"/>
-      <c r="J3" s="81"/>
+      <c r="G3" s="73"/>
+      <c r="H3" s="73"/>
+      <c r="I3" s="67"/>
+      <c r="J3" s="76"/>
       <c r="L3" s="38"/>
       <c r="M3" s="23"/>
       <c r="N3" s="23"/>
@@ -5064,10 +5219,10 @@
       <c r="C4" t="s">
         <v>250</v>
       </c>
-      <c r="G4" s="60"/>
-      <c r="H4" s="60"/>
-      <c r="I4" s="74"/>
-      <c r="J4" s="81"/>
+      <c r="G4" s="73"/>
+      <c r="H4" s="73"/>
+      <c r="I4" s="67"/>
+      <c r="J4" s="76"/>
       <c r="L4" s="38"/>
       <c r="M4" s="23"/>
       <c r="N4" s="23"/>
@@ -5085,10 +5240,10 @@
       <c r="C5" t="s">
         <v>251</v>
       </c>
-      <c r="G5" s="59"/>
-      <c r="H5" s="59"/>
-      <c r="I5" s="75"/>
-      <c r="J5" s="82"/>
+      <c r="G5" s="74"/>
+      <c r="H5" s="74"/>
+      <c r="I5" s="68"/>
+      <c r="J5" s="77"/>
       <c r="L5" s="38"/>
       <c r="M5" s="23"/>
       <c r="N5" s="23"/>
@@ -5103,22 +5258,22 @@
       <c r="W5" s="23"/>
     </row>
     <row r="6" spans="1:23" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="70" t="s">
+      <c r="A6" s="44" t="s">
         <v>252</v>
       </c>
       <c r="B6" t="s">
         <v>253</v>
       </c>
-      <c r="G6" s="58">
+      <c r="G6" s="72">
         <v>2</v>
       </c>
-      <c r="H6" s="58" t="s">
+      <c r="H6" s="72" t="s">
         <v>59</v>
       </c>
-      <c r="I6" s="73" t="s">
+      <c r="I6" s="66" t="s">
         <v>60</v>
       </c>
-      <c r="J6" s="83" t="s">
+      <c r="J6" s="78" t="s">
         <v>72</v>
       </c>
       <c r="M6" s="26"/>
@@ -5130,20 +5285,20 @@
       <c r="C7" t="s">
         <v>254</v>
       </c>
-      <c r="G7" s="60"/>
-      <c r="H7" s="60"/>
-      <c r="I7" s="74"/>
-      <c r="J7" s="84"/>
+      <c r="G7" s="73"/>
+      <c r="H7" s="73"/>
+      <c r="I7" s="67"/>
+      <c r="J7" s="79"/>
       <c r="M7" s="26"/>
     </row>
     <row r="8" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
         <v>255</v>
       </c>
-      <c r="G8" s="60"/>
-      <c r="H8" s="60"/>
-      <c r="I8" s="74"/>
-      <c r="J8" s="84"/>
+      <c r="G8" s="73"/>
+      <c r="H8" s="73"/>
+      <c r="I8" s="67"/>
+      <c r="J8" s="79"/>
       <c r="M8" s="26"/>
     </row>
     <row r="9" spans="1:23" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -5153,29 +5308,29 @@
       <c r="C9" t="s">
         <v>256</v>
       </c>
-      <c r="G9" s="59"/>
-      <c r="H9" s="59"/>
-      <c r="I9" s="75"/>
-      <c r="J9" s="85"/>
+      <c r="G9" s="74"/>
+      <c r="H9" s="74"/>
+      <c r="I9" s="68"/>
+      <c r="J9" s="80"/>
       <c r="M9" s="26"/>
     </row>
     <row r="10" spans="1:23" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="70" t="s">
+      <c r="A10" s="44" t="s">
         <v>257</v>
       </c>
       <c r="B10" t="s">
         <v>258</v>
       </c>
-      <c r="G10" s="58">
+      <c r="G10" s="72">
         <v>3</v>
       </c>
-      <c r="H10" s="58" t="s">
+      <c r="H10" s="72" t="s">
         <v>61</v>
       </c>
-      <c r="I10" s="73" t="s">
+      <c r="I10" s="66" t="s">
         <v>62</v>
       </c>
-      <c r="J10" s="83" t="s">
+      <c r="J10" s="78" t="s">
         <v>63</v>
       </c>
     </row>
@@ -5186,10 +5341,10 @@
       <c r="C11" t="s">
         <v>259</v>
       </c>
-      <c r="G11" s="60"/>
-      <c r="H11" s="60"/>
-      <c r="I11" s="74"/>
-      <c r="J11" s="84"/>
+      <c r="G11" s="73"/>
+      <c r="H11" s="73"/>
+      <c r="I11" s="67"/>
+      <c r="J11" s="79"/>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
@@ -5198,43 +5353,43 @@
       <c r="C12" t="s">
         <v>260</v>
       </c>
-      <c r="G12" s="60"/>
-      <c r="H12" s="60"/>
-      <c r="I12" s="74"/>
-      <c r="J12" s="84"/>
+      <c r="G12" s="73"/>
+      <c r="H12" s="73"/>
+      <c r="I12" s="67"/>
+      <c r="J12" s="79"/>
     </row>
     <row r="13" spans="1:23" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="70" t="s">
+      <c r="A13" s="44" t="s">
         <v>261</v>
       </c>
       <c r="B13" t="s">
         <v>262</v>
       </c>
-      <c r="G13" s="58">
+      <c r="G13" s="72">
         <v>4</v>
       </c>
-      <c r="H13" s="58" t="s">
+      <c r="H13" s="72" t="s">
         <v>66</v>
       </c>
-      <c r="I13" s="73" t="s">
+      <c r="I13" s="66" t="s">
         <v>65</v>
       </c>
-      <c r="J13" s="58"/>
-      <c r="K13" s="55" t="s">
+      <c r="J13" s="72"/>
+      <c r="K13" s="81" t="s">
         <v>69</v>
       </c>
-      <c r="L13" s="45"/>
-      <c r="M13" s="45"/>
-      <c r="N13" s="45"/>
-      <c r="O13" s="45"/>
-      <c r="P13" s="45"/>
-      <c r="Q13" s="45"/>
-      <c r="R13" s="45"/>
-      <c r="S13" s="45"/>
-      <c r="T13" s="45"/>
-      <c r="U13" s="45"/>
-      <c r="V13" s="45"/>
-      <c r="W13" s="45"/>
+      <c r="L13" s="49"/>
+      <c r="M13" s="49"/>
+      <c r="N13" s="49"/>
+      <c r="O13" s="49"/>
+      <c r="P13" s="49"/>
+      <c r="Q13" s="49"/>
+      <c r="R13" s="49"/>
+      <c r="S13" s="49"/>
+      <c r="T13" s="49"/>
+      <c r="U13" s="49"/>
+      <c r="V13" s="49"/>
+      <c r="W13" s="49"/>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
@@ -5243,23 +5398,23 @@
       <c r="C14" t="s">
         <v>263</v>
       </c>
-      <c r="G14" s="60"/>
-      <c r="H14" s="60"/>
-      <c r="I14" s="74"/>
-      <c r="J14" s="60"/>
-      <c r="K14" s="55"/>
-      <c r="L14" s="45"/>
-      <c r="M14" s="45"/>
-      <c r="N14" s="45"/>
-      <c r="O14" s="45"/>
-      <c r="P14" s="45"/>
-      <c r="Q14" s="45"/>
-      <c r="R14" s="45"/>
-      <c r="S14" s="45"/>
-      <c r="T14" s="45"/>
-      <c r="U14" s="45"/>
-      <c r="V14" s="45"/>
-      <c r="W14" s="45"/>
+      <c r="G14" s="73"/>
+      <c r="H14" s="73"/>
+      <c r="I14" s="67"/>
+      <c r="J14" s="73"/>
+      <c r="K14" s="81"/>
+      <c r="L14" s="49"/>
+      <c r="M14" s="49"/>
+      <c r="N14" s="49"/>
+      <c r="O14" s="49"/>
+      <c r="P14" s="49"/>
+      <c r="Q14" s="49"/>
+      <c r="R14" s="49"/>
+      <c r="S14" s="49"/>
+      <c r="T14" s="49"/>
+      <c r="U14" s="49"/>
+      <c r="V14" s="49"/>
+      <c r="W14" s="49"/>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
@@ -5268,26 +5423,26 @@
       <c r="C15" t="s">
         <v>264</v>
       </c>
-      <c r="G15" s="59"/>
-      <c r="H15" s="59"/>
-      <c r="I15" s="75"/>
-      <c r="J15" s="59"/>
-      <c r="K15" s="55"/>
-      <c r="L15" s="45"/>
-      <c r="M15" s="45"/>
-      <c r="N15" s="45"/>
-      <c r="O15" s="45"/>
-      <c r="P15" s="45"/>
-      <c r="Q15" s="45"/>
-      <c r="R15" s="45"/>
-      <c r="S15" s="45"/>
-      <c r="T15" s="45"/>
-      <c r="U15" s="45"/>
-      <c r="V15" s="45"/>
-      <c r="W15" s="45"/>
+      <c r="G15" s="74"/>
+      <c r="H15" s="74"/>
+      <c r="I15" s="68"/>
+      <c r="J15" s="74"/>
+      <c r="K15" s="81"/>
+      <c r="L15" s="49"/>
+      <c r="M15" s="49"/>
+      <c r="N15" s="49"/>
+      <c r="O15" s="49"/>
+      <c r="P15" s="49"/>
+      <c r="Q15" s="49"/>
+      <c r="R15" s="49"/>
+      <c r="S15" s="49"/>
+      <c r="T15" s="49"/>
+      <c r="U15" s="49"/>
+      <c r="V15" s="49"/>
+      <c r="W15" s="49"/>
     </row>
     <row r="16" spans="1:23" ht="45" x14ac:dyDescent="0.25">
-      <c r="A16" s="70" t="s">
+      <c r="A16" s="44" t="s">
         <v>64</v>
       </c>
       <c r="B16" t="s">
@@ -5303,19 +5458,19 @@
         <v>67</v>
       </c>
       <c r="J16" s="3"/>
-      <c r="K16" s="56"/>
-      <c r="L16" s="45"/>
-      <c r="M16" s="45"/>
-      <c r="N16" s="45"/>
-      <c r="O16" s="45"/>
-      <c r="P16" s="45"/>
-      <c r="Q16" s="45"/>
-      <c r="R16" s="45"/>
-      <c r="S16" s="45"/>
-      <c r="T16" s="45"/>
-      <c r="U16" s="45"/>
-      <c r="V16" s="45"/>
-      <c r="W16" s="45"/>
+      <c r="K16" s="82"/>
+      <c r="L16" s="49"/>
+      <c r="M16" s="49"/>
+      <c r="N16" s="49"/>
+      <c r="O16" s="49"/>
+      <c r="P16" s="49"/>
+      <c r="Q16" s="49"/>
+      <c r="R16" s="49"/>
+      <c r="S16" s="49"/>
+      <c r="T16" s="49"/>
+      <c r="U16" s="49"/>
+      <c r="V16" s="49"/>
+      <c r="W16" s="49"/>
     </row>
     <row r="17" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
@@ -5324,11 +5479,11 @@
       <c r="C17" t="s">
         <v>266</v>
       </c>
-      <c r="G17" s="68"/>
-      <c r="H17" s="68"/>
-      <c r="I17" s="86"/>
-      <c r="J17" s="68"/>
-      <c r="K17" s="87"/>
+      <c r="G17" s="14"/>
+      <c r="H17" s="14"/>
+      <c r="I17" s="45"/>
+      <c r="J17" s="14"/>
+      <c r="K17" s="23"/>
       <c r="L17" s="23"/>
       <c r="M17" s="23"/>
       <c r="N17" s="23"/>
@@ -5410,83 +5565,81 @@
       <c r="J27" s="14"/>
     </row>
     <row r="33" spans="11:22" x14ac:dyDescent="0.25">
-      <c r="K33" s="47" t="s">
+      <c r="K33" s="51" t="s">
         <v>70</v>
       </c>
-      <c r="L33" s="45"/>
-      <c r="M33" s="45"/>
-      <c r="N33" s="45"/>
-      <c r="O33" s="45"/>
-      <c r="P33" s="45"/>
-      <c r="Q33" s="45"/>
-      <c r="R33" s="45"/>
-      <c r="S33" s="45"/>
-      <c r="T33" s="45"/>
-      <c r="U33" s="45"/>
-      <c r="V33" s="45"/>
+      <c r="L33" s="49"/>
+      <c r="M33" s="49"/>
+      <c r="N33" s="49"/>
+      <c r="O33" s="49"/>
+      <c r="P33" s="49"/>
+      <c r="Q33" s="49"/>
+      <c r="R33" s="49"/>
+      <c r="S33" s="49"/>
+      <c r="T33" s="49"/>
+      <c r="U33" s="49"/>
+      <c r="V33" s="49"/>
     </row>
     <row r="34" spans="11:22" x14ac:dyDescent="0.25">
-      <c r="K34" s="45"/>
-      <c r="L34" s="45"/>
-      <c r="M34" s="45"/>
-      <c r="N34" s="45"/>
-      <c r="O34" s="45"/>
-      <c r="P34" s="45"/>
-      <c r="Q34" s="45"/>
-      <c r="R34" s="45"/>
-      <c r="S34" s="45"/>
-      <c r="T34" s="45"/>
-      <c r="U34" s="45"/>
-      <c r="V34" s="45"/>
+      <c r="K34" s="49"/>
+      <c r="L34" s="49"/>
+      <c r="M34" s="49"/>
+      <c r="N34" s="49"/>
+      <c r="O34" s="49"/>
+      <c r="P34" s="49"/>
+      <c r="Q34" s="49"/>
+      <c r="R34" s="49"/>
+      <c r="S34" s="49"/>
+      <c r="T34" s="49"/>
+      <c r="U34" s="49"/>
+      <c r="V34" s="49"/>
     </row>
     <row r="35" spans="11:22" x14ac:dyDescent="0.25">
-      <c r="K35" s="45"/>
-      <c r="L35" s="45"/>
-      <c r="M35" s="45"/>
-      <c r="N35" s="45"/>
-      <c r="O35" s="45"/>
-      <c r="P35" s="45"/>
-      <c r="Q35" s="45"/>
-      <c r="R35" s="45"/>
-      <c r="S35" s="45"/>
-      <c r="T35" s="45"/>
-      <c r="U35" s="45"/>
-      <c r="V35" s="45"/>
+      <c r="K35" s="49"/>
+      <c r="L35" s="49"/>
+      <c r="M35" s="49"/>
+      <c r="N35" s="49"/>
+      <c r="O35" s="49"/>
+      <c r="P35" s="49"/>
+      <c r="Q35" s="49"/>
+      <c r="R35" s="49"/>
+      <c r="S35" s="49"/>
+      <c r="T35" s="49"/>
+      <c r="U35" s="49"/>
+      <c r="V35" s="49"/>
     </row>
     <row r="51" spans="11:22" x14ac:dyDescent="0.25">
-      <c r="K51" s="54" t="s">
+      <c r="K51" s="58" t="s">
         <v>71</v>
       </c>
-      <c r="L51" s="45"/>
-      <c r="M51" s="45"/>
-      <c r="N51" s="45"/>
-      <c r="O51" s="45"/>
-      <c r="P51" s="45"/>
-      <c r="Q51" s="45"/>
-      <c r="R51" s="45"/>
-      <c r="S51" s="45"/>
-      <c r="T51" s="45"/>
-      <c r="U51" s="45"/>
-      <c r="V51" s="45"/>
+      <c r="L51" s="49"/>
+      <c r="M51" s="49"/>
+      <c r="N51" s="49"/>
+      <c r="O51" s="49"/>
+      <c r="P51" s="49"/>
+      <c r="Q51" s="49"/>
+      <c r="R51" s="49"/>
+      <c r="S51" s="49"/>
+      <c r="T51" s="49"/>
+      <c r="U51" s="49"/>
+      <c r="V51" s="49"/>
     </row>
     <row r="52" spans="11:22" x14ac:dyDescent="0.25">
-      <c r="K52" s="45"/>
-      <c r="L52" s="45"/>
-      <c r="M52" s="45"/>
-      <c r="N52" s="45"/>
-      <c r="O52" s="45"/>
-      <c r="P52" s="45"/>
-      <c r="Q52" s="45"/>
-      <c r="R52" s="45"/>
-      <c r="S52" s="45"/>
-      <c r="T52" s="45"/>
-      <c r="U52" s="45"/>
-      <c r="V52" s="45"/>
+      <c r="K52" s="49"/>
+      <c r="L52" s="49"/>
+      <c r="M52" s="49"/>
+      <c r="N52" s="49"/>
+      <c r="O52" s="49"/>
+      <c r="P52" s="49"/>
+      <c r="Q52" s="49"/>
+      <c r="R52" s="49"/>
+      <c r="S52" s="49"/>
+      <c r="T52" s="49"/>
+      <c r="U52" s="49"/>
+      <c r="V52" s="49"/>
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="G13:G15"/>
-    <mergeCell ref="H13:H15"/>
     <mergeCell ref="I13:I15"/>
     <mergeCell ref="J13:J15"/>
     <mergeCell ref="L2:W2"/>
@@ -5505,6 +5658,8 @@
     <mergeCell ref="H10:H12"/>
     <mergeCell ref="I10:I12"/>
     <mergeCell ref="J10:J12"/>
+    <mergeCell ref="G13:G15"/>
+    <mergeCell ref="H13:H15"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="J2" r:id="rId1" xr:uid="{3D14D563-A18C-4362-B2CD-8D8339C1C427}"/>
@@ -5575,14 +5730,14 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="57" t="s">
+      <c r="A7" s="83" t="s">
         <v>79</v>
       </c>
-      <c r="B7" s="45"/>
+      <c r="B7" s="49"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="45"/>
-      <c r="B8" s="45"/>
+      <c r="A8" s="49"/>
+      <c r="B8" s="49"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
@@ -5780,511 +5935,1771 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D5CC180-ABEC-4096-BF7B-D59D7E76A5ED}">
-  <dimension ref="A1:M19"/>
+  <dimension ref="A1:P77"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
+    <sheetView tabSelected="1" zoomScale="95" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="42.5703125" customWidth="1"/>
-    <col min="3" max="3" width="108.28515625" customWidth="1"/>
-    <col min="4" max="4" width="70" customWidth="1"/>
-    <col min="5" max="5" width="17.140625" customWidth="1"/>
+    <col min="1" max="1" width="43.140625" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" customWidth="1"/>
+    <col min="3" max="3" width="175.28515625" customWidth="1"/>
+    <col min="5" max="5" width="42.5703125" customWidth="1"/>
+    <col min="6" max="6" width="108.28515625" customWidth="1"/>
+    <col min="7" max="7" width="70" customWidth="1"/>
+    <col min="8" max="8" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="33" t="s">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="D1" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="30" t="s">
+      <c r="E1" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="30" t="s">
+      <c r="F1" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="30" t="s">
+      <c r="G1" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="33" t="s">
+      <c r="H1" s="33" t="s">
         <v>121</v>
       </c>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
       <c r="I1" s="30"/>
       <c r="J1" s="30"/>
       <c r="K1" s="30"/>
       <c r="L1" s="30"/>
       <c r="M1" s="30"/>
-    </row>
-    <row r="2" spans="1:13" ht="112.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3">
+      <c r="N1" s="30"/>
+      <c r="O1" s="30"/>
+      <c r="P1" s="30"/>
+    </row>
+    <row r="2" spans="1:16" ht="112.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>268</v>
+      </c>
+      <c r="B2" t="s">
+        <v>269</v>
+      </c>
+      <c r="D2" s="72">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="E2" s="72" t="s">
         <v>119</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="F2" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="G2" s="11" t="s">
         <v>120</v>
       </c>
-      <c r="E2" s="3">
+      <c r="H2" s="3">
         <v>8</v>
       </c>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
-    </row>
-    <row r="3" spans="1:13" ht="180" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
-        <v>2</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="E3" s="3">
-        <v>8</v>
-      </c>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+    </row>
+    <row r="3" spans="1:16" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>218</v>
+      </c>
+      <c r="C3" t="s">
+        <v>270</v>
+      </c>
+      <c r="D3" s="73"/>
+      <c r="E3" s="73"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="3"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
-    </row>
-    <row r="4" spans="1:13" ht="210" x14ac:dyDescent="0.25">
-      <c r="A4" s="31">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="D4" s="9" t="s">
-        <v>126</v>
-      </c>
-      <c r="E4" s="3">
-        <v>8</v>
-      </c>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
+    </row>
+    <row r="4" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>271</v>
+      </c>
+      <c r="D4" s="73"/>
+      <c r="E4" s="73"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="3"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
-    </row>
-    <row r="5" spans="1:13" ht="150" x14ac:dyDescent="0.25">
-      <c r="A5" s="31">
-        <v>4</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>155</v>
-      </c>
-      <c r="E5" s="31">
-        <v>8</v>
-      </c>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
+    </row>
+    <row r="5" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>249</v>
+      </c>
+      <c r="C5" t="s">
+        <v>272</v>
+      </c>
+      <c r="D5" s="74"/>
+      <c r="E5" s="74"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="3"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
-    </row>
-    <row r="6" spans="1:13" ht="270" x14ac:dyDescent="0.25">
-      <c r="A6" s="31">
-        <v>5</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>131</v>
-      </c>
-      <c r="D6" s="9" t="s">
-        <v>156</v>
-      </c>
-      <c r="E6" s="31">
-        <v>9</v>
-      </c>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
+      <c r="N5" s="1"/>
+      <c r="O5" s="1"/>
+      <c r="P5" s="1"/>
+    </row>
+    <row r="6" spans="1:16" ht="180" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>273</v>
+      </c>
+      <c r="B6" t="s">
+        <v>274</v>
+      </c>
+      <c r="D6" s="72">
+        <v>2</v>
+      </c>
+      <c r="E6" s="72" t="s">
+        <v>122</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="H6" s="3">
+        <v>8</v>
+      </c>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
-    </row>
-    <row r="7" spans="1:13" ht="75" x14ac:dyDescent="0.25">
-      <c r="A7" s="31">
-        <v>6</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>133</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>157</v>
-      </c>
-      <c r="E7" s="31">
-        <v>8</v>
-      </c>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+      <c r="P6" s="1"/>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>218</v>
+      </c>
+      <c r="C7" t="s">
+        <v>275</v>
+      </c>
+      <c r="D7" s="73"/>
+      <c r="E7" s="73"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="3"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
-    </row>
-    <row r="8" spans="1:13" ht="90" x14ac:dyDescent="0.25">
-      <c r="A8" s="3">
-        <v>7</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>135</v>
-      </c>
-      <c r="D8" s="1"/>
-      <c r="E8" s="31">
-        <v>7</v>
-      </c>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
+      <c r="P7" s="1"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>276</v>
+      </c>
+      <c r="D8" s="73"/>
+      <c r="E8" s="73"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="3"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
-    </row>
-    <row r="9" spans="1:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="3">
-        <v>8</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>137</v>
-      </c>
-      <c r="D9" s="9" t="s">
-        <v>158</v>
-      </c>
-      <c r="E9" s="31">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+      <c r="P8" s="1"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>249</v>
+      </c>
+      <c r="C9" t="s">
+        <v>277</v>
+      </c>
+      <c r="D9" s="74"/>
+      <c r="E9" s="74"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="3"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="31">
-        <v>9</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="D10" s="9" t="s">
-        <v>159</v>
-      </c>
-      <c r="E10" s="31">
-        <v>9</v>
-      </c>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1"/>
+      <c r="P9" s="1"/>
+    </row>
+    <row r="10" spans="1:16" ht="150.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>125</v>
+      </c>
+      <c r="B10" t="s">
+        <v>278</v>
+      </c>
+      <c r="D10" s="84">
+        <v>3</v>
+      </c>
+      <c r="E10" s="84" t="s">
+        <v>125</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="H10" s="3">
+        <v>8</v>
+      </c>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
       <c r="M10" s="1"/>
-    </row>
-    <row r="11" spans="1:13" ht="90" x14ac:dyDescent="0.25">
-      <c r="A11" s="31">
-        <v>10</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="D11" s="9" t="s">
-        <v>160</v>
-      </c>
-      <c r="E11" s="34">
-        <v>9</v>
-      </c>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
+      <c r="N10" s="1"/>
+      <c r="O10" s="1"/>
+      <c r="P10" s="1"/>
+    </row>
+    <row r="11" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>218</v>
+      </c>
+      <c r="C11" t="s">
+        <v>279</v>
+      </c>
+      <c r="D11" s="85"/>
+      <c r="E11" s="85"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="3"/>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
       <c r="M11" s="1"/>
-    </row>
-    <row r="12" spans="1:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" s="31">
-        <v>11</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="D12" s="9" t="s">
-        <v>161</v>
-      </c>
-      <c r="E12" s="31">
-        <v>10</v>
-      </c>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
+      <c r="N11" s="1"/>
+      <c r="O11" s="1"/>
+      <c r="P11" s="1"/>
+    </row>
+    <row r="12" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>280</v>
+      </c>
+      <c r="D12" s="85"/>
+      <c r="E12" s="85"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="3"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
       <c r="M12" s="1"/>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="31">
-        <v>12</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="D13" s="9" t="s">
-        <v>163</v>
-      </c>
-      <c r="E13" s="31">
-        <v>12</v>
-      </c>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
+      <c r="N12" s="1"/>
+      <c r="O12" s="1"/>
+      <c r="P12" s="1"/>
+    </row>
+    <row r="13" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>249</v>
+      </c>
+      <c r="C13" t="s">
+        <v>272</v>
+      </c>
+      <c r="D13" s="86"/>
+      <c r="E13" s="86"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="3"/>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
       <c r="L13" s="1"/>
       <c r="M13" s="1"/>
-    </row>
-    <row r="14" spans="1:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="A14" s="31">
-        <v>13</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>146</v>
-      </c>
-      <c r="D14" s="9" t="s">
-        <v>162</v>
-      </c>
-      <c r="E14" s="31">
-        <v>14</v>
-      </c>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
+      <c r="P13" s="1"/>
+    </row>
+    <row r="14" spans="1:16" ht="175.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>128</v>
+      </c>
+      <c r="B14" t="s">
+        <v>281</v>
+      </c>
+      <c r="D14" s="84">
+        <v>4</v>
+      </c>
+      <c r="E14" s="72" t="s">
+        <v>128</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="G14" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="H14" s="31">
+        <v>8</v>
+      </c>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
       <c r="M14" s="1"/>
-    </row>
-    <row r="15" spans="1:13" ht="135" x14ac:dyDescent="0.25">
-      <c r="A15" s="31">
-        <v>14</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>148</v>
-      </c>
-      <c r="D15" s="9" t="s">
-        <v>164</v>
-      </c>
-      <c r="E15" s="31">
-        <v>15</v>
-      </c>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
+      <c r="N14" s="1"/>
+      <c r="O14" s="1"/>
+      <c r="P14" s="1"/>
+    </row>
+    <row r="15" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>218</v>
+      </c>
+      <c r="C15" t="s">
+        <v>282</v>
+      </c>
+      <c r="D15" s="85"/>
+      <c r="E15" s="73"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="31"/>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
       <c r="M15" s="1"/>
-    </row>
-    <row r="16" spans="1:13" ht="75" x14ac:dyDescent="0.25">
-      <c r="A16" s="31">
-        <v>15</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>149</v>
-      </c>
-      <c r="D16" s="9" t="s">
-        <v>165</v>
-      </c>
-      <c r="E16" s="31">
-        <v>16</v>
-      </c>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
+      <c r="N15" s="1"/>
+      <c r="O15" s="1"/>
+      <c r="P15" s="1"/>
+    </row>
+    <row r="16" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>249</v>
+      </c>
+      <c r="D16" s="85"/>
+      <c r="E16" s="73"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="31"/>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
       <c r="M16" s="1"/>
-    </row>
-    <row r="17" spans="1:13" ht="150" x14ac:dyDescent="0.25">
-      <c r="A17" s="32">
-        <v>16</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>152</v>
-      </c>
-      <c r="D17" s="9" t="s">
-        <v>166</v>
-      </c>
-      <c r="E17" s="31">
-        <v>16</v>
-      </c>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
+      <c r="N16" s="1"/>
+      <c r="O16" s="1"/>
+      <c r="P16" s="1"/>
+    </row>
+    <row r="17" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D17" s="86"/>
+      <c r="E17" s="74"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="31"/>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
       <c r="M17" s="1"/>
-    </row>
-    <row r="18" spans="1:13" ht="195" x14ac:dyDescent="0.25">
-      <c r="A18" s="3">
-        <v>17</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="D18" s="9" t="s">
-        <v>167</v>
-      </c>
-      <c r="E18" s="31">
-        <v>16</v>
-      </c>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
+      <c r="N17" s="1"/>
+      <c r="O17" s="1"/>
+      <c r="P17" s="1"/>
+    </row>
+    <row r="18" spans="1:16" ht="270" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>130</v>
+      </c>
+      <c r="B18" t="s">
+        <v>283</v>
+      </c>
+      <c r="D18" s="84">
+        <v>5</v>
+      </c>
+      <c r="E18" s="72" t="s">
+        <v>130</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="G18" s="9" t="s">
+        <v>156</v>
+      </c>
+      <c r="H18" s="31">
+        <v>9</v>
+      </c>
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
       <c r="M18" s="1"/>
-    </row>
-    <row r="19" spans="1:13" ht="60" x14ac:dyDescent="0.25">
-      <c r="A19" s="31">
-        <v>18</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>170</v>
-      </c>
-      <c r="D19" s="9" t="s">
-        <v>171</v>
-      </c>
-      <c r="E19" s="31">
-        <v>8</v>
-      </c>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
+      <c r="N18" s="1"/>
+      <c r="O18" s="1"/>
+      <c r="P18" s="1"/>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>218</v>
+      </c>
+      <c r="C19" t="s">
+        <v>284</v>
+      </c>
+      <c r="D19" s="85"/>
+      <c r="E19" s="73"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="31"/>
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
       <c r="L19" s="1"/>
       <c r="M19" s="1"/>
+      <c r="N19" s="1"/>
+      <c r="O19" s="1"/>
+      <c r="P19" s="1"/>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>285</v>
+      </c>
+      <c r="D20" s="85"/>
+      <c r="E20" s="73"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="31"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
+      <c r="K20" s="1"/>
+      <c r="L20" s="1"/>
+      <c r="M20" s="1"/>
+      <c r="N20" s="1"/>
+      <c r="O20" s="1"/>
+      <c r="P20" s="1"/>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>287</v>
+      </c>
+      <c r="D21" s="85"/>
+      <c r="E21" s="73"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="9"/>
+      <c r="H21" s="31"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+      <c r="K21" s="1"/>
+      <c r="L21" s="1"/>
+      <c r="M21" s="1"/>
+      <c r="N21" s="1"/>
+      <c r="O21" s="1"/>
+      <c r="P21" s="1"/>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>288</v>
+      </c>
+      <c r="D22" s="85"/>
+      <c r="E22" s="73"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="9"/>
+      <c r="H22" s="31"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
+      <c r="K22" s="1"/>
+      <c r="L22" s="1"/>
+      <c r="M22" s="1"/>
+      <c r="N22" s="1"/>
+      <c r="O22" s="1"/>
+      <c r="P22" s="1"/>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C23" t="s">
+        <v>286</v>
+      </c>
+      <c r="D23" s="85"/>
+      <c r="E23" s="73"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="9"/>
+      <c r="H23" s="31"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+      <c r="K23" s="1"/>
+      <c r="L23" s="1"/>
+      <c r="M23" s="1"/>
+      <c r="N23" s="1"/>
+      <c r="O23" s="1"/>
+      <c r="P23" s="1"/>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>249</v>
+      </c>
+      <c r="C24" t="s">
+        <v>289</v>
+      </c>
+      <c r="D24" s="85"/>
+      <c r="E24" s="73"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="9"/>
+      <c r="H24" s="31"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
+      <c r="K24" s="1"/>
+      <c r="L24" s="1"/>
+      <c r="M24" s="1"/>
+      <c r="N24" s="1"/>
+      <c r="O24" s="1"/>
+      <c r="P24" s="1"/>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C25" t="s">
+        <v>290</v>
+      </c>
+      <c r="D25" s="86"/>
+      <c r="E25" s="74"/>
+      <c r="F25" s="6"/>
+      <c r="G25" s="9"/>
+      <c r="H25" s="31"/>
+      <c r="I25" s="1"/>
+      <c r="J25" s="1"/>
+      <c r="K25" s="1"/>
+      <c r="L25" s="1"/>
+      <c r="M25" s="1"/>
+      <c r="N25" s="1"/>
+      <c r="O25" s="1"/>
+      <c r="P25" s="1"/>
+    </row>
+    <row r="26" spans="1:16" ht="75" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>132</v>
+      </c>
+      <c r="B26" t="s">
+        <v>291</v>
+      </c>
+      <c r="D26" s="84">
+        <v>6</v>
+      </c>
+      <c r="E26" s="72" t="s">
+        <v>132</v>
+      </c>
+      <c r="F26" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="G26" s="9" t="s">
+        <v>157</v>
+      </c>
+      <c r="H26" s="31">
+        <v>8</v>
+      </c>
+      <c r="I26" s="1"/>
+      <c r="J26" s="1"/>
+      <c r="K26" s="1"/>
+      <c r="L26" s="1"/>
+      <c r="M26" s="1"/>
+      <c r="N26" s="1"/>
+      <c r="O26" s="1"/>
+      <c r="P26" s="1"/>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>218</v>
+      </c>
+      <c r="C27" t="s">
+        <v>292</v>
+      </c>
+      <c r="D27" s="85"/>
+      <c r="E27" s="73"/>
+      <c r="F27" s="6"/>
+      <c r="G27" s="9"/>
+      <c r="H27" s="31"/>
+      <c r="I27" s="1"/>
+      <c r="J27" s="1"/>
+      <c r="K27" s="1"/>
+      <c r="L27" s="1"/>
+      <c r="M27" s="1"/>
+      <c r="N27" s="1"/>
+      <c r="O27" s="1"/>
+      <c r="P27" s="1"/>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C28" t="s">
+        <v>293</v>
+      </c>
+      <c r="D28" s="85"/>
+      <c r="E28" s="73"/>
+      <c r="F28" s="6"/>
+      <c r="G28" s="9"/>
+      <c r="H28" s="31"/>
+      <c r="I28" s="1"/>
+      <c r="J28" s="1"/>
+      <c r="K28" s="1"/>
+      <c r="L28" s="1"/>
+      <c r="M28" s="1"/>
+      <c r="N28" s="1"/>
+      <c r="O28" s="1"/>
+      <c r="P28" s="1"/>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>249</v>
+      </c>
+      <c r="C29" t="s">
+        <v>294</v>
+      </c>
+      <c r="D29" s="86"/>
+      <c r="E29" s="74"/>
+      <c r="F29" s="6"/>
+      <c r="G29" s="9"/>
+      <c r="H29" s="31"/>
+      <c r="I29" s="1"/>
+      <c r="J29" s="1"/>
+      <c r="K29" s="1"/>
+      <c r="L29" s="1"/>
+      <c r="M29" s="1"/>
+      <c r="N29" s="1"/>
+      <c r="O29" s="1"/>
+      <c r="P29" s="1"/>
+    </row>
+    <row r="30" spans="1:16" ht="90" x14ac:dyDescent="0.25">
+      <c r="A30" s="46" t="s">
+        <v>134</v>
+      </c>
+      <c r="B30" t="s">
+        <v>295</v>
+      </c>
+      <c r="D30" s="72">
+        <v>7</v>
+      </c>
+      <c r="E30" s="72" t="s">
+        <v>134</v>
+      </c>
+      <c r="F30" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="G30" s="1"/>
+      <c r="H30" s="31">
+        <v>7</v>
+      </c>
+      <c r="I30" s="1"/>
+      <c r="J30" s="1"/>
+      <c r="K30" s="1"/>
+      <c r="L30" s="1"/>
+      <c r="M30" s="1"/>
+      <c r="N30" s="1"/>
+      <c r="O30" s="1"/>
+      <c r="P30" s="1"/>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>218</v>
+      </c>
+      <c r="C31" t="s">
+        <v>296</v>
+      </c>
+      <c r="D31" s="73"/>
+      <c r="E31" s="73"/>
+      <c r="F31" s="5"/>
+      <c r="G31" s="1"/>
+      <c r="H31" s="31"/>
+      <c r="I31" s="1"/>
+      <c r="J31" s="1"/>
+      <c r="K31" s="1"/>
+      <c r="L31" s="1"/>
+      <c r="M31" s="1"/>
+      <c r="N31" s="1"/>
+      <c r="O31" s="1"/>
+      <c r="P31" s="1"/>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C32" t="s">
+        <v>297</v>
+      </c>
+      <c r="D32" s="73"/>
+      <c r="E32" s="73"/>
+      <c r="F32" s="5"/>
+      <c r="G32" s="1"/>
+      <c r="H32" s="31"/>
+      <c r="I32" s="1"/>
+      <c r="J32" s="1"/>
+      <c r="K32" s="1"/>
+      <c r="L32" s="1"/>
+      <c r="M32" s="1"/>
+      <c r="N32" s="1"/>
+      <c r="O32" s="1"/>
+      <c r="P32" s="1"/>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>249</v>
+      </c>
+      <c r="C33" t="s">
+        <v>298</v>
+      </c>
+      <c r="D33" s="74"/>
+      <c r="E33" s="74"/>
+      <c r="F33" s="5"/>
+      <c r="G33" s="1"/>
+      <c r="H33" s="31"/>
+      <c r="I33" s="1"/>
+      <c r="J33" s="1"/>
+      <c r="K33" s="1"/>
+      <c r="L33" s="1"/>
+      <c r="M33" s="1"/>
+      <c r="N33" s="1"/>
+      <c r="O33" s="1"/>
+      <c r="P33" s="1"/>
+    </row>
+    <row r="34" spans="1:16" ht="100.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="46" t="s">
+        <v>136</v>
+      </c>
+      <c r="B34" t="s">
+        <v>299</v>
+      </c>
+      <c r="D34" s="72">
+        <v>8</v>
+      </c>
+      <c r="E34" s="72" t="s">
+        <v>136</v>
+      </c>
+      <c r="F34" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="G34" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="H34" s="31">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="I34" s="1"/>
+      <c r="J34" s="1"/>
+      <c r="K34" s="1"/>
+      <c r="L34" s="1"/>
+      <c r="M34" s="1"/>
+      <c r="N34" s="1"/>
+      <c r="O34" s="1"/>
+      <c r="P34" s="1"/>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>218</v>
+      </c>
+      <c r="C35" t="s">
+        <v>300</v>
+      </c>
+      <c r="D35" s="73"/>
+      <c r="E35" s="73"/>
+      <c r="F35" s="5"/>
+      <c r="G35" s="9"/>
+      <c r="H35" s="31"/>
+      <c r="I35" s="1"/>
+      <c r="J35" s="1"/>
+      <c r="K35" s="1"/>
+      <c r="L35" s="1"/>
+      <c r="M35" s="1"/>
+      <c r="N35" s="1"/>
+      <c r="O35" s="1"/>
+      <c r="P35" s="1"/>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C36" t="s">
+        <v>301</v>
+      </c>
+      <c r="D36" s="73"/>
+      <c r="E36" s="73"/>
+      <c r="F36" s="5"/>
+      <c r="G36" s="9"/>
+      <c r="H36" s="31"/>
+      <c r="I36" s="1"/>
+      <c r="J36" s="1"/>
+      <c r="K36" s="1"/>
+      <c r="L36" s="1"/>
+      <c r="M36" s="1"/>
+      <c r="N36" s="1"/>
+      <c r="O36" s="1"/>
+      <c r="P36" s="1"/>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>249</v>
+      </c>
+      <c r="C37" t="s">
+        <v>302</v>
+      </c>
+      <c r="D37" s="73"/>
+      <c r="E37" s="73"/>
+      <c r="F37" s="5"/>
+      <c r="G37" s="9"/>
+      <c r="H37" s="31"/>
+      <c r="I37" s="1"/>
+      <c r="J37" s="1"/>
+      <c r="K37" s="1"/>
+      <c r="L37" s="1"/>
+      <c r="M37" s="1"/>
+      <c r="N37" s="1"/>
+      <c r="O37" s="1"/>
+      <c r="P37" s="1"/>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C38" t="s">
+        <v>304</v>
+      </c>
+      <c r="D38" s="73"/>
+      <c r="E38" s="73"/>
+      <c r="F38" s="5"/>
+      <c r="G38" s="9"/>
+      <c r="H38" s="31"/>
+      <c r="I38" s="1"/>
+      <c r="J38" s="1"/>
+      <c r="K38" s="1"/>
+      <c r="L38" s="1"/>
+      <c r="M38" s="1"/>
+      <c r="N38" s="1"/>
+      <c r="O38" s="1"/>
+      <c r="P38" s="1"/>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C39" t="s">
+        <v>303</v>
+      </c>
+      <c r="D39" s="74"/>
+      <c r="E39" s="74"/>
+      <c r="F39" s="5"/>
+      <c r="G39" s="9"/>
+      <c r="H39" s="31"/>
+      <c r="I39" s="1"/>
+      <c r="J39" s="1"/>
+      <c r="K39" s="1"/>
+      <c r="L39" s="1"/>
+      <c r="M39" s="1"/>
+      <c r="N39" s="1"/>
+      <c r="O39" s="1"/>
+      <c r="P39" s="1"/>
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>138</v>
+      </c>
+      <c r="B40" t="s">
+        <v>306</v>
+      </c>
+      <c r="D40" s="84">
+        <v>9</v>
+      </c>
+      <c r="E40" s="84" t="s">
+        <v>138</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="G40" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="H40" s="31">
+        <v>9</v>
+      </c>
+      <c r="I40" s="1"/>
+      <c r="J40" s="1"/>
+      <c r="K40" s="1"/>
+      <c r="L40" s="1"/>
+      <c r="M40" s="1"/>
+      <c r="N40" s="1"/>
+      <c r="O40" s="1"/>
+      <c r="P40" s="1"/>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>218</v>
+      </c>
+      <c r="C41" t="s">
+        <v>307</v>
+      </c>
+      <c r="D41" s="85"/>
+      <c r="E41" s="85"/>
+      <c r="F41" s="1"/>
+      <c r="G41" s="9"/>
+      <c r="H41" s="34"/>
+      <c r="I41" s="1"/>
+      <c r="J41" s="1"/>
+      <c r="K41" s="1"/>
+      <c r="L41" s="1"/>
+      <c r="M41" s="1"/>
+      <c r="N41" s="1"/>
+      <c r="O41" s="1"/>
+      <c r="P41" s="1"/>
+    </row>
+    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>249</v>
+      </c>
+      <c r="C42" t="s">
+        <v>305</v>
+      </c>
+      <c r="D42" s="86"/>
+      <c r="E42" s="86"/>
+      <c r="F42" s="1"/>
+      <c r="G42" s="9"/>
+      <c r="H42" s="34"/>
+      <c r="I42" s="1"/>
+      <c r="J42" s="1"/>
+      <c r="K42" s="1"/>
+      <c r="L42" s="1"/>
+      <c r="M42" s="1"/>
+      <c r="N42" s="1"/>
+      <c r="O42" s="1"/>
+      <c r="P42" s="1"/>
+    </row>
+    <row r="43" spans="1:16" ht="90" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>139</v>
+      </c>
+      <c r="B43" t="s">
+        <v>308</v>
+      </c>
+      <c r="D43" s="84">
+        <v>10</v>
+      </c>
+      <c r="E43" s="72" t="s">
+        <v>139</v>
+      </c>
+      <c r="F43" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="G43" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="H43" s="34">
+        <v>9</v>
+      </c>
+      <c r="I43" s="1"/>
+      <c r="J43" s="1"/>
+      <c r="K43" s="1"/>
+      <c r="L43" s="1"/>
+      <c r="M43" s="1"/>
+      <c r="N43" s="1"/>
+      <c r="O43" s="1"/>
+      <c r="P43" s="1"/>
+    </row>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
+        <v>218</v>
+      </c>
+      <c r="C44" t="s">
+        <v>309</v>
+      </c>
+      <c r="D44" s="85"/>
+      <c r="E44" s="73"/>
+      <c r="F44" s="6"/>
+      <c r="G44" s="9"/>
+      <c r="H44" s="34"/>
+      <c r="I44" s="1"/>
+      <c r="J44" s="1"/>
+      <c r="K44" s="1"/>
+      <c r="L44" s="1"/>
+      <c r="M44" s="1"/>
+      <c r="N44" s="1"/>
+      <c r="O44" s="1"/>
+      <c r="P44" s="1"/>
+    </row>
+    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C45" t="s">
+        <v>310</v>
+      </c>
+      <c r="D45" s="85"/>
+      <c r="E45" s="73"/>
+      <c r="F45" s="6"/>
+      <c r="G45" s="9"/>
+      <c r="H45" s="34"/>
+      <c r="I45" s="1"/>
+      <c r="J45" s="1"/>
+      <c r="K45" s="1"/>
+      <c r="L45" s="1"/>
+      <c r="M45" s="1"/>
+      <c r="N45" s="1"/>
+      <c r="O45" s="1"/>
+      <c r="P45" s="1"/>
+    </row>
+    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
+        <v>249</v>
+      </c>
+      <c r="C46" t="s">
+        <v>311</v>
+      </c>
+      <c r="D46" s="85"/>
+      <c r="E46" s="73"/>
+      <c r="F46" s="6"/>
+      <c r="G46" s="9"/>
+      <c r="H46" s="34"/>
+      <c r="I46" s="1"/>
+      <c r="J46" s="1"/>
+      <c r="K46" s="1"/>
+      <c r="L46" s="1"/>
+      <c r="M46" s="1"/>
+      <c r="N46" s="1"/>
+      <c r="O46" s="1"/>
+      <c r="P46" s="1"/>
+    </row>
+    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C47" t="s">
+        <v>305</v>
+      </c>
+      <c r="D47" s="86"/>
+      <c r="E47" s="74"/>
+      <c r="F47" s="6"/>
+      <c r="G47" s="9"/>
+      <c r="H47" s="34"/>
+      <c r="I47" s="1"/>
+      <c r="J47" s="1"/>
+      <c r="K47" s="1"/>
+      <c r="L47" s="1"/>
+      <c r="M47" s="1"/>
+      <c r="N47" s="1"/>
+      <c r="O47" s="1"/>
+      <c r="P47" s="1"/>
+    </row>
+    <row r="48" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>141</v>
+      </c>
+      <c r="B48" t="s">
+        <v>312</v>
+      </c>
+      <c r="D48" s="84">
+        <v>11</v>
+      </c>
+      <c r="E48" s="84" t="s">
+        <v>141</v>
+      </c>
+      <c r="F48" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="G48" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="H48" s="31">
+        <v>10</v>
+      </c>
+      <c r="I48" s="1"/>
+      <c r="J48" s="1"/>
+      <c r="K48" s="1"/>
+      <c r="L48" s="1"/>
+      <c r="M48" s="1"/>
+      <c r="N48" s="1"/>
+      <c r="O48" s="1"/>
+      <c r="P48" s="1"/>
+    </row>
+    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B49" t="s">
+        <v>218</v>
+      </c>
+      <c r="C49" t="s">
+        <v>313</v>
+      </c>
+      <c r="D49" s="85"/>
+      <c r="E49" s="85"/>
+      <c r="F49" s="4"/>
+      <c r="G49" s="9"/>
+      <c r="H49" s="31"/>
+      <c r="I49" s="1"/>
+      <c r="J49" s="1"/>
+      <c r="K49" s="1"/>
+      <c r="L49" s="1"/>
+      <c r="M49" s="1"/>
+      <c r="N49" s="1"/>
+      <c r="O49" s="1"/>
+      <c r="P49" s="1"/>
+    </row>
+    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C50" t="s">
+        <v>314</v>
+      </c>
+      <c r="D50" s="85"/>
+      <c r="E50" s="85"/>
+      <c r="F50" s="4"/>
+      <c r="G50" s="9"/>
+      <c r="H50" s="31"/>
+      <c r="I50" s="1"/>
+      <c r="J50" s="1"/>
+      <c r="K50" s="1"/>
+      <c r="L50" s="1"/>
+      <c r="M50" s="1"/>
+      <c r="N50" s="1"/>
+      <c r="O50" s="1"/>
+      <c r="P50" s="1"/>
+    </row>
+    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B51" t="s">
+        <v>249</v>
+      </c>
+      <c r="C51" t="s">
+        <v>315</v>
+      </c>
+      <c r="D51" s="86"/>
+      <c r="E51" s="86"/>
+      <c r="F51" s="4"/>
+      <c r="G51" s="9"/>
+      <c r="H51" s="31"/>
+      <c r="I51" s="1"/>
+      <c r="J51" s="1"/>
+      <c r="K51" s="1"/>
+      <c r="L51" s="1"/>
+      <c r="M51" s="1"/>
+      <c r="N51" s="1"/>
+      <c r="O51" s="1"/>
+      <c r="P51" s="1"/>
+    </row>
+    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>143</v>
+      </c>
+      <c r="B52" t="s">
+        <v>316</v>
+      </c>
+      <c r="D52" s="84">
+        <v>12</v>
+      </c>
+      <c r="E52" s="84" t="s">
+        <v>143</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="G52" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="H52" s="31">
+        <v>12</v>
+      </c>
+      <c r="I52" s="1"/>
+      <c r="J52" s="1"/>
+      <c r="K52" s="1"/>
+      <c r="L52" s="1"/>
+      <c r="M52" s="1"/>
+      <c r="N52" s="1"/>
+      <c r="O52" s="1"/>
+      <c r="P52" s="1"/>
+    </row>
+    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B53" t="s">
+        <v>218</v>
+      </c>
+      <c r="C53" t="s">
+        <v>317</v>
+      </c>
+      <c r="D53" s="85"/>
+      <c r="E53" s="85"/>
+      <c r="F53" s="1"/>
+      <c r="G53" s="9"/>
+      <c r="H53" s="31"/>
+      <c r="I53" s="1"/>
+      <c r="J53" s="1"/>
+      <c r="K53" s="1"/>
+      <c r="L53" s="1"/>
+      <c r="M53" s="1"/>
+      <c r="N53" s="1"/>
+      <c r="O53" s="1"/>
+      <c r="P53" s="1"/>
+    </row>
+    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C54" t="s">
+        <v>318</v>
+      </c>
+      <c r="D54" s="85"/>
+      <c r="E54" s="85"/>
+      <c r="F54" s="1"/>
+      <c r="G54" s="9"/>
+      <c r="H54" s="31"/>
+      <c r="I54" s="1"/>
+      <c r="J54" s="1"/>
+      <c r="K54" s="1"/>
+      <c r="L54" s="1"/>
+      <c r="M54" s="1"/>
+      <c r="N54" s="1"/>
+      <c r="O54" s="1"/>
+      <c r="P54" s="1"/>
+    </row>
+    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B55" t="s">
+        <v>249</v>
+      </c>
+      <c r="C55" t="s">
+        <v>319</v>
+      </c>
+      <c r="D55" s="85"/>
+      <c r="E55" s="85"/>
+      <c r="F55" s="1"/>
+      <c r="G55" s="9"/>
+      <c r="H55" s="31"/>
+      <c r="I55" s="1"/>
+      <c r="J55" s="1"/>
+      <c r="K55" s="1"/>
+      <c r="L55" s="1"/>
+      <c r="M55" s="1"/>
+      <c r="N55" s="1"/>
+      <c r="O55" s="1"/>
+      <c r="P55" s="1"/>
+    </row>
+    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C56" t="s">
+        <v>320</v>
+      </c>
+      <c r="D56" s="86"/>
+      <c r="E56" s="86"/>
+      <c r="F56" s="1"/>
+      <c r="G56" s="9"/>
+      <c r="H56" s="31"/>
+      <c r="I56" s="1"/>
+      <c r="J56" s="1"/>
+      <c r="K56" s="1"/>
+      <c r="L56" s="1"/>
+      <c r="M56" s="1"/>
+      <c r="N56" s="1"/>
+      <c r="O56" s="1"/>
+      <c r="P56" s="1"/>
+    </row>
+    <row r="57" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+      <c r="A57" s="14" t="s">
+        <v>145</v>
+      </c>
+      <c r="B57" t="s">
+        <v>321</v>
+      </c>
+      <c r="D57" s="84">
+        <v>13</v>
+      </c>
+      <c r="E57" s="72" t="s">
+        <v>145</v>
+      </c>
+      <c r="F57" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="G57" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="H57" s="31">
+        <v>14</v>
+      </c>
+      <c r="I57" s="1"/>
+      <c r="J57" s="1"/>
+      <c r="K57" s="1"/>
+      <c r="L57" s="1"/>
+      <c r="M57" s="1"/>
+      <c r="N57" s="1"/>
+      <c r="O57" s="1"/>
+      <c r="P57" s="1"/>
+    </row>
+    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B58" t="s">
+        <v>218</v>
+      </c>
+      <c r="D58" s="85"/>
+      <c r="E58" s="73"/>
+      <c r="F58" s="5"/>
+      <c r="G58" s="9"/>
+      <c r="H58" s="31"/>
+      <c r="I58" s="1"/>
+      <c r="J58" s="1"/>
+      <c r="K58" s="1"/>
+      <c r="L58" s="1"/>
+      <c r="M58" s="1"/>
+      <c r="N58" s="1"/>
+      <c r="O58" s="1"/>
+      <c r="P58" s="1"/>
+    </row>
+    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B59" t="s">
+        <v>249</v>
+      </c>
+      <c r="D59" s="86"/>
+      <c r="E59" s="74"/>
+      <c r="F59" s="5"/>
+      <c r="G59" s="9"/>
+      <c r="H59" s="31"/>
+      <c r="I59" s="1"/>
+      <c r="J59" s="1"/>
+      <c r="K59" s="1"/>
+      <c r="L59" s="1"/>
+      <c r="M59" s="1"/>
+      <c r="N59" s="1"/>
+      <c r="O59" s="1"/>
+      <c r="P59" s="1"/>
+    </row>
+    <row r="60" spans="1:16" ht="135" x14ac:dyDescent="0.25">
+      <c r="A60" s="15" t="s">
+        <v>147</v>
+      </c>
+      <c r="B60" t="s">
+        <v>322</v>
+      </c>
+      <c r="D60" s="84">
+        <v>14</v>
+      </c>
+      <c r="E60" s="72" t="s">
+        <v>147</v>
+      </c>
+      <c r="F60" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="G60" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="H60" s="31">
+        <v>15</v>
+      </c>
+      <c r="I60" s="1"/>
+      <c r="J60" s="1"/>
+      <c r="K60" s="1"/>
+      <c r="L60" s="1"/>
+      <c r="M60" s="1"/>
+      <c r="N60" s="1"/>
+      <c r="O60" s="1"/>
+      <c r="P60" s="1"/>
+    </row>
+    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B61" t="s">
+        <v>218</v>
+      </c>
+      <c r="C61" t="s">
+        <v>323</v>
+      </c>
+      <c r="D61" s="85"/>
+      <c r="E61" s="73"/>
+      <c r="F61" s="6"/>
+      <c r="G61" s="9"/>
+      <c r="H61" s="31"/>
+      <c r="I61" s="1"/>
+      <c r="J61" s="1"/>
+      <c r="K61" s="1"/>
+      <c r="L61" s="1"/>
+      <c r="M61" s="1"/>
+      <c r="N61" s="1"/>
+      <c r="O61" s="1"/>
+      <c r="P61" s="1"/>
+    </row>
+    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C62" t="s">
+        <v>324</v>
+      </c>
+      <c r="D62" s="85"/>
+      <c r="E62" s="73"/>
+      <c r="F62" s="6"/>
+      <c r="G62" s="9"/>
+      <c r="H62" s="31"/>
+      <c r="I62" s="1"/>
+      <c r="J62" s="1"/>
+      <c r="K62" s="1"/>
+      <c r="L62" s="1"/>
+      <c r="M62" s="1"/>
+      <c r="N62" s="1"/>
+      <c r="O62" s="1"/>
+      <c r="P62" s="1"/>
+    </row>
+    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B63" t="s">
+        <v>249</v>
+      </c>
+      <c r="C63" t="s">
+        <v>325</v>
+      </c>
+      <c r="D63" s="86"/>
+      <c r="E63" s="74"/>
+      <c r="F63" s="6"/>
+      <c r="G63" s="9"/>
+      <c r="H63" s="31"/>
+      <c r="I63" s="1"/>
+      <c r="J63" s="1"/>
+      <c r="K63" s="1"/>
+      <c r="L63" s="1"/>
+      <c r="M63" s="1"/>
+      <c r="N63" s="1"/>
+      <c r="O63" s="1"/>
+      <c r="P63" s="1"/>
+    </row>
+    <row r="64" spans="1:16" ht="75" x14ac:dyDescent="0.25">
+      <c r="A64" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="B64" t="s">
+        <v>326</v>
+      </c>
+      <c r="D64" s="84">
+        <v>15</v>
+      </c>
+      <c r="E64" s="72" t="s">
+        <v>150</v>
+      </c>
+      <c r="F64" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="G64" s="9" t="s">
+        <v>165</v>
+      </c>
+      <c r="H64" s="31">
+        <v>16</v>
+      </c>
+      <c r="I64" s="1"/>
+      <c r="J64" s="1"/>
+      <c r="K64" s="1"/>
+      <c r="L64" s="1"/>
+      <c r="M64" s="1"/>
+      <c r="N64" s="1"/>
+      <c r="O64" s="1"/>
+      <c r="P64" s="1"/>
+    </row>
+    <row r="65" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B65" t="s">
+        <v>218</v>
+      </c>
+      <c r="C65" t="s">
+        <v>327</v>
+      </c>
+      <c r="D65" s="85"/>
+      <c r="E65" s="73"/>
+      <c r="F65" s="5"/>
+      <c r="G65" s="9"/>
+      <c r="H65" s="31"/>
+      <c r="I65" s="1"/>
+      <c r="J65" s="1"/>
+      <c r="K65" s="1"/>
+      <c r="L65" s="1"/>
+      <c r="M65" s="1"/>
+      <c r="N65" s="1"/>
+      <c r="O65" s="1"/>
+      <c r="P65" s="1"/>
+    </row>
+    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C66" t="s">
+        <v>328</v>
+      </c>
+      <c r="D66" s="85"/>
+      <c r="E66" s="73"/>
+      <c r="F66" s="5"/>
+      <c r="G66" s="9"/>
+      <c r="H66" s="31"/>
+      <c r="I66" s="1"/>
+      <c r="J66" s="1"/>
+      <c r="K66" s="1"/>
+      <c r="L66" s="1"/>
+      <c r="M66" s="1"/>
+      <c r="N66" s="1"/>
+      <c r="O66" s="1"/>
+      <c r="P66" s="1"/>
+    </row>
+    <row r="67" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B67" t="s">
+        <v>249</v>
+      </c>
+      <c r="C67" t="s">
+        <v>329</v>
+      </c>
+      <c r="D67" s="85"/>
+      <c r="E67" s="74"/>
+      <c r="F67" s="5"/>
+      <c r="G67" s="9"/>
+      <c r="H67" s="31"/>
+      <c r="I67" s="1"/>
+      <c r="J67" s="1"/>
+      <c r="K67" s="1"/>
+      <c r="L67" s="1"/>
+      <c r="M67" s="1"/>
+      <c r="N67" s="1"/>
+      <c r="O67" s="1"/>
+      <c r="P67" s="1"/>
+    </row>
+    <row r="68" spans="1:16" ht="150" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>151</v>
+      </c>
+      <c r="B68" t="s">
+        <v>330</v>
+      </c>
+      <c r="D68" s="32">
+        <v>16</v>
+      </c>
+      <c r="E68" s="72" t="s">
+        <v>151</v>
+      </c>
+      <c r="F68" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="G68" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="H68" s="31">
+        <v>16</v>
+      </c>
+      <c r="I68" s="1"/>
+      <c r="J68" s="1"/>
+      <c r="K68" s="1"/>
+      <c r="L68" s="1"/>
+      <c r="M68" s="1"/>
+      <c r="N68" s="1"/>
+      <c r="O68" s="1"/>
+      <c r="P68" s="1"/>
+    </row>
+    <row r="69" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B69" t="s">
+        <v>218</v>
+      </c>
+      <c r="C69" t="s">
+        <v>331</v>
+      </c>
+      <c r="D69" s="32"/>
+      <c r="E69" s="73"/>
+      <c r="F69" s="6"/>
+      <c r="G69" s="9"/>
+      <c r="H69" s="31"/>
+      <c r="I69" s="1"/>
+      <c r="J69" s="1"/>
+      <c r="K69" s="1"/>
+      <c r="L69" s="1"/>
+      <c r="M69" s="1"/>
+      <c r="N69" s="1"/>
+      <c r="O69" s="1"/>
+      <c r="P69" s="1"/>
+    </row>
+    <row r="70" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B70" t="s">
+        <v>249</v>
+      </c>
+      <c r="C70" t="s">
+        <v>332</v>
+      </c>
+      <c r="D70" s="32"/>
+      <c r="E70" s="73"/>
+      <c r="F70" s="6"/>
+      <c r="G70" s="9"/>
+      <c r="H70" s="31"/>
+      <c r="I70" s="1"/>
+      <c r="J70" s="1"/>
+      <c r="K70" s="1"/>
+      <c r="L70" s="1"/>
+      <c r="M70" s="1"/>
+      <c r="N70" s="1"/>
+      <c r="O70" s="1"/>
+      <c r="P70" s="1"/>
+    </row>
+    <row r="71" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C71" t="s">
+        <v>333</v>
+      </c>
+      <c r="D71" s="32"/>
+      <c r="E71" s="74"/>
+      <c r="F71" s="6"/>
+      <c r="G71" s="9"/>
+      <c r="H71" s="31"/>
+      <c r="I71" s="1"/>
+      <c r="J71" s="1"/>
+      <c r="K71" s="1"/>
+      <c r="L71" s="1"/>
+      <c r="M71" s="1"/>
+      <c r="N71" s="1"/>
+      <c r="O71" s="1"/>
+      <c r="P71" s="1"/>
+    </row>
+    <row r="72" spans="1:16" ht="195" x14ac:dyDescent="0.25">
+      <c r="A72" s="14" t="s">
+        <v>153</v>
+      </c>
+      <c r="B72" t="s">
+        <v>334</v>
+      </c>
+      <c r="D72" s="72">
+        <v>17</v>
+      </c>
+      <c r="E72" s="72" t="s">
+        <v>153</v>
+      </c>
+      <c r="F72" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="G72" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="H72" s="31">
+        <v>16</v>
+      </c>
+      <c r="I72" s="1"/>
+      <c r="J72" s="1"/>
+      <c r="K72" s="1"/>
+      <c r="L72" s="1"/>
+      <c r="M72" s="1"/>
+      <c r="N72" s="1"/>
+      <c r="O72" s="1"/>
+      <c r="P72" s="1"/>
+    </row>
+    <row r="73" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B73" t="s">
+        <v>218</v>
+      </c>
+      <c r="C73" t="s">
+        <v>335</v>
+      </c>
+      <c r="D73" s="73"/>
+      <c r="E73" s="73"/>
+      <c r="F73" s="5"/>
+      <c r="G73" s="9"/>
+      <c r="H73" s="31"/>
+      <c r="I73" s="1"/>
+      <c r="J73" s="1"/>
+      <c r="K73" s="1"/>
+      <c r="L73" s="1"/>
+      <c r="M73" s="1"/>
+      <c r="N73" s="1"/>
+      <c r="O73" s="1"/>
+      <c r="P73" s="1"/>
+    </row>
+    <row r="74" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B74" t="s">
+        <v>249</v>
+      </c>
+      <c r="C74" t="s">
+        <v>337</v>
+      </c>
+      <c r="D74" s="74"/>
+      <c r="E74" s="74"/>
+      <c r="F74" s="5"/>
+      <c r="G74" s="9"/>
+      <c r="H74" s="31"/>
+      <c r="I74" s="1"/>
+      <c r="J74" s="1"/>
+      <c r="K74" s="1"/>
+      <c r="L74" s="1"/>
+      <c r="M74" s="1"/>
+      <c r="N74" s="1"/>
+      <c r="O74" s="1"/>
+      <c r="P74" s="1"/>
+    </row>
+    <row r="75" spans="1:16" ht="60" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>169</v>
+      </c>
+      <c r="B75" t="s">
+        <v>336</v>
+      </c>
+      <c r="D75" s="31">
+        <v>18</v>
+      </c>
+      <c r="E75" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="F75" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="G75" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="H75" s="31">
+        <v>8</v>
+      </c>
+      <c r="I75" s="1"/>
+      <c r="J75" s="1"/>
+      <c r="K75" s="1"/>
+      <c r="L75" s="1"/>
+      <c r="M75" s="1"/>
+      <c r="N75" s="1"/>
+      <c r="O75" s="1"/>
+      <c r="P75" s="1"/>
+    </row>
+    <row r="76" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B76" t="s">
+        <v>218</v>
+      </c>
+      <c r="C76" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="77" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B77" t="s">
+        <v>249</v>
+      </c>
+      <c r="C77" t="s">
+        <v>339</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="33">
+    <mergeCell ref="D60:D63"/>
+    <mergeCell ref="E60:E63"/>
+    <mergeCell ref="E72:E74"/>
+    <mergeCell ref="D72:D74"/>
+    <mergeCell ref="D64:D67"/>
+    <mergeCell ref="E64:E67"/>
+    <mergeCell ref="E68:E71"/>
+    <mergeCell ref="D57:D59"/>
+    <mergeCell ref="E57:E59"/>
+    <mergeCell ref="D52:D56"/>
+    <mergeCell ref="E52:E56"/>
+    <mergeCell ref="D48:D51"/>
+    <mergeCell ref="E48:E51"/>
+    <mergeCell ref="D43:D47"/>
+    <mergeCell ref="E43:E47"/>
+    <mergeCell ref="D40:D42"/>
+    <mergeCell ref="E40:E42"/>
+    <mergeCell ref="D34:D39"/>
+    <mergeCell ref="E34:E39"/>
+    <mergeCell ref="D30:D33"/>
+    <mergeCell ref="E30:E33"/>
+    <mergeCell ref="D26:D29"/>
+    <mergeCell ref="E26:E29"/>
+    <mergeCell ref="D18:D25"/>
+    <mergeCell ref="E18:E25"/>
+    <mergeCell ref="D2:D5"/>
+    <mergeCell ref="E2:E5"/>
+    <mergeCell ref="D14:D17"/>
+    <mergeCell ref="E14:E17"/>
+    <mergeCell ref="D10:D13"/>
+    <mergeCell ref="E10:E13"/>
+    <mergeCell ref="D6:D9"/>
+    <mergeCell ref="E6:E9"/>
+  </mergeCells>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{BD266EE8-9EE9-410E-A73B-7BCBE7209954}"/>
-    <hyperlink ref="D4" r:id="rId2" xr:uid="{61BCAF91-187D-4E55-9A08-AC7DFBC537EF}"/>
-    <hyperlink ref="D5" r:id="rId3" xr:uid="{265D7779-3692-4D46-8D2F-36DDAC43DD3A}"/>
-    <hyperlink ref="D6" r:id="rId4" location="java-module-system" xr:uid="{7CF071A5-697F-456A-857B-6B68A89A54E2}"/>
-    <hyperlink ref="D7" r:id="rId5" xr:uid="{5E418898-2A4E-495A-A104-C7A030278692}"/>
-    <hyperlink ref="D9" r:id="rId6" xr:uid="{CB359587-5F3C-4D3B-B2F0-2FB99D3A9967}"/>
-    <hyperlink ref="D10" r:id="rId7" xr:uid="{BDB8C26B-4ABE-45A2-B5D1-4544AD7FA68B}"/>
-    <hyperlink ref="D11" r:id="rId8" location="private-interface-methods" xr:uid="{03D7CE78-B00A-40EC-B5F3-2AA3BD25A3F8}"/>
-    <hyperlink ref="D12" r:id="rId9" location="local-variable-type-inference" xr:uid="{ABC6A97A-A492-4F1E-B376-6B08FCF1FF79}"/>
-    <hyperlink ref="D13" r:id="rId10" xr:uid="{C5C0004D-306F-4C4E-8BB7-B950CCF159EA}"/>
-    <hyperlink ref="D14" r:id="rId11" location="switch-expressions" xr:uid="{9C27DA53-F783-4DE8-BF63-0D5BC42DFF78}"/>
-    <hyperlink ref="D15" r:id="rId12" location="using-text-blocks" xr:uid="{AF940015-A731-45B2-AF55-D061E7728FA6}"/>
-    <hyperlink ref="D16" r:id="rId13" xr:uid="{B62A518E-DC89-418B-A066-017A0CDEEBDB}"/>
-    <hyperlink ref="D17" r:id="rId14" xr:uid="{1673A8AC-A268-453A-A526-36C81C723CFF}"/>
-    <hyperlink ref="D18" r:id="rId15" xr:uid="{24EB30BC-5EF8-4524-9F31-9D4139905188}"/>
-    <hyperlink ref="D19" r:id="rId16" location="repeating-annotations" xr:uid="{056F707C-428B-48F4-87B1-E2564C8A4EC9}"/>
+    <hyperlink ref="G2" r:id="rId1" xr:uid="{BD266EE8-9EE9-410E-A73B-7BCBE7209954}"/>
+    <hyperlink ref="G10" r:id="rId2" xr:uid="{61BCAF91-187D-4E55-9A08-AC7DFBC537EF}"/>
+    <hyperlink ref="G14" r:id="rId3" xr:uid="{265D7779-3692-4D46-8D2F-36DDAC43DD3A}"/>
+    <hyperlink ref="G18" r:id="rId4" location="java-module-system" xr:uid="{7CF071A5-697F-456A-857B-6B68A89A54E2}"/>
+    <hyperlink ref="G26" r:id="rId5" xr:uid="{5E418898-2A4E-495A-A104-C7A030278692}"/>
+    <hyperlink ref="G34" r:id="rId6" xr:uid="{CB359587-5F3C-4D3B-B2F0-2FB99D3A9967}"/>
+    <hyperlink ref="G40" r:id="rId7" xr:uid="{BDB8C26B-4ABE-45A2-B5D1-4544AD7FA68B}"/>
+    <hyperlink ref="G43" r:id="rId8" location="private-interface-methods" xr:uid="{03D7CE78-B00A-40EC-B5F3-2AA3BD25A3F8}"/>
+    <hyperlink ref="G48" r:id="rId9" location="local-variable-type-inference" xr:uid="{ABC6A97A-A492-4F1E-B376-6B08FCF1FF79}"/>
+    <hyperlink ref="G52" r:id="rId10" xr:uid="{C5C0004D-306F-4C4E-8BB7-B950CCF159EA}"/>
+    <hyperlink ref="G57" r:id="rId11" location="switch-expressions" xr:uid="{9C27DA53-F783-4DE8-BF63-0D5BC42DFF78}"/>
+    <hyperlink ref="G60" r:id="rId12" location="using-text-blocks" xr:uid="{AF940015-A731-45B2-AF55-D061E7728FA6}"/>
+    <hyperlink ref="G64" r:id="rId13" xr:uid="{B62A518E-DC89-418B-A066-017A0CDEEBDB}"/>
+    <hyperlink ref="G68" r:id="rId14" xr:uid="{1673A8AC-A268-453A-A526-36C81C723CFF}"/>
+    <hyperlink ref="G72" r:id="rId15" xr:uid="{24EB30BC-5EF8-4524-9F31-9D4139905188}"/>
+    <hyperlink ref="G75" r:id="rId16" location="repeating-annotations" xr:uid="{056F707C-428B-48F4-87B1-E2564C8A4EC9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId17"/>
@@ -6556,7 +7971,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83D713CF-1264-4070-BA73-824C7A1D0A05}">
   <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A8" workbookViewId="0">
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
@@ -6606,10 +8021,10 @@
       <c r="I2" s="14"/>
     </row>
     <row r="3" spans="1:9" ht="297" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="58">
+      <c r="A3" s="72">
         <v>2</v>
       </c>
-      <c r="B3" s="58" t="s">
+      <c r="B3" s="72" t="s">
         <v>192</v>
       </c>
       <c r="C3" s="41" t="s">
@@ -6625,8 +8040,8 @@
       <c r="I3" s="14"/>
     </row>
     <row r="4" spans="1:9" ht="333.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="60"/>
-      <c r="B4" s="59"/>
+      <c r="A4" s="73"/>
+      <c r="B4" s="74"/>
       <c r="C4" s="3"/>
       <c r="D4" s="37" t="s">
         <v>208</v>
@@ -6638,14 +8053,14 @@
       <c r="I4" s="14"/>
     </row>
     <row r="5" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="60"/>
+      <c r="A5" s="73"/>
       <c r="B5" s="3" t="s">
         <v>194</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>197</v>
       </c>
-      <c r="D5" s="61" t="s">
+      <c r="D5" s="87" t="s">
         <v>210</v>
       </c>
       <c r="E5" s="14"/>
@@ -6655,14 +8070,14 @@
       <c r="I5" s="14"/>
     </row>
     <row r="6" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A6" s="60"/>
+      <c r="A6" s="73"/>
       <c r="B6" s="3" t="s">
         <v>195</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>199</v>
       </c>
-      <c r="D6" s="62"/>
+      <c r="D6" s="88"/>
       <c r="E6" s="14"/>
       <c r="F6" s="14"/>
       <c r="G6" s="14"/>
@@ -6670,14 +8085,14 @@
       <c r="I6" s="14"/>
     </row>
     <row r="7" spans="1:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="A7" s="60"/>
+      <c r="A7" s="73"/>
       <c r="B7" s="3" t="s">
         <v>196</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>198</v>
       </c>
-      <c r="D7" s="62"/>
+      <c r="D7" s="88"/>
       <c r="E7" s="14"/>
       <c r="F7" s="14"/>
       <c r="G7" s="14"/>
@@ -6685,7 +8100,7 @@
       <c r="I7" s="14"/>
     </row>
     <row r="8" spans="1:9" ht="90" x14ac:dyDescent="0.25">
-      <c r="A8" s="59"/>
+      <c r="A8" s="74"/>
       <c r="B8" s="3" t="s">
         <v>200</v>
       </c>
@@ -6740,16 +8155,16 @@
       <c r="I10" s="14"/>
     </row>
     <row r="11" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="63">
+      <c r="A11" s="59">
         <v>5</v>
       </c>
-      <c r="B11" s="63" t="s">
+      <c r="B11" s="59" t="s">
         <v>211</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>212</v>
       </c>
-      <c r="D11" s="64" t="s">
+      <c r="D11" s="63" t="s">
         <v>207</v>
       </c>
       <c r="E11" s="14"/>
@@ -6759,12 +8174,12 @@
       <c r="I11" s="14"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="63"/>
-      <c r="B12" s="63"/>
+      <c r="A12" s="59"/>
+      <c r="B12" s="59"/>
       <c r="C12" s="3" t="s">
         <v>213</v>
       </c>
-      <c r="D12" s="65"/>
+      <c r="D12" s="64"/>
       <c r="E12" s="14"/>
       <c r="F12" s="14"/>
       <c r="G12" s="14"/>
@@ -6772,12 +8187,12 @@
       <c r="I12" s="14"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="63"/>
-      <c r="B13" s="63"/>
+      <c r="A13" s="59"/>
+      <c r="B13" s="59"/>
       <c r="C13" s="3" t="s">
         <v>214</v>
       </c>
-      <c r="D13" s="66"/>
+      <c r="D13" s="65"/>
       <c r="E13" s="14"/>
       <c r="F13" s="14"/>
       <c r="G13" s="14"/>

</xml_diff>

<commit_message>
cập nhật tóm tắt file excel
</commit_message>
<xml_diff>
--- a/Task_Result.xlsx
+++ b/Task_Result.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\beetech\java\stage1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8A99C37-DD67-4AE7-A85C-D0F6B18F9F3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54FC373F-E970-4092-A2BF-7911E735AFA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="428">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="427">
   <si>
     <t>STT</t>
   </si>
@@ -3278,189 +3278,6 @@
   </si>
   <si>
     <t>nhưng sẽ ném exception nếu không có transaction nào tồn tại</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve"> là một thuộc tính quan trọng của Transaction để xác định cách thức các Transaction nội tuyến và các Transaction liên quan tương tác với nhau.
-Có thể có nhiều Transaction trong một ứng dụng Spring. Khi một phương thức được gọi trong một Transaction đã tồn tại, các phương thức này có thể sử dụng cùng một Transaction đã tồn tại hoặc tạo một Transaction mới.
-Propagation có thể E45được đặt trực tiếp trên annotation @</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Transactional</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Các giá trị Propagation có thể được đặt trong @Transactional như sau:
-REQUIRED</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">: Nếu một Transaction đang tồn tại, các phương thức được gọi sẽ tham gia vào Transaction đó. Nếu không có Transaction nào tồn tại, một Transaction mới sẽ được tạo ra.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>SUPPORTS</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">:  là sử dụng lại transaction hiện đang hoạt động. Nếu không thì method được gọi sẽ thực thi mà không được đặt trong một transactional context nào
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>MANDATORY</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">: Chỉ có thể được sử dụng trong một Transaction đang tồn tại. Nếu không có Transaction nào tồn tại, một ngoại lệ sẽ được ném ra.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>REQUIRES_NEW</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">: Luôn tạo ra một Transaction mới, bất kể Transaction nào đang tồn tại. Nếu có Transaction đang tồn tại, nó sẽ tạm thời được tạm dừng cho đến khi Transaction mới hoàn tất. Và cả 2 Transaction này độc lập với nhau
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>NOT_SUPPORTED</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">: Transaction sẽ không được tạo ra cho phương thức được gọi. Nếu Transaction nào đang tồn tại, nó sẽ tạm thời bị treo.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>NEVER</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">: Transaction không được tạo ra. Nếu một Transaction đang tồn tại, một ngoại lệ sẽ được ném ra.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>NESTED</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>: Method được gọi sẽ tạo một transaction mới nếu không có transaction nào đang hoạt động. Nếu method được gọi với một transaction đang hoạt động Spring sẽ tạo một savepoint và rollback tại đây nếu có Exception xảy ra</t>
-    </r>
   </si>
   <si>
     <t>SUPPORTS</t>
@@ -3828,6 +3645,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3841,6 +3659,27 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -3882,27 +3721,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3940,6 +3758,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
@@ -3948,14 +3775,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -3966,13 +3790,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -4040,13 +3857,13 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>952499</xdr:colOff>
+      <xdr:colOff>952498</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>103908</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>2043183</xdr:colOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>1102177</xdr:colOff>
       <xdr:row>63</xdr:row>
       <xdr:rowOff>86105</xdr:rowOff>
     </xdr:to>
@@ -4071,8 +3888,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11880272" y="6199908"/>
-          <a:ext cx="3532548" cy="8935697"/>
+          <a:off x="12015105" y="6199908"/>
+          <a:ext cx="4789715" cy="8935697"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5064,8 +4881,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="P1:V16"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="U18" sqref="U18"/>
+    <sheetView topLeftCell="F6" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="Q7" sqref="Q7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5081,27 +4898,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="16:22" x14ac:dyDescent="0.25">
-      <c r="P1" s="49" t="s">
+      <c r="P1" s="50" t="s">
         <v>17</v>
       </c>
-      <c r="Q1" s="50"/>
-      <c r="R1" s="50"/>
-      <c r="S1" s="50"/>
-      <c r="T1" s="50"/>
+      <c r="Q1" s="51"/>
+      <c r="R1" s="51"/>
+      <c r="S1" s="51"/>
+      <c r="T1" s="51"/>
     </row>
     <row r="2" spans="16:22" x14ac:dyDescent="0.25">
-      <c r="P2" s="50"/>
-      <c r="Q2" s="50"/>
-      <c r="R2" s="50"/>
-      <c r="S2" s="50"/>
-      <c r="T2" s="50"/>
+      <c r="P2" s="51"/>
+      <c r="Q2" s="51"/>
+      <c r="R2" s="51"/>
+      <c r="S2" s="51"/>
+      <c r="T2" s="51"/>
     </row>
     <row r="3" spans="16:22" x14ac:dyDescent="0.25">
-      <c r="P3" s="51"/>
-      <c r="Q3" s="51"/>
-      <c r="R3" s="51"/>
-      <c r="S3" s="51"/>
-      <c r="T3" s="51"/>
+      <c r="P3" s="52"/>
+      <c r="Q3" s="52"/>
+      <c r="R3" s="52"/>
+      <c r="S3" s="52"/>
+      <c r="T3" s="52"/>
     </row>
     <row r="4" spans="16:22" x14ac:dyDescent="0.25">
       <c r="P4" s="7" t="s">
@@ -5110,11 +4927,11 @@
       <c r="Q4" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="R4" s="48" t="s">
+      <c r="R4" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="S4" s="48"/>
-      <c r="T4" s="48"/>
+      <c r="S4" s="49"/>
+      <c r="T4" s="49"/>
       <c r="U4" s="7" t="s">
         <v>18</v>
       </c>
@@ -5268,24 +5085,24 @@
       </c>
     </row>
     <row r="14" spans="16:22" x14ac:dyDescent="0.25">
-      <c r="P14" s="52" t="s">
+      <c r="P14" s="53" t="s">
         <v>73</v>
       </c>
-      <c r="Q14" s="50"/>
-      <c r="R14" s="50"/>
-      <c r="S14" s="50"/>
+      <c r="Q14" s="51"/>
+      <c r="R14" s="51"/>
+      <c r="S14" s="51"/>
     </row>
     <row r="15" spans="16:22" x14ac:dyDescent="0.25">
-      <c r="P15" s="50"/>
-      <c r="Q15" s="50"/>
-      <c r="R15" s="50"/>
-      <c r="S15" s="50"/>
+      <c r="P15" s="51"/>
+      <c r="Q15" s="51"/>
+      <c r="R15" s="51"/>
+      <c r="S15" s="51"/>
     </row>
     <row r="16" spans="16:22" x14ac:dyDescent="0.25">
-      <c r="P16" s="50"/>
-      <c r="Q16" s="50"/>
-      <c r="R16" s="50"/>
-      <c r="S16" s="50"/>
+      <c r="P16" s="51"/>
+      <c r="Q16" s="51"/>
+      <c r="R16" s="51"/>
+      <c r="S16" s="51"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -5311,8 +5128,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25977106-C04A-4BDF-83D6-AA6BE76B6728}">
   <dimension ref="A1:AD89"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="O3" sqref="O3"/>
+    <sheetView topLeftCell="M11" zoomScale="154" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="Q5" sqref="Q5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5330,24 +5147,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:30" ht="49.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="66" t="s">
+      <c r="A1" s="54" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="67"/>
-      <c r="C1" s="67"/>
-      <c r="D1" s="67"/>
-      <c r="E1" s="67"/>
-      <c r="F1" s="67"/>
-      <c r="G1" s="67"/>
-      <c r="H1" s="67"/>
-      <c r="I1" s="67"/>
-      <c r="J1" s="67"/>
-      <c r="K1" s="67"/>
-      <c r="L1" s="67"/>
-      <c r="M1" s="67"/>
-      <c r="N1" s="67"/>
-      <c r="O1" s="67"/>
-      <c r="P1" s="67"/>
+      <c r="B1" s="55"/>
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="55"/>
+      <c r="G1" s="55"/>
+      <c r="H1" s="55"/>
+      <c r="I1" s="55"/>
+      <c r="J1" s="55"/>
+      <c r="K1" s="55"/>
+      <c r="L1" s="55"/>
+      <c r="M1" s="55"/>
+      <c r="N1" s="55"/>
+      <c r="O1" s="55"/>
+      <c r="P1" s="55"/>
       <c r="Q1" s="39"/>
       <c r="R1" s="39"/>
       <c r="S1" s="39"/>
@@ -5439,16 +5256,16 @@
       <c r="P4" t="s">
         <v>214</v>
       </c>
-      <c r="AA4" s="57">
+      <c r="AA4" s="65">
         <v>3</v>
       </c>
-      <c r="AB4" s="57" t="s">
+      <c r="AB4" s="65" t="s">
         <v>35</v>
       </c>
-      <c r="AC4" s="60" t="s">
+      <c r="AC4" s="68" t="s">
         <v>38</v>
       </c>
-      <c r="AD4" s="63" t="s">
+      <c r="AD4" s="71" t="s">
         <v>32</v>
       </c>
     </row>
@@ -5460,10 +5277,10 @@
       <c r="P5" t="s">
         <v>215</v>
       </c>
-      <c r="AA5" s="58"/>
-      <c r="AB5" s="58"/>
-      <c r="AC5" s="61"/>
-      <c r="AD5" s="64"/>
+      <c r="AA5" s="66"/>
+      <c r="AB5" s="66"/>
+      <c r="AC5" s="69"/>
+      <c r="AD5" s="72"/>
     </row>
     <row r="6" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="14"/>
@@ -5476,10 +5293,10 @@
       <c r="P6" t="s">
         <v>217</v>
       </c>
-      <c r="AA6" s="59"/>
-      <c r="AB6" s="59"/>
-      <c r="AC6" s="62"/>
-      <c r="AD6" s="65"/>
+      <c r="AA6" s="67"/>
+      <c r="AB6" s="67"/>
+      <c r="AC6" s="70"/>
+      <c r="AD6" s="73"/>
     </row>
     <row r="7" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="14"/>
@@ -5492,16 +5309,16 @@
       <c r="P7" t="s">
         <v>218</v>
       </c>
-      <c r="AA7" s="57">
+      <c r="AA7" s="65">
         <v>4</v>
       </c>
-      <c r="AB7" s="57" t="s">
+      <c r="AB7" s="65" t="s">
         <v>36</v>
       </c>
-      <c r="AC7" s="60" t="s">
+      <c r="AC7" s="68" t="s">
         <v>39</v>
       </c>
-      <c r="AD7" s="63" t="s">
+      <c r="AD7" s="71" t="s">
         <v>40</v>
       </c>
     </row>
@@ -5513,10 +5330,10 @@
       <c r="P8" t="s">
         <v>219</v>
       </c>
-      <c r="AA8" s="58"/>
-      <c r="AB8" s="58"/>
-      <c r="AC8" s="61"/>
-      <c r="AD8" s="64"/>
+      <c r="AA8" s="66"/>
+      <c r="AB8" s="66"/>
+      <c r="AC8" s="69"/>
+      <c r="AD8" s="72"/>
     </row>
     <row r="9" spans="1:30" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="14"/>
@@ -5529,19 +5346,19 @@
       <c r="P9" t="s">
         <v>220</v>
       </c>
-      <c r="AA9" s="59"/>
-      <c r="AB9" s="59"/>
-      <c r="AC9" s="62"/>
-      <c r="AD9" s="65"/>
+      <c r="AA9" s="67"/>
+      <c r="AB9" s="67"/>
+      <c r="AC9" s="70"/>
+      <c r="AD9" s="73"/>
     </row>
     <row r="10" spans="1:30" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="68" t="s">
+      <c r="A10" s="56" t="s">
         <v>54</v>
       </c>
-      <c r="B10" s="69"/>
-      <c r="C10" s="69"/>
-      <c r="D10" s="69"/>
-      <c r="E10" s="69"/>
+      <c r="B10" s="57"/>
+      <c r="C10" s="57"/>
+      <c r="D10" s="57"/>
+      <c r="E10" s="57"/>
       <c r="F10" s="19"/>
       <c r="G10" s="19"/>
       <c r="H10" s="19"/>
@@ -5552,16 +5369,16 @@
       <c r="P10" t="s">
         <v>222</v>
       </c>
-      <c r="AA10" s="53">
+      <c r="AA10" s="61">
         <v>5</v>
       </c>
-      <c r="AB10" s="54" t="s">
+      <c r="AB10" s="62" t="s">
         <v>37</v>
       </c>
-      <c r="AC10" s="55" t="s">
+      <c r="AC10" s="63" t="s">
         <v>51</v>
       </c>
-      <c r="AD10" s="56" t="s">
+      <c r="AD10" s="64" t="s">
         <v>52</v>
       </c>
     </row>
@@ -5572,19 +5389,19 @@
       <c r="P11" t="s">
         <v>223</v>
       </c>
-      <c r="AA11" s="53"/>
-      <c r="AB11" s="54"/>
-      <c r="AC11" s="55"/>
-      <c r="AD11" s="56"/>
+      <c r="AA11" s="61"/>
+      <c r="AB11" s="62"/>
+      <c r="AC11" s="63"/>
+      <c r="AD11" s="64"/>
     </row>
     <row r="12" spans="1:30" x14ac:dyDescent="0.25">
       <c r="P12" t="s">
         <v>224</v>
       </c>
-      <c r="AA12" s="53"/>
-      <c r="AB12" s="54"/>
-      <c r="AC12" s="55"/>
-      <c r="AD12" s="56"/>
+      <c r="AA12" s="61"/>
+      <c r="AB12" s="62"/>
+      <c r="AC12" s="63"/>
+      <c r="AD12" s="64"/>
     </row>
     <row r="13" spans="1:30" x14ac:dyDescent="0.25">
       <c r="O13" t="s">
@@ -5593,10 +5410,10 @@
       <c r="P13" t="s">
         <v>225</v>
       </c>
-      <c r="AA13" s="53"/>
-      <c r="AB13" s="54"/>
-      <c r="AC13" s="55"/>
-      <c r="AD13" s="56"/>
+      <c r="AA13" s="61"/>
+      <c r="AB13" s="62"/>
+      <c r="AC13" s="63"/>
+      <c r="AD13" s="64"/>
     </row>
     <row r="14" spans="1:30" x14ac:dyDescent="0.25">
       <c r="N14" s="43" t="s">
@@ -5605,10 +5422,10 @@
       <c r="P14" t="s">
         <v>228</v>
       </c>
-      <c r="AA14" s="53"/>
-      <c r="AB14" s="54"/>
-      <c r="AC14" s="55"/>
-      <c r="AD14" s="56"/>
+      <c r="AA14" s="61"/>
+      <c r="AB14" s="62"/>
+      <c r="AC14" s="63"/>
+      <c r="AD14" s="64"/>
     </row>
     <row r="15" spans="1:30" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="40"/>
@@ -5626,10 +5443,10 @@
       <c r="P15" t="s">
         <v>227</v>
       </c>
-      <c r="AA15" s="53"/>
-      <c r="AB15" s="54"/>
-      <c r="AC15" s="55"/>
-      <c r="AD15" s="56"/>
+      <c r="AA15" s="61"/>
+      <c r="AB15" s="62"/>
+      <c r="AC15" s="63"/>
+      <c r="AD15" s="64"/>
     </row>
     <row r="16" spans="1:30" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="40"/>
@@ -5644,10 +5461,10 @@
       <c r="P16" t="s">
         <v>223</v>
       </c>
-      <c r="AA16" s="53"/>
-      <c r="AB16" s="54"/>
-      <c r="AC16" s="55"/>
-      <c r="AD16" s="56"/>
+      <c r="AA16" s="61"/>
+      <c r="AB16" s="62"/>
+      <c r="AC16" s="63"/>
+      <c r="AD16" s="64"/>
     </row>
     <row r="17" spans="1:30" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="40"/>
@@ -5662,10 +5479,10 @@
       <c r="P17" t="s">
         <v>224</v>
       </c>
-      <c r="AA17" s="53"/>
-      <c r="AB17" s="54"/>
-      <c r="AC17" s="55"/>
-      <c r="AD17" s="56"/>
+      <c r="AA17" s="61"/>
+      <c r="AB17" s="62"/>
+      <c r="AC17" s="63"/>
+      <c r="AD17" s="64"/>
     </row>
     <row r="18" spans="1:30" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="40"/>
@@ -5683,10 +5500,10 @@
       <c r="P18" t="s">
         <v>225</v>
       </c>
-      <c r="AA18" s="53"/>
-      <c r="AB18" s="54"/>
-      <c r="AC18" s="55"/>
-      <c r="AD18" s="56"/>
+      <c r="AA18" s="61"/>
+      <c r="AB18" s="62"/>
+      <c r="AC18" s="63"/>
+      <c r="AD18" s="64"/>
     </row>
     <row r="19" spans="1:30" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="40"/>
@@ -5704,10 +5521,10 @@
       <c r="P19" t="s">
         <v>230</v>
       </c>
-      <c r="AA19" s="53"/>
-      <c r="AB19" s="54"/>
-      <c r="AC19" s="55"/>
-      <c r="AD19" s="56"/>
+      <c r="AA19" s="61"/>
+      <c r="AB19" s="62"/>
+      <c r="AC19" s="63"/>
+      <c r="AD19" s="64"/>
     </row>
     <row r="20" spans="1:30" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="40"/>
@@ -5725,10 +5542,10 @@
       <c r="O20" t="s">
         <v>232</v>
       </c>
-      <c r="AA20" s="53"/>
-      <c r="AB20" s="54"/>
-      <c r="AC20" s="55"/>
-      <c r="AD20" s="56"/>
+      <c r="AA20" s="61"/>
+      <c r="AB20" s="62"/>
+      <c r="AC20" s="63"/>
+      <c r="AD20" s="64"/>
     </row>
     <row r="21" spans="1:30" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="40"/>
@@ -5746,10 +5563,10 @@
       <c r="P21" t="s">
         <v>233</v>
       </c>
-      <c r="AA21" s="53"/>
-      <c r="AB21" s="54"/>
-      <c r="AC21" s="55"/>
-      <c r="AD21" s="56"/>
+      <c r="AA21" s="61"/>
+      <c r="AB21" s="62"/>
+      <c r="AC21" s="63"/>
+      <c r="AD21" s="64"/>
     </row>
     <row r="22" spans="1:30" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="40"/>
@@ -5767,10 +5584,10 @@
       <c r="P22" t="s">
         <v>234</v>
       </c>
-      <c r="AA22" s="53"/>
-      <c r="AB22" s="54"/>
-      <c r="AC22" s="55"/>
-      <c r="AD22" s="56"/>
+      <c r="AA22" s="61"/>
+      <c r="AB22" s="62"/>
+      <c r="AC22" s="63"/>
+      <c r="AD22" s="64"/>
     </row>
     <row r="23" spans="1:30" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="40"/>
@@ -5788,10 +5605,10 @@
       <c r="O23" t="s">
         <v>236</v>
       </c>
-      <c r="AA23" s="53"/>
-      <c r="AB23" s="54"/>
-      <c r="AC23" s="55"/>
-      <c r="AD23" s="56"/>
+      <c r="AA23" s="61"/>
+      <c r="AB23" s="62"/>
+      <c r="AC23" s="63"/>
+      <c r="AD23" s="64"/>
     </row>
     <row r="24" spans="1:30" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="40"/>
@@ -5809,10 +5626,10 @@
       <c r="P24" t="s">
         <v>237</v>
       </c>
-      <c r="AA24" s="53"/>
-      <c r="AB24" s="54"/>
-      <c r="AC24" s="55"/>
-      <c r="AD24" s="56"/>
+      <c r="AA24" s="61"/>
+      <c r="AB24" s="62"/>
+      <c r="AC24" s="63"/>
+      <c r="AD24" s="64"/>
     </row>
     <row r="25" spans="1:30" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="40"/>
@@ -5830,25 +5647,25 @@
       <c r="P25" t="s">
         <v>238</v>
       </c>
-      <c r="AA25" s="53"/>
-      <c r="AB25" s="54"/>
-      <c r="AC25" s="55"/>
-      <c r="AD25" s="56"/>
+      <c r="AA25" s="61"/>
+      <c r="AB25" s="62"/>
+      <c r="AC25" s="63"/>
+      <c r="AD25" s="64"/>
     </row>
     <row r="26" spans="1:30" ht="108" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="52" t="s">
+      <c r="A26" s="53" t="s">
         <v>42</v>
       </c>
-      <c r="B26" s="52"/>
-      <c r="C26" s="52"/>
-      <c r="D26" s="52" t="s">
+      <c r="B26" s="53"/>
+      <c r="C26" s="53"/>
+      <c r="D26" s="53" t="s">
         <v>43</v>
       </c>
-      <c r="E26" s="52"/>
-      <c r="F26" s="52"/>
-      <c r="G26" s="52"/>
-      <c r="H26" s="52"/>
-      <c r="I26" s="52"/>
+      <c r="E26" s="53"/>
+      <c r="F26" s="53"/>
+      <c r="G26" s="53"/>
+      <c r="H26" s="53"/>
+      <c r="I26" s="53"/>
       <c r="J26" s="42"/>
       <c r="K26" s="42"/>
       <c r="L26" s="42"/>
@@ -5878,15 +5695,15 @@
       <c r="AD26" s="1"/>
     </row>
     <row r="27" spans="1:30" ht="139.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="52"/>
-      <c r="B27" s="52"/>
-      <c r="C27" s="52"/>
-      <c r="D27" s="52"/>
-      <c r="E27" s="52"/>
-      <c r="F27" s="52"/>
-      <c r="G27" s="52"/>
-      <c r="H27" s="52"/>
-      <c r="I27" s="52"/>
+      <c r="A27" s="53"/>
+      <c r="B27" s="53"/>
+      <c r="C27" s="53"/>
+      <c r="D27" s="53"/>
+      <c r="E27" s="53"/>
+      <c r="F27" s="53"/>
+      <c r="G27" s="53"/>
+      <c r="H27" s="53"/>
+      <c r="I27" s="53"/>
       <c r="J27" s="42"/>
       <c r="K27" s="42"/>
       <c r="L27" s="42"/>
@@ -5916,78 +5733,70 @@
       <c r="AD27" s="1"/>
     </row>
     <row r="54" spans="1:10" ht="42" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="D54" s="72" t="s">
+      <c r="D54" s="60" t="s">
         <v>44</v>
       </c>
-      <c r="E54" s="72"/>
-      <c r="F54" s="72"/>
-      <c r="G54" s="72"/>
-      <c r="H54" s="72"/>
-      <c r="I54" s="72"/>
-      <c r="J54" s="72"/>
+      <c r="E54" s="60"/>
+      <c r="F54" s="60"/>
+      <c r="G54" s="60"/>
+      <c r="H54" s="60"/>
+      <c r="I54" s="60"/>
+      <c r="J54" s="60"/>
     </row>
     <row r="58" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A58" s="71" t="s">
+      <c r="A58" s="59" t="s">
         <v>41</v>
       </c>
-      <c r="B58" s="71"/>
-      <c r="C58" s="71"/>
+      <c r="B58" s="59"/>
+      <c r="C58" s="59"/>
       <c r="D58" s="20"/>
     </row>
     <row r="59" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="71"/>
-      <c r="B59" s="71"/>
-      <c r="C59" s="71"/>
+      <c r="A59" s="59"/>
+      <c r="B59" s="59"/>
+      <c r="C59" s="59"/>
     </row>
     <row r="60" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="71"/>
-      <c r="B60" s="71"/>
-      <c r="C60" s="71"/>
+      <c r="A60" s="59"/>
+      <c r="B60" s="59"/>
+      <c r="C60" s="59"/>
     </row>
     <row r="61" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="71"/>
-      <c r="B61" s="71"/>
-      <c r="C61" s="71"/>
+      <c r="A61" s="59"/>
+      <c r="B61" s="59"/>
+      <c r="C61" s="59"/>
     </row>
     <row r="62" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="52" t="s">
+      <c r="A62" s="53" t="s">
         <v>45</v>
       </c>
-      <c r="B62" s="52"/>
-      <c r="C62" s="52"/>
+      <c r="B62" s="53"/>
+      <c r="C62" s="53"/>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A63" s="52"/>
-      <c r="B63" s="52"/>
-      <c r="C63" s="52"/>
+      <c r="A63" s="53"/>
+      <c r="B63" s="53"/>
+      <c r="C63" s="53"/>
     </row>
     <row r="87" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="70" t="s">
+      <c r="A87" s="58" t="s">
         <v>46</v>
       </c>
-      <c r="B87" s="70"/>
-      <c r="C87" s="70"/>
+      <c r="B87" s="58"/>
+      <c r="C87" s="58"/>
     </row>
     <row r="88" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="70"/>
-      <c r="B88" s="70"/>
-      <c r="C88" s="70"/>
+      <c r="A88" s="58"/>
+      <c r="B88" s="58"/>
+      <c r="C88" s="58"/>
     </row>
     <row r="89" spans="1:3" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="70"/>
-      <c r="B89" s="70"/>
-      <c r="C89" s="70"/>
+      <c r="A89" s="58"/>
+      <c r="B89" s="58"/>
+      <c r="C89" s="58"/>
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="A1:P1"/>
-    <mergeCell ref="A10:E10"/>
-    <mergeCell ref="A87:C89"/>
-    <mergeCell ref="A58:C61"/>
-    <mergeCell ref="A26:C27"/>
-    <mergeCell ref="A62:C63"/>
-    <mergeCell ref="D26:I27"/>
-    <mergeCell ref="D54:J54"/>
     <mergeCell ref="AA10:AA25"/>
     <mergeCell ref="AB10:AB25"/>
     <mergeCell ref="AC10:AC25"/>
@@ -6000,6 +5809,14 @@
     <mergeCell ref="AB7:AB9"/>
     <mergeCell ref="AC7:AC9"/>
     <mergeCell ref="AD7:AD9"/>
+    <mergeCell ref="A1:P1"/>
+    <mergeCell ref="A10:E10"/>
+    <mergeCell ref="A87:C89"/>
+    <mergeCell ref="A58:C61"/>
+    <mergeCell ref="A26:C27"/>
+    <mergeCell ref="A62:C63"/>
+    <mergeCell ref="D26:I27"/>
+    <mergeCell ref="D54:J54"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="AD2" r:id="rId1" display="https://stackoverflow.com/questions/15070513/how-to-test-a-non-thread-safe-class" xr:uid="{AF80577A-A125-48C9-AA50-5BBE662AA378}"/>
@@ -6061,32 +5878,32 @@
       <c r="B2" t="s">
         <v>242</v>
       </c>
-      <c r="G2" s="73">
+      <c r="G2" s="74">
         <v>1</v>
       </c>
-      <c r="H2" s="73" t="s">
+      <c r="H2" s="74" t="s">
         <v>56</v>
       </c>
-      <c r="I2" s="60" t="s">
+      <c r="I2" s="68" t="s">
         <v>57</v>
       </c>
-      <c r="J2" s="78" t="s">
+      <c r="J2" s="79" t="s">
         <v>58</v>
       </c>
-      <c r="L2" s="52" t="s">
+      <c r="L2" s="53" t="s">
         <v>68</v>
       </c>
-      <c r="M2" s="50"/>
-      <c r="N2" s="50"/>
-      <c r="O2" s="50"/>
-      <c r="P2" s="50"/>
-      <c r="Q2" s="50"/>
-      <c r="R2" s="50"/>
-      <c r="S2" s="50"/>
-      <c r="T2" s="50"/>
-      <c r="U2" s="50"/>
-      <c r="V2" s="50"/>
-      <c r="W2" s="50"/>
+      <c r="M2" s="51"/>
+      <c r="N2" s="51"/>
+      <c r="O2" s="51"/>
+      <c r="P2" s="51"/>
+      <c r="Q2" s="51"/>
+      <c r="R2" s="51"/>
+      <c r="S2" s="51"/>
+      <c r="T2" s="51"/>
+      <c r="U2" s="51"/>
+      <c r="V2" s="51"/>
+      <c r="W2" s="51"/>
     </row>
     <row r="3" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B3" t="s">
@@ -6095,10 +5912,10 @@
       <c r="C3" t="s">
         <v>243</v>
       </c>
-      <c r="G3" s="74"/>
-      <c r="H3" s="74"/>
-      <c r="I3" s="61"/>
-      <c r="J3" s="79"/>
+      <c r="G3" s="75"/>
+      <c r="H3" s="75"/>
+      <c r="I3" s="69"/>
+      <c r="J3" s="80"/>
       <c r="L3" s="38"/>
       <c r="M3" s="23"/>
       <c r="N3" s="23"/>
@@ -6119,10 +5936,10 @@
       <c r="C4" t="s">
         <v>245</v>
       </c>
-      <c r="G4" s="74"/>
-      <c r="H4" s="74"/>
-      <c r="I4" s="61"/>
-      <c r="J4" s="79"/>
+      <c r="G4" s="75"/>
+      <c r="H4" s="75"/>
+      <c r="I4" s="69"/>
+      <c r="J4" s="80"/>
       <c r="L4" s="38"/>
       <c r="M4" s="23"/>
       <c r="N4" s="23"/>
@@ -6140,10 +5957,10 @@
       <c r="C5" t="s">
         <v>246</v>
       </c>
-      <c r="G5" s="75"/>
-      <c r="H5" s="75"/>
-      <c r="I5" s="62"/>
-      <c r="J5" s="80"/>
+      <c r="G5" s="76"/>
+      <c r="H5" s="76"/>
+      <c r="I5" s="70"/>
+      <c r="J5" s="81"/>
       <c r="L5" s="38"/>
       <c r="M5" s="23"/>
       <c r="N5" s="23"/>
@@ -6164,16 +5981,16 @@
       <c r="B6" t="s">
         <v>248</v>
       </c>
-      <c r="G6" s="73">
+      <c r="G6" s="74">
         <v>2</v>
       </c>
-      <c r="H6" s="73" t="s">
+      <c r="H6" s="74" t="s">
         <v>59</v>
       </c>
-      <c r="I6" s="60" t="s">
+      <c r="I6" s="68" t="s">
         <v>60</v>
       </c>
-      <c r="J6" s="81" t="s">
+      <c r="J6" s="82" t="s">
         <v>72</v>
       </c>
       <c r="M6" s="26"/>
@@ -6185,20 +6002,20 @@
       <c r="C7" t="s">
         <v>249</v>
       </c>
-      <c r="G7" s="74"/>
-      <c r="H7" s="74"/>
-      <c r="I7" s="61"/>
-      <c r="J7" s="82"/>
+      <c r="G7" s="75"/>
+      <c r="H7" s="75"/>
+      <c r="I7" s="69"/>
+      <c r="J7" s="83"/>
       <c r="M7" s="26"/>
     </row>
     <row r="8" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
         <v>250</v>
       </c>
-      <c r="G8" s="74"/>
-      <c r="H8" s="74"/>
-      <c r="I8" s="61"/>
-      <c r="J8" s="82"/>
+      <c r="G8" s="75"/>
+      <c r="H8" s="75"/>
+      <c r="I8" s="69"/>
+      <c r="J8" s="83"/>
       <c r="M8" s="26"/>
     </row>
     <row r="9" spans="1:23" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -6208,10 +6025,10 @@
       <c r="C9" t="s">
         <v>251</v>
       </c>
-      <c r="G9" s="75"/>
-      <c r="H9" s="75"/>
-      <c r="I9" s="62"/>
-      <c r="J9" s="83"/>
+      <c r="G9" s="76"/>
+      <c r="H9" s="76"/>
+      <c r="I9" s="70"/>
+      <c r="J9" s="84"/>
       <c r="M9" s="26"/>
     </row>
     <row r="10" spans="1:23" ht="90" customHeight="1" x14ac:dyDescent="0.25">
@@ -6221,16 +6038,16 @@
       <c r="B10" t="s">
         <v>253</v>
       </c>
-      <c r="G10" s="73">
+      <c r="G10" s="74">
         <v>3</v>
       </c>
-      <c r="H10" s="73" t="s">
+      <c r="H10" s="74" t="s">
         <v>61</v>
       </c>
-      <c r="I10" s="60" t="s">
+      <c r="I10" s="68" t="s">
         <v>62</v>
       </c>
-      <c r="J10" s="81" t="s">
+      <c r="J10" s="82" t="s">
         <v>63</v>
       </c>
     </row>
@@ -6241,10 +6058,10 @@
       <c r="C11" t="s">
         <v>254</v>
       </c>
-      <c r="G11" s="74"/>
-      <c r="H11" s="74"/>
-      <c r="I11" s="61"/>
-      <c r="J11" s="82"/>
+      <c r="G11" s="75"/>
+      <c r="H11" s="75"/>
+      <c r="I11" s="69"/>
+      <c r="J11" s="83"/>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
@@ -6253,10 +6070,10 @@
       <c r="C12" t="s">
         <v>255</v>
       </c>
-      <c r="G12" s="74"/>
-      <c r="H12" s="74"/>
-      <c r="I12" s="61"/>
-      <c r="J12" s="82"/>
+      <c r="G12" s="75"/>
+      <c r="H12" s="75"/>
+      <c r="I12" s="69"/>
+      <c r="J12" s="83"/>
     </row>
     <row r="13" spans="1:23" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="43" t="s">
@@ -6265,31 +6082,31 @@
       <c r="B13" t="s">
         <v>257</v>
       </c>
-      <c r="G13" s="73">
+      <c r="G13" s="74">
         <v>4</v>
       </c>
-      <c r="H13" s="73" t="s">
+      <c r="H13" s="74" t="s">
         <v>66</v>
       </c>
-      <c r="I13" s="60" t="s">
+      <c r="I13" s="68" t="s">
         <v>65</v>
       </c>
-      <c r="J13" s="73"/>
-      <c r="K13" s="76" t="s">
+      <c r="J13" s="74"/>
+      <c r="K13" s="77" t="s">
         <v>69</v>
       </c>
-      <c r="L13" s="50"/>
-      <c r="M13" s="50"/>
-      <c r="N13" s="50"/>
-      <c r="O13" s="50"/>
-      <c r="P13" s="50"/>
-      <c r="Q13" s="50"/>
-      <c r="R13" s="50"/>
-      <c r="S13" s="50"/>
-      <c r="T13" s="50"/>
-      <c r="U13" s="50"/>
-      <c r="V13" s="50"/>
-      <c r="W13" s="50"/>
+      <c r="L13" s="51"/>
+      <c r="M13" s="51"/>
+      <c r="N13" s="51"/>
+      <c r="O13" s="51"/>
+      <c r="P13" s="51"/>
+      <c r="Q13" s="51"/>
+      <c r="R13" s="51"/>
+      <c r="S13" s="51"/>
+      <c r="T13" s="51"/>
+      <c r="U13" s="51"/>
+      <c r="V13" s="51"/>
+      <c r="W13" s="51"/>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
@@ -6298,23 +6115,23 @@
       <c r="C14" t="s">
         <v>258</v>
       </c>
-      <c r="G14" s="74"/>
-      <c r="H14" s="74"/>
-      <c r="I14" s="61"/>
-      <c r="J14" s="74"/>
-      <c r="K14" s="76"/>
-      <c r="L14" s="50"/>
-      <c r="M14" s="50"/>
-      <c r="N14" s="50"/>
-      <c r="O14" s="50"/>
-      <c r="P14" s="50"/>
-      <c r="Q14" s="50"/>
-      <c r="R14" s="50"/>
-      <c r="S14" s="50"/>
-      <c r="T14" s="50"/>
-      <c r="U14" s="50"/>
-      <c r="V14" s="50"/>
-      <c r="W14" s="50"/>
+      <c r="G14" s="75"/>
+      <c r="H14" s="75"/>
+      <c r="I14" s="69"/>
+      <c r="J14" s="75"/>
+      <c r="K14" s="77"/>
+      <c r="L14" s="51"/>
+      <c r="M14" s="51"/>
+      <c r="N14" s="51"/>
+      <c r="O14" s="51"/>
+      <c r="P14" s="51"/>
+      <c r="Q14" s="51"/>
+      <c r="R14" s="51"/>
+      <c r="S14" s="51"/>
+      <c r="T14" s="51"/>
+      <c r="U14" s="51"/>
+      <c r="V14" s="51"/>
+      <c r="W14" s="51"/>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
@@ -6323,23 +6140,23 @@
       <c r="C15" t="s">
         <v>259</v>
       </c>
-      <c r="G15" s="75"/>
-      <c r="H15" s="75"/>
-      <c r="I15" s="62"/>
-      <c r="J15" s="75"/>
-      <c r="K15" s="76"/>
-      <c r="L15" s="50"/>
-      <c r="M15" s="50"/>
-      <c r="N15" s="50"/>
-      <c r="O15" s="50"/>
-      <c r="P15" s="50"/>
-      <c r="Q15" s="50"/>
-      <c r="R15" s="50"/>
-      <c r="S15" s="50"/>
-      <c r="T15" s="50"/>
-      <c r="U15" s="50"/>
-      <c r="V15" s="50"/>
-      <c r="W15" s="50"/>
+      <c r="G15" s="76"/>
+      <c r="H15" s="76"/>
+      <c r="I15" s="70"/>
+      <c r="J15" s="76"/>
+      <c r="K15" s="77"/>
+      <c r="L15" s="51"/>
+      <c r="M15" s="51"/>
+      <c r="N15" s="51"/>
+      <c r="O15" s="51"/>
+      <c r="P15" s="51"/>
+      <c r="Q15" s="51"/>
+      <c r="R15" s="51"/>
+      <c r="S15" s="51"/>
+      <c r="T15" s="51"/>
+      <c r="U15" s="51"/>
+      <c r="V15" s="51"/>
+      <c r="W15" s="51"/>
     </row>
     <row r="16" spans="1:23" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="43" t="s">
@@ -6358,19 +6175,19 @@
         <v>67</v>
       </c>
       <c r="J16" s="3"/>
-      <c r="K16" s="77"/>
-      <c r="L16" s="50"/>
-      <c r="M16" s="50"/>
-      <c r="N16" s="50"/>
-      <c r="O16" s="50"/>
-      <c r="P16" s="50"/>
-      <c r="Q16" s="50"/>
-      <c r="R16" s="50"/>
-      <c r="S16" s="50"/>
-      <c r="T16" s="50"/>
-      <c r="U16" s="50"/>
-      <c r="V16" s="50"/>
-      <c r="W16" s="50"/>
+      <c r="K16" s="78"/>
+      <c r="L16" s="51"/>
+      <c r="M16" s="51"/>
+      <c r="N16" s="51"/>
+      <c r="O16" s="51"/>
+      <c r="P16" s="51"/>
+      <c r="Q16" s="51"/>
+      <c r="R16" s="51"/>
+      <c r="S16" s="51"/>
+      <c r="T16" s="51"/>
+      <c r="U16" s="51"/>
+      <c r="V16" s="51"/>
+      <c r="W16" s="51"/>
     </row>
     <row r="17" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
@@ -6465,88 +6282,83 @@
       <c r="J27" s="14"/>
     </row>
     <row r="33" spans="11:22" x14ac:dyDescent="0.25">
-      <c r="K33" s="52" t="s">
+      <c r="K33" s="53" t="s">
         <v>70</v>
       </c>
-      <c r="L33" s="50"/>
-      <c r="M33" s="50"/>
-      <c r="N33" s="50"/>
-      <c r="O33" s="50"/>
-      <c r="P33" s="50"/>
-      <c r="Q33" s="50"/>
-      <c r="R33" s="50"/>
-      <c r="S33" s="50"/>
-      <c r="T33" s="50"/>
-      <c r="U33" s="50"/>
-      <c r="V33" s="50"/>
+      <c r="L33" s="51"/>
+      <c r="M33" s="51"/>
+      <c r="N33" s="51"/>
+      <c r="O33" s="51"/>
+      <c r="P33" s="51"/>
+      <c r="Q33" s="51"/>
+      <c r="R33" s="51"/>
+      <c r="S33" s="51"/>
+      <c r="T33" s="51"/>
+      <c r="U33" s="51"/>
+      <c r="V33" s="51"/>
     </row>
     <row r="34" spans="11:22" x14ac:dyDescent="0.25">
-      <c r="K34" s="50"/>
-      <c r="L34" s="50"/>
-      <c r="M34" s="50"/>
-      <c r="N34" s="50"/>
-      <c r="O34" s="50"/>
-      <c r="P34" s="50"/>
-      <c r="Q34" s="50"/>
-      <c r="R34" s="50"/>
-      <c r="S34" s="50"/>
-      <c r="T34" s="50"/>
-      <c r="U34" s="50"/>
-      <c r="V34" s="50"/>
+      <c r="K34" s="51"/>
+      <c r="L34" s="51"/>
+      <c r="M34" s="51"/>
+      <c r="N34" s="51"/>
+      <c r="O34" s="51"/>
+      <c r="P34" s="51"/>
+      <c r="Q34" s="51"/>
+      <c r="R34" s="51"/>
+      <c r="S34" s="51"/>
+      <c r="T34" s="51"/>
+      <c r="U34" s="51"/>
+      <c r="V34" s="51"/>
     </row>
     <row r="35" spans="11:22" x14ac:dyDescent="0.25">
-      <c r="K35" s="50"/>
-      <c r="L35" s="50"/>
-      <c r="M35" s="50"/>
-      <c r="N35" s="50"/>
-      <c r="O35" s="50"/>
-      <c r="P35" s="50"/>
-      <c r="Q35" s="50"/>
-      <c r="R35" s="50"/>
-      <c r="S35" s="50"/>
-      <c r="T35" s="50"/>
-      <c r="U35" s="50"/>
-      <c r="V35" s="50"/>
+      <c r="K35" s="51"/>
+      <c r="L35" s="51"/>
+      <c r="M35" s="51"/>
+      <c r="N35" s="51"/>
+      <c r="O35" s="51"/>
+      <c r="P35" s="51"/>
+      <c r="Q35" s="51"/>
+      <c r="R35" s="51"/>
+      <c r="S35" s="51"/>
+      <c r="T35" s="51"/>
+      <c r="U35" s="51"/>
+      <c r="V35" s="51"/>
     </row>
     <row r="51" spans="11:22" x14ac:dyDescent="0.25">
-      <c r="K51" s="72" t="s">
+      <c r="K51" s="60" t="s">
         <v>71</v>
       </c>
-      <c r="L51" s="50"/>
-      <c r="M51" s="50"/>
-      <c r="N51" s="50"/>
-      <c r="O51" s="50"/>
-      <c r="P51" s="50"/>
-      <c r="Q51" s="50"/>
-      <c r="R51" s="50"/>
-      <c r="S51" s="50"/>
-      <c r="T51" s="50"/>
-      <c r="U51" s="50"/>
-      <c r="V51" s="50"/>
+      <c r="L51" s="51"/>
+      <c r="M51" s="51"/>
+      <c r="N51" s="51"/>
+      <c r="O51" s="51"/>
+      <c r="P51" s="51"/>
+      <c r="Q51" s="51"/>
+      <c r="R51" s="51"/>
+      <c r="S51" s="51"/>
+      <c r="T51" s="51"/>
+      <c r="U51" s="51"/>
+      <c r="V51" s="51"/>
     </row>
     <row r="52" spans="11:22" x14ac:dyDescent="0.25">
-      <c r="K52" s="50"/>
-      <c r="L52" s="50"/>
-      <c r="M52" s="50"/>
-      <c r="N52" s="50"/>
-      <c r="O52" s="50"/>
-      <c r="P52" s="50"/>
-      <c r="Q52" s="50"/>
-      <c r="R52" s="50"/>
-      <c r="S52" s="50"/>
-      <c r="T52" s="50"/>
-      <c r="U52" s="50"/>
-      <c r="V52" s="50"/>
+      <c r="K52" s="51"/>
+      <c r="L52" s="51"/>
+      <c r="M52" s="51"/>
+      <c r="N52" s="51"/>
+      <c r="O52" s="51"/>
+      <c r="P52" s="51"/>
+      <c r="Q52" s="51"/>
+      <c r="R52" s="51"/>
+      <c r="S52" s="51"/>
+      <c r="T52" s="51"/>
+      <c r="U52" s="51"/>
+      <c r="V52" s="51"/>
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="G10:G12"/>
-    <mergeCell ref="H10:H12"/>
-    <mergeCell ref="I10:I12"/>
-    <mergeCell ref="J10:J12"/>
-    <mergeCell ref="G13:G15"/>
-    <mergeCell ref="H13:H15"/>
-    <mergeCell ref="I13:I15"/>
+    <mergeCell ref="K33:V35"/>
+    <mergeCell ref="K51:V52"/>
     <mergeCell ref="G2:G5"/>
     <mergeCell ref="H2:H5"/>
     <mergeCell ref="I2:I5"/>
@@ -6555,11 +6367,16 @@
     <mergeCell ref="H6:H9"/>
     <mergeCell ref="I6:I9"/>
     <mergeCell ref="J6:J9"/>
+    <mergeCell ref="G10:G12"/>
+    <mergeCell ref="H10:H12"/>
+    <mergeCell ref="I10:I12"/>
+    <mergeCell ref="J10:J12"/>
+    <mergeCell ref="G13:G15"/>
+    <mergeCell ref="H13:H15"/>
+    <mergeCell ref="I13:I15"/>
     <mergeCell ref="J13:J15"/>
     <mergeCell ref="L2:W2"/>
     <mergeCell ref="K13:W16"/>
-    <mergeCell ref="K33:V35"/>
-    <mergeCell ref="K51:V52"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="J2" r:id="rId1" xr:uid="{3D14D563-A18C-4362-B2CD-8D8339C1C427}"/>
@@ -6630,14 +6447,14 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="84" t="s">
+      <c r="A7" s="85" t="s">
         <v>79</v>
       </c>
-      <c r="B7" s="50"/>
+      <c r="B7" s="51"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="50"/>
-      <c r="B8" s="50"/>
+      <c r="A8" s="51"/>
+      <c r="B8" s="51"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
@@ -6884,10 +6701,10 @@
       <c r="B2" t="s">
         <v>264</v>
       </c>
-      <c r="D2" s="73">
+      <c r="D2" s="74">
         <v>1</v>
       </c>
-      <c r="E2" s="73" t="s">
+      <c r="E2" s="74" t="s">
         <v>119</v>
       </c>
       <c r="F2" s="6" t="s">
@@ -6915,8 +6732,8 @@
       <c r="C3" t="s">
         <v>265</v>
       </c>
-      <c r="D3" s="74"/>
-      <c r="E3" s="74"/>
+      <c r="D3" s="75"/>
+      <c r="E3" s="75"/>
       <c r="F3" s="6"/>
       <c r="G3" s="11"/>
       <c r="H3" s="3"/>
@@ -6933,8 +6750,8 @@
       <c r="C4" t="s">
         <v>266</v>
       </c>
-      <c r="D4" s="74"/>
-      <c r="E4" s="74"/>
+      <c r="D4" s="75"/>
+      <c r="E4" s="75"/>
       <c r="F4" s="6"/>
       <c r="G4" s="11"/>
       <c r="H4" s="3"/>
@@ -6954,8 +6771,8 @@
       <c r="C5" t="s">
         <v>267</v>
       </c>
-      <c r="D5" s="75"/>
-      <c r="E5" s="75"/>
+      <c r="D5" s="76"/>
+      <c r="E5" s="76"/>
       <c r="F5" s="6"/>
       <c r="G5" s="11"/>
       <c r="H5" s="3"/>
@@ -6975,10 +6792,10 @@
       <c r="B6" t="s">
         <v>269</v>
       </c>
-      <c r="D6" s="73">
+      <c r="D6" s="74">
         <v>2</v>
       </c>
-      <c r="E6" s="73" t="s">
+      <c r="E6" s="74" t="s">
         <v>122</v>
       </c>
       <c r="F6" s="5" t="s">
@@ -7006,8 +6823,8 @@
       <c r="C7" t="s">
         <v>270</v>
       </c>
-      <c r="D7" s="74"/>
-      <c r="E7" s="74"/>
+      <c r="D7" s="75"/>
+      <c r="E7" s="75"/>
       <c r="F7" s="5"/>
       <c r="G7" s="4"/>
       <c r="H7" s="3"/>
@@ -7024,8 +6841,8 @@
       <c r="C8" t="s">
         <v>271</v>
       </c>
-      <c r="D8" s="74"/>
-      <c r="E8" s="74"/>
+      <c r="D8" s="75"/>
+      <c r="E8" s="75"/>
       <c r="F8" s="5"/>
       <c r="G8" s="4"/>
       <c r="H8" s="3"/>
@@ -7045,8 +6862,8 @@
       <c r="C9" t="s">
         <v>272</v>
       </c>
-      <c r="D9" s="75"/>
-      <c r="E9" s="75"/>
+      <c r="D9" s="76"/>
+      <c r="E9" s="76"/>
       <c r="F9" s="5"/>
       <c r="G9" s="4"/>
       <c r="H9" s="3"/>
@@ -7066,13 +6883,13 @@
       <c r="B10" t="s">
         <v>273</v>
       </c>
-      <c r="D10" s="85">
+      <c r="D10" s="89">
         <v>3</v>
       </c>
-      <c r="E10" s="85" t="s">
+      <c r="E10" s="89" t="s">
         <v>125</v>
       </c>
-      <c r="F10" s="88" t="s">
+      <c r="F10" s="86" t="s">
         <v>127</v>
       </c>
       <c r="G10" s="9" t="s">
@@ -7097,9 +6914,9 @@
       <c r="C11" t="s">
         <v>274</v>
       </c>
-      <c r="D11" s="86"/>
-      <c r="E11" s="86"/>
-      <c r="F11" s="89"/>
+      <c r="D11" s="90"/>
+      <c r="E11" s="90"/>
+      <c r="F11" s="87"/>
       <c r="G11" s="9"/>
       <c r="H11" s="3"/>
       <c r="I11" s="1"/>
@@ -7115,9 +6932,9 @@
       <c r="C12" t="s">
         <v>275</v>
       </c>
-      <c r="D12" s="86"/>
-      <c r="E12" s="86"/>
-      <c r="F12" s="89"/>
+      <c r="D12" s="90"/>
+      <c r="E12" s="90"/>
+      <c r="F12" s="87"/>
       <c r="G12" s="9"/>
       <c r="H12" s="3"/>
       <c r="I12" s="1"/>
@@ -7136,9 +6953,9 @@
       <c r="C13" t="s">
         <v>267</v>
       </c>
-      <c r="D13" s="87"/>
-      <c r="E13" s="87"/>
-      <c r="F13" s="90"/>
+      <c r="D13" s="91"/>
+      <c r="E13" s="91"/>
+      <c r="F13" s="88"/>
       <c r="G13" s="9"/>
       <c r="H13" s="3"/>
       <c r="I13" s="1"/>
@@ -7157,10 +6974,10 @@
       <c r="B14" t="s">
         <v>276</v>
       </c>
-      <c r="D14" s="85">
+      <c r="D14" s="89">
         <v>4</v>
       </c>
-      <c r="E14" s="73" t="s">
+      <c r="E14" s="74" t="s">
         <v>128</v>
       </c>
       <c r="F14" s="6" t="s">
@@ -7188,8 +7005,8 @@
       <c r="C15" t="s">
         <v>277</v>
       </c>
-      <c r="D15" s="86"/>
-      <c r="E15" s="74"/>
+      <c r="D15" s="90"/>
+      <c r="E15" s="75"/>
       <c r="F15" s="6"/>
       <c r="G15" s="9"/>
       <c r="H15" s="31"/>
@@ -7206,8 +7023,8 @@
       <c r="B16" t="s">
         <v>244</v>
       </c>
-      <c r="D16" s="86"/>
-      <c r="E16" s="74"/>
+      <c r="D16" s="90"/>
+      <c r="E16" s="75"/>
       <c r="F16" s="6"/>
       <c r="G16" s="9"/>
       <c r="H16" s="31"/>
@@ -7221,8 +7038,8 @@
       <c r="P16" s="1"/>
     </row>
     <row r="17" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D17" s="87"/>
-      <c r="E17" s="75"/>
+      <c r="D17" s="91"/>
+      <c r="E17" s="76"/>
       <c r="F17" s="6"/>
       <c r="G17" s="9"/>
       <c r="H17" s="31"/>
@@ -7242,10 +7059,10 @@
       <c r="B18" t="s">
         <v>278</v>
       </c>
-      <c r="D18" s="85">
+      <c r="D18" s="89">
         <v>5</v>
       </c>
-      <c r="E18" s="73" t="s">
+      <c r="E18" s="74" t="s">
         <v>130</v>
       </c>
       <c r="F18" s="6" t="s">
@@ -7273,8 +7090,8 @@
       <c r="C19" t="s">
         <v>279</v>
       </c>
-      <c r="D19" s="86"/>
-      <c r="E19" s="74"/>
+      <c r="D19" s="90"/>
+      <c r="E19" s="75"/>
       <c r="F19" s="6"/>
       <c r="G19" s="9"/>
       <c r="H19" s="31"/>
@@ -7291,8 +7108,8 @@
       <c r="C20" t="s">
         <v>280</v>
       </c>
-      <c r="D20" s="86"/>
-      <c r="E20" s="74"/>
+      <c r="D20" s="90"/>
+      <c r="E20" s="75"/>
       <c r="F20" s="6"/>
       <c r="G20" s="9"/>
       <c r="H20" s="31"/>
@@ -7309,8 +7126,8 @@
       <c r="C21" t="s">
         <v>282</v>
       </c>
-      <c r="D21" s="86"/>
-      <c r="E21" s="74"/>
+      <c r="D21" s="90"/>
+      <c r="E21" s="75"/>
       <c r="F21" s="6"/>
       <c r="G21" s="9"/>
       <c r="H21" s="31"/>
@@ -7327,8 +7144,8 @@
       <c r="C22" t="s">
         <v>283</v>
       </c>
-      <c r="D22" s="86"/>
-      <c r="E22" s="74"/>
+      <c r="D22" s="90"/>
+      <c r="E22" s="75"/>
       <c r="F22" s="6"/>
       <c r="G22" s="9"/>
       <c r="H22" s="31"/>
@@ -7345,8 +7162,8 @@
       <c r="C23" t="s">
         <v>281</v>
       </c>
-      <c r="D23" s="86"/>
-      <c r="E23" s="74"/>
+      <c r="D23" s="90"/>
+      <c r="E23" s="75"/>
       <c r="F23" s="6"/>
       <c r="G23" s="9"/>
       <c r="H23" s="31"/>
@@ -7366,8 +7183,8 @@
       <c r="C24" t="s">
         <v>284</v>
       </c>
-      <c r="D24" s="86"/>
-      <c r="E24" s="74"/>
+      <c r="D24" s="90"/>
+      <c r="E24" s="75"/>
       <c r="F24" s="6"/>
       <c r="G24" s="9"/>
       <c r="H24" s="31"/>
@@ -7384,8 +7201,8 @@
       <c r="C25" t="s">
         <v>285</v>
       </c>
-      <c r="D25" s="87"/>
-      <c r="E25" s="75"/>
+      <c r="D25" s="91"/>
+      <c r="E25" s="76"/>
       <c r="F25" s="6"/>
       <c r="G25" s="9"/>
       <c r="H25" s="31"/>
@@ -7405,10 +7222,10 @@
       <c r="B26" t="s">
         <v>286</v>
       </c>
-      <c r="D26" s="85">
+      <c r="D26" s="89">
         <v>6</v>
       </c>
-      <c r="E26" s="73" t="s">
+      <c r="E26" s="74" t="s">
         <v>132</v>
       </c>
       <c r="F26" s="6" t="s">
@@ -7436,8 +7253,8 @@
       <c r="C27" t="s">
         <v>287</v>
       </c>
-      <c r="D27" s="86"/>
-      <c r="E27" s="74"/>
+      <c r="D27" s="90"/>
+      <c r="E27" s="75"/>
       <c r="F27" s="6"/>
       <c r="G27" s="9"/>
       <c r="H27" s="31"/>
@@ -7454,8 +7271,8 @@
       <c r="C28" t="s">
         <v>288</v>
       </c>
-      <c r="D28" s="86"/>
-      <c r="E28" s="74"/>
+      <c r="D28" s="90"/>
+      <c r="E28" s="75"/>
       <c r="F28" s="6"/>
       <c r="G28" s="9"/>
       <c r="H28" s="31"/>
@@ -7475,8 +7292,8 @@
       <c r="C29" t="s">
         <v>289</v>
       </c>
-      <c r="D29" s="87"/>
-      <c r="E29" s="75"/>
+      <c r="D29" s="91"/>
+      <c r="E29" s="76"/>
       <c r="F29" s="6"/>
       <c r="G29" s="9"/>
       <c r="H29" s="31"/>
@@ -7496,10 +7313,10 @@
       <c r="B30" t="s">
         <v>290</v>
       </c>
-      <c r="D30" s="73">
+      <c r="D30" s="74">
         <v>7</v>
       </c>
-      <c r="E30" s="73" t="s">
+      <c r="E30" s="74" t="s">
         <v>134</v>
       </c>
       <c r="F30" s="5" t="s">
@@ -7525,8 +7342,8 @@
       <c r="C31" t="s">
         <v>291</v>
       </c>
-      <c r="D31" s="74"/>
-      <c r="E31" s="74"/>
+      <c r="D31" s="75"/>
+      <c r="E31" s="75"/>
       <c r="F31" s="5"/>
       <c r="G31" s="1"/>
       <c r="H31" s="31"/>
@@ -7543,8 +7360,8 @@
       <c r="C32" t="s">
         <v>292</v>
       </c>
-      <c r="D32" s="74"/>
-      <c r="E32" s="74"/>
+      <c r="D32" s="75"/>
+      <c r="E32" s="75"/>
       <c r="F32" s="5"/>
       <c r="G32" s="1"/>
       <c r="H32" s="31"/>
@@ -7564,8 +7381,8 @@
       <c r="C33" t="s">
         <v>293</v>
       </c>
-      <c r="D33" s="75"/>
-      <c r="E33" s="75"/>
+      <c r="D33" s="76"/>
+      <c r="E33" s="76"/>
       <c r="F33" s="5"/>
       <c r="G33" s="1"/>
       <c r="H33" s="31"/>
@@ -7585,10 +7402,10 @@
       <c r="B34" t="s">
         <v>331</v>
       </c>
-      <c r="D34" s="73">
+      <c r="D34" s="74">
         <v>8</v>
       </c>
-      <c r="E34" s="73" t="s">
+      <c r="E34" s="74" t="s">
         <v>136</v>
       </c>
       <c r="F34" s="5" t="s">
@@ -7616,8 +7433,8 @@
       <c r="C35" t="s">
         <v>294</v>
       </c>
-      <c r="D35" s="74"/>
-      <c r="E35" s="74"/>
+      <c r="D35" s="75"/>
+      <c r="E35" s="75"/>
       <c r="F35" s="5"/>
       <c r="G35" s="9"/>
       <c r="H35" s="31"/>
@@ -7634,8 +7451,8 @@
       <c r="C36" t="s">
         <v>330</v>
       </c>
-      <c r="D36" s="74"/>
-      <c r="E36" s="74"/>
+      <c r="D36" s="75"/>
+      <c r="E36" s="75"/>
       <c r="F36" s="5"/>
       <c r="G36" s="9"/>
       <c r="H36" s="31"/>
@@ -7655,8 +7472,8 @@
       <c r="C37" t="s">
         <v>295</v>
       </c>
-      <c r="D37" s="74"/>
-      <c r="E37" s="74"/>
+      <c r="D37" s="75"/>
+      <c r="E37" s="75"/>
       <c r="F37" s="5"/>
       <c r="G37" s="9"/>
       <c r="H37" s="31"/>
@@ -7673,8 +7490,8 @@
       <c r="C38" t="s">
         <v>297</v>
       </c>
-      <c r="D38" s="74"/>
-      <c r="E38" s="74"/>
+      <c r="D38" s="75"/>
+      <c r="E38" s="75"/>
       <c r="F38" s="5"/>
       <c r="G38" s="9"/>
       <c r="H38" s="31"/>
@@ -7691,8 +7508,8 @@
       <c r="C39" t="s">
         <v>296</v>
       </c>
-      <c r="D39" s="75"/>
-      <c r="E39" s="75"/>
+      <c r="D39" s="76"/>
+      <c r="E39" s="76"/>
       <c r="F39" s="5"/>
       <c r="G39" s="9"/>
       <c r="H39" s="31"/>
@@ -7712,10 +7529,10 @@
       <c r="B40" t="s">
         <v>299</v>
       </c>
-      <c r="D40" s="85">
+      <c r="D40" s="89">
         <v>9</v>
       </c>
-      <c r="E40" s="85" t="s">
+      <c r="E40" s="89" t="s">
         <v>138</v>
       </c>
       <c r="F40" s="1" t="s">
@@ -7743,8 +7560,8 @@
       <c r="C41" t="s">
         <v>300</v>
       </c>
-      <c r="D41" s="86"/>
-      <c r="E41" s="86"/>
+      <c r="D41" s="90"/>
+      <c r="E41" s="90"/>
       <c r="F41" s="1"/>
       <c r="G41" s="9"/>
       <c r="H41" s="34"/>
@@ -7764,8 +7581,8 @@
       <c r="C42" t="s">
         <v>298</v>
       </c>
-      <c r="D42" s="87"/>
-      <c r="E42" s="87"/>
+      <c r="D42" s="91"/>
+      <c r="E42" s="91"/>
       <c r="F42" s="1"/>
       <c r="G42" s="9"/>
       <c r="H42" s="34"/>
@@ -7785,10 +7602,10 @@
       <c r="B43" t="s">
         <v>301</v>
       </c>
-      <c r="D43" s="85">
+      <c r="D43" s="89">
         <v>10</v>
       </c>
-      <c r="E43" s="73" t="s">
+      <c r="E43" s="74" t="s">
         <v>139</v>
       </c>
       <c r="F43" s="6" t="s">
@@ -7816,8 +7633,8 @@
       <c r="C44" t="s">
         <v>302</v>
       </c>
-      <c r="D44" s="86"/>
-      <c r="E44" s="74"/>
+      <c r="D44" s="90"/>
+      <c r="E44" s="75"/>
       <c r="F44" s="6"/>
       <c r="G44" s="9"/>
       <c r="H44" s="34"/>
@@ -7834,8 +7651,8 @@
       <c r="C45" t="s">
         <v>303</v>
       </c>
-      <c r="D45" s="86"/>
-      <c r="E45" s="74"/>
+      <c r="D45" s="90"/>
+      <c r="E45" s="75"/>
       <c r="F45" s="6"/>
       <c r="G45" s="9"/>
       <c r="H45" s="34"/>
@@ -7855,8 +7672,8 @@
       <c r="C46" t="s">
         <v>304</v>
       </c>
-      <c r="D46" s="86"/>
-      <c r="E46" s="74"/>
+      <c r="D46" s="90"/>
+      <c r="E46" s="75"/>
       <c r="F46" s="6"/>
       <c r="G46" s="9"/>
       <c r="H46" s="34"/>
@@ -7873,8 +7690,8 @@
       <c r="C47" t="s">
         <v>298</v>
       </c>
-      <c r="D47" s="87"/>
-      <c r="E47" s="75"/>
+      <c r="D47" s="91"/>
+      <c r="E47" s="76"/>
       <c r="F47" s="6"/>
       <c r="G47" s="9"/>
       <c r="H47" s="34"/>
@@ -7894,10 +7711,10 @@
       <c r="B48" t="s">
         <v>305</v>
       </c>
-      <c r="D48" s="85">
+      <c r="D48" s="89">
         <v>11</v>
       </c>
-      <c r="E48" s="85" t="s">
+      <c r="E48" s="89" t="s">
         <v>141</v>
       </c>
       <c r="F48" s="4" t="s">
@@ -7925,8 +7742,8 @@
       <c r="C49" t="s">
         <v>306</v>
       </c>
-      <c r="D49" s="86"/>
-      <c r="E49" s="86"/>
+      <c r="D49" s="90"/>
+      <c r="E49" s="90"/>
       <c r="F49" s="4"/>
       <c r="G49" s="9"/>
       <c r="H49" s="31"/>
@@ -7943,8 +7760,8 @@
       <c r="C50" t="s">
         <v>307</v>
       </c>
-      <c r="D50" s="86"/>
-      <c r="E50" s="86"/>
+      <c r="D50" s="90"/>
+      <c r="E50" s="90"/>
       <c r="F50" s="4"/>
       <c r="G50" s="9"/>
       <c r="H50" s="31"/>
@@ -7964,8 +7781,8 @@
       <c r="C51" t="s">
         <v>308</v>
       </c>
-      <c r="D51" s="87"/>
-      <c r="E51" s="87"/>
+      <c r="D51" s="91"/>
+      <c r="E51" s="91"/>
       <c r="F51" s="4"/>
       <c r="G51" s="9"/>
       <c r="H51" s="31"/>
@@ -7985,10 +7802,10 @@
       <c r="B52" t="s">
         <v>309</v>
       </c>
-      <c r="D52" s="85">
+      <c r="D52" s="89">
         <v>12</v>
       </c>
-      <c r="E52" s="85" t="s">
+      <c r="E52" s="89" t="s">
         <v>143</v>
       </c>
       <c r="F52" s="1" t="s">
@@ -8016,8 +7833,8 @@
       <c r="C53" t="s">
         <v>310</v>
       </c>
-      <c r="D53" s="86"/>
-      <c r="E53" s="86"/>
+      <c r="D53" s="90"/>
+      <c r="E53" s="90"/>
       <c r="F53" s="1"/>
       <c r="G53" s="9"/>
       <c r="H53" s="31"/>
@@ -8034,8 +7851,8 @@
       <c r="C54" t="s">
         <v>311</v>
       </c>
-      <c r="D54" s="86"/>
-      <c r="E54" s="86"/>
+      <c r="D54" s="90"/>
+      <c r="E54" s="90"/>
       <c r="F54" s="1"/>
       <c r="G54" s="9"/>
       <c r="H54" s="31"/>
@@ -8055,8 +7872,8 @@
       <c r="C55" t="s">
         <v>312</v>
       </c>
-      <c r="D55" s="86"/>
-      <c r="E55" s="86"/>
+      <c r="D55" s="90"/>
+      <c r="E55" s="90"/>
       <c r="F55" s="1"/>
       <c r="G55" s="9"/>
       <c r="H55" s="31"/>
@@ -8076,10 +7893,10 @@
       <c r="B56" t="s">
         <v>332</v>
       </c>
-      <c r="D56" s="85">
+      <c r="D56" s="89">
         <v>13</v>
       </c>
-      <c r="E56" s="73" t="s">
+      <c r="E56" s="74" t="s">
         <v>145</v>
       </c>
       <c r="F56" s="5" t="s">
@@ -8104,8 +7921,8 @@
       <c r="B57" t="s">
         <v>213</v>
       </c>
-      <c r="D57" s="86"/>
-      <c r="E57" s="74"/>
+      <c r="D57" s="90"/>
+      <c r="E57" s="75"/>
       <c r="F57" s="5"/>
       <c r="G57" s="9"/>
       <c r="H57" s="31"/>
@@ -8122,8 +7939,8 @@
       <c r="B58" t="s">
         <v>244</v>
       </c>
-      <c r="D58" s="87"/>
-      <c r="E58" s="75"/>
+      <c r="D58" s="91"/>
+      <c r="E58" s="76"/>
       <c r="F58" s="5"/>
       <c r="G58" s="9"/>
       <c r="H58" s="31"/>
@@ -8143,10 +7960,10 @@
       <c r="B59" t="s">
         <v>313</v>
       </c>
-      <c r="D59" s="85">
+      <c r="D59" s="89">
         <v>14</v>
       </c>
-      <c r="E59" s="73" t="s">
+      <c r="E59" s="74" t="s">
         <v>146</v>
       </c>
       <c r="F59" s="6" t="s">
@@ -8174,8 +7991,8 @@
       <c r="C60" t="s">
         <v>314</v>
       </c>
-      <c r="D60" s="86"/>
-      <c r="E60" s="74"/>
+      <c r="D60" s="90"/>
+      <c r="E60" s="75"/>
       <c r="F60" s="6"/>
       <c r="G60" s="9"/>
       <c r="H60" s="31"/>
@@ -8192,8 +8009,8 @@
       <c r="C61" t="s">
         <v>315</v>
       </c>
-      <c r="D61" s="86"/>
-      <c r="E61" s="74"/>
+      <c r="D61" s="90"/>
+      <c r="E61" s="75"/>
       <c r="F61" s="6"/>
       <c r="G61" s="9"/>
       <c r="H61" s="31"/>
@@ -8213,8 +8030,8 @@
       <c r="C62" t="s">
         <v>316</v>
       </c>
-      <c r="D62" s="87"/>
-      <c r="E62" s="75"/>
+      <c r="D62" s="91"/>
+      <c r="E62" s="76"/>
       <c r="F62" s="6"/>
       <c r="G62" s="9"/>
       <c r="H62" s="31"/>
@@ -8234,10 +8051,10 @@
       <c r="B63" t="s">
         <v>317</v>
       </c>
-      <c r="D63" s="85">
+      <c r="D63" s="89">
         <v>15</v>
       </c>
-      <c r="E63" s="73" t="s">
+      <c r="E63" s="74" t="s">
         <v>149</v>
       </c>
       <c r="F63" s="5" t="s">
@@ -8265,8 +8082,8 @@
       <c r="C64" t="s">
         <v>318</v>
       </c>
-      <c r="D64" s="86"/>
-      <c r="E64" s="74"/>
+      <c r="D64" s="90"/>
+      <c r="E64" s="75"/>
       <c r="F64" s="5"/>
       <c r="G64" s="9"/>
       <c r="H64" s="31"/>
@@ -8283,8 +8100,8 @@
       <c r="C65" t="s">
         <v>319</v>
       </c>
-      <c r="D65" s="86"/>
-      <c r="E65" s="74"/>
+      <c r="D65" s="90"/>
+      <c r="E65" s="75"/>
       <c r="F65" s="5"/>
       <c r="G65" s="9"/>
       <c r="H65" s="31"/>
@@ -8304,8 +8121,8 @@
       <c r="C66" t="s">
         <v>320</v>
       </c>
-      <c r="D66" s="86"/>
-      <c r="E66" s="75"/>
+      <c r="D66" s="90"/>
+      <c r="E66" s="76"/>
       <c r="F66" s="5"/>
       <c r="G66" s="9"/>
       <c r="H66" s="31"/>
@@ -8328,7 +8145,7 @@
       <c r="D67" s="32">
         <v>16</v>
       </c>
-      <c r="E67" s="73" t="s">
+      <c r="E67" s="74" t="s">
         <v>150</v>
       </c>
       <c r="F67" s="6" t="s">
@@ -8357,7 +8174,7 @@
         <v>322</v>
       </c>
       <c r="D68" s="32"/>
-      <c r="E68" s="74"/>
+      <c r="E68" s="75"/>
       <c r="F68" s="6"/>
       <c r="G68" s="9"/>
       <c r="H68" s="31"/>
@@ -8378,7 +8195,7 @@
         <v>323</v>
       </c>
       <c r="D69" s="32"/>
-      <c r="E69" s="74"/>
+      <c r="E69" s="75"/>
       <c r="F69" s="6"/>
       <c r="G69" s="9"/>
       <c r="H69" s="31"/>
@@ -8396,7 +8213,7 @@
         <v>324</v>
       </c>
       <c r="D70" s="32"/>
-      <c r="E70" s="75"/>
+      <c r="E70" s="76"/>
       <c r="F70" s="6"/>
       <c r="G70" s="9"/>
       <c r="H70" s="31"/>
@@ -8416,10 +8233,10 @@
       <c r="B71" t="s">
         <v>334</v>
       </c>
-      <c r="D71" s="73">
+      <c r="D71" s="74">
         <v>17</v>
       </c>
-      <c r="E71" s="73" t="s">
+      <c r="E71" s="74" t="s">
         <v>152</v>
       </c>
       <c r="F71" s="5" t="s">
@@ -8447,8 +8264,8 @@
       <c r="C72" t="s">
         <v>325</v>
       </c>
-      <c r="D72" s="74"/>
-      <c r="E72" s="74"/>
+      <c r="D72" s="75"/>
+      <c r="E72" s="75"/>
       <c r="F72" s="5"/>
       <c r="G72" s="9"/>
       <c r="H72" s="31"/>
@@ -8468,8 +8285,8 @@
       <c r="C73" t="s">
         <v>327</v>
       </c>
-      <c r="D73" s="75"/>
-      <c r="E73" s="75"/>
+      <c r="D73" s="76"/>
+      <c r="E73" s="76"/>
       <c r="F73" s="5"/>
       <c r="G73" s="9"/>
       <c r="H73" s="31"/>
@@ -8531,6 +8348,31 @@
     </row>
   </sheetData>
   <mergeCells count="34">
+    <mergeCell ref="D59:D62"/>
+    <mergeCell ref="E59:E62"/>
+    <mergeCell ref="E71:E73"/>
+    <mergeCell ref="D71:D73"/>
+    <mergeCell ref="D63:D66"/>
+    <mergeCell ref="E63:E66"/>
+    <mergeCell ref="E67:E70"/>
+    <mergeCell ref="D56:D58"/>
+    <mergeCell ref="E56:E58"/>
+    <mergeCell ref="D52:D55"/>
+    <mergeCell ref="E52:E55"/>
+    <mergeCell ref="D48:D51"/>
+    <mergeCell ref="E48:E51"/>
+    <mergeCell ref="D43:D47"/>
+    <mergeCell ref="E43:E47"/>
+    <mergeCell ref="D40:D42"/>
+    <mergeCell ref="E40:E42"/>
+    <mergeCell ref="D34:D39"/>
+    <mergeCell ref="E34:E39"/>
+    <mergeCell ref="D30:D33"/>
+    <mergeCell ref="E30:E33"/>
+    <mergeCell ref="D26:D29"/>
+    <mergeCell ref="E26:E29"/>
+    <mergeCell ref="D18:D25"/>
+    <mergeCell ref="E18:E25"/>
     <mergeCell ref="F10:F13"/>
     <mergeCell ref="D2:D5"/>
     <mergeCell ref="E2:E5"/>
@@ -8540,31 +8382,6 @@
     <mergeCell ref="E10:E13"/>
     <mergeCell ref="D6:D9"/>
     <mergeCell ref="E6:E9"/>
-    <mergeCell ref="D30:D33"/>
-    <mergeCell ref="E30:E33"/>
-    <mergeCell ref="D26:D29"/>
-    <mergeCell ref="E26:E29"/>
-    <mergeCell ref="D18:D25"/>
-    <mergeCell ref="E18:E25"/>
-    <mergeCell ref="D43:D47"/>
-    <mergeCell ref="E43:E47"/>
-    <mergeCell ref="D40:D42"/>
-    <mergeCell ref="E40:E42"/>
-    <mergeCell ref="D34:D39"/>
-    <mergeCell ref="E34:E39"/>
-    <mergeCell ref="D56:D58"/>
-    <mergeCell ref="E56:E58"/>
-    <mergeCell ref="D52:D55"/>
-    <mergeCell ref="E52:E55"/>
-    <mergeCell ref="D48:D51"/>
-    <mergeCell ref="E48:E51"/>
-    <mergeCell ref="D59:D62"/>
-    <mergeCell ref="E59:E62"/>
-    <mergeCell ref="E71:E73"/>
-    <mergeCell ref="D71:D73"/>
-    <mergeCell ref="D63:D66"/>
-    <mergeCell ref="E63:E66"/>
-    <mergeCell ref="E67:E70"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="G2" r:id="rId1" xr:uid="{BD266EE8-9EE9-410E-A73B-7BCBE7209954}"/>
@@ -8593,7 +8410,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A3AF180-2B8D-4C19-A7E4-B0AE9B7543FC}">
   <dimension ref="A1:N17"/>
   <sheetViews>
-    <sheetView topLeftCell="D2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
@@ -8635,16 +8452,16 @@
       <c r="B2" t="s">
         <v>336</v>
       </c>
-      <c r="E2" s="73">
+      <c r="E2" s="74">
         <v>1</v>
       </c>
-      <c r="F2" s="73" t="s">
+      <c r="F2" s="74" t="s">
         <v>171</v>
       </c>
-      <c r="G2" s="60" t="s">
+      <c r="G2" s="68" t="s">
         <v>174</v>
       </c>
-      <c r="H2" s="78" t="s">
+      <c r="H2" s="79" t="s">
         <v>175</v>
       </c>
     </row>
@@ -8659,10 +8476,10 @@
       <c r="D3" t="s">
         <v>346</v>
       </c>
-      <c r="E3" s="74"/>
-      <c r="F3" s="74"/>
-      <c r="G3" s="61"/>
-      <c r="H3" s="79"/>
+      <c r="E3" s="75"/>
+      <c r="F3" s="75"/>
+      <c r="G3" s="69"/>
+      <c r="H3" s="80"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="42"/>
@@ -8673,10 +8490,10 @@
       <c r="D4" t="s">
         <v>345</v>
       </c>
-      <c r="E4" s="74"/>
-      <c r="F4" s="74"/>
-      <c r="G4" s="61"/>
-      <c r="H4" s="79"/>
+      <c r="E4" s="75"/>
+      <c r="F4" s="75"/>
+      <c r="G4" s="69"/>
+      <c r="H4" s="80"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="42"/>
@@ -8687,10 +8504,10 @@
       <c r="D5" t="s">
         <v>344</v>
       </c>
-      <c r="E5" s="75"/>
-      <c r="F5" s="75"/>
-      <c r="G5" s="62"/>
-      <c r="H5" s="80"/>
+      <c r="E5" s="76"/>
+      <c r="F5" s="76"/>
+      <c r="G5" s="70"/>
+      <c r="H5" s="81"/>
     </row>
     <row r="6" spans="1:14" ht="180" x14ac:dyDescent="0.25">
       <c r="A6" s="42" t="s">
@@ -8818,7 +8635,7 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8956,8 +8773,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83D713CF-1264-4070-BA73-824C7A1D0A05}">
   <dimension ref="A1:N53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="83" workbookViewId="0">
-      <selection activeCell="M23" sqref="M23"/>
+    <sheetView tabSelected="1" zoomScale="83" workbookViewId="0">
+      <selection activeCell="E49" sqref="E49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8998,13 +8815,13 @@
       <c r="B2" t="s">
         <v>355</v>
       </c>
-      <c r="F2" s="73">
+      <c r="F2" s="74">
         <v>1</v>
       </c>
-      <c r="G2" s="73" t="s">
+      <c r="G2" s="74" t="s">
         <v>189</v>
       </c>
-      <c r="H2" s="60" t="s">
+      <c r="H2" s="68" t="s">
         <v>190</v>
       </c>
       <c r="I2" s="37" t="s">
@@ -9023,9 +8840,9 @@
       <c r="C3" t="s">
         <v>357</v>
       </c>
-      <c r="F3" s="74"/>
-      <c r="G3" s="74"/>
-      <c r="H3" s="61"/>
+      <c r="F3" s="75"/>
+      <c r="G3" s="75"/>
+      <c r="H3" s="69"/>
       <c r="I3" s="37"/>
       <c r="J3" s="14"/>
       <c r="K3" s="14"/>
@@ -9040,9 +8857,9 @@
       <c r="C4" t="s">
         <v>359</v>
       </c>
-      <c r="F4" s="75"/>
-      <c r="G4" s="75"/>
-      <c r="H4" s="62"/>
+      <c r="F4" s="76"/>
+      <c r="G4" s="76"/>
+      <c r="H4" s="70"/>
       <c r="I4" s="37"/>
       <c r="J4" s="14"/>
       <c r="K4" s="14"/>
@@ -9054,13 +8871,13 @@
       <c r="B5" t="s">
         <v>360</v>
       </c>
-      <c r="F5" s="73">
+      <c r="F5" s="74">
         <v>2</v>
       </c>
-      <c r="G5" s="73" t="s">
+      <c r="G5" s="74" t="s">
         <v>191</v>
       </c>
-      <c r="H5" s="91" t="s">
+      <c r="H5" s="94" t="s">
         <v>369</v>
       </c>
       <c r="I5" s="41" t="s">
@@ -9079,9 +8896,9 @@
       <c r="C6" t="s">
         <v>362</v>
       </c>
-      <c r="F6" s="74"/>
-      <c r="G6" s="74"/>
-      <c r="H6" s="92"/>
+      <c r="F6" s="75"/>
+      <c r="G6" s="75"/>
+      <c r="H6" s="95"/>
       <c r="I6" s="41"/>
       <c r="J6" s="14"/>
       <c r="K6" s="14"/>
@@ -9096,9 +8913,9 @@
       <c r="C7" t="s">
         <v>364</v>
       </c>
-      <c r="F7" s="74"/>
-      <c r="G7" s="74"/>
-      <c r="H7" s="92"/>
+      <c r="F7" s="75"/>
+      <c r="G7" s="75"/>
+      <c r="H7" s="95"/>
       <c r="I7" s="41"/>
       <c r="J7" s="14"/>
       <c r="K7" s="14"/>
@@ -9113,9 +8930,9 @@
       <c r="C8" t="s">
         <v>368</v>
       </c>
-      <c r="F8" s="74"/>
-      <c r="G8" s="74"/>
-      <c r="H8" s="92"/>
+      <c r="F8" s="75"/>
+      <c r="G8" s="75"/>
+      <c r="H8" s="95"/>
       <c r="I8" s="41"/>
       <c r="J8" s="14"/>
       <c r="K8" s="14"/>
@@ -9130,9 +8947,9 @@
       <c r="C9" t="s">
         <v>366</v>
       </c>
-      <c r="F9" s="74"/>
-      <c r="G9" s="74"/>
-      <c r="H9" s="93"/>
+      <c r="F9" s="75"/>
+      <c r="G9" s="75"/>
+      <c r="H9" s="96"/>
       <c r="I9" s="41"/>
       <c r="J9" s="14"/>
       <c r="K9" s="14"/>
@@ -9149,8 +8966,8 @@
       </c>
       <c r="D10" s="47"/>
       <c r="E10" s="47"/>
-      <c r="F10" s="74"/>
-      <c r="G10" s="75"/>
+      <c r="F10" s="75"/>
+      <c r="G10" s="76"/>
       <c r="H10" s="3"/>
       <c r="I10" s="37" t="s">
         <v>203</v>
@@ -9162,20 +8979,20 @@
       <c r="N10" s="14"/>
     </row>
     <row r="11" spans="1:14" ht="45" x14ac:dyDescent="0.25">
-      <c r="B11" s="50" t="s">
+      <c r="B11" s="51" t="s">
         <v>192</v>
       </c>
       <c r="C11" t="s">
         <v>372</v>
       </c>
-      <c r="F11" s="74"/>
-      <c r="G11" s="73" t="s">
+      <c r="F11" s="75"/>
+      <c r="G11" s="74" t="s">
         <v>192</v>
       </c>
       <c r="H11" s="5" t="s">
         <v>195</v>
       </c>
-      <c r="I11" s="94" t="s">
+      <c r="I11" s="92" t="s">
         <v>205</v>
       </c>
       <c r="J11" s="14"/>
@@ -9185,14 +9002,14 @@
       <c r="N11" s="14"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B12" s="50"/>
+      <c r="B12" s="51"/>
       <c r="C12" t="s">
         <v>373</v>
       </c>
-      <c r="F12" s="74"/>
-      <c r="G12" s="74"/>
+      <c r="F12" s="75"/>
+      <c r="G12" s="75"/>
       <c r="H12" s="5"/>
-      <c r="I12" s="94"/>
+      <c r="I12" s="92"/>
       <c r="J12" s="14"/>
       <c r="K12" s="14"/>
       <c r="L12" s="14"/>
@@ -9204,10 +9021,10 @@
       <c r="C13" t="s">
         <v>387</v>
       </c>
-      <c r="F13" s="74"/>
-      <c r="G13" s="75"/>
+      <c r="F13" s="75"/>
+      <c r="G13" s="76"/>
       <c r="H13" s="5"/>
-      <c r="I13" s="94"/>
+      <c r="I13" s="92"/>
       <c r="J13" s="14"/>
       <c r="K13" s="14"/>
       <c r="L13" s="14"/>
@@ -9215,20 +9032,20 @@
       <c r="N13" s="14"/>
     </row>
     <row r="14" spans="1:14" ht="60" x14ac:dyDescent="0.25">
-      <c r="B14" s="50" t="s">
+      <c r="B14" s="51" t="s">
         <v>374</v>
       </c>
       <c r="C14" t="s">
         <v>376</v>
       </c>
-      <c r="F14" s="74"/>
-      <c r="G14" s="73" t="s">
+      <c r="F14" s="75"/>
+      <c r="G14" s="74" t="s">
         <v>193</v>
       </c>
       <c r="H14" s="5" t="s">
         <v>197</v>
       </c>
-      <c r="I14" s="95"/>
+      <c r="I14" s="93"/>
       <c r="J14" s="14"/>
       <c r="K14" s="14"/>
       <c r="L14" s="14"/>
@@ -9236,14 +9053,14 @@
       <c r="N14" s="14"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B15" s="50"/>
+      <c r="B15" s="51"/>
       <c r="C15" t="s">
         <v>378</v>
       </c>
-      <c r="F15" s="74"/>
-      <c r="G15" s="74"/>
+      <c r="F15" s="75"/>
+      <c r="G15" s="75"/>
       <c r="H15" s="5"/>
-      <c r="I15" s="95"/>
+      <c r="I15" s="93"/>
       <c r="J15" s="14"/>
       <c r="K15" s="14"/>
       <c r="L15" s="14"/>
@@ -9255,10 +9072,10 @@
       <c r="C16" t="s">
         <v>388</v>
       </c>
-      <c r="F16" s="74"/>
-      <c r="G16" s="75"/>
+      <c r="F16" s="75"/>
+      <c r="G16" s="76"/>
       <c r="H16" s="5"/>
-      <c r="I16" s="95"/>
+      <c r="I16" s="93"/>
       <c r="J16" s="14"/>
       <c r="K16" s="14"/>
       <c r="L16" s="14"/>
@@ -9266,20 +9083,20 @@
       <c r="N16" s="14"/>
     </row>
     <row r="17" spans="2:14" ht="75" x14ac:dyDescent="0.25">
-      <c r="B17" s="50" t="s">
+      <c r="B17" s="51" t="s">
         <v>194</v>
       </c>
       <c r="C17" t="s">
         <v>377</v>
       </c>
-      <c r="F17" s="74"/>
-      <c r="G17" s="73" t="s">
+      <c r="F17" s="75"/>
+      <c r="G17" s="74" t="s">
         <v>194</v>
       </c>
       <c r="H17" s="5" t="s">
         <v>196</v>
       </c>
-      <c r="I17" s="95"/>
+      <c r="I17" s="93"/>
       <c r="J17" s="14"/>
       <c r="K17" s="14"/>
       <c r="L17" s="14"/>
@@ -9287,12 +9104,12 @@
       <c r="N17" s="14"/>
     </row>
     <row r="18" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B18" s="50"/>
+      <c r="B18" s="51"/>
       <c r="C18" t="s">
         <v>379</v>
       </c>
-      <c r="F18" s="74"/>
-      <c r="G18" s="74"/>
+      <c r="F18" s="75"/>
+      <c r="G18" s="75"/>
       <c r="H18" s="5"/>
       <c r="I18" s="46"/>
       <c r="J18" s="14"/>
@@ -9306,8 +9123,8 @@
       <c r="C19" t="s">
         <v>389</v>
       </c>
-      <c r="F19" s="74"/>
-      <c r="G19" s="75"/>
+      <c r="F19" s="75"/>
+      <c r="G19" s="76"/>
       <c r="H19" s="5"/>
       <c r="I19" s="46"/>
       <c r="J19" s="14"/>
@@ -9326,11 +9143,11 @@
       <c r="D20" t="s">
         <v>383</v>
       </c>
-      <c r="F20" s="74"/>
-      <c r="G20" s="73" t="s">
+      <c r="F20" s="75"/>
+      <c r="G20" s="74" t="s">
         <v>375</v>
       </c>
-      <c r="H20" s="60" t="s">
+      <c r="H20" s="68" t="s">
         <v>198</v>
       </c>
       <c r="I20" s="37" t="s">
@@ -9350,9 +9167,9 @@
       <c r="D21" t="s">
         <v>384</v>
       </c>
-      <c r="F21" s="74"/>
-      <c r="G21" s="74"/>
-      <c r="H21" s="61"/>
+      <c r="F21" s="75"/>
+      <c r="G21" s="75"/>
+      <c r="H21" s="69"/>
       <c r="I21" s="37"/>
       <c r="J21" s="14"/>
       <c r="K21" s="14"/>
@@ -9368,9 +9185,9 @@
       <c r="D22" t="s">
         <v>386</v>
       </c>
-      <c r="F22" s="75"/>
-      <c r="G22" s="75"/>
-      <c r="H22" s="62"/>
+      <c r="F22" s="76"/>
+      <c r="G22" s="76"/>
+      <c r="H22" s="70"/>
       <c r="I22" s="37"/>
       <c r="J22" s="14"/>
       <c r="K22" s="14"/>
@@ -9385,17 +9202,17 @@
       <c r="C23" t="s">
         <v>390</v>
       </c>
-      <c r="F23" s="73">
+      <c r="F23" s="74">
         <v>3</v>
       </c>
-      <c r="G23" s="73" t="s">
+      <c r="G23" s="74" t="s">
         <v>199</v>
       </c>
-      <c r="H23" s="60" t="s">
+      <c r="H23" s="68" t="s">
         <v>400</v>
       </c>
       <c r="I23" s="41" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="J23" s="14"/>
       <c r="K23" s="14"/>
@@ -9410,9 +9227,9 @@
       <c r="D24" t="s">
         <v>403</v>
       </c>
-      <c r="F24" s="74"/>
-      <c r="G24" s="74"/>
-      <c r="H24" s="61"/>
+      <c r="F24" s="75"/>
+      <c r="G24" s="75"/>
+      <c r="H24" s="69"/>
       <c r="I24" s="41"/>
       <c r="J24" s="14"/>
       <c r="K24" s="14"/>
@@ -9424,9 +9241,9 @@
       <c r="D25" t="s">
         <v>404</v>
       </c>
-      <c r="F25" s="74"/>
-      <c r="G25" s="74"/>
-      <c r="H25" s="61"/>
+      <c r="F25" s="75"/>
+      <c r="G25" s="75"/>
+      <c r="H25" s="69"/>
       <c r="I25" s="41"/>
       <c r="J25" s="14"/>
       <c r="K25" s="14"/>
@@ -9438,9 +9255,9 @@
       <c r="D26" t="s">
         <v>405</v>
       </c>
-      <c r="F26" s="74"/>
-      <c r="G26" s="74"/>
-      <c r="H26" s="61"/>
+      <c r="F26" s="75"/>
+      <c r="G26" s="75"/>
+      <c r="H26" s="69"/>
       <c r="I26" s="41"/>
       <c r="J26" s="14"/>
       <c r="K26" s="14"/>
@@ -9455,9 +9272,9 @@
       <c r="D27" t="s">
         <v>406</v>
       </c>
-      <c r="F27" s="74"/>
-      <c r="G27" s="74"/>
-      <c r="H27" s="61"/>
+      <c r="F27" s="75"/>
+      <c r="G27" s="75"/>
+      <c r="H27" s="69"/>
       <c r="I27" s="41"/>
       <c r="J27" s="14"/>
       <c r="K27" s="14"/>
@@ -9469,9 +9286,9 @@
       <c r="D28" t="s">
         <v>407</v>
       </c>
-      <c r="F28" s="74"/>
-      <c r="G28" s="74"/>
-      <c r="H28" s="61"/>
+      <c r="F28" s="75"/>
+      <c r="G28" s="75"/>
+      <c r="H28" s="69"/>
       <c r="I28" s="41"/>
       <c r="J28" s="14"/>
       <c r="K28" s="14"/>
@@ -9486,9 +9303,9 @@
       <c r="E29" t="s">
         <v>409</v>
       </c>
-      <c r="F29" s="74"/>
-      <c r="G29" s="74"/>
-      <c r="H29" s="61"/>
+      <c r="F29" s="75"/>
+      <c r="G29" s="75"/>
+      <c r="H29" s="69"/>
       <c r="I29" s="41"/>
       <c r="J29" s="14"/>
       <c r="K29" s="14"/>
@@ -9503,9 +9320,9 @@
       <c r="E30" t="s">
         <v>411</v>
       </c>
-      <c r="F30" s="74"/>
-      <c r="G30" s="74"/>
-      <c r="H30" s="61"/>
+      <c r="F30" s="75"/>
+      <c r="G30" s="75"/>
+      <c r="H30" s="69"/>
       <c r="I30" s="41"/>
       <c r="J30" s="14"/>
       <c r="K30" s="14"/>
@@ -9514,15 +9331,15 @@
       <c r="N30" s="14"/>
     </row>
     <row r="31" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="C31" s="96" t="s">
+      <c r="C31" s="48" t="s">
+        <v>422</v>
+      </c>
+      <c r="D31" t="s">
         <v>423</v>
       </c>
-      <c r="D31" t="s">
-        <v>424</v>
-      </c>
-      <c r="F31" s="74"/>
-      <c r="G31" s="74"/>
-      <c r="H31" s="61"/>
+      <c r="F31" s="75"/>
+      <c r="G31" s="75"/>
+      <c r="H31" s="69"/>
       <c r="I31" s="41"/>
       <c r="J31" s="14"/>
       <c r="K31" s="14"/>
@@ -9531,13 +9348,13 @@
       <c r="N31" s="14"/>
     </row>
     <row r="32" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="C32" s="96"/>
+      <c r="C32" s="48"/>
       <c r="D32" t="s">
-        <v>426</v>
-      </c>
-      <c r="F32" s="74"/>
-      <c r="G32" s="74"/>
-      <c r="H32" s="61"/>
+        <v>425</v>
+      </c>
+      <c r="F32" s="75"/>
+      <c r="G32" s="75"/>
+      <c r="H32" s="69"/>
       <c r="I32" s="41"/>
       <c r="J32" s="14"/>
       <c r="K32" s="14"/>
@@ -9550,11 +9367,11 @@
         <v>412</v>
       </c>
       <c r="D33" t="s">
-        <v>425</v>
-      </c>
-      <c r="F33" s="74"/>
-      <c r="G33" s="74"/>
-      <c r="H33" s="61"/>
+        <v>424</v>
+      </c>
+      <c r="F33" s="75"/>
+      <c r="G33" s="75"/>
+      <c r="H33" s="69"/>
       <c r="I33" s="41"/>
       <c r="J33" s="14"/>
       <c r="K33" s="14"/>
@@ -9566,9 +9383,9 @@
       <c r="D34" t="s">
         <v>413</v>
       </c>
-      <c r="F34" s="74"/>
-      <c r="G34" s="74"/>
-      <c r="H34" s="61"/>
+      <c r="F34" s="75"/>
+      <c r="G34" s="75"/>
+      <c r="H34" s="69"/>
       <c r="I34" s="41"/>
       <c r="J34" s="14"/>
       <c r="K34" s="14"/>
@@ -9578,14 +9395,14 @@
     </row>
     <row r="35" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C35" t="s">
+        <v>414</v>
+      </c>
+      <c r="D35" t="s">
         <v>415</v>
       </c>
-      <c r="D35" t="s">
-        <v>416</v>
-      </c>
-      <c r="F35" s="74"/>
-      <c r="G35" s="74"/>
-      <c r="H35" s="61"/>
+      <c r="F35" s="75"/>
+      <c r="G35" s="75"/>
+      <c r="H35" s="69"/>
       <c r="I35" s="41"/>
       <c r="J35" s="14"/>
       <c r="K35" s="14"/>
@@ -9595,11 +9412,11 @@
     </row>
     <row r="36" spans="2:14" x14ac:dyDescent="0.25">
       <c r="D36" t="s">
-        <v>422</v>
-      </c>
-      <c r="F36" s="74"/>
-      <c r="G36" s="74"/>
-      <c r="H36" s="61"/>
+        <v>421</v>
+      </c>
+      <c r="F36" s="75"/>
+      <c r="G36" s="75"/>
+      <c r="H36" s="69"/>
       <c r="I36" s="41"/>
       <c r="J36" s="14"/>
       <c r="K36" s="14"/>
@@ -9609,14 +9426,14 @@
     </row>
     <row r="37" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C37" t="s">
+        <v>416</v>
+      </c>
+      <c r="D37" t="s">
         <v>417</v>
       </c>
-      <c r="D37" t="s">
-        <v>418</v>
-      </c>
-      <c r="F37" s="74"/>
-      <c r="G37" s="74"/>
-      <c r="H37" s="61"/>
+      <c r="F37" s="75"/>
+      <c r="G37" s="75"/>
+      <c r="H37" s="69"/>
       <c r="I37" s="41"/>
       <c r="J37" s="14"/>
       <c r="K37" s="14"/>
@@ -9626,11 +9443,11 @@
     </row>
     <row r="38" spans="2:14" x14ac:dyDescent="0.25">
       <c r="D38" t="s">
-        <v>419</v>
-      </c>
-      <c r="F38" s="74"/>
-      <c r="G38" s="74"/>
-      <c r="H38" s="61"/>
+        <v>418</v>
+      </c>
+      <c r="F38" s="75"/>
+      <c r="G38" s="75"/>
+      <c r="H38" s="69"/>
       <c r="I38" s="41"/>
       <c r="J38" s="14"/>
       <c r="K38" s="14"/>
@@ -9640,14 +9457,14 @@
     </row>
     <row r="39" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C39" t="s">
+        <v>419</v>
+      </c>
+      <c r="D39" t="s">
         <v>420</v>
       </c>
-      <c r="D39" t="s">
-        <v>421</v>
-      </c>
-      <c r="F39" s="74"/>
-      <c r="G39" s="74"/>
-      <c r="H39" s="61"/>
+      <c r="F39" s="75"/>
+      <c r="G39" s="75"/>
+      <c r="H39" s="69"/>
       <c r="I39" s="41"/>
       <c r="J39" s="14"/>
       <c r="K39" s="14"/>
@@ -9657,11 +9474,11 @@
     </row>
     <row r="40" spans="2:14" x14ac:dyDescent="0.25">
       <c r="D40" t="s">
-        <v>422</v>
-      </c>
-      <c r="F40" s="75"/>
-      <c r="G40" s="75"/>
-      <c r="H40" s="62"/>
+        <v>421</v>
+      </c>
+      <c r="F40" s="76"/>
+      <c r="G40" s="76"/>
+      <c r="H40" s="70"/>
       <c r="I40" s="41"/>
       <c r="J40" s="14"/>
       <c r="K40" s="14"/>
@@ -9701,16 +9518,16 @@
       <c r="C42" t="s">
         <v>394</v>
       </c>
-      <c r="F42" s="53">
+      <c r="F42" s="61">
         <v>5</v>
       </c>
-      <c r="G42" s="53" t="s">
+      <c r="G42" s="61" t="s">
         <v>206</v>
       </c>
       <c r="H42" s="5" t="s">
         <v>207</v>
       </c>
-      <c r="I42" s="57" t="s">
+      <c r="I42" s="65" t="s">
         <v>202</v>
       </c>
       <c r="J42" s="14"/>
@@ -9729,12 +9546,12 @@
       <c r="E43" t="s">
         <v>398</v>
       </c>
-      <c r="F43" s="53"/>
-      <c r="G43" s="53"/>
+      <c r="F43" s="61"/>
+      <c r="G43" s="61"/>
       <c r="H43" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="I43" s="58"/>
+      <c r="I43" s="66"/>
       <c r="J43" s="14"/>
       <c r="K43" s="14"/>
       <c r="L43" s="14"/>
@@ -9748,12 +9565,12 @@
       <c r="E44" t="s">
         <v>399</v>
       </c>
-      <c r="F44" s="53"/>
-      <c r="G44" s="53"/>
+      <c r="F44" s="61"/>
+      <c r="G44" s="61"/>
       <c r="H44" s="3" t="s">
         <v>209</v>
       </c>
-      <c r="I44" s="59"/>
+      <c r="I44" s="67"/>
       <c r="J44" s="14"/>
       <c r="K44" s="14"/>
       <c r="L44" s="14"/>
@@ -9793,13 +9610,24 @@
       <c r="M47" s="14"/>
       <c r="N47" s="14"/>
     </row>
-    <row r="53" spans="5:5" ht="330" x14ac:dyDescent="0.25">
-      <c r="E53" s="47" t="s">
-        <v>414</v>
-      </c>
+    <row r="53" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E53" s="47"/>
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="F5:F22"/>
+    <mergeCell ref="G11:G13"/>
+    <mergeCell ref="G14:G16"/>
+    <mergeCell ref="G17:G19"/>
+    <mergeCell ref="G20:G22"/>
+    <mergeCell ref="F2:F4"/>
+    <mergeCell ref="G2:G4"/>
+    <mergeCell ref="H2:H4"/>
+    <mergeCell ref="H5:H9"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="G5:G10"/>
     <mergeCell ref="I11:I17"/>
     <mergeCell ref="G42:G44"/>
     <mergeCell ref="F42:F44"/>
@@ -9808,19 +9636,6 @@
     <mergeCell ref="F23:F40"/>
     <mergeCell ref="G23:G40"/>
     <mergeCell ref="H23:H40"/>
-    <mergeCell ref="F2:F4"/>
-    <mergeCell ref="G2:G4"/>
-    <mergeCell ref="H2:H4"/>
-    <mergeCell ref="H5:H9"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="G5:G10"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="F5:F22"/>
-    <mergeCell ref="G11:G13"/>
-    <mergeCell ref="G14:G16"/>
-    <mergeCell ref="G17:G19"/>
-    <mergeCell ref="G20:G22"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="I23" r:id="rId1" display="https://www.baeldung.com/spring-transactional-propagation-isolation" xr:uid="{48BFAE5D-1145-4E0D-A5BD-44A48408A956}"/>

</xml_diff>

<commit_message>
cập nhật tất cả các file và thêm file mới
</commit_message>
<xml_diff>
--- a/Task_Result.xlsx
+++ b/Task_Result.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\beetech\java\stage1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54FC373F-E970-4092-A2BF-7911E735AFA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CE96A3C-B826-4BAF-BA4A-39FBDCFD8040}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="day2 " sheetId="1" r:id="rId1"/>
@@ -21,9 +21,10 @@
     <sheet name="day7" sheetId="6" r:id="rId6"/>
     <sheet name="day8" sheetId="7" r:id="rId7"/>
     <sheet name="day10" sheetId="8" r:id="rId8"/>
+    <sheet name="day15" sheetId="9" r:id="rId9"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId9"/>
+    <externalReference r:id="rId10"/>
   </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
@@ -46,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="427">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="607" uniqueCount="483">
   <si>
     <t>STT</t>
   </si>
@@ -3322,6 +3323,230 @@
 https://shareprogramming.net/quan-ly-transaction-voi-spring-va-jpa/
 https://stackoverflow.com/questions/12390888/differences-between-requires-new-and-nested-propagation-in-spring-transactions
 https://shareprogramming.net/quan-ly-transaction-voi-spring-va-jpa/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thời gian chờ trong Connection Pool: </t>
+  </si>
+  <si>
+    <t>là thời gian mà chờ 1 connection khi không có connection nào trong pool đang rãnh và không thể tạo connection mới</t>
+  </si>
+  <si>
+    <t>Khi request tới sẽ chờ bao lâu:</t>
+  </si>
+  <si>
+    <t>thời gian này thường được setting và khi quá thời gian chờ sẽ ném 1 ConnectionTimeOutException</t>
+  </si>
+  <si>
+    <t>dependency injection (DI)</t>
+  </si>
+  <si>
+    <t>Aspect Oriented Programming (AOP)</t>
+  </si>
+  <si>
+    <t>là một kỹ thuật lập trình cho phép phân tách chương trình thành cách module riêng rẽ, không phụ thuộc nhau</t>
+  </si>
+  <si>
+    <t>Một số thuật ngữ khác trong AOP</t>
+  </si>
+  <si>
+    <t>Join Point</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">là điểm mà các </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="4" tint="-0.499984740745262"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>advice</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> được thực thi</t>
+    </r>
+  </si>
+  <si>
+    <t>Advice</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">là xử lý được thực hiện tại </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="4" tint="-0.499984740745262"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>join point</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t>Before</t>
+  </si>
+  <si>
+    <t>được thực hiện trước join poin</t>
+  </si>
+  <si>
+    <t>After</t>
+  </si>
+  <si>
+    <t>Around</t>
+  </si>
+  <si>
+    <t>After returning</t>
+  </si>
+  <si>
+    <t>After throwing</t>
+  </si>
+  <si>
+    <t>được thực hiện sau khi join point được kết thúc bằng một Exception</t>
+  </si>
+  <si>
+    <t>Pointcut</t>
+  </si>
+  <si>
+    <r>
+      <t>là cách để xác định</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="4" tint="-0.499984740745262"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> join point </t>
+    </r>
+  </si>
+  <si>
+    <t>Aspect</t>
+  </si>
+  <si>
+    <t>là một class bao gồm các advice và các join point</t>
+  </si>
+  <si>
+    <t>Target object</t>
+  </si>
+  <si>
+    <t>là những đối tượng mà advice được áp dụng</t>
+  </si>
+  <si>
+    <t>Có 5  loại Advice:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">được thực hiện sau join point </t>
+  </si>
+  <si>
+    <t>được thực hiện sau join point được kết thúc với return</t>
+  </si>
+  <si>
+    <t>bao gồm cả 4 advice trên</t>
+  </si>
+  <si>
+    <t>Supported Pointcut Designators</t>
+  </si>
+  <si>
+    <t xml:space="preserve">execution </t>
+  </si>
+  <si>
+    <t xml:space="preserve">within </t>
+  </si>
+  <si>
+    <t xml:space="preserve">this </t>
+  </si>
+  <si>
+    <t xml:space="preserve">target </t>
+  </si>
+  <si>
+    <t xml:space="preserve">args </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> @args</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> @within</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> @annotation</t>
+  </si>
+  <si>
+    <t>bean</t>
+  </si>
+  <si>
+    <t>Introductions</t>
+  </si>
+  <si>
+    <t>https://reflectoring.io/aop-spring/#deeper-look-into-spring-aops-annotations</t>
+  </si>
+  <si>
+    <t>Spring AOP Example Tutorial - Aspect, Advice, Pointcut, JoinPoint, Annotations, XML Configuration | DigitalOcean</t>
+  </si>
+  <si>
+    <t>Spring Core – Phần 5: Spring AOP là gì? code ví dụ với Spring AOP (techmaster.vn)</t>
+  </si>
+  <si>
+    <t>Sử dụng AOP trong Spring Boot và AspectJ (viblo.asia)</t>
+  </si>
+  <si>
+    <t>Giới thiệu Aspect Oriented Programming (AOP) - GP Coder (Lập trình Java)</t>
+  </si>
+  <si>
+    <t>Sử dụng Spring AOP Advise trong Spring | Lê Vũ Nguyên Dạy Học Lập Trình (levunguyen.com)</t>
+  </si>
+  <si>
+    <t>https://www.javatpoint.com/spring-boot-aop</t>
+  </si>
+  <si>
+    <t>Spring AOP</t>
+  </si>
+  <si>
+    <t>AspectJ</t>
+  </si>
+  <si>
+    <t>Weaving</t>
+  </si>
+  <si>
+    <t>dùng để match với các joinPoint method’s signature</t>
+  </si>
+  <si>
+    <t>dùng để match với tất cả phương thức join point có trong class, package, sub-package</t>
+  </si>
+  <si>
+    <t>dùng để match với các tham số của phương thức join point</t>
+  </si>
+  <si>
+    <t>dùng để match với phương thức join point được đánh dấu bởi annotation đã được định nghĩa là pointcut</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dùng để match với tất cả phương thức join point có trong class, package, sub-package bằng cách định nghĩa annotation bên trong nó và đính kèm annotation đó lên các class, package, sub-package </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> @target</t>
   </si>
 </sst>
 </file>
@@ -3530,7 +3755,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="97">
+  <cellXfs count="101">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -3646,6 +3871,16 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3659,27 +3894,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -3721,6 +3935,27 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3729,12 +3964,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3754,7 +3983,22 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
@@ -3767,21 +4011,6 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
@@ -3789,6 +4018,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -4224,7 +4459,7 @@
       <xdr:col>23</xdr:col>
       <xdr:colOff>89339</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>151305</xdr:rowOff>
+      <xdr:rowOff>1038115</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4278,13 +4513,13 @@
     <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>394138</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>43793</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
       <xdr:colOff>488841</xdr:colOff>
-      <xdr:row>31</xdr:row>
+      <xdr:row>33</xdr:row>
       <xdr:rowOff>92404</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -4339,13 +4574,13 @@
     <xdr:from>
       <xdr:col>11</xdr:col>
       <xdr:colOff>580258</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>37</xdr:row>
       <xdr:rowOff>65690</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>152806</xdr:colOff>
-      <xdr:row>49</xdr:row>
+      <xdr:colOff>152805</xdr:colOff>
+      <xdr:row>51</xdr:row>
       <xdr:rowOff>136899</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -4879,6 +5114,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="P1:V16"/>
   <sheetViews>
     <sheetView topLeftCell="F6" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
@@ -4898,27 +5134,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="16:22" x14ac:dyDescent="0.25">
-      <c r="P1" s="50" t="s">
+      <c r="P1" s="54" t="s">
         <v>17</v>
       </c>
-      <c r="Q1" s="51"/>
-      <c r="R1" s="51"/>
-      <c r="S1" s="51"/>
-      <c r="T1" s="51"/>
+      <c r="Q1" s="55"/>
+      <c r="R1" s="55"/>
+      <c r="S1" s="55"/>
+      <c r="T1" s="55"/>
     </row>
     <row r="2" spans="16:22" x14ac:dyDescent="0.25">
-      <c r="P2" s="51"/>
-      <c r="Q2" s="51"/>
-      <c r="R2" s="51"/>
-      <c r="S2" s="51"/>
-      <c r="T2" s="51"/>
+      <c r="P2" s="55"/>
+      <c r="Q2" s="55"/>
+      <c r="R2" s="55"/>
+      <c r="S2" s="55"/>
+      <c r="T2" s="55"/>
     </row>
     <row r="3" spans="16:22" x14ac:dyDescent="0.25">
-      <c r="P3" s="52"/>
-      <c r="Q3" s="52"/>
-      <c r="R3" s="52"/>
-      <c r="S3" s="52"/>
-      <c r="T3" s="52"/>
+      <c r="P3" s="56"/>
+      <c r="Q3" s="56"/>
+      <c r="R3" s="56"/>
+      <c r="S3" s="56"/>
+      <c r="T3" s="56"/>
     </row>
     <row r="4" spans="16:22" x14ac:dyDescent="0.25">
       <c r="P4" s="7" t="s">
@@ -4927,11 +5163,11 @@
       <c r="Q4" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="R4" s="49" t="s">
+      <c r="R4" s="53" t="s">
         <v>2</v>
       </c>
-      <c r="S4" s="49"/>
-      <c r="T4" s="49"/>
+      <c r="S4" s="53"/>
+      <c r="T4" s="53"/>
       <c r="U4" s="7" t="s">
         <v>18</v>
       </c>
@@ -5085,24 +5321,24 @@
       </c>
     </row>
     <row r="14" spans="16:22" x14ac:dyDescent="0.25">
-      <c r="P14" s="53" t="s">
+      <c r="P14" s="57" t="s">
         <v>73</v>
       </c>
-      <c r="Q14" s="51"/>
-      <c r="R14" s="51"/>
-      <c r="S14" s="51"/>
+      <c r="Q14" s="55"/>
+      <c r="R14" s="55"/>
+      <c r="S14" s="55"/>
     </row>
     <row r="15" spans="16:22" x14ac:dyDescent="0.25">
-      <c r="P15" s="51"/>
-      <c r="Q15" s="51"/>
-      <c r="R15" s="51"/>
-      <c r="S15" s="51"/>
+      <c r="P15" s="55"/>
+      <c r="Q15" s="55"/>
+      <c r="R15" s="55"/>
+      <c r="S15" s="55"/>
     </row>
     <row r="16" spans="16:22" x14ac:dyDescent="0.25">
-      <c r="P16" s="51"/>
-      <c r="Q16" s="51"/>
-      <c r="R16" s="51"/>
-      <c r="S16" s="51"/>
+      <c r="P16" s="55"/>
+      <c r="Q16" s="55"/>
+      <c r="R16" s="55"/>
+      <c r="S16" s="55"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -5126,6 +5362,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25977106-C04A-4BDF-83D6-AA6BE76B6728}">
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:AD89"/>
   <sheetViews>
     <sheetView topLeftCell="M11" zoomScale="154" zoomScaleNormal="70" workbookViewId="0">
@@ -5147,24 +5384,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:30" ht="49.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="71" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="55"/>
-      <c r="C1" s="55"/>
-      <c r="D1" s="55"/>
-      <c r="E1" s="55"/>
-      <c r="F1" s="55"/>
-      <c r="G1" s="55"/>
-      <c r="H1" s="55"/>
-      <c r="I1" s="55"/>
-      <c r="J1" s="55"/>
-      <c r="K1" s="55"/>
-      <c r="L1" s="55"/>
-      <c r="M1" s="55"/>
-      <c r="N1" s="55"/>
-      <c r="O1" s="55"/>
-      <c r="P1" s="55"/>
+      <c r="B1" s="72"/>
+      <c r="C1" s="72"/>
+      <c r="D1" s="72"/>
+      <c r="E1" s="72"/>
+      <c r="F1" s="72"/>
+      <c r="G1" s="72"/>
+      <c r="H1" s="72"/>
+      <c r="I1" s="72"/>
+      <c r="J1" s="72"/>
+      <c r="K1" s="72"/>
+      <c r="L1" s="72"/>
+      <c r="M1" s="72"/>
+      <c r="N1" s="72"/>
+      <c r="O1" s="72"/>
+      <c r="P1" s="72"/>
       <c r="Q1" s="39"/>
       <c r="R1" s="39"/>
       <c r="S1" s="39"/>
@@ -5256,16 +5493,16 @@
       <c r="P4" t="s">
         <v>214</v>
       </c>
-      <c r="AA4" s="65">
+      <c r="AA4" s="62">
         <v>3</v>
       </c>
-      <c r="AB4" s="65" t="s">
+      <c r="AB4" s="62" t="s">
         <v>35</v>
       </c>
-      <c r="AC4" s="68" t="s">
+      <c r="AC4" s="65" t="s">
         <v>38</v>
       </c>
-      <c r="AD4" s="71" t="s">
+      <c r="AD4" s="68" t="s">
         <v>32</v>
       </c>
     </row>
@@ -5277,10 +5514,10 @@
       <c r="P5" t="s">
         <v>215</v>
       </c>
-      <c r="AA5" s="66"/>
-      <c r="AB5" s="66"/>
-      <c r="AC5" s="69"/>
-      <c r="AD5" s="72"/>
+      <c r="AA5" s="63"/>
+      <c r="AB5" s="63"/>
+      <c r="AC5" s="66"/>
+      <c r="AD5" s="69"/>
     </row>
     <row r="6" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="14"/>
@@ -5293,10 +5530,10 @@
       <c r="P6" t="s">
         <v>217</v>
       </c>
-      <c r="AA6" s="67"/>
-      <c r="AB6" s="67"/>
-      <c r="AC6" s="70"/>
-      <c r="AD6" s="73"/>
+      <c r="AA6" s="64"/>
+      <c r="AB6" s="64"/>
+      <c r="AC6" s="67"/>
+      <c r="AD6" s="70"/>
     </row>
     <row r="7" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="14"/>
@@ -5309,16 +5546,16 @@
       <c r="P7" t="s">
         <v>218</v>
       </c>
-      <c r="AA7" s="65">
+      <c r="AA7" s="62">
         <v>4</v>
       </c>
-      <c r="AB7" s="65" t="s">
+      <c r="AB7" s="62" t="s">
         <v>36</v>
       </c>
-      <c r="AC7" s="68" t="s">
+      <c r="AC7" s="65" t="s">
         <v>39</v>
       </c>
-      <c r="AD7" s="71" t="s">
+      <c r="AD7" s="68" t="s">
         <v>40</v>
       </c>
     </row>
@@ -5330,10 +5567,10 @@
       <c r="P8" t="s">
         <v>219</v>
       </c>
-      <c r="AA8" s="66"/>
-      <c r="AB8" s="66"/>
-      <c r="AC8" s="69"/>
-      <c r="AD8" s="72"/>
+      <c r="AA8" s="63"/>
+      <c r="AB8" s="63"/>
+      <c r="AC8" s="66"/>
+      <c r="AD8" s="69"/>
     </row>
     <row r="9" spans="1:30" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="14"/>
@@ -5346,19 +5583,19 @@
       <c r="P9" t="s">
         <v>220</v>
       </c>
-      <c r="AA9" s="67"/>
-      <c r="AB9" s="67"/>
-      <c r="AC9" s="70"/>
-      <c r="AD9" s="73"/>
+      <c r="AA9" s="64"/>
+      <c r="AB9" s="64"/>
+      <c r="AC9" s="67"/>
+      <c r="AD9" s="70"/>
     </row>
     <row r="10" spans="1:30" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="56" t="s">
+      <c r="A10" s="73" t="s">
         <v>54</v>
       </c>
-      <c r="B10" s="57"/>
-      <c r="C10" s="57"/>
-      <c r="D10" s="57"/>
-      <c r="E10" s="57"/>
+      <c r="B10" s="74"/>
+      <c r="C10" s="74"/>
+      <c r="D10" s="74"/>
+      <c r="E10" s="74"/>
       <c r="F10" s="19"/>
       <c r="G10" s="19"/>
       <c r="H10" s="19"/>
@@ -5369,16 +5606,16 @@
       <c r="P10" t="s">
         <v>222</v>
       </c>
-      <c r="AA10" s="61">
+      <c r="AA10" s="58">
         <v>5</v>
       </c>
-      <c r="AB10" s="62" t="s">
+      <c r="AB10" s="59" t="s">
         <v>37</v>
       </c>
-      <c r="AC10" s="63" t="s">
+      <c r="AC10" s="60" t="s">
         <v>51</v>
       </c>
-      <c r="AD10" s="64" t="s">
+      <c r="AD10" s="61" t="s">
         <v>52</v>
       </c>
     </row>
@@ -5389,19 +5626,19 @@
       <c r="P11" t="s">
         <v>223</v>
       </c>
-      <c r="AA11" s="61"/>
-      <c r="AB11" s="62"/>
-      <c r="AC11" s="63"/>
-      <c r="AD11" s="64"/>
+      <c r="AA11" s="58"/>
+      <c r="AB11" s="59"/>
+      <c r="AC11" s="60"/>
+      <c r="AD11" s="61"/>
     </row>
     <row r="12" spans="1:30" x14ac:dyDescent="0.25">
       <c r="P12" t="s">
         <v>224</v>
       </c>
-      <c r="AA12" s="61"/>
-      <c r="AB12" s="62"/>
-      <c r="AC12" s="63"/>
-      <c r="AD12" s="64"/>
+      <c r="AA12" s="58"/>
+      <c r="AB12" s="59"/>
+      <c r="AC12" s="60"/>
+      <c r="AD12" s="61"/>
     </row>
     <row r="13" spans="1:30" x14ac:dyDescent="0.25">
       <c r="O13" t="s">
@@ -5410,10 +5647,10 @@
       <c r="P13" t="s">
         <v>225</v>
       </c>
-      <c r="AA13" s="61"/>
-      <c r="AB13" s="62"/>
-      <c r="AC13" s="63"/>
-      <c r="AD13" s="64"/>
+      <c r="AA13" s="58"/>
+      <c r="AB13" s="59"/>
+      <c r="AC13" s="60"/>
+      <c r="AD13" s="61"/>
     </row>
     <row r="14" spans="1:30" x14ac:dyDescent="0.25">
       <c r="N14" s="43" t="s">
@@ -5422,10 +5659,10 @@
       <c r="P14" t="s">
         <v>228</v>
       </c>
-      <c r="AA14" s="61"/>
-      <c r="AB14" s="62"/>
-      <c r="AC14" s="63"/>
-      <c r="AD14" s="64"/>
+      <c r="AA14" s="58"/>
+      <c r="AB14" s="59"/>
+      <c r="AC14" s="60"/>
+      <c r="AD14" s="61"/>
     </row>
     <row r="15" spans="1:30" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="40"/>
@@ -5443,10 +5680,10 @@
       <c r="P15" t="s">
         <v>227</v>
       </c>
-      <c r="AA15" s="61"/>
-      <c r="AB15" s="62"/>
-      <c r="AC15" s="63"/>
-      <c r="AD15" s="64"/>
+      <c r="AA15" s="58"/>
+      <c r="AB15" s="59"/>
+      <c r="AC15" s="60"/>
+      <c r="AD15" s="61"/>
     </row>
     <row r="16" spans="1:30" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="40"/>
@@ -5461,10 +5698,10 @@
       <c r="P16" t="s">
         <v>223</v>
       </c>
-      <c r="AA16" s="61"/>
-      <c r="AB16" s="62"/>
-      <c r="AC16" s="63"/>
-      <c r="AD16" s="64"/>
+      <c r="AA16" s="58"/>
+      <c r="AB16" s="59"/>
+      <c r="AC16" s="60"/>
+      <c r="AD16" s="61"/>
     </row>
     <row r="17" spans="1:30" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="40"/>
@@ -5479,10 +5716,10 @@
       <c r="P17" t="s">
         <v>224</v>
       </c>
-      <c r="AA17" s="61"/>
-      <c r="AB17" s="62"/>
-      <c r="AC17" s="63"/>
-      <c r="AD17" s="64"/>
+      <c r="AA17" s="58"/>
+      <c r="AB17" s="59"/>
+      <c r="AC17" s="60"/>
+      <c r="AD17" s="61"/>
     </row>
     <row r="18" spans="1:30" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="40"/>
@@ -5500,10 +5737,10 @@
       <c r="P18" t="s">
         <v>225</v>
       </c>
-      <c r="AA18" s="61"/>
-      <c r="AB18" s="62"/>
-      <c r="AC18" s="63"/>
-      <c r="AD18" s="64"/>
+      <c r="AA18" s="58"/>
+      <c r="AB18" s="59"/>
+      <c r="AC18" s="60"/>
+      <c r="AD18" s="61"/>
     </row>
     <row r="19" spans="1:30" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="40"/>
@@ -5521,10 +5758,10 @@
       <c r="P19" t="s">
         <v>230</v>
       </c>
-      <c r="AA19" s="61"/>
-      <c r="AB19" s="62"/>
-      <c r="AC19" s="63"/>
-      <c r="AD19" s="64"/>
+      <c r="AA19" s="58"/>
+      <c r="AB19" s="59"/>
+      <c r="AC19" s="60"/>
+      <c r="AD19" s="61"/>
     </row>
     <row r="20" spans="1:30" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="40"/>
@@ -5542,10 +5779,10 @@
       <c r="O20" t="s">
         <v>232</v>
       </c>
-      <c r="AA20" s="61"/>
-      <c r="AB20" s="62"/>
-      <c r="AC20" s="63"/>
-      <c r="AD20" s="64"/>
+      <c r="AA20" s="58"/>
+      <c r="AB20" s="59"/>
+      <c r="AC20" s="60"/>
+      <c r="AD20" s="61"/>
     </row>
     <row r="21" spans="1:30" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="40"/>
@@ -5563,10 +5800,10 @@
       <c r="P21" t="s">
         <v>233</v>
       </c>
-      <c r="AA21" s="61"/>
-      <c r="AB21" s="62"/>
-      <c r="AC21" s="63"/>
-      <c r="AD21" s="64"/>
+      <c r="AA21" s="58"/>
+      <c r="AB21" s="59"/>
+      <c r="AC21" s="60"/>
+      <c r="AD21" s="61"/>
     </row>
     <row r="22" spans="1:30" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="40"/>
@@ -5584,10 +5821,10 @@
       <c r="P22" t="s">
         <v>234</v>
       </c>
-      <c r="AA22" s="61"/>
-      <c r="AB22" s="62"/>
-      <c r="AC22" s="63"/>
-      <c r="AD22" s="64"/>
+      <c r="AA22" s="58"/>
+      <c r="AB22" s="59"/>
+      <c r="AC22" s="60"/>
+      <c r="AD22" s="61"/>
     </row>
     <row r="23" spans="1:30" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="40"/>
@@ -5605,10 +5842,10 @@
       <c r="O23" t="s">
         <v>236</v>
       </c>
-      <c r="AA23" s="61"/>
-      <c r="AB23" s="62"/>
-      <c r="AC23" s="63"/>
-      <c r="AD23" s="64"/>
+      <c r="AA23" s="58"/>
+      <c r="AB23" s="59"/>
+      <c r="AC23" s="60"/>
+      <c r="AD23" s="61"/>
     </row>
     <row r="24" spans="1:30" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="40"/>
@@ -5626,10 +5863,10 @@
       <c r="P24" t="s">
         <v>237</v>
       </c>
-      <c r="AA24" s="61"/>
-      <c r="AB24" s="62"/>
-      <c r="AC24" s="63"/>
-      <c r="AD24" s="64"/>
+      <c r="AA24" s="58"/>
+      <c r="AB24" s="59"/>
+      <c r="AC24" s="60"/>
+      <c r="AD24" s="61"/>
     </row>
     <row r="25" spans="1:30" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="40"/>
@@ -5647,25 +5884,25 @@
       <c r="P25" t="s">
         <v>238</v>
       </c>
-      <c r="AA25" s="61"/>
-      <c r="AB25" s="62"/>
-      <c r="AC25" s="63"/>
-      <c r="AD25" s="64"/>
+      <c r="AA25" s="58"/>
+      <c r="AB25" s="59"/>
+      <c r="AC25" s="60"/>
+      <c r="AD25" s="61"/>
     </row>
     <row r="26" spans="1:30" ht="108" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="53" t="s">
+      <c r="A26" s="57" t="s">
         <v>42</v>
       </c>
-      <c r="B26" s="53"/>
-      <c r="C26" s="53"/>
-      <c r="D26" s="53" t="s">
+      <c r="B26" s="57"/>
+      <c r="C26" s="57"/>
+      <c r="D26" s="57" t="s">
         <v>43</v>
       </c>
-      <c r="E26" s="53"/>
-      <c r="F26" s="53"/>
-      <c r="G26" s="53"/>
-      <c r="H26" s="53"/>
-      <c r="I26" s="53"/>
+      <c r="E26" s="57"/>
+      <c r="F26" s="57"/>
+      <c r="G26" s="57"/>
+      <c r="H26" s="57"/>
+      <c r="I26" s="57"/>
       <c r="J26" s="42"/>
       <c r="K26" s="42"/>
       <c r="L26" s="42"/>
@@ -5695,15 +5932,15 @@
       <c r="AD26" s="1"/>
     </row>
     <row r="27" spans="1:30" ht="139.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="53"/>
-      <c r="B27" s="53"/>
-      <c r="C27" s="53"/>
-      <c r="D27" s="53"/>
-      <c r="E27" s="53"/>
-      <c r="F27" s="53"/>
-      <c r="G27" s="53"/>
-      <c r="H27" s="53"/>
-      <c r="I27" s="53"/>
+      <c r="A27" s="57"/>
+      <c r="B27" s="57"/>
+      <c r="C27" s="57"/>
+      <c r="D27" s="57"/>
+      <c r="E27" s="57"/>
+      <c r="F27" s="57"/>
+      <c r="G27" s="57"/>
+      <c r="H27" s="57"/>
+      <c r="I27" s="57"/>
       <c r="J27" s="42"/>
       <c r="K27" s="42"/>
       <c r="L27" s="42"/>
@@ -5733,70 +5970,78 @@
       <c r="AD27" s="1"/>
     </row>
     <row r="54" spans="1:10" ht="42" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="D54" s="60" t="s">
+      <c r="D54" s="77" t="s">
         <v>44</v>
       </c>
-      <c r="E54" s="60"/>
-      <c r="F54" s="60"/>
-      <c r="G54" s="60"/>
-      <c r="H54" s="60"/>
-      <c r="I54" s="60"/>
-      <c r="J54" s="60"/>
+      <c r="E54" s="77"/>
+      <c r="F54" s="77"/>
+      <c r="G54" s="77"/>
+      <c r="H54" s="77"/>
+      <c r="I54" s="77"/>
+      <c r="J54" s="77"/>
     </row>
     <row r="58" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A58" s="59" t="s">
+      <c r="A58" s="76" t="s">
         <v>41</v>
       </c>
-      <c r="B58" s="59"/>
-      <c r="C58" s="59"/>
+      <c r="B58" s="76"/>
+      <c r="C58" s="76"/>
       <c r="D58" s="20"/>
     </row>
     <row r="59" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="59"/>
-      <c r="B59" s="59"/>
-      <c r="C59" s="59"/>
+      <c r="A59" s="76"/>
+      <c r="B59" s="76"/>
+      <c r="C59" s="76"/>
     </row>
     <row r="60" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="59"/>
-      <c r="B60" s="59"/>
-      <c r="C60" s="59"/>
+      <c r="A60" s="76"/>
+      <c r="B60" s="76"/>
+      <c r="C60" s="76"/>
     </row>
     <row r="61" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="59"/>
-      <c r="B61" s="59"/>
-      <c r="C61" s="59"/>
+      <c r="A61" s="76"/>
+      <c r="B61" s="76"/>
+      <c r="C61" s="76"/>
     </row>
     <row r="62" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="53" t="s">
+      <c r="A62" s="57" t="s">
         <v>45</v>
       </c>
-      <c r="B62" s="53"/>
-      <c r="C62" s="53"/>
+      <c r="B62" s="57"/>
+      <c r="C62" s="57"/>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A63" s="53"/>
-      <c r="B63" s="53"/>
-      <c r="C63" s="53"/>
+      <c r="A63" s="57"/>
+      <c r="B63" s="57"/>
+      <c r="C63" s="57"/>
     </row>
     <row r="87" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="58" t="s">
+      <c r="A87" s="75" t="s">
         <v>46</v>
       </c>
-      <c r="B87" s="58"/>
-      <c r="C87" s="58"/>
+      <c r="B87" s="75"/>
+      <c r="C87" s="75"/>
     </row>
     <row r="88" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="58"/>
-      <c r="B88" s="58"/>
-      <c r="C88" s="58"/>
+      <c r="A88" s="75"/>
+      <c r="B88" s="75"/>
+      <c r="C88" s="75"/>
     </row>
     <row r="89" spans="1:3" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="58"/>
-      <c r="B89" s="58"/>
-      <c r="C89" s="58"/>
+      <c r="A89" s="75"/>
+      <c r="B89" s="75"/>
+      <c r="C89" s="75"/>
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A1:P1"/>
+    <mergeCell ref="A10:E10"/>
+    <mergeCell ref="A87:C89"/>
+    <mergeCell ref="A58:C61"/>
+    <mergeCell ref="A26:C27"/>
+    <mergeCell ref="A62:C63"/>
+    <mergeCell ref="D26:I27"/>
+    <mergeCell ref="D54:J54"/>
     <mergeCell ref="AA10:AA25"/>
     <mergeCell ref="AB10:AB25"/>
     <mergeCell ref="AC10:AC25"/>
@@ -5809,14 +6054,6 @@
     <mergeCell ref="AB7:AB9"/>
     <mergeCell ref="AC7:AC9"/>
     <mergeCell ref="AD7:AD9"/>
-    <mergeCell ref="A1:P1"/>
-    <mergeCell ref="A10:E10"/>
-    <mergeCell ref="A87:C89"/>
-    <mergeCell ref="A58:C61"/>
-    <mergeCell ref="A26:C27"/>
-    <mergeCell ref="A62:C63"/>
-    <mergeCell ref="D26:I27"/>
-    <mergeCell ref="D54:J54"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="AD2" r:id="rId1" display="https://stackoverflow.com/questions/15070513/how-to-test-a-non-thread-safe-class" xr:uid="{AF80577A-A125-48C9-AA50-5BBE662AA378}"/>
@@ -5833,16 +6070,17 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9C39CBF-243C-46B8-A97D-C9A6BCF6006E}">
-  <dimension ref="A1:W52"/>
+  <sheetPr codeName="Sheet3"/>
+  <dimension ref="A1:W54"/>
   <sheetViews>
-    <sheetView zoomScale="87" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView topLeftCell="A2" zoomScale="87" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.5703125" customWidth="1"/>
-    <col min="2" max="2" width="14.28515625" customWidth="1"/>
+    <col min="2" max="2" width="38.85546875" customWidth="1"/>
     <col min="6" max="6" width="88.5703125" customWidth="1"/>
     <col min="8" max="8" width="22.7109375" customWidth="1"/>
     <col min="9" max="9" width="115.140625" customWidth="1"/>
@@ -5878,32 +6116,32 @@
       <c r="B2" t="s">
         <v>242</v>
       </c>
-      <c r="G2" s="74">
+      <c r="G2" s="78">
         <v>1</v>
       </c>
-      <c r="H2" s="74" t="s">
+      <c r="H2" s="78" t="s">
         <v>56</v>
       </c>
-      <c r="I2" s="68" t="s">
+      <c r="I2" s="65" t="s">
         <v>57</v>
       </c>
-      <c r="J2" s="79" t="s">
+      <c r="J2" s="81" t="s">
         <v>58</v>
       </c>
-      <c r="L2" s="53" t="s">
+      <c r="L2" s="57" t="s">
         <v>68</v>
       </c>
-      <c r="M2" s="51"/>
-      <c r="N2" s="51"/>
-      <c r="O2" s="51"/>
-      <c r="P2" s="51"/>
-      <c r="Q2" s="51"/>
-      <c r="R2" s="51"/>
-      <c r="S2" s="51"/>
-      <c r="T2" s="51"/>
-      <c r="U2" s="51"/>
-      <c r="V2" s="51"/>
-      <c r="W2" s="51"/>
+      <c r="M2" s="55"/>
+      <c r="N2" s="55"/>
+      <c r="O2" s="55"/>
+      <c r="P2" s="55"/>
+      <c r="Q2" s="55"/>
+      <c r="R2" s="55"/>
+      <c r="S2" s="55"/>
+      <c r="T2" s="55"/>
+      <c r="U2" s="55"/>
+      <c r="V2" s="55"/>
+      <c r="W2" s="55"/>
     </row>
     <row r="3" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B3" t="s">
@@ -5912,10 +6150,10 @@
       <c r="C3" t="s">
         <v>243</v>
       </c>
-      <c r="G3" s="75"/>
-      <c r="H3" s="75"/>
-      <c r="I3" s="69"/>
-      <c r="J3" s="80"/>
+      <c r="G3" s="79"/>
+      <c r="H3" s="79"/>
+      <c r="I3" s="66"/>
+      <c r="J3" s="82"/>
       <c r="L3" s="38"/>
       <c r="M3" s="23"/>
       <c r="N3" s="23"/>
@@ -5936,10 +6174,10 @@
       <c r="C4" t="s">
         <v>245</v>
       </c>
-      <c r="G4" s="75"/>
-      <c r="H4" s="75"/>
-      <c r="I4" s="69"/>
-      <c r="J4" s="80"/>
+      <c r="G4" s="79"/>
+      <c r="H4" s="79"/>
+      <c r="I4" s="66"/>
+      <c r="J4" s="82"/>
       <c r="L4" s="38"/>
       <c r="M4" s="23"/>
       <c r="N4" s="23"/>
@@ -5957,10 +6195,10 @@
       <c r="C5" t="s">
         <v>246</v>
       </c>
-      <c r="G5" s="76"/>
-      <c r="H5" s="76"/>
-      <c r="I5" s="70"/>
-      <c r="J5" s="81"/>
+      <c r="G5" s="80"/>
+      <c r="H5" s="80"/>
+      <c r="I5" s="67"/>
+      <c r="J5" s="83"/>
       <c r="L5" s="38"/>
       <c r="M5" s="23"/>
       <c r="N5" s="23"/>
@@ -5981,16 +6219,16 @@
       <c r="B6" t="s">
         <v>248</v>
       </c>
-      <c r="G6" s="74">
+      <c r="G6" s="78">
         <v>2</v>
       </c>
-      <c r="H6" s="74" t="s">
+      <c r="H6" s="78" t="s">
         <v>59</v>
       </c>
-      <c r="I6" s="68" t="s">
+      <c r="I6" s="65" t="s">
         <v>60</v>
       </c>
-      <c r="J6" s="82" t="s">
+      <c r="J6" s="84" t="s">
         <v>72</v>
       </c>
       <c r="M6" s="26"/>
@@ -6002,20 +6240,20 @@
       <c r="C7" t="s">
         <v>249</v>
       </c>
-      <c r="G7" s="75"/>
-      <c r="H7" s="75"/>
-      <c r="I7" s="69"/>
-      <c r="J7" s="83"/>
+      <c r="G7" s="79"/>
+      <c r="H7" s="79"/>
+      <c r="I7" s="66"/>
+      <c r="J7" s="85"/>
       <c r="M7" s="26"/>
     </row>
     <row r="8" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
         <v>250</v>
       </c>
-      <c r="G8" s="75"/>
-      <c r="H8" s="75"/>
-      <c r="I8" s="69"/>
-      <c r="J8" s="83"/>
+      <c r="G8" s="79"/>
+      <c r="H8" s="79"/>
+      <c r="I8" s="66"/>
+      <c r="J8" s="85"/>
       <c r="M8" s="26"/>
     </row>
     <row r="9" spans="1:23" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -6025,340 +6263,369 @@
       <c r="C9" t="s">
         <v>251</v>
       </c>
-      <c r="G9" s="76"/>
-      <c r="H9" s="76"/>
-      <c r="I9" s="70"/>
-      <c r="J9" s="84"/>
+      <c r="G9" s="80"/>
+      <c r="H9" s="80"/>
+      <c r="I9" s="67"/>
+      <c r="J9" s="86"/>
       <c r="M9" s="26"/>
     </row>
-    <row r="10" spans="1:23" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="43" t="s">
+    <row r="10" spans="1:23" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>427</v>
+      </c>
+      <c r="C10" t="s">
+        <v>428</v>
+      </c>
+      <c r="G10" s="50"/>
+      <c r="H10" s="50"/>
+      <c r="I10" s="49"/>
+      <c r="J10" s="51"/>
+      <c r="M10" s="26"/>
+    </row>
+    <row r="11" spans="1:23" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>429</v>
+      </c>
+      <c r="C11" t="s">
+        <v>430</v>
+      </c>
+      <c r="G11" s="50"/>
+      <c r="H11" s="50"/>
+      <c r="I11" s="49"/>
+      <c r="J11" s="51"/>
+      <c r="M11" s="26"/>
+    </row>
+    <row r="12" spans="1:23" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="43" t="s">
         <v>252</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B12" t="s">
         <v>253</v>
       </c>
-      <c r="G10" s="74">
+      <c r="G12" s="78">
         <v>3</v>
       </c>
-      <c r="H10" s="74" t="s">
+      <c r="H12" s="78" t="s">
         <v>61</v>
       </c>
-      <c r="I10" s="68" t="s">
+      <c r="I12" s="65" t="s">
         <v>62</v>
       </c>
-      <c r="J10" s="82" t="s">
+      <c r="J12" s="84" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
         <v>213</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C13" t="s">
         <v>254</v>
       </c>
-      <c r="G11" s="75"/>
-      <c r="H11" s="75"/>
-      <c r="I11" s="69"/>
-      <c r="J11" s="83"/>
-    </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
-        <v>244</v>
-      </c>
-      <c r="C12" t="s">
-        <v>255</v>
-      </c>
-      <c r="G12" s="75"/>
-      <c r="H12" s="75"/>
-      <c r="I12" s="69"/>
-      <c r="J12" s="83"/>
-    </row>
-    <row r="13" spans="1:23" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="43" t="s">
-        <v>256</v>
-      </c>
-      <c r="B13" t="s">
-        <v>257</v>
-      </c>
-      <c r="G13" s="74">
-        <v>4</v>
-      </c>
-      <c r="H13" s="74" t="s">
-        <v>66</v>
-      </c>
-      <c r="I13" s="68" t="s">
-        <v>65</v>
-      </c>
-      <c r="J13" s="74"/>
-      <c r="K13" s="77" t="s">
-        <v>69</v>
-      </c>
-      <c r="L13" s="51"/>
-      <c r="M13" s="51"/>
-      <c r="N13" s="51"/>
-      <c r="O13" s="51"/>
-      <c r="P13" s="51"/>
-      <c r="Q13" s="51"/>
-      <c r="R13" s="51"/>
-      <c r="S13" s="51"/>
-      <c r="T13" s="51"/>
-      <c r="U13" s="51"/>
-      <c r="V13" s="51"/>
-      <c r="W13" s="51"/>
+      <c r="G13" s="79"/>
+      <c r="H13" s="79"/>
+      <c r="I13" s="66"/>
+      <c r="J13" s="85"/>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
+        <v>244</v>
+      </c>
+      <c r="C14" t="s">
+        <v>255</v>
+      </c>
+      <c r="G14" s="79"/>
+      <c r="H14" s="79"/>
+      <c r="I14" s="66"/>
+      <c r="J14" s="85"/>
+    </row>
+    <row r="15" spans="1:23" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="43" t="s">
+        <v>256</v>
+      </c>
+      <c r="B15" t="s">
+        <v>257</v>
+      </c>
+      <c r="G15" s="78">
+        <v>4</v>
+      </c>
+      <c r="H15" s="78" t="s">
+        <v>66</v>
+      </c>
+      <c r="I15" s="65" t="s">
+        <v>65</v>
+      </c>
+      <c r="J15" s="78"/>
+      <c r="K15" s="87" t="s">
+        <v>69</v>
+      </c>
+      <c r="L15" s="55"/>
+      <c r="M15" s="55"/>
+      <c r="N15" s="55"/>
+      <c r="O15" s="55"/>
+      <c r="P15" s="55"/>
+      <c r="Q15" s="55"/>
+      <c r="R15" s="55"/>
+      <c r="S15" s="55"/>
+      <c r="T15" s="55"/>
+      <c r="U15" s="55"/>
+      <c r="V15" s="55"/>
+      <c r="W15" s="55"/>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
         <v>213</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C16" t="s">
         <v>258</v>
       </c>
-      <c r="G14" s="75"/>
-      <c r="H14" s="75"/>
-      <c r="I14" s="69"/>
-      <c r="J14" s="75"/>
-      <c r="K14" s="77"/>
-      <c r="L14" s="51"/>
-      <c r="M14" s="51"/>
-      <c r="N14" s="51"/>
-      <c r="O14" s="51"/>
-      <c r="P14" s="51"/>
-      <c r="Q14" s="51"/>
-      <c r="R14" s="51"/>
-      <c r="S14" s="51"/>
-      <c r="T14" s="51"/>
-      <c r="U14" s="51"/>
-      <c r="V14" s="51"/>
-      <c r="W14" s="51"/>
-    </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
+      <c r="G16" s="79"/>
+      <c r="H16" s="79"/>
+      <c r="I16" s="66"/>
+      <c r="J16" s="79"/>
+      <c r="K16" s="87"/>
+      <c r="L16" s="55"/>
+      <c r="M16" s="55"/>
+      <c r="N16" s="55"/>
+      <c r="O16" s="55"/>
+      <c r="P16" s="55"/>
+      <c r="Q16" s="55"/>
+      <c r="R16" s="55"/>
+      <c r="S16" s="55"/>
+      <c r="T16" s="55"/>
+      <c r="U16" s="55"/>
+      <c r="V16" s="55"/>
+      <c r="W16" s="55"/>
+    </row>
+    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
         <v>244</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C17" t="s">
         <v>259</v>
       </c>
-      <c r="G15" s="76"/>
-      <c r="H15" s="76"/>
-      <c r="I15" s="70"/>
-      <c r="J15" s="76"/>
-      <c r="K15" s="77"/>
-      <c r="L15" s="51"/>
-      <c r="M15" s="51"/>
-      <c r="N15" s="51"/>
-      <c r="O15" s="51"/>
-      <c r="P15" s="51"/>
-      <c r="Q15" s="51"/>
-      <c r="R15" s="51"/>
-      <c r="S15" s="51"/>
-      <c r="T15" s="51"/>
-      <c r="U15" s="51"/>
-      <c r="V15" s="51"/>
-      <c r="W15" s="51"/>
-    </row>
-    <row r="16" spans="1:23" ht="45" x14ac:dyDescent="0.25">
-      <c r="A16" s="43" t="s">
+      <c r="G17" s="80"/>
+      <c r="H17" s="80"/>
+      <c r="I17" s="67"/>
+      <c r="J17" s="80"/>
+      <c r="K17" s="87"/>
+      <c r="L17" s="55"/>
+      <c r="M17" s="55"/>
+      <c r="N17" s="55"/>
+      <c r="O17" s="55"/>
+      <c r="P17" s="55"/>
+      <c r="Q17" s="55"/>
+      <c r="R17" s="55"/>
+      <c r="S17" s="55"/>
+      <c r="T17" s="55"/>
+      <c r="U17" s="55"/>
+      <c r="V17" s="55"/>
+      <c r="W17" s="55"/>
+    </row>
+    <row r="18" spans="1:23" ht="45" x14ac:dyDescent="0.25">
+      <c r="A18" s="43" t="s">
         <v>64</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B18" t="s">
         <v>260</v>
       </c>
-      <c r="G16" s="3">
+      <c r="G18" s="3">
         <v>5</v>
       </c>
-      <c r="H16" s="3" t="s">
+      <c r="H18" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="I16" s="5" t="s">
+      <c r="I18" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="J16" s="3"/>
-      <c r="K16" s="78"/>
-      <c r="L16" s="51"/>
-      <c r="M16" s="51"/>
-      <c r="N16" s="51"/>
-      <c r="O16" s="51"/>
-      <c r="P16" s="51"/>
-      <c r="Q16" s="51"/>
-      <c r="R16" s="51"/>
-      <c r="S16" s="51"/>
-      <c r="T16" s="51"/>
-      <c r="U16" s="51"/>
-      <c r="V16" s="51"/>
-      <c r="W16" s="51"/>
-    </row>
-    <row r="17" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
+      <c r="J18" s="3"/>
+      <c r="K18" s="88"/>
+      <c r="L18" s="55"/>
+      <c r="M18" s="55"/>
+      <c r="N18" s="55"/>
+      <c r="O18" s="55"/>
+      <c r="P18" s="55"/>
+      <c r="Q18" s="55"/>
+      <c r="R18" s="55"/>
+      <c r="S18" s="55"/>
+      <c r="T18" s="55"/>
+      <c r="U18" s="55"/>
+      <c r="V18" s="55"/>
+      <c r="W18" s="55"/>
+    </row>
+    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
         <v>213</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C19" t="s">
         <v>261</v>
       </c>
-      <c r="G17" s="14"/>
-      <c r="H17" s="14"/>
-      <c r="I17" s="44"/>
-      <c r="J17" s="14"/>
-      <c r="K17" s="23"/>
-      <c r="L17" s="23"/>
-      <c r="M17" s="23"/>
-      <c r="N17" s="23"/>
-      <c r="O17" s="23"/>
-      <c r="P17" s="23"/>
-      <c r="Q17" s="23"/>
-      <c r="R17" s="23"/>
-      <c r="S17" s="23"/>
-      <c r="T17" s="23"/>
-      <c r="U17" s="23"/>
-      <c r="V17" s="23"/>
-      <c r="W17" s="23"/>
-    </row>
-    <row r="18" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
-        <v>244</v>
-      </c>
-      <c r="C18" t="s">
-        <v>262</v>
-      </c>
-      <c r="G18" s="14"/>
-      <c r="H18" s="14"/>
-      <c r="I18" s="14"/>
-      <c r="J18" s="14"/>
-    </row>
-    <row r="19" spans="2:23" x14ac:dyDescent="0.25">
       <c r="G19" s="14"/>
       <c r="H19" s="14"/>
-      <c r="I19" s="14"/>
+      <c r="I19" s="44"/>
       <c r="J19" s="14"/>
-    </row>
-    <row r="20" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="K19" s="23"/>
+      <c r="L19" s="23"/>
+      <c r="M19" s="23"/>
+      <c r="N19" s="23"/>
+      <c r="O19" s="23"/>
+      <c r="P19" s="23"/>
+      <c r="Q19" s="23"/>
+      <c r="R19" s="23"/>
+      <c r="S19" s="23"/>
+      <c r="T19" s="23"/>
+      <c r="U19" s="23"/>
+      <c r="V19" s="23"/>
+      <c r="W19" s="23"/>
+    </row>
+    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>244</v>
+      </c>
+      <c r="C20" t="s">
+        <v>262</v>
+      </c>
       <c r="G20" s="14"/>
       <c r="H20" s="14"/>
       <c r="I20" s="14"/>
       <c r="J20" s="14"/>
     </row>
-    <row r="21" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
       <c r="G21" s="14"/>
       <c r="H21" s="14"/>
       <c r="I21" s="14"/>
       <c r="J21" s="14"/>
     </row>
-    <row r="22" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
       <c r="G22" s="14"/>
       <c r="H22" s="14"/>
       <c r="I22" s="14"/>
       <c r="J22" s="14"/>
-      <c r="Q22" s="27"/>
-    </row>
-    <row r="23" spans="2:23" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
       <c r="G23" s="14"/>
       <c r="H23" s="14"/>
       <c r="I23" s="14"/>
       <c r="J23" s="14"/>
     </row>
-    <row r="24" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
       <c r="G24" s="14"/>
       <c r="H24" s="14"/>
       <c r="I24" s="14"/>
       <c r="J24" s="14"/>
-    </row>
-    <row r="25" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="Q24" s="27"/>
+    </row>
+    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
       <c r="G25" s="14"/>
       <c r="H25" s="14"/>
       <c r="I25" s="14"/>
       <c r="J25" s="14"/>
     </row>
-    <row r="26" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
       <c r="G26" s="14"/>
       <c r="H26" s="14"/>
       <c r="I26" s="14"/>
       <c r="J26" s="14"/>
     </row>
-    <row r="27" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
       <c r="G27" s="14"/>
       <c r="H27" s="14"/>
       <c r="I27" s="14"/>
       <c r="J27" s="14"/>
     </row>
-    <row r="33" spans="11:22" x14ac:dyDescent="0.25">
-      <c r="K33" s="53" t="s">
+    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="G28" s="14"/>
+      <c r="H28" s="14"/>
+      <c r="I28" s="14"/>
+      <c r="J28" s="14"/>
+    </row>
+    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="G29" s="14"/>
+      <c r="H29" s="14"/>
+      <c r="I29" s="14"/>
+      <c r="J29" s="14"/>
+    </row>
+    <row r="35" spans="11:22" x14ac:dyDescent="0.25">
+      <c r="K35" s="57" t="s">
         <v>70</v>
       </c>
-      <c r="L33" s="51"/>
-      <c r="M33" s="51"/>
-      <c r="N33" s="51"/>
-      <c r="O33" s="51"/>
-      <c r="P33" s="51"/>
-      <c r="Q33" s="51"/>
-      <c r="R33" s="51"/>
-      <c r="S33" s="51"/>
-      <c r="T33" s="51"/>
-      <c r="U33" s="51"/>
-      <c r="V33" s="51"/>
-    </row>
-    <row r="34" spans="11:22" x14ac:dyDescent="0.25">
-      <c r="K34" s="51"/>
-      <c r="L34" s="51"/>
-      <c r="M34" s="51"/>
-      <c r="N34" s="51"/>
-      <c r="O34" s="51"/>
-      <c r="P34" s="51"/>
-      <c r="Q34" s="51"/>
-      <c r="R34" s="51"/>
-      <c r="S34" s="51"/>
-      <c r="T34" s="51"/>
-      <c r="U34" s="51"/>
-      <c r="V34" s="51"/>
-    </row>
-    <row r="35" spans="11:22" x14ac:dyDescent="0.25">
-      <c r="K35" s="51"/>
-      <c r="L35" s="51"/>
-      <c r="M35" s="51"/>
-      <c r="N35" s="51"/>
-      <c r="O35" s="51"/>
-      <c r="P35" s="51"/>
-      <c r="Q35" s="51"/>
-      <c r="R35" s="51"/>
-      <c r="S35" s="51"/>
-      <c r="T35" s="51"/>
-      <c r="U35" s="51"/>
-      <c r="V35" s="51"/>
-    </row>
-    <row r="51" spans="11:22" x14ac:dyDescent="0.25">
-      <c r="K51" s="60" t="s">
+      <c r="L35" s="55"/>
+      <c r="M35" s="55"/>
+      <c r="N35" s="55"/>
+      <c r="O35" s="55"/>
+      <c r="P35" s="55"/>
+      <c r="Q35" s="55"/>
+      <c r="R35" s="55"/>
+      <c r="S35" s="55"/>
+      <c r="T35" s="55"/>
+      <c r="U35" s="55"/>
+      <c r="V35" s="55"/>
+    </row>
+    <row r="36" spans="11:22" x14ac:dyDescent="0.25">
+      <c r="K36" s="55"/>
+      <c r="L36" s="55"/>
+      <c r="M36" s="55"/>
+      <c r="N36" s="55"/>
+      <c r="O36" s="55"/>
+      <c r="P36" s="55"/>
+      <c r="Q36" s="55"/>
+      <c r="R36" s="55"/>
+      <c r="S36" s="55"/>
+      <c r="T36" s="55"/>
+      <c r="U36" s="55"/>
+      <c r="V36" s="55"/>
+    </row>
+    <row r="37" spans="11:22" x14ac:dyDescent="0.25">
+      <c r="K37" s="55"/>
+      <c r="L37" s="55"/>
+      <c r="M37" s="55"/>
+      <c r="N37" s="55"/>
+      <c r="O37" s="55"/>
+      <c r="P37" s="55"/>
+      <c r="Q37" s="55"/>
+      <c r="R37" s="55"/>
+      <c r="S37" s="55"/>
+      <c r="T37" s="55"/>
+      <c r="U37" s="55"/>
+      <c r="V37" s="55"/>
+    </row>
+    <row r="53" spans="11:22" x14ac:dyDescent="0.25">
+      <c r="K53" s="77" t="s">
         <v>71</v>
       </c>
-      <c r="L51" s="51"/>
-      <c r="M51" s="51"/>
-      <c r="N51" s="51"/>
-      <c r="O51" s="51"/>
-      <c r="P51" s="51"/>
-      <c r="Q51" s="51"/>
-      <c r="R51" s="51"/>
-      <c r="S51" s="51"/>
-      <c r="T51" s="51"/>
-      <c r="U51" s="51"/>
-      <c r="V51" s="51"/>
-    </row>
-    <row r="52" spans="11:22" x14ac:dyDescent="0.25">
-      <c r="K52" s="51"/>
-      <c r="L52" s="51"/>
-      <c r="M52" s="51"/>
-      <c r="N52" s="51"/>
-      <c r="O52" s="51"/>
-      <c r="P52" s="51"/>
-      <c r="Q52" s="51"/>
-      <c r="R52" s="51"/>
-      <c r="S52" s="51"/>
-      <c r="T52" s="51"/>
-      <c r="U52" s="51"/>
-      <c r="V52" s="51"/>
+      <c r="L53" s="55"/>
+      <c r="M53" s="55"/>
+      <c r="N53" s="55"/>
+      <c r="O53" s="55"/>
+      <c r="P53" s="55"/>
+      <c r="Q53" s="55"/>
+      <c r="R53" s="55"/>
+      <c r="S53" s="55"/>
+      <c r="T53" s="55"/>
+      <c r="U53" s="55"/>
+      <c r="V53" s="55"/>
+    </row>
+    <row r="54" spans="11:22" x14ac:dyDescent="0.25">
+      <c r="K54" s="55"/>
+      <c r="L54" s="55"/>
+      <c r="M54" s="55"/>
+      <c r="N54" s="55"/>
+      <c r="O54" s="55"/>
+      <c r="P54" s="55"/>
+      <c r="Q54" s="55"/>
+      <c r="R54" s="55"/>
+      <c r="S54" s="55"/>
+      <c r="T54" s="55"/>
+      <c r="U54" s="55"/>
+      <c r="V54" s="55"/>
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="K33:V35"/>
-    <mergeCell ref="K51:V52"/>
+    <mergeCell ref="J15:J17"/>
+    <mergeCell ref="L2:W2"/>
+    <mergeCell ref="K15:W18"/>
+    <mergeCell ref="K35:V37"/>
+    <mergeCell ref="K53:V54"/>
     <mergeCell ref="G2:G5"/>
     <mergeCell ref="H2:H5"/>
     <mergeCell ref="I2:I5"/>
@@ -6367,21 +6634,18 @@
     <mergeCell ref="H6:H9"/>
     <mergeCell ref="I6:I9"/>
     <mergeCell ref="J6:J9"/>
-    <mergeCell ref="G10:G12"/>
-    <mergeCell ref="H10:H12"/>
-    <mergeCell ref="I10:I12"/>
-    <mergeCell ref="J10:J12"/>
-    <mergeCell ref="G13:G15"/>
-    <mergeCell ref="H13:H15"/>
-    <mergeCell ref="I13:I15"/>
-    <mergeCell ref="J13:J15"/>
-    <mergeCell ref="L2:W2"/>
-    <mergeCell ref="K13:W16"/>
+    <mergeCell ref="G12:G14"/>
+    <mergeCell ref="H12:H14"/>
+    <mergeCell ref="I12:I14"/>
+    <mergeCell ref="J12:J14"/>
+    <mergeCell ref="G15:G17"/>
+    <mergeCell ref="H15:H17"/>
+    <mergeCell ref="I15:I17"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="J2" r:id="rId1" xr:uid="{3D14D563-A18C-4362-B2CD-8D8339C1C427}"/>
     <hyperlink ref="J6" r:id="rId2" display="https://www.baeldung.com/java-connection-pooling" xr:uid="{C6D19347-A59D-426C-9D1E-C2B07B6CDCC2}"/>
-    <hyperlink ref="J10" r:id="rId3" display="https://viblo.asia/p/string-pool-la-gi-_x000a_" xr:uid="{6F55EEC8-830E-42C3-9431-2030A8B28A12}"/>
+    <hyperlink ref="J12" r:id="rId3" display="https://viblo.asia/p/string-pool-la-gi-_x000a_" xr:uid="{6F55EEC8-830E-42C3-9431-2030A8B28A12}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId4"/>
@@ -6391,6 +6655,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{341EEE2D-1F16-40EE-ACD5-5E90DCDB2717}">
+  <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6447,14 +6712,14 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="85" t="s">
+      <c r="A7" s="89" t="s">
         <v>79</v>
       </c>
-      <c r="B7" s="51"/>
+      <c r="B7" s="55"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="51"/>
-      <c r="B8" s="51"/>
+      <c r="A8" s="55"/>
+      <c r="B8" s="55"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
@@ -6652,6 +6917,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D5CC180-ABEC-4096-BF7B-D59D7E76A5ED}">
+  <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:P76"/>
   <sheetViews>
     <sheetView topLeftCell="A61" zoomScale="95" workbookViewId="0">
@@ -6701,10 +6967,10 @@
       <c r="B2" t="s">
         <v>264</v>
       </c>
-      <c r="D2" s="74">
+      <c r="D2" s="78">
         <v>1</v>
       </c>
-      <c r="E2" s="74" t="s">
+      <c r="E2" s="78" t="s">
         <v>119</v>
       </c>
       <c r="F2" s="6" t="s">
@@ -6732,8 +6998,8 @@
       <c r="C3" t="s">
         <v>265</v>
       </c>
-      <c r="D3" s="75"/>
-      <c r="E3" s="75"/>
+      <c r="D3" s="79"/>
+      <c r="E3" s="79"/>
       <c r="F3" s="6"/>
       <c r="G3" s="11"/>
       <c r="H3" s="3"/>
@@ -6750,8 +7016,8 @@
       <c r="C4" t="s">
         <v>266</v>
       </c>
-      <c r="D4" s="75"/>
-      <c r="E4" s="75"/>
+      <c r="D4" s="79"/>
+      <c r="E4" s="79"/>
       <c r="F4" s="6"/>
       <c r="G4" s="11"/>
       <c r="H4" s="3"/>
@@ -6771,8 +7037,8 @@
       <c r="C5" t="s">
         <v>267</v>
       </c>
-      <c r="D5" s="76"/>
-      <c r="E5" s="76"/>
+      <c r="D5" s="80"/>
+      <c r="E5" s="80"/>
       <c r="F5" s="6"/>
       <c r="G5" s="11"/>
       <c r="H5" s="3"/>
@@ -6792,10 +7058,10 @@
       <c r="B6" t="s">
         <v>269</v>
       </c>
-      <c r="D6" s="74">
+      <c r="D6" s="78">
         <v>2</v>
       </c>
-      <c r="E6" s="74" t="s">
+      <c r="E6" s="78" t="s">
         <v>122</v>
       </c>
       <c r="F6" s="5" t="s">
@@ -6823,8 +7089,8 @@
       <c r="C7" t="s">
         <v>270</v>
       </c>
-      <c r="D7" s="75"/>
-      <c r="E7" s="75"/>
+      <c r="D7" s="79"/>
+      <c r="E7" s="79"/>
       <c r="F7" s="5"/>
       <c r="G7" s="4"/>
       <c r="H7" s="3"/>
@@ -6841,8 +7107,8 @@
       <c r="C8" t="s">
         <v>271</v>
       </c>
-      <c r="D8" s="75"/>
-      <c r="E8" s="75"/>
+      <c r="D8" s="79"/>
+      <c r="E8" s="79"/>
       <c r="F8" s="5"/>
       <c r="G8" s="4"/>
       <c r="H8" s="3"/>
@@ -6862,8 +7128,8 @@
       <c r="C9" t="s">
         <v>272</v>
       </c>
-      <c r="D9" s="76"/>
-      <c r="E9" s="76"/>
+      <c r="D9" s="80"/>
+      <c r="E9" s="80"/>
       <c r="F9" s="5"/>
       <c r="G9" s="4"/>
       <c r="H9" s="3"/>
@@ -6883,13 +7149,13 @@
       <c r="B10" t="s">
         <v>273</v>
       </c>
-      <c r="D10" s="89">
+      <c r="D10" s="90">
         <v>3</v>
       </c>
-      <c r="E10" s="89" t="s">
+      <c r="E10" s="90" t="s">
         <v>125</v>
       </c>
-      <c r="F10" s="86" t="s">
+      <c r="F10" s="93" t="s">
         <v>127</v>
       </c>
       <c r="G10" s="9" t="s">
@@ -6914,9 +7180,9 @@
       <c r="C11" t="s">
         <v>274</v>
       </c>
-      <c r="D11" s="90"/>
-      <c r="E11" s="90"/>
-      <c r="F11" s="87"/>
+      <c r="D11" s="91"/>
+      <c r="E11" s="91"/>
+      <c r="F11" s="94"/>
       <c r="G11" s="9"/>
       <c r="H11" s="3"/>
       <c r="I11" s="1"/>
@@ -6932,9 +7198,9 @@
       <c r="C12" t="s">
         <v>275</v>
       </c>
-      <c r="D12" s="90"/>
-      <c r="E12" s="90"/>
-      <c r="F12" s="87"/>
+      <c r="D12" s="91"/>
+      <c r="E12" s="91"/>
+      <c r="F12" s="94"/>
       <c r="G12" s="9"/>
       <c r="H12" s="3"/>
       <c r="I12" s="1"/>
@@ -6953,9 +7219,9 @@
       <c r="C13" t="s">
         <v>267</v>
       </c>
-      <c r="D13" s="91"/>
-      <c r="E13" s="91"/>
-      <c r="F13" s="88"/>
+      <c r="D13" s="92"/>
+      <c r="E13" s="92"/>
+      <c r="F13" s="95"/>
       <c r="G13" s="9"/>
       <c r="H13" s="3"/>
       <c r="I13" s="1"/>
@@ -6974,10 +7240,10 @@
       <c r="B14" t="s">
         <v>276</v>
       </c>
-      <c r="D14" s="89">
+      <c r="D14" s="90">
         <v>4</v>
       </c>
-      <c r="E14" s="74" t="s">
+      <c r="E14" s="78" t="s">
         <v>128</v>
       </c>
       <c r="F14" s="6" t="s">
@@ -7005,8 +7271,8 @@
       <c r="C15" t="s">
         <v>277</v>
       </c>
-      <c r="D15" s="90"/>
-      <c r="E15" s="75"/>
+      <c r="D15" s="91"/>
+      <c r="E15" s="79"/>
       <c r="F15" s="6"/>
       <c r="G15" s="9"/>
       <c r="H15" s="31"/>
@@ -7023,8 +7289,8 @@
       <c r="B16" t="s">
         <v>244</v>
       </c>
-      <c r="D16" s="90"/>
-      <c r="E16" s="75"/>
+      <c r="D16" s="91"/>
+      <c r="E16" s="79"/>
       <c r="F16" s="6"/>
       <c r="G16" s="9"/>
       <c r="H16" s="31"/>
@@ -7038,8 +7304,8 @@
       <c r="P16" s="1"/>
     </row>
     <row r="17" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D17" s="91"/>
-      <c r="E17" s="76"/>
+      <c r="D17" s="92"/>
+      <c r="E17" s="80"/>
       <c r="F17" s="6"/>
       <c r="G17" s="9"/>
       <c r="H17" s="31"/>
@@ -7059,10 +7325,10 @@
       <c r="B18" t="s">
         <v>278</v>
       </c>
-      <c r="D18" s="89">
+      <c r="D18" s="90">
         <v>5</v>
       </c>
-      <c r="E18" s="74" t="s">
+      <c r="E18" s="78" t="s">
         <v>130</v>
       </c>
       <c r="F18" s="6" t="s">
@@ -7090,8 +7356,8 @@
       <c r="C19" t="s">
         <v>279</v>
       </c>
-      <c r="D19" s="90"/>
-      <c r="E19" s="75"/>
+      <c r="D19" s="91"/>
+      <c r="E19" s="79"/>
       <c r="F19" s="6"/>
       <c r="G19" s="9"/>
       <c r="H19" s="31"/>
@@ -7108,8 +7374,8 @@
       <c r="C20" t="s">
         <v>280</v>
       </c>
-      <c r="D20" s="90"/>
-      <c r="E20" s="75"/>
+      <c r="D20" s="91"/>
+      <c r="E20" s="79"/>
       <c r="F20" s="6"/>
       <c r="G20" s="9"/>
       <c r="H20" s="31"/>
@@ -7126,8 +7392,8 @@
       <c r="C21" t="s">
         <v>282</v>
       </c>
-      <c r="D21" s="90"/>
-      <c r="E21" s="75"/>
+      <c r="D21" s="91"/>
+      <c r="E21" s="79"/>
       <c r="F21" s="6"/>
       <c r="G21" s="9"/>
       <c r="H21" s="31"/>
@@ -7144,8 +7410,8 @@
       <c r="C22" t="s">
         <v>283</v>
       </c>
-      <c r="D22" s="90"/>
-      <c r="E22" s="75"/>
+      <c r="D22" s="91"/>
+      <c r="E22" s="79"/>
       <c r="F22" s="6"/>
       <c r="G22" s="9"/>
       <c r="H22" s="31"/>
@@ -7162,8 +7428,8 @@
       <c r="C23" t="s">
         <v>281</v>
       </c>
-      <c r="D23" s="90"/>
-      <c r="E23" s="75"/>
+      <c r="D23" s="91"/>
+      <c r="E23" s="79"/>
       <c r="F23" s="6"/>
       <c r="G23" s="9"/>
       <c r="H23" s="31"/>
@@ -7183,8 +7449,8 @@
       <c r="C24" t="s">
         <v>284</v>
       </c>
-      <c r="D24" s="90"/>
-      <c r="E24" s="75"/>
+      <c r="D24" s="91"/>
+      <c r="E24" s="79"/>
       <c r="F24" s="6"/>
       <c r="G24" s="9"/>
       <c r="H24" s="31"/>
@@ -7201,8 +7467,8 @@
       <c r="C25" t="s">
         <v>285</v>
       </c>
-      <c r="D25" s="91"/>
-      <c r="E25" s="76"/>
+      <c r="D25" s="92"/>
+      <c r="E25" s="80"/>
       <c r="F25" s="6"/>
       <c r="G25" s="9"/>
       <c r="H25" s="31"/>
@@ -7222,10 +7488,10 @@
       <c r="B26" t="s">
         <v>286</v>
       </c>
-      <c r="D26" s="89">
+      <c r="D26" s="90">
         <v>6</v>
       </c>
-      <c r="E26" s="74" t="s">
+      <c r="E26" s="78" t="s">
         <v>132</v>
       </c>
       <c r="F26" s="6" t="s">
@@ -7253,8 +7519,8 @@
       <c r="C27" t="s">
         <v>287</v>
       </c>
-      <c r="D27" s="90"/>
-      <c r="E27" s="75"/>
+      <c r="D27" s="91"/>
+      <c r="E27" s="79"/>
       <c r="F27" s="6"/>
       <c r="G27" s="9"/>
       <c r="H27" s="31"/>
@@ -7271,8 +7537,8 @@
       <c r="C28" t="s">
         <v>288</v>
       </c>
-      <c r="D28" s="90"/>
-      <c r="E28" s="75"/>
+      <c r="D28" s="91"/>
+      <c r="E28" s="79"/>
       <c r="F28" s="6"/>
       <c r="G28" s="9"/>
       <c r="H28" s="31"/>
@@ -7292,8 +7558,8 @@
       <c r="C29" t="s">
         <v>289</v>
       </c>
-      <c r="D29" s="91"/>
-      <c r="E29" s="76"/>
+      <c r="D29" s="92"/>
+      <c r="E29" s="80"/>
       <c r="F29" s="6"/>
       <c r="G29" s="9"/>
       <c r="H29" s="31"/>
@@ -7313,10 +7579,10 @@
       <c r="B30" t="s">
         <v>290</v>
       </c>
-      <c r="D30" s="74">
+      <c r="D30" s="78">
         <v>7</v>
       </c>
-      <c r="E30" s="74" t="s">
+      <c r="E30" s="78" t="s">
         <v>134</v>
       </c>
       <c r="F30" s="5" t="s">
@@ -7342,8 +7608,8 @@
       <c r="C31" t="s">
         <v>291</v>
       </c>
-      <c r="D31" s="75"/>
-      <c r="E31" s="75"/>
+      <c r="D31" s="79"/>
+      <c r="E31" s="79"/>
       <c r="F31" s="5"/>
       <c r="G31" s="1"/>
       <c r="H31" s="31"/>
@@ -7360,8 +7626,8 @@
       <c r="C32" t="s">
         <v>292</v>
       </c>
-      <c r="D32" s="75"/>
-      <c r="E32" s="75"/>
+      <c r="D32" s="79"/>
+      <c r="E32" s="79"/>
       <c r="F32" s="5"/>
       <c r="G32" s="1"/>
       <c r="H32" s="31"/>
@@ -7381,8 +7647,8 @@
       <c r="C33" t="s">
         <v>293</v>
       </c>
-      <c r="D33" s="76"/>
-      <c r="E33" s="76"/>
+      <c r="D33" s="80"/>
+      <c r="E33" s="80"/>
       <c r="F33" s="5"/>
       <c r="G33" s="1"/>
       <c r="H33" s="31"/>
@@ -7402,10 +7668,10 @@
       <c r="B34" t="s">
         <v>331</v>
       </c>
-      <c r="D34" s="74">
+      <c r="D34" s="78">
         <v>8</v>
       </c>
-      <c r="E34" s="74" t="s">
+      <c r="E34" s="78" t="s">
         <v>136</v>
       </c>
       <c r="F34" s="5" t="s">
@@ -7433,8 +7699,8 @@
       <c r="C35" t="s">
         <v>294</v>
       </c>
-      <c r="D35" s="75"/>
-      <c r="E35" s="75"/>
+      <c r="D35" s="79"/>
+      <c r="E35" s="79"/>
       <c r="F35" s="5"/>
       <c r="G35" s="9"/>
       <c r="H35" s="31"/>
@@ -7451,8 +7717,8 @@
       <c r="C36" t="s">
         <v>330</v>
       </c>
-      <c r="D36" s="75"/>
-      <c r="E36" s="75"/>
+      <c r="D36" s="79"/>
+      <c r="E36" s="79"/>
       <c r="F36" s="5"/>
       <c r="G36" s="9"/>
       <c r="H36" s="31"/>
@@ -7472,8 +7738,8 @@
       <c r="C37" t="s">
         <v>295</v>
       </c>
-      <c r="D37" s="75"/>
-      <c r="E37" s="75"/>
+      <c r="D37" s="79"/>
+      <c r="E37" s="79"/>
       <c r="F37" s="5"/>
       <c r="G37" s="9"/>
       <c r="H37" s="31"/>
@@ -7490,8 +7756,8 @@
       <c r="C38" t="s">
         <v>297</v>
       </c>
-      <c r="D38" s="75"/>
-      <c r="E38" s="75"/>
+      <c r="D38" s="79"/>
+      <c r="E38" s="79"/>
       <c r="F38" s="5"/>
       <c r="G38" s="9"/>
       <c r="H38" s="31"/>
@@ -7508,8 +7774,8 @@
       <c r="C39" t="s">
         <v>296</v>
       </c>
-      <c r="D39" s="76"/>
-      <c r="E39" s="76"/>
+      <c r="D39" s="80"/>
+      <c r="E39" s="80"/>
       <c r="F39" s="5"/>
       <c r="G39" s="9"/>
       <c r="H39" s="31"/>
@@ -7529,10 +7795,10 @@
       <c r="B40" t="s">
         <v>299</v>
       </c>
-      <c r="D40" s="89">
+      <c r="D40" s="90">
         <v>9</v>
       </c>
-      <c r="E40" s="89" t="s">
+      <c r="E40" s="90" t="s">
         <v>138</v>
       </c>
       <c r="F40" s="1" t="s">
@@ -7560,8 +7826,8 @@
       <c r="C41" t="s">
         <v>300</v>
       </c>
-      <c r="D41" s="90"/>
-      <c r="E41" s="90"/>
+      <c r="D41" s="91"/>
+      <c r="E41" s="91"/>
       <c r="F41" s="1"/>
       <c r="G41" s="9"/>
       <c r="H41" s="34"/>
@@ -7581,8 +7847,8 @@
       <c r="C42" t="s">
         <v>298</v>
       </c>
-      <c r="D42" s="91"/>
-      <c r="E42" s="91"/>
+      <c r="D42" s="92"/>
+      <c r="E42" s="92"/>
       <c r="F42" s="1"/>
       <c r="G42" s="9"/>
       <c r="H42" s="34"/>
@@ -7602,10 +7868,10 @@
       <c r="B43" t="s">
         <v>301</v>
       </c>
-      <c r="D43" s="89">
+      <c r="D43" s="90">
         <v>10</v>
       </c>
-      <c r="E43" s="74" t="s">
+      <c r="E43" s="78" t="s">
         <v>139</v>
       </c>
       <c r="F43" s="6" t="s">
@@ -7633,8 +7899,8 @@
       <c r="C44" t="s">
         <v>302</v>
       </c>
-      <c r="D44" s="90"/>
-      <c r="E44" s="75"/>
+      <c r="D44" s="91"/>
+      <c r="E44" s="79"/>
       <c r="F44" s="6"/>
       <c r="G44" s="9"/>
       <c r="H44" s="34"/>
@@ -7651,8 +7917,8 @@
       <c r="C45" t="s">
         <v>303</v>
       </c>
-      <c r="D45" s="90"/>
-      <c r="E45" s="75"/>
+      <c r="D45" s="91"/>
+      <c r="E45" s="79"/>
       <c r="F45" s="6"/>
       <c r="G45" s="9"/>
       <c r="H45" s="34"/>
@@ -7672,8 +7938,8 @@
       <c r="C46" t="s">
         <v>304</v>
       </c>
-      <c r="D46" s="90"/>
-      <c r="E46" s="75"/>
+      <c r="D46" s="91"/>
+      <c r="E46" s="79"/>
       <c r="F46" s="6"/>
       <c r="G46" s="9"/>
       <c r="H46" s="34"/>
@@ -7690,8 +7956,8 @@
       <c r="C47" t="s">
         <v>298</v>
       </c>
-      <c r="D47" s="91"/>
-      <c r="E47" s="76"/>
+      <c r="D47" s="92"/>
+      <c r="E47" s="80"/>
       <c r="F47" s="6"/>
       <c r="G47" s="9"/>
       <c r="H47" s="34"/>
@@ -7711,10 +7977,10 @@
       <c r="B48" t="s">
         <v>305</v>
       </c>
-      <c r="D48" s="89">
+      <c r="D48" s="90">
         <v>11</v>
       </c>
-      <c r="E48" s="89" t="s">
+      <c r="E48" s="90" t="s">
         <v>141</v>
       </c>
       <c r="F48" s="4" t="s">
@@ -7742,8 +8008,8 @@
       <c r="C49" t="s">
         <v>306</v>
       </c>
-      <c r="D49" s="90"/>
-      <c r="E49" s="90"/>
+      <c r="D49" s="91"/>
+      <c r="E49" s="91"/>
       <c r="F49" s="4"/>
       <c r="G49" s="9"/>
       <c r="H49" s="31"/>
@@ -7760,8 +8026,8 @@
       <c r="C50" t="s">
         <v>307</v>
       </c>
-      <c r="D50" s="90"/>
-      <c r="E50" s="90"/>
+      <c r="D50" s="91"/>
+      <c r="E50" s="91"/>
       <c r="F50" s="4"/>
       <c r="G50" s="9"/>
       <c r="H50" s="31"/>
@@ -7781,8 +8047,8 @@
       <c r="C51" t="s">
         <v>308</v>
       </c>
-      <c r="D51" s="91"/>
-      <c r="E51" s="91"/>
+      <c r="D51" s="92"/>
+      <c r="E51" s="92"/>
       <c r="F51" s="4"/>
       <c r="G51" s="9"/>
       <c r="H51" s="31"/>
@@ -7802,10 +8068,10 @@
       <c r="B52" t="s">
         <v>309</v>
       </c>
-      <c r="D52" s="89">
+      <c r="D52" s="90">
         <v>12</v>
       </c>
-      <c r="E52" s="89" t="s">
+      <c r="E52" s="90" t="s">
         <v>143</v>
       </c>
       <c r="F52" s="1" t="s">
@@ -7833,8 +8099,8 @@
       <c r="C53" t="s">
         <v>310</v>
       </c>
-      <c r="D53" s="90"/>
-      <c r="E53" s="90"/>
+      <c r="D53" s="91"/>
+      <c r="E53" s="91"/>
       <c r="F53" s="1"/>
       <c r="G53" s="9"/>
       <c r="H53" s="31"/>
@@ -7851,8 +8117,8 @@
       <c r="C54" t="s">
         <v>311</v>
       </c>
-      <c r="D54" s="90"/>
-      <c r="E54" s="90"/>
+      <c r="D54" s="91"/>
+      <c r="E54" s="91"/>
       <c r="F54" s="1"/>
       <c r="G54" s="9"/>
       <c r="H54" s="31"/>
@@ -7872,8 +8138,8 @@
       <c r="C55" t="s">
         <v>312</v>
       </c>
-      <c r="D55" s="90"/>
-      <c r="E55" s="90"/>
+      <c r="D55" s="91"/>
+      <c r="E55" s="91"/>
       <c r="F55" s="1"/>
       <c r="G55" s="9"/>
       <c r="H55" s="31"/>
@@ -7893,10 +8159,10 @@
       <c r="B56" t="s">
         <v>332</v>
       </c>
-      <c r="D56" s="89">
+      <c r="D56" s="90">
         <v>13</v>
       </c>
-      <c r="E56" s="74" t="s">
+      <c r="E56" s="78" t="s">
         <v>145</v>
       </c>
       <c r="F56" s="5" t="s">
@@ -7921,8 +8187,8 @@
       <c r="B57" t="s">
         <v>213</v>
       </c>
-      <c r="D57" s="90"/>
-      <c r="E57" s="75"/>
+      <c r="D57" s="91"/>
+      <c r="E57" s="79"/>
       <c r="F57" s="5"/>
       <c r="G57" s="9"/>
       <c r="H57" s="31"/>
@@ -7939,8 +8205,8 @@
       <c r="B58" t="s">
         <v>244</v>
       </c>
-      <c r="D58" s="91"/>
-      <c r="E58" s="76"/>
+      <c r="D58" s="92"/>
+      <c r="E58" s="80"/>
       <c r="F58" s="5"/>
       <c r="G58" s="9"/>
       <c r="H58" s="31"/>
@@ -7960,10 +8226,10 @@
       <c r="B59" t="s">
         <v>313</v>
       </c>
-      <c r="D59" s="89">
+      <c r="D59" s="90">
         <v>14</v>
       </c>
-      <c r="E59" s="74" t="s">
+      <c r="E59" s="78" t="s">
         <v>146</v>
       </c>
       <c r="F59" s="6" t="s">
@@ -7991,8 +8257,8 @@
       <c r="C60" t="s">
         <v>314</v>
       </c>
-      <c r="D60" s="90"/>
-      <c r="E60" s="75"/>
+      <c r="D60" s="91"/>
+      <c r="E60" s="79"/>
       <c r="F60" s="6"/>
       <c r="G60" s="9"/>
       <c r="H60" s="31"/>
@@ -8009,8 +8275,8 @@
       <c r="C61" t="s">
         <v>315</v>
       </c>
-      <c r="D61" s="90"/>
-      <c r="E61" s="75"/>
+      <c r="D61" s="91"/>
+      <c r="E61" s="79"/>
       <c r="F61" s="6"/>
       <c r="G61" s="9"/>
       <c r="H61" s="31"/>
@@ -8030,8 +8296,8 @@
       <c r="C62" t="s">
         <v>316</v>
       </c>
-      <c r="D62" s="91"/>
-      <c r="E62" s="76"/>
+      <c r="D62" s="92"/>
+      <c r="E62" s="80"/>
       <c r="F62" s="6"/>
       <c r="G62" s="9"/>
       <c r="H62" s="31"/>
@@ -8051,10 +8317,10 @@
       <c r="B63" t="s">
         <v>317</v>
       </c>
-      <c r="D63" s="89">
+      <c r="D63" s="90">
         <v>15</v>
       </c>
-      <c r="E63" s="74" t="s">
+      <c r="E63" s="78" t="s">
         <v>149</v>
       </c>
       <c r="F63" s="5" t="s">
@@ -8082,8 +8348,8 @@
       <c r="C64" t="s">
         <v>318</v>
       </c>
-      <c r="D64" s="90"/>
-      <c r="E64" s="75"/>
+      <c r="D64" s="91"/>
+      <c r="E64" s="79"/>
       <c r="F64" s="5"/>
       <c r="G64" s="9"/>
       <c r="H64" s="31"/>
@@ -8100,8 +8366,8 @@
       <c r="C65" t="s">
         <v>319</v>
       </c>
-      <c r="D65" s="90"/>
-      <c r="E65" s="75"/>
+      <c r="D65" s="91"/>
+      <c r="E65" s="79"/>
       <c r="F65" s="5"/>
       <c r="G65" s="9"/>
       <c r="H65" s="31"/>
@@ -8121,8 +8387,8 @@
       <c r="C66" t="s">
         <v>320</v>
       </c>
-      <c r="D66" s="90"/>
-      <c r="E66" s="76"/>
+      <c r="D66" s="91"/>
+      <c r="E66" s="80"/>
       <c r="F66" s="5"/>
       <c r="G66" s="9"/>
       <c r="H66" s="31"/>
@@ -8145,7 +8411,7 @@
       <c r="D67" s="32">
         <v>16</v>
       </c>
-      <c r="E67" s="74" t="s">
+      <c r="E67" s="78" t="s">
         <v>150</v>
       </c>
       <c r="F67" s="6" t="s">
@@ -8174,7 +8440,7 @@
         <v>322</v>
       </c>
       <c r="D68" s="32"/>
-      <c r="E68" s="75"/>
+      <c r="E68" s="79"/>
       <c r="F68" s="6"/>
       <c r="G68" s="9"/>
       <c r="H68" s="31"/>
@@ -8195,7 +8461,7 @@
         <v>323</v>
       </c>
       <c r="D69" s="32"/>
-      <c r="E69" s="75"/>
+      <c r="E69" s="79"/>
       <c r="F69" s="6"/>
       <c r="G69" s="9"/>
       <c r="H69" s="31"/>
@@ -8213,7 +8479,7 @@
         <v>324</v>
       </c>
       <c r="D70" s="32"/>
-      <c r="E70" s="76"/>
+      <c r="E70" s="80"/>
       <c r="F70" s="6"/>
       <c r="G70" s="9"/>
       <c r="H70" s="31"/>
@@ -8233,10 +8499,10 @@
       <c r="B71" t="s">
         <v>334</v>
       </c>
-      <c r="D71" s="74">
+      <c r="D71" s="78">
         <v>17</v>
       </c>
-      <c r="E71" s="74" t="s">
+      <c r="E71" s="78" t="s">
         <v>152</v>
       </c>
       <c r="F71" s="5" t="s">
@@ -8264,8 +8530,8 @@
       <c r="C72" t="s">
         <v>325</v>
       </c>
-      <c r="D72" s="75"/>
-      <c r="E72" s="75"/>
+      <c r="D72" s="79"/>
+      <c r="E72" s="79"/>
       <c r="F72" s="5"/>
       <c r="G72" s="9"/>
       <c r="H72" s="31"/>
@@ -8285,8 +8551,8 @@
       <c r="C73" t="s">
         <v>327</v>
       </c>
-      <c r="D73" s="76"/>
-      <c r="E73" s="76"/>
+      <c r="D73" s="80"/>
+      <c r="E73" s="80"/>
       <c r="F73" s="5"/>
       <c r="G73" s="9"/>
       <c r="H73" s="31"/>
@@ -8348,31 +8614,6 @@
     </row>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="D59:D62"/>
-    <mergeCell ref="E59:E62"/>
-    <mergeCell ref="E71:E73"/>
-    <mergeCell ref="D71:D73"/>
-    <mergeCell ref="D63:D66"/>
-    <mergeCell ref="E63:E66"/>
-    <mergeCell ref="E67:E70"/>
-    <mergeCell ref="D56:D58"/>
-    <mergeCell ref="E56:E58"/>
-    <mergeCell ref="D52:D55"/>
-    <mergeCell ref="E52:E55"/>
-    <mergeCell ref="D48:D51"/>
-    <mergeCell ref="E48:E51"/>
-    <mergeCell ref="D43:D47"/>
-    <mergeCell ref="E43:E47"/>
-    <mergeCell ref="D40:D42"/>
-    <mergeCell ref="E40:E42"/>
-    <mergeCell ref="D34:D39"/>
-    <mergeCell ref="E34:E39"/>
-    <mergeCell ref="D30:D33"/>
-    <mergeCell ref="E30:E33"/>
-    <mergeCell ref="D26:D29"/>
-    <mergeCell ref="E26:E29"/>
-    <mergeCell ref="D18:D25"/>
-    <mergeCell ref="E18:E25"/>
     <mergeCell ref="F10:F13"/>
     <mergeCell ref="D2:D5"/>
     <mergeCell ref="E2:E5"/>
@@ -8382,6 +8623,31 @@
     <mergeCell ref="E10:E13"/>
     <mergeCell ref="D6:D9"/>
     <mergeCell ref="E6:E9"/>
+    <mergeCell ref="D30:D33"/>
+    <mergeCell ref="E30:E33"/>
+    <mergeCell ref="D26:D29"/>
+    <mergeCell ref="E26:E29"/>
+    <mergeCell ref="D18:D25"/>
+    <mergeCell ref="E18:E25"/>
+    <mergeCell ref="D43:D47"/>
+    <mergeCell ref="E43:E47"/>
+    <mergeCell ref="D40:D42"/>
+    <mergeCell ref="E40:E42"/>
+    <mergeCell ref="D34:D39"/>
+    <mergeCell ref="E34:E39"/>
+    <mergeCell ref="D56:D58"/>
+    <mergeCell ref="E56:E58"/>
+    <mergeCell ref="D52:D55"/>
+    <mergeCell ref="E52:E55"/>
+    <mergeCell ref="D48:D51"/>
+    <mergeCell ref="E48:E51"/>
+    <mergeCell ref="D59:D62"/>
+    <mergeCell ref="E59:E62"/>
+    <mergeCell ref="E71:E73"/>
+    <mergeCell ref="D71:D73"/>
+    <mergeCell ref="D63:D66"/>
+    <mergeCell ref="E63:E66"/>
+    <mergeCell ref="E67:E70"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="G2" r:id="rId1" xr:uid="{BD266EE8-9EE9-410E-A73B-7BCBE7209954}"/>
@@ -8408,10 +8674,11 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A3AF180-2B8D-4C19-A7E4-B0AE9B7543FC}">
+  <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:N17"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8452,16 +8719,16 @@
       <c r="B2" t="s">
         <v>336</v>
       </c>
-      <c r="E2" s="74">
+      <c r="E2" s="78">
         <v>1</v>
       </c>
-      <c r="F2" s="74" t="s">
+      <c r="F2" s="78" t="s">
         <v>171</v>
       </c>
-      <c r="G2" s="68" t="s">
+      <c r="G2" s="65" t="s">
         <v>174</v>
       </c>
-      <c r="H2" s="79" t="s">
+      <c r="H2" s="81" t="s">
         <v>175</v>
       </c>
     </row>
@@ -8476,10 +8743,10 @@
       <c r="D3" t="s">
         <v>346</v>
       </c>
-      <c r="E3" s="75"/>
-      <c r="F3" s="75"/>
-      <c r="G3" s="69"/>
-      <c r="H3" s="80"/>
+      <c r="E3" s="79"/>
+      <c r="F3" s="79"/>
+      <c r="G3" s="66"/>
+      <c r="H3" s="82"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="42"/>
@@ -8490,10 +8757,10 @@
       <c r="D4" t="s">
         <v>345</v>
       </c>
-      <c r="E4" s="75"/>
-      <c r="F4" s="75"/>
-      <c r="G4" s="69"/>
-      <c r="H4" s="80"/>
+      <c r="E4" s="79"/>
+      <c r="F4" s="79"/>
+      <c r="G4" s="66"/>
+      <c r="H4" s="82"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="42"/>
@@ -8504,10 +8771,10 @@
       <c r="D5" t="s">
         <v>344</v>
       </c>
-      <c r="E5" s="76"/>
-      <c r="F5" s="76"/>
-      <c r="G5" s="70"/>
-      <c r="H5" s="81"/>
+      <c r="E5" s="80"/>
+      <c r="F5" s="80"/>
+      <c r="G5" s="67"/>
+      <c r="H5" s="83"/>
     </row>
     <row r="6" spans="1:14" ht="180" x14ac:dyDescent="0.25">
       <c r="A6" s="42" t="s">
@@ -8632,10 +8899,11 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F79DFAC0-397F-4C98-B2DF-6497ADE191DD}">
+  <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8771,9 +9039,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83D713CF-1264-4070-BA73-824C7A1D0A05}">
+  <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:N53"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="83" workbookViewId="0">
+    <sheetView topLeftCell="A10" zoomScale="83" workbookViewId="0">
       <selection activeCell="E49" sqref="E49"/>
     </sheetView>
   </sheetViews>
@@ -8815,13 +9084,13 @@
       <c r="B2" t="s">
         <v>355</v>
       </c>
-      <c r="F2" s="74">
+      <c r="F2" s="78">
         <v>1</v>
       </c>
-      <c r="G2" s="74" t="s">
+      <c r="G2" s="78" t="s">
         <v>189</v>
       </c>
-      <c r="H2" s="68" t="s">
+      <c r="H2" s="65" t="s">
         <v>190</v>
       </c>
       <c r="I2" s="37" t="s">
@@ -8840,9 +9109,9 @@
       <c r="C3" t="s">
         <v>357</v>
       </c>
-      <c r="F3" s="75"/>
-      <c r="G3" s="75"/>
-      <c r="H3" s="69"/>
+      <c r="F3" s="79"/>
+      <c r="G3" s="79"/>
+      <c r="H3" s="66"/>
       <c r="I3" s="37"/>
       <c r="J3" s="14"/>
       <c r="K3" s="14"/>
@@ -8857,9 +9126,9 @@
       <c r="C4" t="s">
         <v>359</v>
       </c>
-      <c r="F4" s="76"/>
-      <c r="G4" s="76"/>
-      <c r="H4" s="70"/>
+      <c r="F4" s="80"/>
+      <c r="G4" s="80"/>
+      <c r="H4" s="67"/>
       <c r="I4" s="37"/>
       <c r="J4" s="14"/>
       <c r="K4" s="14"/>
@@ -8871,13 +9140,13 @@
       <c r="B5" t="s">
         <v>360</v>
       </c>
-      <c r="F5" s="74">
+      <c r="F5" s="78">
         <v>2</v>
       </c>
-      <c r="G5" s="74" t="s">
+      <c r="G5" s="78" t="s">
         <v>191</v>
       </c>
-      <c r="H5" s="94" t="s">
+      <c r="H5" s="96" t="s">
         <v>369</v>
       </c>
       <c r="I5" s="41" t="s">
@@ -8896,9 +9165,9 @@
       <c r="C6" t="s">
         <v>362</v>
       </c>
-      <c r="F6" s="75"/>
-      <c r="G6" s="75"/>
-      <c r="H6" s="95"/>
+      <c r="F6" s="79"/>
+      <c r="G6" s="79"/>
+      <c r="H6" s="97"/>
       <c r="I6" s="41"/>
       <c r="J6" s="14"/>
       <c r="K6" s="14"/>
@@ -8913,9 +9182,9 @@
       <c r="C7" t="s">
         <v>364</v>
       </c>
-      <c r="F7" s="75"/>
-      <c r="G7" s="75"/>
-      <c r="H7" s="95"/>
+      <c r="F7" s="79"/>
+      <c r="G7" s="79"/>
+      <c r="H7" s="97"/>
       <c r="I7" s="41"/>
       <c r="J7" s="14"/>
       <c r="K7" s="14"/>
@@ -8930,9 +9199,9 @@
       <c r="C8" t="s">
         <v>368</v>
       </c>
-      <c r="F8" s="75"/>
-      <c r="G8" s="75"/>
-      <c r="H8" s="95"/>
+      <c r="F8" s="79"/>
+      <c r="G8" s="79"/>
+      <c r="H8" s="97"/>
       <c r="I8" s="41"/>
       <c r="J8" s="14"/>
       <c r="K8" s="14"/>
@@ -8947,9 +9216,9 @@
       <c r="C9" t="s">
         <v>366</v>
       </c>
-      <c r="F9" s="75"/>
-      <c r="G9" s="75"/>
-      <c r="H9" s="96"/>
+      <c r="F9" s="79"/>
+      <c r="G9" s="79"/>
+      <c r="H9" s="98"/>
       <c r="I9" s="41"/>
       <c r="J9" s="14"/>
       <c r="K9" s="14"/>
@@ -8966,8 +9235,8 @@
       </c>
       <c r="D10" s="47"/>
       <c r="E10" s="47"/>
-      <c r="F10" s="75"/>
-      <c r="G10" s="76"/>
+      <c r="F10" s="79"/>
+      <c r="G10" s="80"/>
       <c r="H10" s="3"/>
       <c r="I10" s="37" t="s">
         <v>203</v>
@@ -8979,20 +9248,20 @@
       <c r="N10" s="14"/>
     </row>
     <row r="11" spans="1:14" ht="45" x14ac:dyDescent="0.25">
-      <c r="B11" s="51" t="s">
+      <c r="B11" s="55" t="s">
         <v>192</v>
       </c>
       <c r="C11" t="s">
         <v>372</v>
       </c>
-      <c r="F11" s="75"/>
-      <c r="G11" s="74" t="s">
+      <c r="F11" s="79"/>
+      <c r="G11" s="78" t="s">
         <v>192</v>
       </c>
       <c r="H11" s="5" t="s">
         <v>195</v>
       </c>
-      <c r="I11" s="92" t="s">
+      <c r="I11" s="99" t="s">
         <v>205</v>
       </c>
       <c r="J11" s="14"/>
@@ -9002,14 +9271,14 @@
       <c r="N11" s="14"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B12" s="51"/>
+      <c r="B12" s="55"/>
       <c r="C12" t="s">
         <v>373</v>
       </c>
-      <c r="F12" s="75"/>
-      <c r="G12" s="75"/>
+      <c r="F12" s="79"/>
+      <c r="G12" s="79"/>
       <c r="H12" s="5"/>
-      <c r="I12" s="92"/>
+      <c r="I12" s="99"/>
       <c r="J12" s="14"/>
       <c r="K12" s="14"/>
       <c r="L12" s="14"/>
@@ -9021,10 +9290,10 @@
       <c r="C13" t="s">
         <v>387</v>
       </c>
-      <c r="F13" s="75"/>
-      <c r="G13" s="76"/>
+      <c r="F13" s="79"/>
+      <c r="G13" s="80"/>
       <c r="H13" s="5"/>
-      <c r="I13" s="92"/>
+      <c r="I13" s="99"/>
       <c r="J13" s="14"/>
       <c r="K13" s="14"/>
       <c r="L13" s="14"/>
@@ -9032,20 +9301,20 @@
       <c r="N13" s="14"/>
     </row>
     <row r="14" spans="1:14" ht="60" x14ac:dyDescent="0.25">
-      <c r="B14" s="51" t="s">
+      <c r="B14" s="55" t="s">
         <v>374</v>
       </c>
       <c r="C14" t="s">
         <v>376</v>
       </c>
-      <c r="F14" s="75"/>
-      <c r="G14" s="74" t="s">
+      <c r="F14" s="79"/>
+      <c r="G14" s="78" t="s">
         <v>193</v>
       </c>
       <c r="H14" s="5" t="s">
         <v>197</v>
       </c>
-      <c r="I14" s="93"/>
+      <c r="I14" s="100"/>
       <c r="J14" s="14"/>
       <c r="K14" s="14"/>
       <c r="L14" s="14"/>
@@ -9053,14 +9322,14 @@
       <c r="N14" s="14"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B15" s="51"/>
+      <c r="B15" s="55"/>
       <c r="C15" t="s">
         <v>378</v>
       </c>
-      <c r="F15" s="75"/>
-      <c r="G15" s="75"/>
+      <c r="F15" s="79"/>
+      <c r="G15" s="79"/>
       <c r="H15" s="5"/>
-      <c r="I15" s="93"/>
+      <c r="I15" s="100"/>
       <c r="J15" s="14"/>
       <c r="K15" s="14"/>
       <c r="L15" s="14"/>
@@ -9072,10 +9341,10 @@
       <c r="C16" t="s">
         <v>388</v>
       </c>
-      <c r="F16" s="75"/>
-      <c r="G16" s="76"/>
+      <c r="F16" s="79"/>
+      <c r="G16" s="80"/>
       <c r="H16" s="5"/>
-      <c r="I16" s="93"/>
+      <c r="I16" s="100"/>
       <c r="J16" s="14"/>
       <c r="K16" s="14"/>
       <c r="L16" s="14"/>
@@ -9083,20 +9352,20 @@
       <c r="N16" s="14"/>
     </row>
     <row r="17" spans="2:14" ht="75" x14ac:dyDescent="0.25">
-      <c r="B17" s="51" t="s">
+      <c r="B17" s="55" t="s">
         <v>194</v>
       </c>
       <c r="C17" t="s">
         <v>377</v>
       </c>
-      <c r="F17" s="75"/>
-      <c r="G17" s="74" t="s">
+      <c r="F17" s="79"/>
+      <c r="G17" s="78" t="s">
         <v>194</v>
       </c>
       <c r="H17" s="5" t="s">
         <v>196</v>
       </c>
-      <c r="I17" s="93"/>
+      <c r="I17" s="100"/>
       <c r="J17" s="14"/>
       <c r="K17" s="14"/>
       <c r="L17" s="14"/>
@@ -9104,12 +9373,12 @@
       <c r="N17" s="14"/>
     </row>
     <row r="18" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B18" s="51"/>
+      <c r="B18" s="55"/>
       <c r="C18" t="s">
         <v>379</v>
       </c>
-      <c r="F18" s="75"/>
-      <c r="G18" s="75"/>
+      <c r="F18" s="79"/>
+      <c r="G18" s="79"/>
       <c r="H18" s="5"/>
       <c r="I18" s="46"/>
       <c r="J18" s="14"/>
@@ -9123,8 +9392,8 @@
       <c r="C19" t="s">
         <v>389</v>
       </c>
-      <c r="F19" s="75"/>
-      <c r="G19" s="76"/>
+      <c r="F19" s="79"/>
+      <c r="G19" s="80"/>
       <c r="H19" s="5"/>
       <c r="I19" s="46"/>
       <c r="J19" s="14"/>
@@ -9143,11 +9412,11 @@
       <c r="D20" t="s">
         <v>383</v>
       </c>
-      <c r="F20" s="75"/>
-      <c r="G20" s="74" t="s">
+      <c r="F20" s="79"/>
+      <c r="G20" s="78" t="s">
         <v>375</v>
       </c>
-      <c r="H20" s="68" t="s">
+      <c r="H20" s="65" t="s">
         <v>198</v>
       </c>
       <c r="I20" s="37" t="s">
@@ -9167,9 +9436,9 @@
       <c r="D21" t="s">
         <v>384</v>
       </c>
-      <c r="F21" s="75"/>
-      <c r="G21" s="75"/>
-      <c r="H21" s="69"/>
+      <c r="F21" s="79"/>
+      <c r="G21" s="79"/>
+      <c r="H21" s="66"/>
       <c r="I21" s="37"/>
       <c r="J21" s="14"/>
       <c r="K21" s="14"/>
@@ -9185,9 +9454,9 @@
       <c r="D22" t="s">
         <v>386</v>
       </c>
-      <c r="F22" s="76"/>
-      <c r="G22" s="76"/>
-      <c r="H22" s="70"/>
+      <c r="F22" s="80"/>
+      <c r="G22" s="80"/>
+      <c r="H22" s="67"/>
       <c r="I22" s="37"/>
       <c r="J22" s="14"/>
       <c r="K22" s="14"/>
@@ -9202,13 +9471,13 @@
       <c r="C23" t="s">
         <v>390</v>
       </c>
-      <c r="F23" s="74">
+      <c r="F23" s="78">
         <v>3</v>
       </c>
-      <c r="G23" s="74" t="s">
+      <c r="G23" s="78" t="s">
         <v>199</v>
       </c>
-      <c r="H23" s="68" t="s">
+      <c r="H23" s="65" t="s">
         <v>400</v>
       </c>
       <c r="I23" s="41" t="s">
@@ -9227,9 +9496,9 @@
       <c r="D24" t="s">
         <v>403</v>
       </c>
-      <c r="F24" s="75"/>
-      <c r="G24" s="75"/>
-      <c r="H24" s="69"/>
+      <c r="F24" s="79"/>
+      <c r="G24" s="79"/>
+      <c r="H24" s="66"/>
       <c r="I24" s="41"/>
       <c r="J24" s="14"/>
       <c r="K24" s="14"/>
@@ -9241,9 +9510,9 @@
       <c r="D25" t="s">
         <v>404</v>
       </c>
-      <c r="F25" s="75"/>
-      <c r="G25" s="75"/>
-      <c r="H25" s="69"/>
+      <c r="F25" s="79"/>
+      <c r="G25" s="79"/>
+      <c r="H25" s="66"/>
       <c r="I25" s="41"/>
       <c r="J25" s="14"/>
       <c r="K25" s="14"/>
@@ -9255,9 +9524,9 @@
       <c r="D26" t="s">
         <v>405</v>
       </c>
-      <c r="F26" s="75"/>
-      <c r="G26" s="75"/>
-      <c r="H26" s="69"/>
+      <c r="F26" s="79"/>
+      <c r="G26" s="79"/>
+      <c r="H26" s="66"/>
       <c r="I26" s="41"/>
       <c r="J26" s="14"/>
       <c r="K26" s="14"/>
@@ -9272,9 +9541,9 @@
       <c r="D27" t="s">
         <v>406</v>
       </c>
-      <c r="F27" s="75"/>
-      <c r="G27" s="75"/>
-      <c r="H27" s="69"/>
+      <c r="F27" s="79"/>
+      <c r="G27" s="79"/>
+      <c r="H27" s="66"/>
       <c r="I27" s="41"/>
       <c r="J27" s="14"/>
       <c r="K27" s="14"/>
@@ -9286,9 +9555,9 @@
       <c r="D28" t="s">
         <v>407</v>
       </c>
-      <c r="F28" s="75"/>
-      <c r="G28" s="75"/>
-      <c r="H28" s="69"/>
+      <c r="F28" s="79"/>
+      <c r="G28" s="79"/>
+      <c r="H28" s="66"/>
       <c r="I28" s="41"/>
       <c r="J28" s="14"/>
       <c r="K28" s="14"/>
@@ -9303,9 +9572,9 @@
       <c r="E29" t="s">
         <v>409</v>
       </c>
-      <c r="F29" s="75"/>
-      <c r="G29" s="75"/>
-      <c r="H29" s="69"/>
+      <c r="F29" s="79"/>
+      <c r="G29" s="79"/>
+      <c r="H29" s="66"/>
       <c r="I29" s="41"/>
       <c r="J29" s="14"/>
       <c r="K29" s="14"/>
@@ -9320,9 +9589,9 @@
       <c r="E30" t="s">
         <v>411</v>
       </c>
-      <c r="F30" s="75"/>
-      <c r="G30" s="75"/>
-      <c r="H30" s="69"/>
+      <c r="F30" s="79"/>
+      <c r="G30" s="79"/>
+      <c r="H30" s="66"/>
       <c r="I30" s="41"/>
       <c r="J30" s="14"/>
       <c r="K30" s="14"/>
@@ -9337,9 +9606,9 @@
       <c r="D31" t="s">
         <v>423</v>
       </c>
-      <c r="F31" s="75"/>
-      <c r="G31" s="75"/>
-      <c r="H31" s="69"/>
+      <c r="F31" s="79"/>
+      <c r="G31" s="79"/>
+      <c r="H31" s="66"/>
       <c r="I31" s="41"/>
       <c r="J31" s="14"/>
       <c r="K31" s="14"/>
@@ -9352,9 +9621,9 @@
       <c r="D32" t="s">
         <v>425</v>
       </c>
-      <c r="F32" s="75"/>
-      <c r="G32" s="75"/>
-      <c r="H32" s="69"/>
+      <c r="F32" s="79"/>
+      <c r="G32" s="79"/>
+      <c r="H32" s="66"/>
       <c r="I32" s="41"/>
       <c r="J32" s="14"/>
       <c r="K32" s="14"/>
@@ -9369,9 +9638,9 @@
       <c r="D33" t="s">
         <v>424</v>
       </c>
-      <c r="F33" s="75"/>
-      <c r="G33" s="75"/>
-      <c r="H33" s="69"/>
+      <c r="F33" s="79"/>
+      <c r="G33" s="79"/>
+      <c r="H33" s="66"/>
       <c r="I33" s="41"/>
       <c r="J33" s="14"/>
       <c r="K33" s="14"/>
@@ -9383,9 +9652,9 @@
       <c r="D34" t="s">
         <v>413</v>
       </c>
-      <c r="F34" s="75"/>
-      <c r="G34" s="75"/>
-      <c r="H34" s="69"/>
+      <c r="F34" s="79"/>
+      <c r="G34" s="79"/>
+      <c r="H34" s="66"/>
       <c r="I34" s="41"/>
       <c r="J34" s="14"/>
       <c r="K34" s="14"/>
@@ -9400,9 +9669,9 @@
       <c r="D35" t="s">
         <v>415</v>
       </c>
-      <c r="F35" s="75"/>
-      <c r="G35" s="75"/>
-      <c r="H35" s="69"/>
+      <c r="F35" s="79"/>
+      <c r="G35" s="79"/>
+      <c r="H35" s="66"/>
       <c r="I35" s="41"/>
       <c r="J35" s="14"/>
       <c r="K35" s="14"/>
@@ -9414,9 +9683,9 @@
       <c r="D36" t="s">
         <v>421</v>
       </c>
-      <c r="F36" s="75"/>
-      <c r="G36" s="75"/>
-      <c r="H36" s="69"/>
+      <c r="F36" s="79"/>
+      <c r="G36" s="79"/>
+      <c r="H36" s="66"/>
       <c r="I36" s="41"/>
       <c r="J36" s="14"/>
       <c r="K36" s="14"/>
@@ -9431,9 +9700,9 @@
       <c r="D37" t="s">
         <v>417</v>
       </c>
-      <c r="F37" s="75"/>
-      <c r="G37" s="75"/>
-      <c r="H37" s="69"/>
+      <c r="F37" s="79"/>
+      <c r="G37" s="79"/>
+      <c r="H37" s="66"/>
       <c r="I37" s="41"/>
       <c r="J37" s="14"/>
       <c r="K37" s="14"/>
@@ -9445,9 +9714,9 @@
       <c r="D38" t="s">
         <v>418</v>
       </c>
-      <c r="F38" s="75"/>
-      <c r="G38" s="75"/>
-      <c r="H38" s="69"/>
+      <c r="F38" s="79"/>
+      <c r="G38" s="79"/>
+      <c r="H38" s="66"/>
       <c r="I38" s="41"/>
       <c r="J38" s="14"/>
       <c r="K38" s="14"/>
@@ -9462,9 +9731,9 @@
       <c r="D39" t="s">
         <v>420</v>
       </c>
-      <c r="F39" s="75"/>
-      <c r="G39" s="75"/>
-      <c r="H39" s="69"/>
+      <c r="F39" s="79"/>
+      <c r="G39" s="79"/>
+      <c r="H39" s="66"/>
       <c r="I39" s="41"/>
       <c r="J39" s="14"/>
       <c r="K39" s="14"/>
@@ -9476,9 +9745,9 @@
       <c r="D40" t="s">
         <v>421</v>
       </c>
-      <c r="F40" s="76"/>
-      <c r="G40" s="76"/>
-      <c r="H40" s="70"/>
+      <c r="F40" s="80"/>
+      <c r="G40" s="80"/>
+      <c r="H40" s="67"/>
       <c r="I40" s="41"/>
       <c r="J40" s="14"/>
       <c r="K40" s="14"/>
@@ -9518,16 +9787,16 @@
       <c r="C42" t="s">
         <v>394</v>
       </c>
-      <c r="F42" s="61">
+      <c r="F42" s="58">
         <v>5</v>
       </c>
-      <c r="G42" s="61" t="s">
+      <c r="G42" s="58" t="s">
         <v>206</v>
       </c>
       <c r="H42" s="5" t="s">
         <v>207</v>
       </c>
-      <c r="I42" s="65" t="s">
+      <c r="I42" s="62" t="s">
         <v>202</v>
       </c>
       <c r="J42" s="14"/>
@@ -9546,12 +9815,12 @@
       <c r="E43" t="s">
         <v>398</v>
       </c>
-      <c r="F43" s="61"/>
-      <c r="G43" s="61"/>
+      <c r="F43" s="58"/>
+      <c r="G43" s="58"/>
       <c r="H43" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="I43" s="66"/>
+      <c r="I43" s="63"/>
       <c r="J43" s="14"/>
       <c r="K43" s="14"/>
       <c r="L43" s="14"/>
@@ -9565,12 +9834,12 @@
       <c r="E44" t="s">
         <v>399</v>
       </c>
-      <c r="F44" s="61"/>
-      <c r="G44" s="61"/>
+      <c r="F44" s="58"/>
+      <c r="G44" s="58"/>
       <c r="H44" s="3" t="s">
         <v>209</v>
       </c>
-      <c r="I44" s="67"/>
+      <c r="I44" s="64"/>
       <c r="J44" s="14"/>
       <c r="K44" s="14"/>
       <c r="L44" s="14"/>
@@ -9615,19 +9884,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="F5:F22"/>
-    <mergeCell ref="G11:G13"/>
-    <mergeCell ref="G14:G16"/>
-    <mergeCell ref="G17:G19"/>
-    <mergeCell ref="G20:G22"/>
-    <mergeCell ref="F2:F4"/>
-    <mergeCell ref="G2:G4"/>
-    <mergeCell ref="H2:H4"/>
-    <mergeCell ref="H5:H9"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="G5:G10"/>
     <mergeCell ref="I11:I17"/>
     <mergeCell ref="G42:G44"/>
     <mergeCell ref="F42:F44"/>
@@ -9636,6 +9892,19 @@
     <mergeCell ref="F23:F40"/>
     <mergeCell ref="G23:G40"/>
     <mergeCell ref="H23:H40"/>
+    <mergeCell ref="F2:F4"/>
+    <mergeCell ref="G2:G4"/>
+    <mergeCell ref="H2:H4"/>
+    <mergeCell ref="H5:H9"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="G5:G10"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="F5:F22"/>
+    <mergeCell ref="G11:G13"/>
+    <mergeCell ref="G14:G16"/>
+    <mergeCell ref="G17:G19"/>
+    <mergeCell ref="G20:G22"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="I23" r:id="rId1" display="https://www.baeldung.com/spring-transactional-propagation-isolation" xr:uid="{48BFAE5D-1145-4E0D-A5BD-44A48408A956}"/>
@@ -9650,4 +9919,268 @@
   <pageSetup orientation="portrait" r:id="rId8"/>
   <drawing r:id="rId9"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCA47C9C-6F99-4F74-8F04-233056ABBE4B}">
+  <sheetPr codeName="Sheet9"/>
+  <dimension ref="A1:H39"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q21" sqref="Q21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="34.42578125" customWidth="1"/>
+    <col min="2" max="2" width="14" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="42" t="s">
+        <v>431</v>
+      </c>
+      <c r="B1" t="s">
+        <v>354</v>
+      </c>
+      <c r="H1" s="52" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="42" t="s">
+        <v>432</v>
+      </c>
+      <c r="B2" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="42" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>435</v>
+      </c>
+      <c r="C4" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>437</v>
+      </c>
+      <c r="C5" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>439</v>
+      </c>
+      <c r="E7" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
+        <v>444</v>
+      </c>
+      <c r="E8" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>443</v>
+      </c>
+      <c r="E9" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
+        <v>441</v>
+      </c>
+      <c r="E10" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
+        <v>442</v>
+      </c>
+      <c r="E11" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>446</v>
+      </c>
+      <c r="C12" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>448</v>
+      </c>
+      <c r="C13" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>450</v>
+      </c>
+      <c r="C16" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="42" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>457</v>
+      </c>
+      <c r="C18" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>458</v>
+      </c>
+      <c r="C19" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>461</v>
+      </c>
+      <c r="C22" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>463</v>
+      </c>
+      <c r="C25" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>464</v>
+      </c>
+      <c r="C26" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="52" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="52" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="52" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="52" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="52" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="52" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>474</v>
+      </c>
+      <c r="B38" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="52" t="s">
+        <v>473</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="H1" r:id="rId1" xr:uid="{FD790352-9AB3-438A-B805-4E38FEE8BA22}"/>
+    <hyperlink ref="A28" r:id="rId2" location="deeper-look-into-spring-aops-annotations" xr:uid="{78DCEF18-00D2-4EFA-B107-E7CA18D0D8FE}"/>
+    <hyperlink ref="A29" r:id="rId3" display="https://www.digitalocean.com/community/tutorials/spring-aop-example-tutorial-aspect-advice-pointcut-joinpoint-annotations" xr:uid="{BCFC0ACD-33E1-483E-9A2A-1F45EF2A9DA9}"/>
+    <hyperlink ref="A30" r:id="rId4" location=":~:text=Aspect%20Oriented%20Programming%20(AOP)%20l%C3%A0,tr%E1%BA%A3%20v%E1%BB%81%20m%E1%BB%99t%20k%E1%BA%BFt%20qu%E1%BA%A3" display="https://techmaster.vn/posts/36087/spring-core-phan-5-spring-aop-la-gi-code-vi-du-voi-spring-aop - :~:text=Aspect%20Oriented%20Programming%20(AOP)%20l%C3%A0,tr%E1%BA%A3%20v%E1%BB%81%20m%E1%BB%99t%20k%E1%BA%BFt%20qu%E1%BA%A3" xr:uid="{70145C8E-A03B-4CE2-A6DA-970F7CB3F0C9}"/>
+    <hyperlink ref="A31" r:id="rId5" display="https://viblo.asia/p/su-dung-aop-trong-spring-boot-va-aspectj-vyDZOkbaZwj" xr:uid="{E9ED52EB-6172-4E9F-A0BD-111D6CCA182F}"/>
+    <hyperlink ref="A32" r:id="rId6" display="https://gpcoder.com/5112-gioi-thieu-aspect-oriented-programming-aop/" xr:uid="{0F8D92B0-260D-4D69-9F99-EAD6314460DD}"/>
+    <hyperlink ref="A33" r:id="rId7" display="https://levunguyen.com/laptrinhspring/2020/04/27/su-dung-aop-advise-trong-spring/" xr:uid="{197D74B0-CBE3-492E-BB4F-8EEC42746249}"/>
+    <hyperlink ref="A39" r:id="rId8" xr:uid="{DEDB1230-9B57-4D7C-BF68-766DD4B6BEC4}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId9"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
cập nhật task trong file excel
</commit_message>
<xml_diff>
--- a/Task_Result.xlsx
+++ b/Task_Result.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\beetech\java\stage1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE7B8E33-F005-49D2-AC3E-9B4AE6CF7F2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C678C64-1690-414A-A666-9726405F2FEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="5" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="5" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="day2 " sheetId="1" r:id="rId1"/>
@@ -4882,6 +4882,27 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -4921,27 +4942,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4950,6 +4950,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -4969,22 +4975,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
@@ -4997,6 +4988,21 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
@@ -5004,12 +5010,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -6400,8 +6400,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9601CE73-AAA1-4817-B4FF-196A7817E766}">
   <dimension ref="A1:W137"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="C72" sqref="C72"/>
+    <sheetView topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="F49" sqref="F49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7379,7 +7379,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99F636C8-1563-4E93-9E63-868EB37CCEF7}">
   <dimension ref="A1:K38"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
@@ -7677,24 +7677,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:30" ht="49.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="79" t="s">
+      <c r="A1" s="66" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="80"/>
-      <c r="C1" s="80"/>
-      <c r="D1" s="80"/>
-      <c r="E1" s="80"/>
-      <c r="F1" s="80"/>
-      <c r="G1" s="80"/>
-      <c r="H1" s="80"/>
-      <c r="I1" s="80"/>
-      <c r="J1" s="80"/>
-      <c r="K1" s="80"/>
-      <c r="L1" s="80"/>
-      <c r="M1" s="80"/>
-      <c r="N1" s="80"/>
-      <c r="O1" s="80"/>
-      <c r="P1" s="80"/>
+      <c r="B1" s="67"/>
+      <c r="C1" s="67"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="67"/>
+      <c r="F1" s="67"/>
+      <c r="G1" s="67"/>
+      <c r="H1" s="67"/>
+      <c r="I1" s="67"/>
+      <c r="J1" s="67"/>
+      <c r="K1" s="67"/>
+      <c r="L1" s="67"/>
+      <c r="M1" s="67"/>
+      <c r="N1" s="67"/>
+      <c r="O1" s="67"/>
+      <c r="P1" s="67"/>
       <c r="Q1" s="39"/>
       <c r="R1" s="39"/>
       <c r="S1" s="39"/>
@@ -7786,16 +7786,16 @@
       <c r="P4" t="s">
         <v>214</v>
       </c>
-      <c r="AA4" s="70">
+      <c r="AA4" s="77">
         <v>3</v>
       </c>
-      <c r="AB4" s="70" t="s">
+      <c r="AB4" s="77" t="s">
         <v>35</v>
       </c>
-      <c r="AC4" s="73" t="s">
+      <c r="AC4" s="80" t="s">
         <v>38</v>
       </c>
-      <c r="AD4" s="76" t="s">
+      <c r="AD4" s="83" t="s">
         <v>32</v>
       </c>
     </row>
@@ -7807,10 +7807,10 @@
       <c r="P5" t="s">
         <v>215</v>
       </c>
-      <c r="AA5" s="71"/>
-      <c r="AB5" s="71"/>
-      <c r="AC5" s="74"/>
-      <c r="AD5" s="77"/>
+      <c r="AA5" s="78"/>
+      <c r="AB5" s="78"/>
+      <c r="AC5" s="81"/>
+      <c r="AD5" s="84"/>
     </row>
     <row r="6" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="14"/>
@@ -7823,10 +7823,10 @@
       <c r="P6" t="s">
         <v>217</v>
       </c>
-      <c r="AA6" s="72"/>
-      <c r="AB6" s="72"/>
-      <c r="AC6" s="75"/>
-      <c r="AD6" s="78"/>
+      <c r="AA6" s="79"/>
+      <c r="AB6" s="79"/>
+      <c r="AC6" s="82"/>
+      <c r="AD6" s="85"/>
     </row>
     <row r="7" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="14"/>
@@ -7839,16 +7839,16 @@
       <c r="P7" t="s">
         <v>218</v>
       </c>
-      <c r="AA7" s="70">
+      <c r="AA7" s="77">
         <v>4</v>
       </c>
-      <c r="AB7" s="70" t="s">
+      <c r="AB7" s="77" t="s">
         <v>36</v>
       </c>
-      <c r="AC7" s="73" t="s">
+      <c r="AC7" s="80" t="s">
         <v>39</v>
       </c>
-      <c r="AD7" s="76" t="s">
+      <c r="AD7" s="83" t="s">
         <v>40</v>
       </c>
     </row>
@@ -7860,10 +7860,10 @@
       <c r="P8" t="s">
         <v>219</v>
       </c>
-      <c r="AA8" s="71"/>
-      <c r="AB8" s="71"/>
-      <c r="AC8" s="74"/>
-      <c r="AD8" s="77"/>
+      <c r="AA8" s="78"/>
+      <c r="AB8" s="78"/>
+      <c r="AC8" s="81"/>
+      <c r="AD8" s="84"/>
     </row>
     <row r="9" spans="1:30" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="14"/>
@@ -7876,19 +7876,19 @@
       <c r="P9" t="s">
         <v>220</v>
       </c>
-      <c r="AA9" s="72"/>
-      <c r="AB9" s="72"/>
-      <c r="AC9" s="75"/>
-      <c r="AD9" s="78"/>
+      <c r="AA9" s="79"/>
+      <c r="AB9" s="79"/>
+      <c r="AC9" s="82"/>
+      <c r="AD9" s="85"/>
     </row>
     <row r="10" spans="1:30" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="81" t="s">
+      <c r="A10" s="68" t="s">
         <v>54</v>
       </c>
-      <c r="B10" s="82"/>
-      <c r="C10" s="82"/>
-      <c r="D10" s="82"/>
-      <c r="E10" s="82"/>
+      <c r="B10" s="69"/>
+      <c r="C10" s="69"/>
+      <c r="D10" s="69"/>
+      <c r="E10" s="69"/>
       <c r="F10" s="19"/>
       <c r="G10" s="19"/>
       <c r="H10" s="19"/>
@@ -7899,16 +7899,16 @@
       <c r="P10" t="s">
         <v>222</v>
       </c>
-      <c r="AA10" s="66">
+      <c r="AA10" s="73">
         <v>5</v>
       </c>
-      <c r="AB10" s="67" t="s">
+      <c r="AB10" s="74" t="s">
         <v>37</v>
       </c>
-      <c r="AC10" s="68" t="s">
+      <c r="AC10" s="75" t="s">
         <v>51</v>
       </c>
-      <c r="AD10" s="69" t="s">
+      <c r="AD10" s="76" t="s">
         <v>52</v>
       </c>
     </row>
@@ -7919,19 +7919,19 @@
       <c r="P11" t="s">
         <v>223</v>
       </c>
-      <c r="AA11" s="66"/>
-      <c r="AB11" s="67"/>
-      <c r="AC11" s="68"/>
-      <c r="AD11" s="69"/>
+      <c r="AA11" s="73"/>
+      <c r="AB11" s="74"/>
+      <c r="AC11" s="75"/>
+      <c r="AD11" s="76"/>
     </row>
     <row r="12" spans="1:30" x14ac:dyDescent="0.25">
       <c r="P12" t="s">
         <v>224</v>
       </c>
-      <c r="AA12" s="66"/>
-      <c r="AB12" s="67"/>
-      <c r="AC12" s="68"/>
-      <c r="AD12" s="69"/>
+      <c r="AA12" s="73"/>
+      <c r="AB12" s="74"/>
+      <c r="AC12" s="75"/>
+      <c r="AD12" s="76"/>
     </row>
     <row r="13" spans="1:30" x14ac:dyDescent="0.25">
       <c r="O13" t="s">
@@ -7940,10 +7940,10 @@
       <c r="P13" t="s">
         <v>225</v>
       </c>
-      <c r="AA13" s="66"/>
-      <c r="AB13" s="67"/>
-      <c r="AC13" s="68"/>
-      <c r="AD13" s="69"/>
+      <c r="AA13" s="73"/>
+      <c r="AB13" s="74"/>
+      <c r="AC13" s="75"/>
+      <c r="AD13" s="76"/>
     </row>
     <row r="14" spans="1:30" x14ac:dyDescent="0.25">
       <c r="N14" s="43" t="s">
@@ -7952,10 +7952,10 @@
       <c r="P14" t="s">
         <v>228</v>
       </c>
-      <c r="AA14" s="66"/>
-      <c r="AB14" s="67"/>
-      <c r="AC14" s="68"/>
-      <c r="AD14" s="69"/>
+      <c r="AA14" s="73"/>
+      <c r="AB14" s="74"/>
+      <c r="AC14" s="75"/>
+      <c r="AD14" s="76"/>
     </row>
     <row r="15" spans="1:30" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="40"/>
@@ -7973,10 +7973,10 @@
       <c r="P15" t="s">
         <v>227</v>
       </c>
-      <c r="AA15" s="66"/>
-      <c r="AB15" s="67"/>
-      <c r="AC15" s="68"/>
-      <c r="AD15" s="69"/>
+      <c r="AA15" s="73"/>
+      <c r="AB15" s="74"/>
+      <c r="AC15" s="75"/>
+      <c r="AD15" s="76"/>
     </row>
     <row r="16" spans="1:30" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="40"/>
@@ -7991,10 +7991,10 @@
       <c r="P16" t="s">
         <v>223</v>
       </c>
-      <c r="AA16" s="66"/>
-      <c r="AB16" s="67"/>
-      <c r="AC16" s="68"/>
-      <c r="AD16" s="69"/>
+      <c r="AA16" s="73"/>
+      <c r="AB16" s="74"/>
+      <c r="AC16" s="75"/>
+      <c r="AD16" s="76"/>
     </row>
     <row r="17" spans="1:30" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="40"/>
@@ -8009,10 +8009,10 @@
       <c r="P17" t="s">
         <v>224</v>
       </c>
-      <c r="AA17" s="66"/>
-      <c r="AB17" s="67"/>
-      <c r="AC17" s="68"/>
-      <c r="AD17" s="69"/>
+      <c r="AA17" s="73"/>
+      <c r="AB17" s="74"/>
+      <c r="AC17" s="75"/>
+      <c r="AD17" s="76"/>
     </row>
     <row r="18" spans="1:30" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="40"/>
@@ -8030,10 +8030,10 @@
       <c r="P18" t="s">
         <v>225</v>
       </c>
-      <c r="AA18" s="66"/>
-      <c r="AB18" s="67"/>
-      <c r="AC18" s="68"/>
-      <c r="AD18" s="69"/>
+      <c r="AA18" s="73"/>
+      <c r="AB18" s="74"/>
+      <c r="AC18" s="75"/>
+      <c r="AD18" s="76"/>
     </row>
     <row r="19" spans="1:30" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="40"/>
@@ -8051,10 +8051,10 @@
       <c r="P19" t="s">
         <v>230</v>
       </c>
-      <c r="AA19" s="66"/>
-      <c r="AB19" s="67"/>
-      <c r="AC19" s="68"/>
-      <c r="AD19" s="69"/>
+      <c r="AA19" s="73"/>
+      <c r="AB19" s="74"/>
+      <c r="AC19" s="75"/>
+      <c r="AD19" s="76"/>
     </row>
     <row r="20" spans="1:30" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="40"/>
@@ -8072,10 +8072,10 @@
       <c r="O20" t="s">
         <v>232</v>
       </c>
-      <c r="AA20" s="66"/>
-      <c r="AB20" s="67"/>
-      <c r="AC20" s="68"/>
-      <c r="AD20" s="69"/>
+      <c r="AA20" s="73"/>
+      <c r="AB20" s="74"/>
+      <c r="AC20" s="75"/>
+      <c r="AD20" s="76"/>
     </row>
     <row r="21" spans="1:30" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="40"/>
@@ -8093,10 +8093,10 @@
       <c r="P21" t="s">
         <v>233</v>
       </c>
-      <c r="AA21" s="66"/>
-      <c r="AB21" s="67"/>
-      <c r="AC21" s="68"/>
-      <c r="AD21" s="69"/>
+      <c r="AA21" s="73"/>
+      <c r="AB21" s="74"/>
+      <c r="AC21" s="75"/>
+      <c r="AD21" s="76"/>
     </row>
     <row r="22" spans="1:30" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="40"/>
@@ -8114,10 +8114,10 @@
       <c r="P22" t="s">
         <v>234</v>
       </c>
-      <c r="AA22" s="66"/>
-      <c r="AB22" s="67"/>
-      <c r="AC22" s="68"/>
-      <c r="AD22" s="69"/>
+      <c r="AA22" s="73"/>
+      <c r="AB22" s="74"/>
+      <c r="AC22" s="75"/>
+      <c r="AD22" s="76"/>
     </row>
     <row r="23" spans="1:30" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="40"/>
@@ -8135,10 +8135,10 @@
       <c r="O23" t="s">
         <v>236</v>
       </c>
-      <c r="AA23" s="66"/>
-      <c r="AB23" s="67"/>
-      <c r="AC23" s="68"/>
-      <c r="AD23" s="69"/>
+      <c r="AA23" s="73"/>
+      <c r="AB23" s="74"/>
+      <c r="AC23" s="75"/>
+      <c r="AD23" s="76"/>
     </row>
     <row r="24" spans="1:30" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="40"/>
@@ -8156,10 +8156,10 @@
       <c r="P24" t="s">
         <v>237</v>
       </c>
-      <c r="AA24" s="66"/>
-      <c r="AB24" s="67"/>
-      <c r="AC24" s="68"/>
-      <c r="AD24" s="69"/>
+      <c r="AA24" s="73"/>
+      <c r="AB24" s="74"/>
+      <c r="AC24" s="75"/>
+      <c r="AD24" s="76"/>
     </row>
     <row r="25" spans="1:30" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="40"/>
@@ -8177,10 +8177,10 @@
       <c r="P25" t="s">
         <v>238</v>
       </c>
-      <c r="AA25" s="66"/>
-      <c r="AB25" s="67"/>
-      <c r="AC25" s="68"/>
-      <c r="AD25" s="69"/>
+      <c r="AA25" s="73"/>
+      <c r="AB25" s="74"/>
+      <c r="AC25" s="75"/>
+      <c r="AD25" s="76"/>
     </row>
     <row r="26" spans="1:30" ht="108" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="65" t="s">
@@ -8263,38 +8263,38 @@
       <c r="AD27" s="1"/>
     </row>
     <row r="54" spans="1:10" ht="42" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="D54" s="85" t="s">
+      <c r="D54" s="72" t="s">
         <v>44</v>
       </c>
-      <c r="E54" s="85"/>
-      <c r="F54" s="85"/>
-      <c r="G54" s="85"/>
-      <c r="H54" s="85"/>
-      <c r="I54" s="85"/>
-      <c r="J54" s="85"/>
+      <c r="E54" s="72"/>
+      <c r="F54" s="72"/>
+      <c r="G54" s="72"/>
+      <c r="H54" s="72"/>
+      <c r="I54" s="72"/>
+      <c r="J54" s="72"/>
     </row>
     <row r="58" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A58" s="84" t="s">
+      <c r="A58" s="71" t="s">
         <v>41</v>
       </c>
-      <c r="B58" s="84"/>
-      <c r="C58" s="84"/>
+      <c r="B58" s="71"/>
+      <c r="C58" s="71"/>
       <c r="D58" s="20"/>
     </row>
     <row r="59" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="84"/>
-      <c r="B59" s="84"/>
-      <c r="C59" s="84"/>
+      <c r="A59" s="71"/>
+      <c r="B59" s="71"/>
+      <c r="C59" s="71"/>
     </row>
     <row r="60" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="84"/>
-      <c r="B60" s="84"/>
-      <c r="C60" s="84"/>
+      <c r="A60" s="71"/>
+      <c r="B60" s="71"/>
+      <c r="C60" s="71"/>
     </row>
     <row r="61" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="84"/>
-      <c r="B61" s="84"/>
-      <c r="C61" s="84"/>
+      <c r="A61" s="71"/>
+      <c r="B61" s="71"/>
+      <c r="C61" s="71"/>
     </row>
     <row r="62" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="65" t="s">
@@ -8309,32 +8309,24 @@
       <c r="C63" s="65"/>
     </row>
     <row r="87" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="83" t="s">
+      <c r="A87" s="70" t="s">
         <v>46</v>
       </c>
-      <c r="B87" s="83"/>
-      <c r="C87" s="83"/>
+      <c r="B87" s="70"/>
+      <c r="C87" s="70"/>
     </row>
     <row r="88" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="83"/>
-      <c r="B88" s="83"/>
-      <c r="C88" s="83"/>
+      <c r="A88" s="70"/>
+      <c r="B88" s="70"/>
+      <c r="C88" s="70"/>
     </row>
     <row r="89" spans="1:3" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="83"/>
-      <c r="B89" s="83"/>
-      <c r="C89" s="83"/>
+      <c r="A89" s="70"/>
+      <c r="B89" s="70"/>
+      <c r="C89" s="70"/>
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="A1:P1"/>
-    <mergeCell ref="A10:E10"/>
-    <mergeCell ref="A87:C89"/>
-    <mergeCell ref="A58:C61"/>
-    <mergeCell ref="A26:C27"/>
-    <mergeCell ref="A62:C63"/>
-    <mergeCell ref="D26:I27"/>
-    <mergeCell ref="D54:J54"/>
     <mergeCell ref="AA10:AA25"/>
     <mergeCell ref="AB10:AB25"/>
     <mergeCell ref="AC10:AC25"/>
@@ -8347,6 +8339,14 @@
     <mergeCell ref="AB7:AB9"/>
     <mergeCell ref="AC7:AC9"/>
     <mergeCell ref="AD7:AD9"/>
+    <mergeCell ref="A1:P1"/>
+    <mergeCell ref="A10:E10"/>
+    <mergeCell ref="A87:C89"/>
+    <mergeCell ref="A58:C61"/>
+    <mergeCell ref="A26:C27"/>
+    <mergeCell ref="A62:C63"/>
+    <mergeCell ref="D26:I27"/>
+    <mergeCell ref="D54:J54"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="AD2" r:id="rId1" display="https://stackoverflow.com/questions/15070513/how-to-test-a-non-thread-safe-class" xr:uid="{AF80577A-A125-48C9-AA50-5BBE662AA378}"/>
@@ -8415,10 +8415,10 @@
       <c r="H2" s="86" t="s">
         <v>56</v>
       </c>
-      <c r="I2" s="73" t="s">
+      <c r="I2" s="80" t="s">
         <v>57</v>
       </c>
-      <c r="J2" s="89" t="s">
+      <c r="J2" s="91" t="s">
         <v>58</v>
       </c>
       <c r="L2" s="65" t="s">
@@ -8445,8 +8445,8 @@
       </c>
       <c r="G3" s="87"/>
       <c r="H3" s="87"/>
-      <c r="I3" s="74"/>
-      <c r="J3" s="90"/>
+      <c r="I3" s="81"/>
+      <c r="J3" s="92"/>
       <c r="L3" s="38"/>
       <c r="M3" s="23"/>
       <c r="N3" s="23"/>
@@ -8469,8 +8469,8 @@
       </c>
       <c r="G4" s="87"/>
       <c r="H4" s="87"/>
-      <c r="I4" s="74"/>
-      <c r="J4" s="90"/>
+      <c r="I4" s="81"/>
+      <c r="J4" s="92"/>
       <c r="L4" s="38"/>
       <c r="M4" s="23"/>
       <c r="N4" s="23"/>
@@ -8490,8 +8490,8 @@
       </c>
       <c r="G5" s="88"/>
       <c r="H5" s="88"/>
-      <c r="I5" s="75"/>
-      <c r="J5" s="91"/>
+      <c r="I5" s="82"/>
+      <c r="J5" s="93"/>
       <c r="L5" s="38"/>
       <c r="M5" s="23"/>
       <c r="N5" s="23"/>
@@ -8518,10 +8518,10 @@
       <c r="H6" s="86" t="s">
         <v>59</v>
       </c>
-      <c r="I6" s="73" t="s">
+      <c r="I6" s="80" t="s">
         <v>60</v>
       </c>
-      <c r="J6" s="92" t="s">
+      <c r="J6" s="94" t="s">
         <v>72</v>
       </c>
       <c r="M6" s="26"/>
@@ -8535,8 +8535,8 @@
       </c>
       <c r="G7" s="87"/>
       <c r="H7" s="87"/>
-      <c r="I7" s="74"/>
-      <c r="J7" s="93"/>
+      <c r="I7" s="81"/>
+      <c r="J7" s="95"/>
       <c r="M7" s="26"/>
     </row>
     <row r="8" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -8545,8 +8545,8 @@
       </c>
       <c r="G8" s="87"/>
       <c r="H8" s="87"/>
-      <c r="I8" s="74"/>
-      <c r="J8" s="93"/>
+      <c r="I8" s="81"/>
+      <c r="J8" s="95"/>
       <c r="M8" s="26"/>
     </row>
     <row r="9" spans="1:23" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -8558,8 +8558,8 @@
       </c>
       <c r="G9" s="88"/>
       <c r="H9" s="88"/>
-      <c r="I9" s="75"/>
-      <c r="J9" s="94"/>
+      <c r="I9" s="82"/>
+      <c r="J9" s="96"/>
       <c r="M9" s="26"/>
     </row>
     <row r="10" spans="1:23" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -8601,10 +8601,10 @@
       <c r="H12" s="86" t="s">
         <v>61</v>
       </c>
-      <c r="I12" s="73" t="s">
+      <c r="I12" s="80" t="s">
         <v>62</v>
       </c>
-      <c r="J12" s="92" t="s">
+      <c r="J12" s="94" t="s">
         <v>63</v>
       </c>
     </row>
@@ -8617,8 +8617,8 @@
       </c>
       <c r="G13" s="87"/>
       <c r="H13" s="87"/>
-      <c r="I13" s="74"/>
-      <c r="J13" s="93"/>
+      <c r="I13" s="81"/>
+      <c r="J13" s="95"/>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
@@ -8629,8 +8629,8 @@
       </c>
       <c r="G14" s="87"/>
       <c r="H14" s="87"/>
-      <c r="I14" s="74"/>
-      <c r="J14" s="93"/>
+      <c r="I14" s="81"/>
+      <c r="J14" s="95"/>
     </row>
     <row r="15" spans="1:23" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="43" t="s">
@@ -8645,11 +8645,11 @@
       <c r="H15" s="86" t="s">
         <v>66</v>
       </c>
-      <c r="I15" s="73" t="s">
+      <c r="I15" s="80" t="s">
         <v>65</v>
       </c>
       <c r="J15" s="86"/>
-      <c r="K15" s="95" t="s">
+      <c r="K15" s="89" t="s">
         <v>69</v>
       </c>
       <c r="L15" s="63"/>
@@ -8674,9 +8674,9 @@
       </c>
       <c r="G16" s="87"/>
       <c r="H16" s="87"/>
-      <c r="I16" s="74"/>
+      <c r="I16" s="81"/>
       <c r="J16" s="87"/>
-      <c r="K16" s="95"/>
+      <c r="K16" s="89"/>
       <c r="L16" s="63"/>
       <c r="M16" s="63"/>
       <c r="N16" s="63"/>
@@ -8699,9 +8699,9 @@
       </c>
       <c r="G17" s="88"/>
       <c r="H17" s="88"/>
-      <c r="I17" s="75"/>
+      <c r="I17" s="82"/>
       <c r="J17" s="88"/>
-      <c r="K17" s="95"/>
+      <c r="K17" s="89"/>
       <c r="L17" s="63"/>
       <c r="M17" s="63"/>
       <c r="N17" s="63"/>
@@ -8732,7 +8732,7 @@
         <v>67</v>
       </c>
       <c r="J18" s="3"/>
-      <c r="K18" s="96"/>
+      <c r="K18" s="90"/>
       <c r="L18" s="63"/>
       <c r="M18" s="63"/>
       <c r="N18" s="63"/>
@@ -8883,7 +8883,7 @@
       <c r="V37" s="63"/>
     </row>
     <row r="53" spans="11:22" x14ac:dyDescent="0.25">
-      <c r="K53" s="85" t="s">
+      <c r="K53" s="72" t="s">
         <v>71</v>
       </c>
       <c r="L53" s="63"/>
@@ -8914,11 +8914,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="I15:I17"/>
-    <mergeCell ref="J15:J17"/>
-    <mergeCell ref="L2:W2"/>
-    <mergeCell ref="K15:W18"/>
-    <mergeCell ref="K35:V37"/>
     <mergeCell ref="K53:V54"/>
     <mergeCell ref="G2:G5"/>
     <mergeCell ref="H2:H5"/>
@@ -8934,6 +8929,11 @@
     <mergeCell ref="J12:J14"/>
     <mergeCell ref="G15:G17"/>
     <mergeCell ref="H15:H17"/>
+    <mergeCell ref="I15:I17"/>
+    <mergeCell ref="J15:J17"/>
+    <mergeCell ref="L2:W2"/>
+    <mergeCell ref="K15:W18"/>
+    <mergeCell ref="K35:V37"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="J2" r:id="rId1" xr:uid="{3D14D563-A18C-4362-B2CD-8D8339C1C427}"/>
@@ -9442,13 +9442,13 @@
       <c r="B10" t="s">
         <v>273</v>
       </c>
-      <c r="D10" s="98">
+      <c r="D10" s="101">
         <v>3</v>
       </c>
-      <c r="E10" s="98" t="s">
+      <c r="E10" s="101" t="s">
         <v>125</v>
       </c>
-      <c r="F10" s="101" t="s">
+      <c r="F10" s="98" t="s">
         <v>127</v>
       </c>
       <c r="G10" s="9" t="s">
@@ -9473,9 +9473,9 @@
       <c r="C11" t="s">
         <v>274</v>
       </c>
-      <c r="D11" s="99"/>
-      <c r="E11" s="99"/>
-      <c r="F11" s="102"/>
+      <c r="D11" s="102"/>
+      <c r="E11" s="102"/>
+      <c r="F11" s="99"/>
       <c r="G11" s="9"/>
       <c r="H11" s="3"/>
       <c r="I11" s="1"/>
@@ -9491,9 +9491,9 @@
       <c r="C12" t="s">
         <v>275</v>
       </c>
-      <c r="D12" s="99"/>
-      <c r="E12" s="99"/>
-      <c r="F12" s="102"/>
+      <c r="D12" s="102"/>
+      <c r="E12" s="102"/>
+      <c r="F12" s="99"/>
       <c r="G12" s="9"/>
       <c r="H12" s="3"/>
       <c r="I12" s="1"/>
@@ -9512,9 +9512,9 @@
       <c r="C13" t="s">
         <v>267</v>
       </c>
-      <c r="D13" s="100"/>
-      <c r="E13" s="100"/>
-      <c r="F13" s="103"/>
+      <c r="D13" s="103"/>
+      <c r="E13" s="103"/>
+      <c r="F13" s="100"/>
       <c r="G13" s="9"/>
       <c r="H13" s="3"/>
       <c r="I13" s="1"/>
@@ -9533,7 +9533,7 @@
       <c r="B14" t="s">
         <v>276</v>
       </c>
-      <c r="D14" s="98">
+      <c r="D14" s="101">
         <v>4</v>
       </c>
       <c r="E14" s="86" t="s">
@@ -9564,7 +9564,7 @@
       <c r="C15" t="s">
         <v>277</v>
       </c>
-      <c r="D15" s="99"/>
+      <c r="D15" s="102"/>
       <c r="E15" s="87"/>
       <c r="F15" s="6"/>
       <c r="G15" s="9"/>
@@ -9582,7 +9582,7 @@
       <c r="B16" t="s">
         <v>244</v>
       </c>
-      <c r="D16" s="99"/>
+      <c r="D16" s="102"/>
       <c r="E16" s="87"/>
       <c r="F16" s="6"/>
       <c r="G16" s="9"/>
@@ -9597,7 +9597,7 @@
       <c r="P16" s="1"/>
     </row>
     <row r="17" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D17" s="100"/>
+      <c r="D17" s="103"/>
       <c r="E17" s="88"/>
       <c r="F17" s="6"/>
       <c r="G17" s="9"/>
@@ -9618,7 +9618,7 @@
       <c r="B18" t="s">
         <v>278</v>
       </c>
-      <c r="D18" s="98">
+      <c r="D18" s="101">
         <v>5</v>
       </c>
       <c r="E18" s="86" t="s">
@@ -9649,7 +9649,7 @@
       <c r="C19" t="s">
         <v>279</v>
       </c>
-      <c r="D19" s="99"/>
+      <c r="D19" s="102"/>
       <c r="E19" s="87"/>
       <c r="F19" s="6"/>
       <c r="G19" s="9"/>
@@ -9667,7 +9667,7 @@
       <c r="C20" t="s">
         <v>280</v>
       </c>
-      <c r="D20" s="99"/>
+      <c r="D20" s="102"/>
       <c r="E20" s="87"/>
       <c r="F20" s="6"/>
       <c r="G20" s="9"/>
@@ -9685,7 +9685,7 @@
       <c r="C21" t="s">
         <v>282</v>
       </c>
-      <c r="D21" s="99"/>
+      <c r="D21" s="102"/>
       <c r="E21" s="87"/>
       <c r="F21" s="6"/>
       <c r="G21" s="9"/>
@@ -9703,7 +9703,7 @@
       <c r="C22" t="s">
         <v>283</v>
       </c>
-      <c r="D22" s="99"/>
+      <c r="D22" s="102"/>
       <c r="E22" s="87"/>
       <c r="F22" s="6"/>
       <c r="G22" s="9"/>
@@ -9721,7 +9721,7 @@
       <c r="C23" t="s">
         <v>281</v>
       </c>
-      <c r="D23" s="99"/>
+      <c r="D23" s="102"/>
       <c r="E23" s="87"/>
       <c r="F23" s="6"/>
       <c r="G23" s="9"/>
@@ -9742,7 +9742,7 @@
       <c r="C24" t="s">
         <v>284</v>
       </c>
-      <c r="D24" s="99"/>
+      <c r="D24" s="102"/>
       <c r="E24" s="87"/>
       <c r="F24" s="6"/>
       <c r="G24" s="9"/>
@@ -9760,7 +9760,7 @@
       <c r="C25" t="s">
         <v>285</v>
       </c>
-      <c r="D25" s="100"/>
+      <c r="D25" s="103"/>
       <c r="E25" s="88"/>
       <c r="F25" s="6"/>
       <c r="G25" s="9"/>
@@ -9781,7 +9781,7 @@
       <c r="B26" t="s">
         <v>286</v>
       </c>
-      <c r="D26" s="98">
+      <c r="D26" s="101">
         <v>6</v>
       </c>
       <c r="E26" s="86" t="s">
@@ -9812,7 +9812,7 @@
       <c r="C27" t="s">
         <v>287</v>
       </c>
-      <c r="D27" s="99"/>
+      <c r="D27" s="102"/>
       <c r="E27" s="87"/>
       <c r="F27" s="6"/>
       <c r="G27" s="9"/>
@@ -9830,7 +9830,7 @@
       <c r="C28" t="s">
         <v>288</v>
       </c>
-      <c r="D28" s="99"/>
+      <c r="D28" s="102"/>
       <c r="E28" s="87"/>
       <c r="F28" s="6"/>
       <c r="G28" s="9"/>
@@ -9851,7 +9851,7 @@
       <c r="C29" t="s">
         <v>289</v>
       </c>
-      <c r="D29" s="100"/>
+      <c r="D29" s="103"/>
       <c r="E29" s="88"/>
       <c r="F29" s="6"/>
       <c r="G29" s="9"/>
@@ -10088,10 +10088,10 @@
       <c r="B40" t="s">
         <v>299</v>
       </c>
-      <c r="D40" s="98">
+      <c r="D40" s="101">
         <v>9</v>
       </c>
-      <c r="E40" s="98" t="s">
+      <c r="E40" s="101" t="s">
         <v>138</v>
       </c>
       <c r="F40" s="1" t="s">
@@ -10119,8 +10119,8 @@
       <c r="C41" t="s">
         <v>300</v>
       </c>
-      <c r="D41" s="99"/>
-      <c r="E41" s="99"/>
+      <c r="D41" s="102"/>
+      <c r="E41" s="102"/>
       <c r="F41" s="1"/>
       <c r="G41" s="9"/>
       <c r="H41" s="34"/>
@@ -10140,8 +10140,8 @@
       <c r="C42" t="s">
         <v>298</v>
       </c>
-      <c r="D42" s="100"/>
-      <c r="E42" s="100"/>
+      <c r="D42" s="103"/>
+      <c r="E42" s="103"/>
       <c r="F42" s="1"/>
       <c r="G42" s="9"/>
       <c r="H42" s="34"/>
@@ -10161,7 +10161,7 @@
       <c r="B43" t="s">
         <v>301</v>
       </c>
-      <c r="D43" s="98">
+      <c r="D43" s="101">
         <v>10</v>
       </c>
       <c r="E43" s="86" t="s">
@@ -10192,7 +10192,7 @@
       <c r="C44" t="s">
         <v>302</v>
       </c>
-      <c r="D44" s="99"/>
+      <c r="D44" s="102"/>
       <c r="E44" s="87"/>
       <c r="F44" s="6"/>
       <c r="G44" s="9"/>
@@ -10210,7 +10210,7 @@
       <c r="C45" t="s">
         <v>303</v>
       </c>
-      <c r="D45" s="99"/>
+      <c r="D45" s="102"/>
       <c r="E45" s="87"/>
       <c r="F45" s="6"/>
       <c r="G45" s="9"/>
@@ -10231,7 +10231,7 @@
       <c r="C46" t="s">
         <v>304</v>
       </c>
-      <c r="D46" s="99"/>
+      <c r="D46" s="102"/>
       <c r="E46" s="87"/>
       <c r="F46" s="6"/>
       <c r="G46" s="9"/>
@@ -10249,7 +10249,7 @@
       <c r="C47" t="s">
         <v>298</v>
       </c>
-      <c r="D47" s="100"/>
+      <c r="D47" s="103"/>
       <c r="E47" s="88"/>
       <c r="F47" s="6"/>
       <c r="G47" s="9"/>
@@ -10270,10 +10270,10 @@
       <c r="B48" t="s">
         <v>305</v>
       </c>
-      <c r="D48" s="98">
+      <c r="D48" s="101">
         <v>11</v>
       </c>
-      <c r="E48" s="98" t="s">
+      <c r="E48" s="101" t="s">
         <v>141</v>
       </c>
       <c r="F48" s="4" t="s">
@@ -10301,8 +10301,8 @@
       <c r="C49" t="s">
         <v>306</v>
       </c>
-      <c r="D49" s="99"/>
-      <c r="E49" s="99"/>
+      <c r="D49" s="102"/>
+      <c r="E49" s="102"/>
       <c r="F49" s="4"/>
       <c r="G49" s="9"/>
       <c r="H49" s="31"/>
@@ -10319,8 +10319,8 @@
       <c r="C50" t="s">
         <v>307</v>
       </c>
-      <c r="D50" s="99"/>
-      <c r="E50" s="99"/>
+      <c r="D50" s="102"/>
+      <c r="E50" s="102"/>
       <c r="F50" s="4"/>
       <c r="G50" s="9"/>
       <c r="H50" s="31"/>
@@ -10340,8 +10340,8 @@
       <c r="C51" t="s">
         <v>308</v>
       </c>
-      <c r="D51" s="100"/>
-      <c r="E51" s="100"/>
+      <c r="D51" s="103"/>
+      <c r="E51" s="103"/>
       <c r="F51" s="4"/>
       <c r="G51" s="9"/>
       <c r="H51" s="31"/>
@@ -10361,10 +10361,10 @@
       <c r="B52" t="s">
         <v>309</v>
       </c>
-      <c r="D52" s="98">
+      <c r="D52" s="101">
         <v>12</v>
       </c>
-      <c r="E52" s="98" t="s">
+      <c r="E52" s="101" t="s">
         <v>143</v>
       </c>
       <c r="F52" s="1" t="s">
@@ -10392,8 +10392,8 @@
       <c r="C53" t="s">
         <v>310</v>
       </c>
-      <c r="D53" s="99"/>
-      <c r="E53" s="99"/>
+      <c r="D53" s="102"/>
+      <c r="E53" s="102"/>
       <c r="F53" s="1"/>
       <c r="G53" s="9"/>
       <c r="H53" s="31"/>
@@ -10410,8 +10410,8 @@
       <c r="C54" t="s">
         <v>311</v>
       </c>
-      <c r="D54" s="99"/>
-      <c r="E54" s="99"/>
+      <c r="D54" s="102"/>
+      <c r="E54" s="102"/>
       <c r="F54" s="1"/>
       <c r="G54" s="9"/>
       <c r="H54" s="31"/>
@@ -10431,8 +10431,8 @@
       <c r="C55" t="s">
         <v>312</v>
       </c>
-      <c r="D55" s="99"/>
-      <c r="E55" s="99"/>
+      <c r="D55" s="102"/>
+      <c r="E55" s="102"/>
       <c r="F55" s="1"/>
       <c r="G55" s="9"/>
       <c r="H55" s="31"/>
@@ -10452,7 +10452,7 @@
       <c r="B56" t="s">
         <v>332</v>
       </c>
-      <c r="D56" s="98">
+      <c r="D56" s="101">
         <v>13</v>
       </c>
       <c r="E56" s="86" t="s">
@@ -10480,7 +10480,7 @@
       <c r="B57" t="s">
         <v>213</v>
       </c>
-      <c r="D57" s="99"/>
+      <c r="D57" s="102"/>
       <c r="E57" s="87"/>
       <c r="F57" s="5"/>
       <c r="G57" s="9"/>
@@ -10498,7 +10498,7 @@
       <c r="B58" t="s">
         <v>244</v>
       </c>
-      <c r="D58" s="100"/>
+      <c r="D58" s="103"/>
       <c r="E58" s="88"/>
       <c r="F58" s="5"/>
       <c r="G58" s="9"/>
@@ -10519,7 +10519,7 @@
       <c r="B59" t="s">
         <v>313</v>
       </c>
-      <c r="D59" s="98">
+      <c r="D59" s="101">
         <v>14</v>
       </c>
       <c r="E59" s="86" t="s">
@@ -10550,7 +10550,7 @@
       <c r="C60" t="s">
         <v>314</v>
       </c>
-      <c r="D60" s="99"/>
+      <c r="D60" s="102"/>
       <c r="E60" s="87"/>
       <c r="F60" s="6"/>
       <c r="G60" s="9"/>
@@ -10568,7 +10568,7 @@
       <c r="C61" t="s">
         <v>315</v>
       </c>
-      <c r="D61" s="99"/>
+      <c r="D61" s="102"/>
       <c r="E61" s="87"/>
       <c r="F61" s="6"/>
       <c r="G61" s="9"/>
@@ -10589,7 +10589,7 @@
       <c r="C62" t="s">
         <v>316</v>
       </c>
-      <c r="D62" s="100"/>
+      <c r="D62" s="103"/>
       <c r="E62" s="88"/>
       <c r="F62" s="6"/>
       <c r="G62" s="9"/>
@@ -10610,7 +10610,7 @@
       <c r="B63" t="s">
         <v>317</v>
       </c>
-      <c r="D63" s="98">
+      <c r="D63" s="101">
         <v>15</v>
       </c>
       <c r="E63" s="86" t="s">
@@ -10641,7 +10641,7 @@
       <c r="C64" t="s">
         <v>318</v>
       </c>
-      <c r="D64" s="99"/>
+      <c r="D64" s="102"/>
       <c r="E64" s="87"/>
       <c r="F64" s="5"/>
       <c r="G64" s="9"/>
@@ -10659,7 +10659,7 @@
       <c r="C65" t="s">
         <v>319</v>
       </c>
-      <c r="D65" s="99"/>
+      <c r="D65" s="102"/>
       <c r="E65" s="87"/>
       <c r="F65" s="5"/>
       <c r="G65" s="9"/>
@@ -10680,7 +10680,7 @@
       <c r="C66" t="s">
         <v>320</v>
       </c>
-      <c r="D66" s="99"/>
+      <c r="D66" s="102"/>
       <c r="E66" s="88"/>
       <c r="F66" s="5"/>
       <c r="G66" s="9"/>
@@ -10907,6 +10907,31 @@
     </row>
   </sheetData>
   <mergeCells count="34">
+    <mergeCell ref="D59:D62"/>
+    <mergeCell ref="E59:E62"/>
+    <mergeCell ref="E71:E73"/>
+    <mergeCell ref="D71:D73"/>
+    <mergeCell ref="D63:D66"/>
+    <mergeCell ref="E63:E66"/>
+    <mergeCell ref="E67:E70"/>
+    <mergeCell ref="D56:D58"/>
+    <mergeCell ref="E56:E58"/>
+    <mergeCell ref="D52:D55"/>
+    <mergeCell ref="E52:E55"/>
+    <mergeCell ref="D48:D51"/>
+    <mergeCell ref="E48:E51"/>
+    <mergeCell ref="D43:D47"/>
+    <mergeCell ref="E43:E47"/>
+    <mergeCell ref="D40:D42"/>
+    <mergeCell ref="E40:E42"/>
+    <mergeCell ref="D34:D39"/>
+    <mergeCell ref="E34:E39"/>
+    <mergeCell ref="D30:D33"/>
+    <mergeCell ref="E30:E33"/>
+    <mergeCell ref="D26:D29"/>
+    <mergeCell ref="E26:E29"/>
+    <mergeCell ref="D18:D25"/>
+    <mergeCell ref="E18:E25"/>
     <mergeCell ref="F10:F13"/>
     <mergeCell ref="D2:D5"/>
     <mergeCell ref="E2:E5"/>
@@ -10916,31 +10941,6 @@
     <mergeCell ref="E10:E13"/>
     <mergeCell ref="D6:D9"/>
     <mergeCell ref="E6:E9"/>
-    <mergeCell ref="D30:D33"/>
-    <mergeCell ref="E30:E33"/>
-    <mergeCell ref="D26:D29"/>
-    <mergeCell ref="E26:E29"/>
-    <mergeCell ref="D18:D25"/>
-    <mergeCell ref="E18:E25"/>
-    <mergeCell ref="D43:D47"/>
-    <mergeCell ref="E43:E47"/>
-    <mergeCell ref="D40:D42"/>
-    <mergeCell ref="E40:E42"/>
-    <mergeCell ref="D34:D39"/>
-    <mergeCell ref="E34:E39"/>
-    <mergeCell ref="D56:D58"/>
-    <mergeCell ref="E56:E58"/>
-    <mergeCell ref="D52:D55"/>
-    <mergeCell ref="E52:E55"/>
-    <mergeCell ref="D48:D51"/>
-    <mergeCell ref="E48:E51"/>
-    <mergeCell ref="D59:D62"/>
-    <mergeCell ref="E59:E62"/>
-    <mergeCell ref="E71:E73"/>
-    <mergeCell ref="D71:D73"/>
-    <mergeCell ref="D63:D66"/>
-    <mergeCell ref="E63:E66"/>
-    <mergeCell ref="E67:E70"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="G2" r:id="rId1" xr:uid="{BD266EE8-9EE9-410E-A73B-7BCBE7209954}"/>
@@ -11018,10 +11018,10 @@
       <c r="F2" s="86" t="s">
         <v>171</v>
       </c>
-      <c r="G2" s="73" t="s">
+      <c r="G2" s="80" t="s">
         <v>174</v>
       </c>
-      <c r="H2" s="89" t="s">
+      <c r="H2" s="91" t="s">
         <v>175</v>
       </c>
     </row>
@@ -11038,8 +11038,8 @@
       </c>
       <c r="E3" s="87"/>
       <c r="F3" s="87"/>
-      <c r="G3" s="74"/>
-      <c r="H3" s="90"/>
+      <c r="G3" s="81"/>
+      <c r="H3" s="92"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="42"/>
@@ -11052,8 +11052,8 @@
       </c>
       <c r="E4" s="87"/>
       <c r="F4" s="87"/>
-      <c r="G4" s="74"/>
-      <c r="H4" s="90"/>
+      <c r="G4" s="81"/>
+      <c r="H4" s="92"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="42"/>
@@ -11066,8 +11066,8 @@
       </c>
       <c r="E5" s="88"/>
       <c r="F5" s="88"/>
-      <c r="G5" s="75"/>
-      <c r="H5" s="91"/>
+      <c r="G5" s="82"/>
+      <c r="H5" s="93"/>
     </row>
     <row r="6" spans="1:14" ht="180" x14ac:dyDescent="0.25">
       <c r="A6" s="42" t="s">
@@ -11335,7 +11335,7 @@
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:N53"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" zoomScale="83" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="83" workbookViewId="0">
       <selection activeCell="D58" sqref="D58"/>
     </sheetView>
   </sheetViews>
@@ -11383,7 +11383,7 @@
       <c r="G2" s="86" t="s">
         <v>189</v>
       </c>
-      <c r="H2" s="73" t="s">
+      <c r="H2" s="80" t="s">
         <v>190</v>
       </c>
       <c r="I2" s="37" t="s">
@@ -11404,7 +11404,7 @@
       </c>
       <c r="F3" s="87"/>
       <c r="G3" s="87"/>
-      <c r="H3" s="74"/>
+      <c r="H3" s="81"/>
       <c r="I3" s="37"/>
       <c r="J3" s="14"/>
       <c r="K3" s="14"/>
@@ -11421,7 +11421,7 @@
       </c>
       <c r="F4" s="88"/>
       <c r="G4" s="88"/>
-      <c r="H4" s="75"/>
+      <c r="H4" s="82"/>
       <c r="I4" s="37"/>
       <c r="J4" s="14"/>
       <c r="K4" s="14"/>
@@ -11439,7 +11439,7 @@
       <c r="G5" s="86" t="s">
         <v>191</v>
       </c>
-      <c r="H5" s="104" t="s">
+      <c r="H5" s="106" t="s">
         <v>369</v>
       </c>
       <c r="I5" s="41" t="s">
@@ -11460,7 +11460,7 @@
       </c>
       <c r="F6" s="87"/>
       <c r="G6" s="87"/>
-      <c r="H6" s="105"/>
+      <c r="H6" s="107"/>
       <c r="I6" s="41"/>
       <c r="J6" s="14"/>
       <c r="K6" s="14"/>
@@ -11477,7 +11477,7 @@
       </c>
       <c r="F7" s="87"/>
       <c r="G7" s="87"/>
-      <c r="H7" s="105"/>
+      <c r="H7" s="107"/>
       <c r="I7" s="41"/>
       <c r="J7" s="14"/>
       <c r="K7" s="14"/>
@@ -11494,7 +11494,7 @@
       </c>
       <c r="F8" s="87"/>
       <c r="G8" s="87"/>
-      <c r="H8" s="105"/>
+      <c r="H8" s="107"/>
       <c r="I8" s="41"/>
       <c r="J8" s="14"/>
       <c r="K8" s="14"/>
@@ -11511,7 +11511,7 @@
       </c>
       <c r="F9" s="87"/>
       <c r="G9" s="87"/>
-      <c r="H9" s="106"/>
+      <c r="H9" s="108"/>
       <c r="I9" s="41"/>
       <c r="J9" s="14"/>
       <c r="K9" s="14"/>
@@ -11554,7 +11554,7 @@
       <c r="H11" s="5" t="s">
         <v>195</v>
       </c>
-      <c r="I11" s="107" t="s">
+      <c r="I11" s="104" t="s">
         <v>205</v>
       </c>
       <c r="J11" s="14"/>
@@ -11571,7 +11571,7 @@
       <c r="F12" s="87"/>
       <c r="G12" s="87"/>
       <c r="H12" s="5"/>
-      <c r="I12" s="107"/>
+      <c r="I12" s="104"/>
       <c r="J12" s="14"/>
       <c r="K12" s="14"/>
       <c r="L12" s="14"/>
@@ -11586,7 +11586,7 @@
       <c r="F13" s="87"/>
       <c r="G13" s="88"/>
       <c r="H13" s="5"/>
-      <c r="I13" s="107"/>
+      <c r="I13" s="104"/>
       <c r="J13" s="14"/>
       <c r="K13" s="14"/>
       <c r="L13" s="14"/>
@@ -11607,7 +11607,7 @@
       <c r="H14" s="5" t="s">
         <v>197</v>
       </c>
-      <c r="I14" s="108"/>
+      <c r="I14" s="105"/>
       <c r="J14" s="14"/>
       <c r="K14" s="14"/>
       <c r="L14" s="14"/>
@@ -11622,7 +11622,7 @@
       <c r="F15" s="87"/>
       <c r="G15" s="87"/>
       <c r="H15" s="5"/>
-      <c r="I15" s="108"/>
+      <c r="I15" s="105"/>
       <c r="J15" s="14"/>
       <c r="K15" s="14"/>
       <c r="L15" s="14"/>
@@ -11637,7 +11637,7 @@
       <c r="F16" s="87"/>
       <c r="G16" s="88"/>
       <c r="H16" s="5"/>
-      <c r="I16" s="108"/>
+      <c r="I16" s="105"/>
       <c r="J16" s="14"/>
       <c r="K16" s="14"/>
       <c r="L16" s="14"/>
@@ -11658,7 +11658,7 @@
       <c r="H17" s="5" t="s">
         <v>196</v>
       </c>
-      <c r="I17" s="108"/>
+      <c r="I17" s="105"/>
       <c r="J17" s="14"/>
       <c r="K17" s="14"/>
       <c r="L17" s="14"/>
@@ -11709,7 +11709,7 @@
       <c r="G20" s="86" t="s">
         <v>375</v>
       </c>
-      <c r="H20" s="73" t="s">
+      <c r="H20" s="80" t="s">
         <v>198</v>
       </c>
       <c r="I20" s="37" t="s">
@@ -11731,7 +11731,7 @@
       </c>
       <c r="F21" s="87"/>
       <c r="G21" s="87"/>
-      <c r="H21" s="74"/>
+      <c r="H21" s="81"/>
       <c r="I21" s="37"/>
       <c r="J21" s="14"/>
       <c r="K21" s="14"/>
@@ -11749,7 +11749,7 @@
       </c>
       <c r="F22" s="88"/>
       <c r="G22" s="88"/>
-      <c r="H22" s="75"/>
+      <c r="H22" s="82"/>
       <c r="I22" s="37"/>
       <c r="J22" s="14"/>
       <c r="K22" s="14"/>
@@ -11770,7 +11770,7 @@
       <c r="G23" s="86" t="s">
         <v>199</v>
       </c>
-      <c r="H23" s="73" t="s">
+      <c r="H23" s="80" t="s">
         <v>400</v>
       </c>
       <c r="I23" s="41" t="s">
@@ -11791,7 +11791,7 @@
       </c>
       <c r="F24" s="87"/>
       <c r="G24" s="87"/>
-      <c r="H24" s="74"/>
+      <c r="H24" s="81"/>
       <c r="I24" s="41"/>
       <c r="J24" s="14"/>
       <c r="K24" s="14"/>
@@ -11805,7 +11805,7 @@
       </c>
       <c r="F25" s="87"/>
       <c r="G25" s="87"/>
-      <c r="H25" s="74"/>
+      <c r="H25" s="81"/>
       <c r="I25" s="41"/>
       <c r="J25" s="14"/>
       <c r="K25" s="14"/>
@@ -11819,7 +11819,7 @@
       </c>
       <c r="F26" s="87"/>
       <c r="G26" s="87"/>
-      <c r="H26" s="74"/>
+      <c r="H26" s="81"/>
       <c r="I26" s="41"/>
       <c r="J26" s="14"/>
       <c r="K26" s="14"/>
@@ -11836,7 +11836,7 @@
       </c>
       <c r="F27" s="87"/>
       <c r="G27" s="87"/>
-      <c r="H27" s="74"/>
+      <c r="H27" s="81"/>
       <c r="I27" s="41"/>
       <c r="J27" s="14"/>
       <c r="K27" s="14"/>
@@ -11850,7 +11850,7 @@
       </c>
       <c r="F28" s="87"/>
       <c r="G28" s="87"/>
-      <c r="H28" s="74"/>
+      <c r="H28" s="81"/>
       <c r="I28" s="41"/>
       <c r="J28" s="14"/>
       <c r="K28" s="14"/>
@@ -11867,7 +11867,7 @@
       </c>
       <c r="F29" s="87"/>
       <c r="G29" s="87"/>
-      <c r="H29" s="74"/>
+      <c r="H29" s="81"/>
       <c r="I29" s="41"/>
       <c r="J29" s="14"/>
       <c r="K29" s="14"/>
@@ -11884,7 +11884,7 @@
       </c>
       <c r="F30" s="87"/>
       <c r="G30" s="87"/>
-      <c r="H30" s="74"/>
+      <c r="H30" s="81"/>
       <c r="I30" s="41"/>
       <c r="J30" s="14"/>
       <c r="K30" s="14"/>
@@ -11901,7 +11901,7 @@
       </c>
       <c r="F31" s="87"/>
       <c r="G31" s="87"/>
-      <c r="H31" s="74"/>
+      <c r="H31" s="81"/>
       <c r="I31" s="41"/>
       <c r="J31" s="14"/>
       <c r="K31" s="14"/>
@@ -11916,7 +11916,7 @@
       </c>
       <c r="F32" s="87"/>
       <c r="G32" s="87"/>
-      <c r="H32" s="74"/>
+      <c r="H32" s="81"/>
       <c r="I32" s="41"/>
       <c r="J32" s="14"/>
       <c r="K32" s="14"/>
@@ -11933,7 +11933,7 @@
       </c>
       <c r="F33" s="87"/>
       <c r="G33" s="87"/>
-      <c r="H33" s="74"/>
+      <c r="H33" s="81"/>
       <c r="I33" s="41"/>
       <c r="J33" s="14"/>
       <c r="K33" s="14"/>
@@ -11947,7 +11947,7 @@
       </c>
       <c r="F34" s="87"/>
       <c r="G34" s="87"/>
-      <c r="H34" s="74"/>
+      <c r="H34" s="81"/>
       <c r="I34" s="41"/>
       <c r="J34" s="14"/>
       <c r="K34" s="14"/>
@@ -11964,7 +11964,7 @@
       </c>
       <c r="F35" s="87"/>
       <c r="G35" s="87"/>
-      <c r="H35" s="74"/>
+      <c r="H35" s="81"/>
       <c r="I35" s="41"/>
       <c r="J35" s="14"/>
       <c r="K35" s="14"/>
@@ -11978,7 +11978,7 @@
       </c>
       <c r="F36" s="87"/>
       <c r="G36" s="87"/>
-      <c r="H36" s="74"/>
+      <c r="H36" s="81"/>
       <c r="I36" s="41"/>
       <c r="J36" s="14"/>
       <c r="K36" s="14"/>
@@ -11995,7 +11995,7 @@
       </c>
       <c r="F37" s="87"/>
       <c r="G37" s="87"/>
-      <c r="H37" s="74"/>
+      <c r="H37" s="81"/>
       <c r="I37" s="41"/>
       <c r="J37" s="14"/>
       <c r="K37" s="14"/>
@@ -12009,7 +12009,7 @@
       </c>
       <c r="F38" s="87"/>
       <c r="G38" s="87"/>
-      <c r="H38" s="74"/>
+      <c r="H38" s="81"/>
       <c r="I38" s="41"/>
       <c r="J38" s="14"/>
       <c r="K38" s="14"/>
@@ -12026,7 +12026,7 @@
       </c>
       <c r="F39" s="87"/>
       <c r="G39" s="87"/>
-      <c r="H39" s="74"/>
+      <c r="H39" s="81"/>
       <c r="I39" s="41"/>
       <c r="J39" s="14"/>
       <c r="K39" s="14"/>
@@ -12040,7 +12040,7 @@
       </c>
       <c r="F40" s="88"/>
       <c r="G40" s="88"/>
-      <c r="H40" s="75"/>
+      <c r="H40" s="82"/>
       <c r="I40" s="41"/>
       <c r="J40" s="14"/>
       <c r="K40" s="14"/>
@@ -12080,16 +12080,16 @@
       <c r="C42" t="s">
         <v>394</v>
       </c>
-      <c r="F42" s="66">
+      <c r="F42" s="73">
         <v>5</v>
       </c>
-      <c r="G42" s="66" t="s">
+      <c r="G42" s="73" t="s">
         <v>206</v>
       </c>
       <c r="H42" s="5" t="s">
         <v>207</v>
       </c>
-      <c r="I42" s="70" t="s">
+      <c r="I42" s="77" t="s">
         <v>202</v>
       </c>
       <c r="J42" s="14"/>
@@ -12108,12 +12108,12 @@
       <c r="E43" t="s">
         <v>398</v>
       </c>
-      <c r="F43" s="66"/>
-      <c r="G43" s="66"/>
+      <c r="F43" s="73"/>
+      <c r="G43" s="73"/>
       <c r="H43" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="I43" s="71"/>
+      <c r="I43" s="78"/>
       <c r="J43" s="14"/>
       <c r="K43" s="14"/>
       <c r="L43" s="14"/>
@@ -12127,12 +12127,12 @@
       <c r="E44" t="s">
         <v>399</v>
       </c>
-      <c r="F44" s="66"/>
-      <c r="G44" s="66"/>
+      <c r="F44" s="73"/>
+      <c r="G44" s="73"/>
       <c r="H44" s="3" t="s">
         <v>209</v>
       </c>
-      <c r="I44" s="72"/>
+      <c r="I44" s="79"/>
       <c r="J44" s="14"/>
       <c r="K44" s="14"/>
       <c r="L44" s="14"/>
@@ -12177,6 +12177,19 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="F5:F22"/>
+    <mergeCell ref="G11:G13"/>
+    <mergeCell ref="G14:G16"/>
+    <mergeCell ref="G17:G19"/>
+    <mergeCell ref="G20:G22"/>
+    <mergeCell ref="F2:F4"/>
+    <mergeCell ref="G2:G4"/>
+    <mergeCell ref="H2:H4"/>
+    <mergeCell ref="H5:H9"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="G5:G10"/>
     <mergeCell ref="I11:I17"/>
     <mergeCell ref="G42:G44"/>
     <mergeCell ref="F42:F44"/>
@@ -12185,19 +12198,6 @@
     <mergeCell ref="F23:F40"/>
     <mergeCell ref="G23:G40"/>
     <mergeCell ref="H23:H40"/>
-    <mergeCell ref="F2:F4"/>
-    <mergeCell ref="G2:G4"/>
-    <mergeCell ref="H2:H4"/>
-    <mergeCell ref="H5:H9"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="G5:G10"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="F5:F22"/>
-    <mergeCell ref="G11:G13"/>
-    <mergeCell ref="G14:G16"/>
-    <mergeCell ref="G17:G19"/>
-    <mergeCell ref="G20:G22"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="I23" r:id="rId1" display="https://www.baeldung.com/spring-transactional-propagation-isolation" xr:uid="{48BFAE5D-1145-4E0D-A5BD-44A48408A956}"/>

</xml_diff>